<commit_message>
adjusting and adding maps
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BD06B0-BA63-D442-9363-310A34C268C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C231B-3F9E-C34E-9589-0DA66E543166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -60,12 +60,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Longitude </t>
-  </si>
-  <si>
-    <t>Latitude </t>
-  </si>
-  <si>
     <t>Office Location( Which town, if no physical office address then "Online")</t>
   </si>
   <si>
@@ -1023,6 +1017,12 @@
   </si>
   <si>
     <t xml:space="preserve">Transportation </t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
   </si>
 </sst>
 </file>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1452,45 +1452,45 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="I2" s="1">
         <v>38.840490000000003</v>
@@ -1499,39 +1499,39 @@
         <v>-77.115129999999994</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="I3" s="1">
         <v>37.538339999999998</v>
@@ -1540,37 +1540,37 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1">
         <v>37.538339999999998</v>
@@ -1579,39 +1579,39 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I5" s="1">
         <v>39.031359999999999</v>
@@ -1620,39 +1620,39 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="I6" s="1">
         <v>39.015009999999997</v>
@@ -1661,39 +1661,39 @@
         <v>-77.400989999999993</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="I7" s="1">
         <v>39.031359999999999</v>
@@ -1702,39 +1702,39 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -1743,39 +1743,39 @@
         <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" s="1">
         <v>39.031359999999999</v>
@@ -1784,37 +1784,37 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I10" s="1">
         <v>39.114306589999998</v>
@@ -1823,39 +1823,39 @@
         <v>-77.539617179999993</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="I11" s="1">
         <v>39.114306589999998</v>
@@ -1864,39 +1864,39 @@
         <v>-77.539617179999993</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="I12" s="1">
         <v>38.917318170000001</v>
@@ -1905,33 +1905,33 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1941,22 +1941,22 @@
     </row>
     <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1966,28 +1966,28 @@
     </row>
     <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I15" s="1">
         <v>39.084557510000003</v>
@@ -1996,39 +1996,39 @@
         <v>-77.555403999999996</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="I16" s="1">
         <v>37.61065696</v>
@@ -2037,39 +2037,39 @@
         <v>-77.340073020000005</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="I17" s="1">
         <v>39.114571660000003</v>
@@ -2078,39 +2078,39 @@
         <v>-77.540547570000001</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -2119,39 +2119,39 @@
         <v>0</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -2160,39 +2160,39 @@
         <v>0</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -2201,39 +2201,39 @@
         <v>0</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -2242,39 +2242,39 @@
         <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -2283,39 +2283,39 @@
         <v>0</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -2324,37 +2324,37 @@
         <v>0</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="I24" s="1">
         <v>40.439188049999998</v>
@@ -2363,39 +2363,39 @@
         <v>-80.001456360000006</v>
       </c>
       <c r="K24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="I25" s="1">
         <v>40.437306100000001</v>
@@ -2404,39 +2404,39 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="I26" s="1">
         <v>40.349269890000002</v>
@@ -2445,39 +2445,39 @@
         <v>-79.832162819999994</v>
       </c>
       <c r="K26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M26" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="I27" s="1">
         <v>40.439132790000002</v>
@@ -2486,78 +2486,78 @@
         <v>-79.994721900000002</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I29" s="1">
         <v>40.40062056</v>
@@ -2566,39 +2566,39 @@
         <v>-79.8352431</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I30" s="1">
         <v>40.40062056</v>
@@ -2607,36 +2607,36 @@
         <v>-79.8352431</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1">
@@ -2646,70 +2646,70 @@
         <v>-79.8352431</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -2719,45 +2719,45 @@
     </row>
     <row r="34" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2768,21 +2768,21 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2793,118 +2793,118 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M39" s="1"/>
     </row>
     <row r="40" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I40" s="1">
         <v>39.114409999999999</v>
@@ -2913,39 +2913,39 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="I41" s="1">
         <v>39.114409999999999</v>
@@ -2954,80 +2954,80 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="I42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="M42" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="I43" s="1">
         <v>39.076819999999998</v>
@@ -3036,39 +3036,39 @@
         <v>-77.549896000000004</v>
       </c>
       <c r="K43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M43" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="I44" s="1">
         <v>39.114409999999999</v>
@@ -3077,39 +3077,39 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="K44" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M44" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="I45" s="1">
         <v>39.115279999999998</v>
@@ -3118,39 +3118,39 @@
         <v>-77.564430000000002</v>
       </c>
       <c r="K45" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="I46" s="1">
         <v>40.741895</v>
@@ -3159,78 +3159,78 @@
         <v>-73.989307999999994</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="F48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="I48" s="1">
         <v>39.108399900000002</v>
@@ -3239,39 +3239,39 @@
         <v>-77.565337</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="F49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="I49" s="1">
         <v>39.114409999999999</v>
@@ -3280,39 +3280,39 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="I50" s="1">
         <v>39.115943000000001</v>
@@ -3321,39 +3321,39 @@
         <v>-77.581795999999997</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="I51" s="1">
         <v>39.114406199999998</v>
@@ -3362,39 +3362,39 @@
         <v>-77.567706299999998</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="I52" s="1">
         <v>37.542472099999998</v>
@@ -3403,39 +3403,39 @@
         <v>-77.435912200000004</v>
       </c>
       <c r="K52" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M52" s="2" t="s">
+      <c r="D53" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="I53" s="1">
         <v>39.117853099999998</v>
@@ -3444,39 +3444,39 @@
         <v>-77.568151900000004</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="I54" s="1">
         <v>37.610656959136698</v>
@@ -3485,119 +3485,119 @@
         <v>-77.340073015724201</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G55" s="1" t="s">
+      <c r="I55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="M55" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="I56" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="I57" s="1">
         <v>40.439779999999999</v>
@@ -3606,240 +3606,240 @@
         <v>-79.998869999999997</v>
       </c>
       <c r="K57" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="M57" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G58" s="1" t="s">
+      <c r="I58" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L58" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="M58" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="M59" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="I60" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G61" s="1" t="s">
+      <c r="I61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="M61" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="I63" s="1">
         <v>40.407960000000003</v>
@@ -3848,39 +3848,39 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K63" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="M63" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>306</v>
       </c>
       <c r="I64" s="1">
         <v>40.405259100000002</v>
@@ -3889,39 +3889,39 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K64" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="M64" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="I65" s="1">
         <v>40.559510000000003</v>
@@ -3930,30 +3930,30 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K65" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="M65" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="L65" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="M65" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3966,19 +3966,19 @@
     </row>
     <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3991,19 +3991,19 @@
     </row>
     <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -4016,19 +4016,19 @@
     </row>
     <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -4041,19 +4041,19 @@
     </row>
     <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -4066,19 +4066,19 @@
     </row>
     <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -4091,19 +4091,19 @@
     </row>
     <row r="72" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -4116,19 +4116,19 @@
     </row>
     <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -4141,19 +4141,19 @@
     </row>
     <row r="74" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>

</xml_diff>

<commit_message>
added maps into ShinyApp
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C231B-3F9E-C34E-9589-0DA66E543166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB700AB2-DBA4-9948-8FC2-F389AB299CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Sources (Stakeholders) If we are going to ask for administrative data, who are we going to ask for data?</t>
   </si>
   <si>
-    <t>Links of programs</t>
-  </si>
-  <si>
     <t>Loudoun</t>
   </si>
   <si>
@@ -1023,6 +1020,9 @@
   </si>
   <si>
     <t>Latitude</t>
+  </si>
+  <si>
+    <t>Website</t>
   </si>
 </sst>
 </file>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1452,10 +1452,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1464,33 +1464,33 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="1">
         <v>38.840490000000003</v>
@@ -1499,39 +1499,39 @@
         <v>-77.115129999999994</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="I3" s="1">
         <v>37.538339999999998</v>
@@ -1540,37 +1540,37 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1">
         <v>37.538339999999998</v>
@@ -1579,39 +1579,39 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="I5" s="1">
         <v>39.031359999999999</v>
@@ -1620,39 +1620,39 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="I6" s="1">
         <v>39.015009999999997</v>
@@ -1661,39 +1661,39 @@
         <v>-77.400989999999993</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="I7" s="1">
         <v>39.031359999999999</v>
@@ -1702,39 +1702,39 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -1743,39 +1743,39 @@
         <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="I9" s="1">
         <v>39.031359999999999</v>
@@ -1784,37 +1784,37 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="I10" s="1">
         <v>39.114306589999998</v>
@@ -1823,39 +1823,39 @@
         <v>-77.539617179999993</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="I11" s="1">
         <v>39.114306589999998</v>
@@ -1864,39 +1864,39 @@
         <v>-77.539617179999993</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I12" s="1">
         <v>38.917318170000001</v>
@@ -1905,33 +1905,33 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1941,22 +1941,22 @@
     </row>
     <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1966,28 +1966,28 @@
     </row>
     <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="I15" s="1">
         <v>39.084557510000003</v>
@@ -1996,39 +1996,39 @@
         <v>-77.555403999999996</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="I16" s="1">
         <v>37.61065696</v>
@@ -2037,39 +2037,39 @@
         <v>-77.340073020000005</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="I17" s="1">
         <v>39.114571660000003</v>
@@ -2078,39 +2078,39 @@
         <v>-77.540547570000001</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -2119,39 +2119,39 @@
         <v>0</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -2160,39 +2160,39 @@
         <v>0</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -2201,39 +2201,39 @@
         <v>0</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -2242,39 +2242,39 @@
         <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -2283,39 +2283,39 @@
         <v>0</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -2324,37 +2324,37 @@
         <v>0</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="I24" s="1">
         <v>40.439188049999998</v>
@@ -2363,39 +2363,39 @@
         <v>-80.001456360000006</v>
       </c>
       <c r="K24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="I25" s="1">
         <v>40.437306100000001</v>
@@ -2404,39 +2404,39 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="M25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="I26" s="1">
         <v>40.349269890000002</v>
@@ -2445,39 +2445,39 @@
         <v>-79.832162819999994</v>
       </c>
       <c r="K26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="I27" s="1">
         <v>40.439132790000002</v>
@@ -2486,78 +2486,78 @@
         <v>-79.994721900000002</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="I29" s="1">
         <v>40.40062056</v>
@@ -2566,39 +2566,39 @@
         <v>-79.8352431</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="I30" s="1">
         <v>40.40062056</v>
@@ -2607,36 +2607,36 @@
         <v>-79.8352431</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1">
@@ -2646,70 +2646,70 @@
         <v>-79.8352431</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M31" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -2719,45 +2719,45 @@
     </row>
     <row r="34" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2768,21 +2768,21 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2793,118 +2793,118 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M39" s="1"/>
     </row>
     <row r="40" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="I40" s="1">
         <v>39.114409999999999</v>
@@ -2913,39 +2913,39 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L40" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M40" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="I41" s="1">
         <v>39.114409999999999</v>
@@ -2954,80 +2954,80 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L42" s="1" t="s">
+      <c r="M42" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="I43" s="1">
         <v>39.076819999999998</v>
@@ -3036,39 +3036,39 @@
         <v>-77.549896000000004</v>
       </c>
       <c r="K43" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="M43" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="I44" s="1">
         <v>39.114409999999999</v>
@@ -3077,39 +3077,39 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="K44" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="I45" s="1">
         <v>39.115279999999998</v>
@@ -3118,39 +3118,39 @@
         <v>-77.564430000000002</v>
       </c>
       <c r="K45" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="I46" s="1">
         <v>40.741895</v>
@@ -3159,78 +3159,78 @@
         <v>-73.989307999999994</v>
       </c>
       <c r="K46" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L46" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="M46" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="I47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L47" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M47" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="I48" s="1">
         <v>39.108399900000002</v>
@@ -3239,39 +3239,39 @@
         <v>-77.565337</v>
       </c>
       <c r="K48" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="M48" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="I49" s="1">
         <v>39.114409999999999</v>
@@ -3280,39 +3280,39 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L49" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M49" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C50" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="I50" s="1">
         <v>39.115943000000001</v>
@@ -3321,39 +3321,39 @@
         <v>-77.581795999999997</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L50" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="M50" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C51" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="I51" s="1">
         <v>39.114406199999998</v>
@@ -3362,39 +3362,39 @@
         <v>-77.567706299999998</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="I52" s="1">
         <v>37.542472099999998</v>
@@ -3403,39 +3403,39 @@
         <v>-77.435912200000004</v>
       </c>
       <c r="K52" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M52" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="I53" s="1">
         <v>39.117853099999998</v>
@@ -3444,39 +3444,39 @@
         <v>-77.568151900000004</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L53" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="M53" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="I54" s="1">
         <v>37.610656959136698</v>
@@ -3485,119 +3485,119 @@
         <v>-77.340073015724201</v>
       </c>
       <c r="K54" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M54" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="I55" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="L55" s="1" t="s">
+      <c r="M55" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="I56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L56" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="M56" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="I57" s="1">
         <v>40.439779999999999</v>
@@ -3606,240 +3606,240 @@
         <v>-79.998869999999997</v>
       </c>
       <c r="K57" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="L57" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="L57" s="1" t="s">
+      <c r="M57" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G58" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="I58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L58" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I58" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L58" s="1" t="s">
+      <c r="M58" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H59" s="1" t="s">
+      <c r="I59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M59" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="I60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G61" s="1" t="s">
+      <c r="H61" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="I61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M61" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="G63" s="1" t="s">
+      <c r="H63" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="I63" s="1">
         <v>40.407960000000003</v>
@@ -3848,39 +3848,39 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K63" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="L63" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="L63" s="1" t="s">
+      <c r="M63" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="I64" s="1">
         <v>40.405259100000002</v>
@@ -3889,39 +3889,39 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K64" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="L64" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="L64" s="1" t="s">
+      <c r="M64" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="H65" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="I65" s="1">
         <v>40.559510000000003</v>
@@ -3930,30 +3930,30 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K65" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="L65" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="L65" s="1" t="s">
+      <c r="M65" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="M65" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3966,19 +3966,19 @@
     </row>
     <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3991,19 +3991,19 @@
     </row>
     <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -4016,19 +4016,19 @@
     </row>
     <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -4041,19 +4041,19 @@
     </row>
     <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -4066,19 +4066,19 @@
     </row>
     <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -4091,19 +4091,19 @@
     </row>
     <row r="72" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -4116,19 +4116,19 @@
     </row>
     <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -4141,19 +4141,19 @@
     </row>
     <row r="74" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>

</xml_diff>

<commit_message>
Added missing info and homeless shelter centers on combined-programs list
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB700AB2-DBA4-9948-8FC2-F389AB299CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7936536-4743-42BA-AB02-93378B200A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="367">
   <si>
     <t>County</t>
   </si>
@@ -1023,13 +1023,131 @@
   </si>
   <si>
     <t>Website</t>
+  </si>
+  <si>
+    <t>Loudoun Homeless Services Center</t>
+  </si>
+  <si>
+    <t>Those who are currently or are at risk of experiencing homelessness</t>
+  </si>
+  <si>
+    <t>provides extensive services to prevent, support and help end homelessness within Loudoun and surrounding counties</t>
+  </si>
+  <si>
+    <t>https://www.voachesapeake.org/lhsc</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/WorkArea/linkit.aspx?LinkIdentifier=id&amp;ItemID=2147486416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegheny County Office of Behavioral Health </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free psychiatric prescription medication </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegheny Couny residents who are or have applied to receive medicaid/third-party prescription coverage and make an adusted income of $500 dollars or less </t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Erie, PA</t>
+  </si>
+  <si>
+    <t>A collection of programs available to Pennsylvania residents who recieve medicaid.</t>
+  </si>
+  <si>
+    <t>http://matp.pa.gov/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Human Services </t>
+  </si>
+  <si>
+    <t>Allegheny County PA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online </t>
+  </si>
+  <si>
+    <t>provides transportation to medical appointments for Medical Assistance recipients who do not have transportation available to them.</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>PortAuthority.org</t>
+  </si>
+  <si>
+    <t>Public transit agency in Alleghany Count</t>
+  </si>
+  <si>
+    <t>https://www.ccac.edu/academics/apprenticeship.php</t>
+  </si>
+  <si>
+    <t> Community College of Allegheny County.</t>
+  </si>
+  <si>
+    <t>career services program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education </t>
+  </si>
+  <si>
+    <t>https://www.ccac.edu/academics/free-and-subsidized.php</t>
+  </si>
+  <si>
+    <t>KEYS is for Temporary Assistance for Needy Families (TANF) cash assistance and some SNAP recipients in Pennsylvania.</t>
+  </si>
+  <si>
+    <t>https://www.ccac.edu/admissions/ged.php</t>
+  </si>
+  <si>
+    <t>Community College of Allegheny County</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awards commonwealth secondary school diplomas </t>
+  </si>
+  <si>
+    <t>Those who do not possess secondary diplomas after successful completion of 30-credit hours in relevant courses.</t>
+  </si>
+  <si>
+    <t>https://www.ccac.edu/workforce/index.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programs designed to provide skills and knowledge needed to remain competitive in a variety of industries.
+</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Resources/Education/DHS-Methods.aspx</t>
+  </si>
+  <si>
+    <t>Individualized support for youth with educational barriers. The Liaison works within the framework of the Department of Human Services to coordinate continued education opportunities.</t>
+  </si>
+  <si>
+    <t>Allegheny County youth with educational barriers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Shepherd Alliance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-profit that offers homeless services and shelters </t>
+  </si>
+  <si>
+    <t>Ahsburn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Sheppard Alliance </t>
+  </si>
+  <si>
+    <t>https://goodshepherdalliance.org/who-we-are/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1056,6 +1174,29 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1078,7 +1219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1088,6 +1229,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1404,13 +1559,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
@@ -1418,7 +1573,7 @@
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
     <col min="7" max="7" width="65.6640625" customWidth="1"/>
-    <col min="8" max="8" width="83.1640625" customWidth="1"/>
+    <col min="8" max="8" width="83.33203125" style="7" customWidth="1"/>
     <col min="9" max="9" width="16.5" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" customWidth="1"/>
     <col min="11" max="11" width="51.5" customWidth="1"/>
@@ -1426,7 +1581,7 @@
     <col min="13" max="13" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1603,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1467,7 +1622,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1489,7 +1644,7 @@
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1">
@@ -1508,7 +1663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1530,7 +1685,7 @@
       <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="1">
@@ -1549,7 +1704,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1724,7 @@
         <v>29</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="1">
@@ -1588,7 +1743,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1610,7 +1765,7 @@
       <c r="G5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="1">
@@ -1629,7 +1784,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1651,7 +1806,7 @@
       <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="5" t="s">
         <v>42</v>
       </c>
       <c r="I6" s="1">
@@ -1670,7 +1825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1692,7 +1847,7 @@
       <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="5" t="s">
         <v>46</v>
       </c>
       <c r="I7" s="1">
@@ -1711,7 +1866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1733,7 +1888,7 @@
       <c r="G8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="5" t="s">
         <v>48</v>
       </c>
       <c r="I8" s="1">
@@ -1752,7 +1907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1774,7 +1929,7 @@
       <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I9" s="1">
@@ -1793,7 +1948,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1813,7 +1968,7 @@
       <c r="G10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="5" t="s">
         <v>55</v>
       </c>
       <c r="I10" s="1">
@@ -1832,7 +1987,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1854,7 +2009,7 @@
       <c r="G11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="5" t="s">
         <v>62</v>
       </c>
       <c r="I11" s="1">
@@ -1873,7 +2028,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1895,7 +2050,7 @@
       <c r="G12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="5" t="s">
         <v>67</v>
       </c>
       <c r="I12" s="1">
@@ -1914,7 +2069,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1930,7 +2085,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="5" t="s">
         <v>71</v>
       </c>
       <c r="I13" s="1"/>
@@ -1939,7 +2094,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1955,7 +2110,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I14" s="1"/>
@@ -1964,7 +2119,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1986,7 +2141,7 @@
       <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I15" s="1">
@@ -2005,7 +2160,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2182,7 @@
       <c r="G16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I16" s="1">
@@ -2046,7 +2201,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -2068,7 +2223,7 @@
       <c r="G17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="5" t="s">
         <v>86</v>
       </c>
       <c r="I17" s="1">
@@ -2087,7 +2242,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -2109,7 +2264,7 @@
       <c r="G18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="5" t="s">
         <v>92</v>
       </c>
       <c r="I18" s="1">
@@ -2128,7 +2283,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -2150,7 +2305,7 @@
       <c r="G19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="5" t="s">
         <v>98</v>
       </c>
       <c r="I19" s="1">
@@ -2169,7 +2324,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -2191,7 +2346,7 @@
       <c r="G20" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="5" t="s">
         <v>102</v>
       </c>
       <c r="I20" s="1">
@@ -2210,7 +2365,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -2232,7 +2387,7 @@
       <c r="G21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="5" t="s">
         <v>106</v>
       </c>
       <c r="I21" s="1">
@@ -2251,7 +2406,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -2273,7 +2428,7 @@
       <c r="G22" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="5" t="s">
         <v>111</v>
       </c>
       <c r="I22" s="1">
@@ -2292,7 +2447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -2314,7 +2469,7 @@
       <c r="G23" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="5" t="s">
         <v>114</v>
       </c>
       <c r="I23" s="1">
@@ -2331,7 +2486,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>264</v>
       </c>
@@ -2353,7 +2508,7 @@
       <c r="G24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="5" t="s">
         <v>119</v>
       </c>
       <c r="I24" s="1">
@@ -2372,7 +2527,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>264</v>
       </c>
@@ -2394,7 +2549,7 @@
       <c r="G25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="5" t="s">
         <v>126</v>
       </c>
       <c r="I25" s="1">
@@ -2413,7 +2568,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>264</v>
       </c>
@@ -2435,7 +2590,7 @@
       <c r="G26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="5" t="s">
         <v>131</v>
       </c>
       <c r="I26" s="1">
@@ -2454,7 +2609,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>264</v>
       </c>
@@ -2476,7 +2631,7 @@
       <c r="G27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="5" t="s">
         <v>137</v>
       </c>
       <c r="I27" s="1">
@@ -2495,7 +2650,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>264</v>
       </c>
@@ -2517,7 +2672,7 @@
       <c r="G28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="5" t="s">
         <v>143</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2534,7 +2689,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>264</v>
       </c>
@@ -2556,7 +2711,7 @@
       <c r="G29" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="5" t="s">
         <v>149</v>
       </c>
       <c r="I29" s="1">
@@ -2575,7 +2730,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>264</v>
       </c>
@@ -2597,7 +2752,7 @@
       <c r="G30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="5" t="s">
         <v>153</v>
       </c>
       <c r="I30" s="1">
@@ -2616,7 +2771,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>264</v>
       </c>
@@ -2638,7 +2793,7 @@
       <c r="G31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="5"/>
       <c r="I31" s="1">
         <v>40.40062056</v>
       </c>
@@ -2655,7 +2810,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>264</v>
       </c>
@@ -2677,7 +2832,7 @@
       <c r="G32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="5" t="s">
         <v>158</v>
       </c>
       <c r="I32" s="1"/>
@@ -2688,7 +2843,7 @@
       </c>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>264</v>
       </c>
@@ -2708,7 +2863,7 @@
       <c r="G33" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" s="5" t="s">
         <v>162</v>
       </c>
       <c r="I33" s="1"/>
@@ -2717,7 +2872,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>264</v>
       </c>
@@ -2735,7 +2890,7 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="5" t="s">
         <v>164</v>
       </c>
       <c r="I34" s="1"/>
@@ -2746,7 +2901,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>264</v>
       </c>
@@ -2762,7 +2917,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="5"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2771,7 +2926,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>264</v>
       </c>
@@ -2787,7 +2942,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2796,7 +2951,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>264</v>
       </c>
@@ -2812,7 +2967,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="5" t="s">
         <v>172</v>
       </c>
       <c r="I37" s="1"/>
@@ -2823,7 +2978,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>264</v>
       </c>
@@ -2841,7 +2996,7 @@
       <c r="G38" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="5" t="s">
         <v>175</v>
       </c>
       <c r="I38" s="1"/>
@@ -2852,7 +3007,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>264</v>
       </c>
@@ -2870,7 +3025,7 @@
       <c r="G39" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="5" t="s">
         <v>177</v>
       </c>
       <c r="I39" s="1"/>
@@ -2881,7 +3036,7 @@
       </c>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -2903,7 +3058,7 @@
       <c r="G40" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="5" t="s">
         <v>182</v>
       </c>
       <c r="I40" s="1">
@@ -2922,7 +3077,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -2944,7 +3099,7 @@
       <c r="G41" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="5" t="s">
         <v>188</v>
       </c>
       <c r="I41" s="1">
@@ -2963,7 +3118,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -2985,7 +3140,7 @@
       <c r="G42" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="5" t="s">
         <v>193</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -3004,7 +3159,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -3026,7 +3181,7 @@
       <c r="G43" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="5" t="s">
         <v>198</v>
       </c>
       <c r="I43" s="1">
@@ -3045,7 +3200,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -3067,7 +3222,7 @@
       <c r="G44" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="5" t="s">
         <v>204</v>
       </c>
       <c r="I44" s="1">
@@ -3086,7 +3241,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -3108,7 +3263,7 @@
       <c r="G45" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="5" t="s">
         <v>211</v>
       </c>
       <c r="I45" s="1">
@@ -3127,7 +3282,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -3149,7 +3304,7 @@
       <c r="G46" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" s="5" t="s">
         <v>217</v>
       </c>
       <c r="I46" s="1">
@@ -3168,7 +3323,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -3190,7 +3345,7 @@
       <c r="G47" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="5" t="s">
         <v>220</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3207,7 +3362,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>223</v>
       </c>
@@ -3229,7 +3384,7 @@
       <c r="G48" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="5" t="s">
         <v>227</v>
       </c>
       <c r="I48" s="1">
@@ -3248,7 +3403,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>223</v>
       </c>
@@ -3270,7 +3425,7 @@
       <c r="G49" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" s="5" t="s">
         <v>232</v>
       </c>
       <c r="I49" s="1">
@@ -3289,7 +3444,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
@@ -3311,7 +3466,7 @@
       <c r="G50" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" s="5" t="s">
         <v>237</v>
       </c>
       <c r="I50" s="1">
@@ -3330,7 +3485,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
@@ -3352,7 +3507,7 @@
       <c r="G51" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H51" s="5" t="s">
         <v>242</v>
       </c>
       <c r="I51" s="1">
@@ -3371,7 +3526,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
@@ -3393,7 +3548,7 @@
       <c r="G52" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H52" s="5" t="s">
         <v>246</v>
       </c>
       <c r="I52" s="1">
@@ -3412,7 +3567,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
@@ -3434,7 +3589,7 @@
       <c r="G53" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="H53" s="5" t="s">
         <v>251</v>
       </c>
       <c r="I53" s="1">
@@ -3453,7 +3608,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
@@ -3475,7 +3630,7 @@
       <c r="G54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="5" t="s">
         <v>256</v>
       </c>
       <c r="I54" s="1">
@@ -3494,7 +3649,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
@@ -3516,7 +3671,7 @@
       <c r="G55" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" s="5" t="s">
         <v>261</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -3535,7 +3690,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>264</v>
       </c>
@@ -3557,7 +3712,7 @@
       <c r="G56" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="5" t="s">
         <v>267</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -3574,7 +3729,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>264</v>
       </c>
@@ -3596,7 +3751,7 @@
       <c r="G57" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="H57" s="5" t="s">
         <v>272</v>
       </c>
       <c r="I57" s="1">
@@ -3615,7 +3770,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>264</v>
       </c>
@@ -3637,7 +3792,7 @@
       <c r="G58" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="H58" s="5" t="s">
         <v>278</v>
       </c>
       <c r="I58" s="1" t="s">
@@ -3656,7 +3811,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>264</v>
       </c>
@@ -3678,7 +3833,7 @@
       <c r="G59" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="H59" s="5" t="s">
         <v>282</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -3697,7 +3852,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>264</v>
       </c>
@@ -3719,7 +3874,7 @@
       <c r="G60" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="H60" s="5" t="s">
         <v>287</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -3738,7 +3893,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>264</v>
       </c>
@@ -3760,7 +3915,7 @@
       <c r="G61" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="H61" s="5" t="s">
         <v>290</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -3779,7 +3934,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>264</v>
       </c>
@@ -3801,7 +3956,7 @@
       <c r="G62" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="H62" s="5" t="s">
         <v>293</v>
       </c>
       <c r="I62" s="1"/>
@@ -3816,7 +3971,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>264</v>
       </c>
@@ -3838,7 +3993,7 @@
       <c r="G63" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H63" s="5" t="s">
         <v>297</v>
       </c>
       <c r="I63" s="1">
@@ -3857,7 +4012,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>264</v>
       </c>
@@ -3879,7 +4034,7 @@
       <c r="G64" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="H64" s="5" t="s">
         <v>303</v>
       </c>
       <c r="I64" s="1">
@@ -3898,7 +4053,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>264</v>
       </c>
@@ -3920,7 +4075,7 @@
       <c r="G65" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="H65" s="5" t="s">
         <v>309</v>
       </c>
       <c r="I65" s="1">
@@ -3939,230 +4094,444 @@
         <v>312</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A66" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="B66" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J66" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K66" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="M66" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E67" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-    </row>
-    <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+      <c r="F67" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="I67" s="9">
+        <v>40.427699869999998</v>
+      </c>
+      <c r="J67" s="9">
+        <v>-80.135979739999996</v>
+      </c>
+      <c r="K67" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="L67" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="M67" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A68" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D67" s="1" t="s">
+      <c r="B68" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="D68" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E68" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-    </row>
-    <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+      <c r="F68" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="I68" s="9">
+        <v>40.427699869999998</v>
+      </c>
+      <c r="J68" s="9">
+        <v>-80.135979739999996</v>
+      </c>
+      <c r="K68" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="L68" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="M68" s="9" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A69" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D68" s="1" t="s">
+      <c r="B69" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D69" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E69" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-    </row>
-    <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="F69" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="I69" s="9">
+        <v>40.427699869999998</v>
+      </c>
+      <c r="J69" s="9">
+        <v>-80.135979739999996</v>
+      </c>
+      <c r="K69" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="L69" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="M69" s="9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A70" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D69" s="1" t="s">
+      <c r="B70" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="D70" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E70" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-    </row>
-    <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+      <c r="F70" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="I70" s="9">
+        <v>40.427699869999998</v>
+      </c>
+      <c r="J70" s="9">
+        <v>-80.135979739999996</v>
+      </c>
+      <c r="K70" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="L70" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="M70" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A71" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D70" s="1" t="s">
+      <c r="B71" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D71" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E71" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-    </row>
-    <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+      <c r="F71" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J71" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K71" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="L71" s="9"/>
+      <c r="M71" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A72" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D71" s="1" t="s">
+      <c r="B72" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E72" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-    </row>
-    <row r="72" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+      <c r="F72" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="J72" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K72" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="L72" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="M72" s="9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A73" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D72" s="1" t="s">
+      <c r="B73" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E73" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-    </row>
-    <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+      <c r="F73" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="G73" s="9"/>
+      <c r="H73" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A74" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D73" s="1" t="s">
+      <c r="B74" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D74" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E74" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-    </row>
-    <row r="74" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D74" s="1" t="s">
+      <c r="F74" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="I74" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J74" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K74" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L74" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="M74" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
+      <c r="F75" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="I75">
+        <v>39.078167000000001</v>
+      </c>
+      <c r="J75">
+        <v>-77.550561000000002</v>
+      </c>
+      <c r="K75" t="s">
+        <v>56</v>
+      </c>
+      <c r="L75" t="s">
+        <v>328</v>
+      </c>
+      <c r="M75" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A76" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="I76">
+        <v>39.045227799999999</v>
+      </c>
+      <c r="J76">
+        <v>-77.486494199999996</v>
+      </c>
+      <c r="K76" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="L76" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M76" t="s">
+        <v>366</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4192,5 +4561,6 @@
     <hyperlink ref="M57" r:id="rId24" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new graphs for tays
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB700AB2-DBA4-9948-8FC2-F389AB299CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CF1EE7-DA04-D04F-94B0-73DF98A03023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -1404,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,7 +1426,7 @@
     <col min="13" max="13" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1466,8 +1466,9 @@
       <c r="M1" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1793,7 +1794,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1939,7 +1940,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1964,7 +1965,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
added farifax info into the shinyApp
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87B4185-8F79-3D4A-9DEE-0E41204AC2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C77A287-C85D-2448-9FE6-66D974791403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="407">
   <si>
     <t>County</t>
   </si>
@@ -705,9 +705,6 @@
   </si>
   <si>
     <t>Work in Loudoun - Loudoun County Economic Development, VA</t>
-  </si>
-  <si>
-    <t>Northern Virginia</t>
   </si>
   <si>
     <t>OAR</t>
@@ -1667,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1716,7 +1713,7 @@
         <v>325</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
@@ -1725,7 +1722,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -1860,7 +1857,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>33</v>
@@ -1901,7 +1898,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>33</v>
@@ -1942,7 +1939,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>33</v>
@@ -1983,7 +1980,7 @@
         <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>33</v>
@@ -2024,7 +2021,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
@@ -2059,13 +2056,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>33</v>
@@ -2100,13 +2097,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>14</v>
@@ -2141,13 +2138,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>14</v>
@@ -2177,12 +2174,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>70</v>
@@ -2207,7 +2204,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>72</v>
@@ -2232,13 +2229,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>33</v>
@@ -2273,13 +2270,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>33</v>
@@ -2314,13 +2311,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>33</v>
@@ -2361,7 +2358,7 @@
         <v>89</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>33</v>
@@ -2402,7 +2399,7 @@
         <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>14</v>
@@ -2437,7 +2434,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>100</v>
@@ -2478,7 +2475,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>105</v>
@@ -2519,7 +2516,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>109</v>
@@ -2560,13 +2557,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>112</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>14</v>
@@ -2596,7 +2593,7 @@
     </row>
     <row r="24" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>11</v>
@@ -2637,10 +2634,10 @@
     </row>
     <row r="25" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>123</v>
@@ -2678,16 +2675,16 @@
     </row>
     <row r="26" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
@@ -2719,16 +2716,16 @@
     </row>
     <row r="27" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>135</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>14</v>
@@ -2760,10 +2757,10 @@
     </row>
     <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>140</v>
@@ -2799,16 +2796,16 @@
     </row>
     <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>14</v>
@@ -2840,16 +2837,16 @@
     </row>
     <row r="30" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>152</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>33</v>
@@ -2881,10 +2878,10 @@
     </row>
     <row r="31" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>154</v>
@@ -2920,16 +2917,16 @@
     </row>
     <row r="32" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>156</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>33</v>
@@ -2953,16 +2950,16 @@
     </row>
     <row r="33" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>160</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>33</v>
@@ -2982,16 +2979,16 @@
     </row>
     <row r="34" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>163</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>110</v>
@@ -3011,7 +3008,7 @@
     </row>
     <row r="35" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>166</v>
@@ -3020,7 +3017,7 @@
         <v>167</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -3036,7 +3033,7 @@
     </row>
     <row r="36" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>166</v>
@@ -3061,7 +3058,7 @@
     </row>
     <row r="37" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>166</v>
@@ -3088,7 +3085,7 @@
     </row>
     <row r="38" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>166</v>
@@ -3117,7 +3114,7 @@
     </row>
     <row r="39" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>166</v>
@@ -3149,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>179</v>
@@ -3190,7 +3187,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>185</v>
@@ -3231,7 +3228,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>190</v>
@@ -3272,7 +3269,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>196</v>
@@ -3313,7 +3310,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>202</v>
@@ -3354,7 +3351,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>208</v>
@@ -3395,7 +3392,7 @@
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>215</v>
@@ -3436,7 +3433,7 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>219</v>
@@ -3472,28 +3469,28 @@
     </row>
     <row r="48" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="I48" s="2">
         <v>39.108399900000002</v>
@@ -3502,39 +3499,39 @@
         <v>-77.565337</v>
       </c>
       <c r="K48" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="M48" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="M48" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>223</v>
+        <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="I49" s="2">
         <v>39.114409999999999</v>
@@ -3546,10 +3543,10 @@
         <v>205</v>
       </c>
       <c r="L49" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="M49" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="M49" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="84" x14ac:dyDescent="0.2">
@@ -3560,7 +3557,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>180</v>
@@ -3572,10 +3569,10 @@
         <v>34</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="I50" s="2">
         <v>39.115943000000001</v>
@@ -3587,10 +3584,10 @@
         <v>212</v>
       </c>
       <c r="L50" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="M50" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="M50" s="4" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3601,7 +3598,7 @@
         <v>11</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>180</v>
@@ -3613,10 +3610,10 @@
         <v>186</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="I51" s="2">
         <v>39.114406199999998</v>
@@ -3628,10 +3625,10 @@
         <v>212</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3651,13 +3648,13 @@
         <v>33</v>
       </c>
       <c r="F52" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="I52" s="2">
         <v>37.542472099999998</v>
@@ -3666,13 +3663,13 @@
         <v>-77.435912200000004</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>82</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="63" x14ac:dyDescent="0.2">
@@ -3683,7 +3680,7 @@
         <v>166</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>180</v>
@@ -3692,13 +3689,13 @@
         <v>33</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G53" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="I53" s="2">
         <v>39.117853099999998</v>
@@ -3710,10 +3707,10 @@
         <v>205</v>
       </c>
       <c r="L53" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="M53" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="63" x14ac:dyDescent="0.2">
@@ -3721,10 +3718,10 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>180</v>
@@ -3736,10 +3733,10 @@
         <v>186</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="I54" s="2">
         <v>37.610656959136698</v>
@@ -3748,13 +3745,13 @@
         <v>-77.340073015724201</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>82</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3762,10 +3759,10 @@
         <v>10</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>180</v>
@@ -3777,10 +3774,10 @@
         <v>186</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>49</v>
@@ -3789,39 +3786,39 @@
         <v>49</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L55" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="M55" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>49</v>
@@ -3831,21 +3828,21 @@
         <v>49</v>
       </c>
       <c r="L56" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="M56" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="M56" s="4" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>180</v>
@@ -3857,10 +3854,10 @@
         <v>186</v>
       </c>
       <c r="G57" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="I57" s="2">
         <v>40.439779999999999</v>
@@ -3869,39 +3866,39 @@
         <v>-79.998869999999997</v>
       </c>
       <c r="K57" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="L57" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="L57" s="2" t="s">
+      <c r="M57" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="M57" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G58" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>49</v>
@@ -3913,36 +3910,36 @@
         <v>49</v>
       </c>
       <c r="L58" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="M58" s="4" t="s">
         <v>279</v>
-      </c>
-      <c r="M58" s="4" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>49</v>
@@ -3954,36 +3951,36 @@
         <v>49</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F60" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>49</v>
@@ -3995,36 +3992,36 @@
         <v>49</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G61" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>49</v>
@@ -4036,36 +4033,36 @@
         <v>49</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2" t="s">
@@ -4073,21 +4070,21 @@
       </c>
       <c r="K62" s="2"/>
       <c r="L62" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>180</v>
@@ -4096,13 +4093,13 @@
         <v>33</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="I63" s="2">
         <v>40.407960000000003</v>
@@ -4111,24 +4108,24 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K63" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L63" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="L63" s="2" t="s">
+      <c r="M63" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="M63" s="4" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>180</v>
@@ -4140,10 +4137,10 @@
         <v>34</v>
       </c>
       <c r="G64" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="I64" s="2">
         <v>40.405259100000002</v>
@@ -4152,24 +4149,24 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K64" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="L64" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="M64" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="M64" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>180</v>
@@ -4181,10 +4178,10 @@
         <v>186</v>
       </c>
       <c r="G65" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>309</v>
       </c>
       <c r="I65" s="2">
         <v>40.559510000000003</v>
@@ -4193,39 +4190,39 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K65" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="L65" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="L65" s="2" t="s">
+      <c r="M65" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="M65" s="4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>129</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>49</v>
@@ -4237,21 +4234,21 @@
         <v>49</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>180</v>
@@ -4263,10 +4260,10 @@
         <v>34</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I67" s="2">
         <v>40.427699869999998</v>
@@ -4275,24 +4272,24 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>180</v>
@@ -4304,10 +4301,10 @@
         <v>34</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I68" s="2">
         <v>40.427699869999998</v>
@@ -4316,24 +4313,24 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>180</v>
@@ -4345,10 +4342,10 @@
         <v>34</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I69" s="2">
         <v>40.427699869999998</v>
@@ -4357,24 +4354,24 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>180</v>
@@ -4386,10 +4383,10 @@
         <v>34</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I70" s="2">
         <v>40.427699869999998</v>
@@ -4398,24 +4395,24 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>180</v>
@@ -4427,10 +4424,10 @@
         <v>34</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>49</v>
@@ -4439,22 +4436,22 @@
         <v>49</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L71" s="2"/>
       <c r="M71" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>180</v>
@@ -4466,36 +4463,36 @@
         <v>186</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>180</v>
@@ -4504,23 +4501,23 @@
         <v>33</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
     </row>
     <row r="74" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>166</v>
@@ -4538,10 +4535,10 @@
         <v>186</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>49</v>
@@ -4553,10 +4550,10 @@
         <v>49</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -4564,10 +4561,10 @@
         <v>10</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>180</v>
@@ -4576,13 +4573,13 @@
         <v>33</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G75" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="I75" s="2">
         <v>39.078167000000001</v>
@@ -4594,10 +4591,10 @@
         <v>56</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="21" x14ac:dyDescent="0.2">
@@ -4605,10 +4602,10 @@
         <v>10</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>180</v>
@@ -4620,10 +4617,10 @@
         <v>186</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I76" s="2">
         <v>39.045227799999999</v>
@@ -4632,39 +4629,39 @@
         <v>-77.486494199999996</v>
       </c>
       <c r="K76" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="L76" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="L76" s="2" t="s">
+      <c r="M76" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="M76" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>368</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G77" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="I77" s="2">
         <v>38.906303508879397</v>
@@ -4673,37 +4670,37 @@
         <v>-77.222641329237604</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L77" s="2"/>
       <c r="M77" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="H78" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="I78" s="2">
         <v>38.875816034503501</v>
@@ -4712,37 +4709,37 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F79" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="G79" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="G79" s="2" t="s">
-        <v>375</v>
-      </c>
       <c r="H79" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I79" s="2">
         <v>38.875816034503501</v>
@@ -4751,37 +4748,37 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F80" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="H80" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="I80" s="2">
         <v>38.873610192974397</v>
@@ -4790,37 +4787,37 @@
         <v>-77.3055466310296</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>110</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I81" s="2">
         <v>38.868590773014198</v>
@@ -4829,37 +4826,37 @@
         <v>-77.224144877053305</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L81" s="2"/>
       <c r="M81" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="168" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="H82" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="I82" s="2">
         <v>38.8060490968736</v>
@@ -4868,37 +4865,37 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L82" s="2"/>
       <c r="M82" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I83" s="2">
         <v>38.8060490968736</v>
@@ -4907,37 +4904,37 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I84" s="2">
         <v>38.8553917225858</v>
@@ -4946,37 +4943,37 @@
         <v>-77.362718702194798</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="210" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G85" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="I85" s="2">
         <v>38.854251580169802</v>
@@ -4985,11 +4982,11 @@
         <v>-77.356579302194902</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Shelters in fairfax to combined sheet
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C77A287-C85D-2448-9FE6-66D974791403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FEB22D-E039-4B8A-9FAD-B892C925D3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="429">
   <si>
     <t>County</t>
   </si>
@@ -1276,12 +1276,79 @@
   <si>
     <t>Both</t>
   </si>
+  <si>
+    <t>Coordinated Services Planning (CSP)</t>
+  </si>
+  <si>
+    <t>Connects Fairfax County residents to county- and community-based services and resources that promote self-sufficiency and enhance well-being.</t>
+  </si>
+  <si>
+    <t>Fairfax County Neighborhood and Community Services</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/</t>
+  </si>
+  <si>
+    <t>Bailey’s Crossroads Community Shelter (Falls Church)</t>
+  </si>
+  <si>
+    <t>Eleanor U. Kennedy Shelter (Richmond Highway – Fort Belvoir)</t>
+  </si>
+  <si>
+    <t>Embry Rucker Community Shelter (Reston)</t>
+  </si>
+  <si>
+    <t>Adults without children who are in need of shelter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides Shelter to those who are homeless </t>
+  </si>
+  <si>
+    <t>Fort Belvoir</t>
+  </si>
+  <si>
+    <t>Reston</t>
+  </si>
+  <si>
+    <t>New Hope Housing, Inc.</t>
+  </si>
+  <si>
+    <t>Cornerstones.</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/homeless/emergency-shelters</t>
+  </si>
+  <si>
+    <t>Katherine K. Hanley Family Shelter (Fairfax)</t>
+  </si>
+  <si>
+    <t>Patrick Henry Family Shelter (Falls Church)</t>
+  </si>
+  <si>
+    <t>Adults with children who are in need of shelter </t>
+  </si>
+  <si>
+    <t>Adults with and without children who are in need of shelter </t>
+  </si>
+  <si>
+    <t>Next Steps Family Program (Main Office)</t>
+  </si>
+  <si>
+    <t>Full service sheltering and supportive services program. 
+Sheltering services are provided in apartment communities located throughout the county.</t>
+  </si>
+  <si>
+    <t>Shelter House, Inc.</t>
+  </si>
+  <si>
+    <t>FACETS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1310,6 +1377,18 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1332,7 +1411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1346,6 +1425,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1662,29 +1749,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="82.33203125" customWidth="1"/>
+    <col min="7" max="7" width="87.08203125" customWidth="1"/>
     <col min="8" max="8" width="83.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" customWidth="1"/>
     <col min="11" max="11" width="51.5" customWidth="1"/>
     <col min="12" max="12" width="40" customWidth="1"/>
-    <col min="13" max="13" width="54" customWidth="1"/>
+    <col min="13" max="13" width="72.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1812,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1766,7 +1853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1807,7 +1894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1846,7 +1933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1887,7 +1974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1928,7 +2015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1969,7 +2056,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +2097,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2051,7 +2138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2092,7 +2179,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2133,7 +2220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2174,7 +2261,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -2199,7 +2286,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2224,7 +2311,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2265,7 +2352,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -2306,7 +2393,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -2347,7 +2434,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -2388,7 +2475,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2429,7 +2516,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -2470,7 +2557,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -2511,7 +2598,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -2552,7 +2639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -2591,7 +2678,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>263</v>
       </c>
@@ -2632,7 +2719,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>263</v>
       </c>
@@ -2673,7 +2760,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>263</v>
       </c>
@@ -2714,7 +2801,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>263</v>
       </c>
@@ -2755,7 +2842,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>263</v>
       </c>
@@ -2794,7 +2881,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>263</v>
       </c>
@@ -2835,7 +2922,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>263</v>
       </c>
@@ -2876,7 +2963,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>263</v>
       </c>
@@ -2915,7 +3002,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>263</v>
       </c>
@@ -2948,7 +3035,7 @@
       </c>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>263</v>
       </c>
@@ -2977,7 +3064,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>263</v>
       </c>
@@ -3006,7 +3093,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>263</v>
       </c>
@@ -3031,7 +3118,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>263</v>
       </c>
@@ -3056,7 +3143,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>263</v>
       </c>
@@ -3083,7 +3170,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>263</v>
       </c>
@@ -3112,7 +3199,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>263</v>
       </c>
@@ -3141,7 +3228,7 @@
       </c>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>10</v>
       </c>
@@ -3182,7 +3269,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
@@ -3223,7 +3310,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
@@ -3264,7 +3351,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -3305,7 +3392,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -3346,7 +3433,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -3387,7 +3474,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>10</v>
       </c>
@@ -3428,7 +3515,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
@@ -3467,7 +3554,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
@@ -3508,7 +3595,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -3549,7 +3636,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>10</v>
       </c>
@@ -3590,7 +3677,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>10</v>
       </c>
@@ -3631,7 +3718,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>10</v>
       </c>
@@ -3672,7 +3759,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>10</v>
       </c>
@@ -3713,7 +3800,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>10</v>
       </c>
@@ -3754,7 +3841,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>10</v>
       </c>
@@ -3795,7 +3882,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>263</v>
       </c>
@@ -3834,7 +3921,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>263</v>
       </c>
@@ -3875,7 +3962,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>263</v>
       </c>
@@ -3916,7 +4003,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>263</v>
       </c>
@@ -3957,7 +4044,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>263</v>
       </c>
@@ -3998,7 +4085,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>263</v>
       </c>
@@ -4039,7 +4126,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>263</v>
       </c>
@@ -4076,7 +4163,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>263</v>
       </c>
@@ -4117,7 +4204,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>263</v>
       </c>
@@ -4158,7 +4245,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>263</v>
       </c>
@@ -4199,7 +4286,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>263</v>
       </c>
@@ -4240,7 +4327,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>263</v>
       </c>
@@ -4281,7 +4368,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>263</v>
       </c>
@@ -4322,7 +4409,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>263</v>
       </c>
@@ -4363,7 +4450,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>263</v>
       </c>
@@ -4404,7 +4491,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>263</v>
       </c>
@@ -4443,7 +4530,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>263</v>
       </c>
@@ -4484,7 +4571,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>263</v>
       </c>
@@ -4515,7 +4602,7 @@
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>263</v>
       </c>
@@ -4556,7 +4643,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>10</v>
       </c>
@@ -4597,7 +4684,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>10</v>
       </c>
@@ -4638,7 +4725,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>400</v>
       </c>
@@ -4677,7 +4764,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>400</v>
       </c>
@@ -4716,7 +4803,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>400</v>
       </c>
@@ -4755,7 +4842,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>400</v>
       </c>
@@ -4794,7 +4881,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>400</v>
       </c>
@@ -4833,7 +4920,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="168" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" ht="164" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>400</v>
       </c>
@@ -4872,7 +4959,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>400</v>
       </c>
@@ -4911,7 +4998,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>400</v>
       </c>
@@ -4950,7 +5037,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="210" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" ht="205" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>400</v>
       </c>
@@ -4987,6 +5074,293 @@
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
         <v>405</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+      <c r="A86" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C86" t="s">
+        <v>407</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="M86" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A87" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C87" t="s">
+        <v>411</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G87" t="s">
+        <v>414</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I87">
+        <v>38.848489999999998</v>
+      </c>
+      <c r="J87">
+        <v>-77.128174999999999</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L87" t="s">
+        <v>418</v>
+      </c>
+      <c r="M87" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A88" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G88" t="s">
+        <v>414</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I88">
+        <v>38.709357400000002</v>
+      </c>
+      <c r="J88">
+        <v>-77.157447599999998</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="L88" t="s">
+        <v>418</v>
+      </c>
+      <c r="M88" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A89" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C89" t="s">
+        <v>413</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G89" t="s">
+        <v>424</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I89">
+        <v>38.962038700000001</v>
+      </c>
+      <c r="J89">
+        <v>-77.3598353</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="M89" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A90" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C90" t="s">
+        <v>421</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G90" t="s">
+        <v>423</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I90">
+        <v>38.843446</v>
+      </c>
+      <c r="J90">
+        <v>-77.339151999999999</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="L90" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="M90" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A91" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C91" t="s">
+        <v>422</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G91" t="s">
+        <v>423</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I91">
+        <v>38.867538452148402</v>
+      </c>
+      <c r="J91">
+        <v>-77.147491455078097</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L91" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="M91" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+      <c r="A92" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G92" t="s">
+        <v>423</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="I92">
+        <v>38.727029999999999</v>
+      </c>
+      <c r="J92">
+        <v>-77.130688000000006</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L92" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="M92" s="9" t="s">
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -5015,8 +5389,12 @@
     <hyperlink ref="M64" r:id="rId22" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
     <hyperlink ref="M65" r:id="rId23" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
     <hyperlink ref="M57" r:id="rId24" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
+    <hyperlink ref="M86" r:id="rId25" xr:uid="{331F533A-9D09-4395-A2D7-E8FBA31E7F3D}"/>
+    <hyperlink ref="M87" r:id="rId26" xr:uid="{F8107525-8BD8-4E17-8327-69D4372A675E}"/>
+    <hyperlink ref="M88:M89" r:id="rId27" display="https://www.fairfaxcounty.gov/homeless/emergency-shelters" xr:uid="{3118F14B-4B01-42AE-BD3B-13E80435DD12}"/>
+    <hyperlink ref="M90:M92" r:id="rId28" display="https://www.fairfaxcounty.gov/homeless/emergency-shelters" xr:uid="{FED8C5B7-572E-4144-8F75-650C52CEF26B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Health and Housing info for fairfax county to combined spreadsheet
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FEB22D-E039-4B8A-9FAD-B892C925D3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694ACB0B-C001-4006-8E92-46AA203C6D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="446">
   <si>
     <t>County</t>
   </si>
@@ -1343,12 +1343,63 @@
   <si>
     <t>FACETS</t>
   </si>
+  <si>
+    <t>Free Prescription Discount Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offer savings on prescription drugs to residents who are without health insurance, a traditional benefits plan, or have prescriptions that are not covered by insurance. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">City of Fairfax </t>
+  </si>
+  <si>
+    <t>https://www.fairfaxva.gov/residents/free-prescription-discount-card</t>
+  </si>
+  <si>
+    <t>First-Time Homebuyers Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Households must not have owned a home within the last three years, must have at least $25,000 in annual income and not more than the income limits outlined on website, be able to qualify for a home loan, have a credit score of at least 620 or more, be able to pay a 2 percent down payment, closing costs and have at least one month of savings, </t>
+  </si>
+  <si>
+    <t>Provides affordable homes primarily through the Affordable Dwelling Unit (ADU) Program to low- and moderate-income families</t>
+  </si>
+  <si>
+    <t>Fairfax County Housing and Community Development</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/housing/homeownership/firsttimehomebuyers</t>
+  </si>
+  <si>
+    <t>Workforce Dwelling Unit Homebuyer Program</t>
+  </si>
+  <si>
+    <t>Homebuyers earning between 70 and 120 percent the Area Median Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides a means for qualified homebuyer to purchase a home at below-market prices near employment centers and transportation options. </t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/housing/homeownership/wduhomebuyers</t>
+  </si>
+  <si>
+    <t>Participants  eceive assistance to rent privately-owned housing units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family’s total income must not exceed 50% of the Area Median Income, at least one member of the household must be a U.S. citizen or U.S. national or have eligible immigration status and all members of the household must provide a complete and accurate social security number (SSN). </t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/housing/rentalhousing/housingchoicevoucher/eligibility</t>
+  </si>
+  <si>
+    <t>Housing Choice Voucher Program</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1376,18 +1427,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1426,13 +1465,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1749,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2138,7 +2177,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="41" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2639,7 +2678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -3118,7 +3157,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>263</v>
       </c>
@@ -3170,7 +3209,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>263</v>
       </c>
@@ -4602,7 +4641,7 @@
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>263</v>
       </c>
@@ -4725,7 +4764,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>400</v>
       </c>
@@ -4881,7 +4920,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>400</v>
       </c>
@@ -5037,7 +5076,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="205" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:13" ht="184.5" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>400</v>
       </c>
@@ -5076,14 +5115,14 @@
         <v>405</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
         <v>400</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="6" t="s">
         <v>407</v>
       </c>
       <c r="D86" s="2" t="s">
@@ -5124,7 +5163,7 @@
       <c r="B87" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="6" t="s">
         <v>411</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -5136,25 +5175,25 @@
       <c r="F87" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87" s="6" t="s">
         <v>414</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I87">
+      <c r="I87" s="6">
         <v>38.848489999999998</v>
       </c>
-      <c r="J87">
+      <c r="J87" s="6">
         <v>-77.128174999999999</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L87" t="s">
+      <c r="L87" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="M87" s="9" t="s">
+      <c r="M87" s="8" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5165,7 +5204,7 @@
       <c r="B88" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="9" t="s">
         <v>412</v>
       </c>
       <c r="D88" s="2" t="s">
@@ -5177,25 +5216,25 @@
       <c r="F88" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" s="6" t="s">
         <v>414</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="6">
         <v>38.709357400000002</v>
       </c>
-      <c r="J88">
+      <c r="J88" s="6">
         <v>-77.157447599999998</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="L88" t="s">
+      <c r="L88" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="M88" s="9" t="s">
+      <c r="M88" s="8" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5206,7 +5245,7 @@
       <c r="B89" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="6" t="s">
         <v>413</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -5218,16 +5257,16 @@
       <c r="F89" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="6" t="s">
         <v>424</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I89">
+      <c r="I89" s="6">
         <v>38.962038700000001</v>
       </c>
-      <c r="J89">
+      <c r="J89" s="6">
         <v>-77.3598353</v>
       </c>
       <c r="K89" s="2" t="s">
@@ -5236,7 +5275,7 @@
       <c r="L89" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="M89" s="9" t="s">
+      <c r="M89" s="8" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5247,7 +5286,7 @@
       <c r="B90" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="6" t="s">
         <v>421</v>
       </c>
       <c r="D90" s="2" t="s">
@@ -5259,16 +5298,16 @@
       <c r="F90" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="6" t="s">
         <v>423</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I90">
+      <c r="I90" s="6">
         <v>38.843446</v>
       </c>
-      <c r="J90">
+      <c r="J90" s="6">
         <v>-77.339151999999999</v>
       </c>
       <c r="K90" s="2" t="s">
@@ -5277,7 +5316,7 @@
       <c r="L90" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="M90" s="9" t="s">
+      <c r="M90" s="8" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5288,7 +5327,7 @@
       <c r="B91" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="6" t="s">
         <v>422</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -5300,16 +5339,16 @@
       <c r="F91" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="6" t="s">
         <v>423</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I91">
+      <c r="I91" s="6">
         <v>38.867538452148402</v>
       </c>
-      <c r="J91">
+      <c r="J91" s="6">
         <v>-77.147491455078097</v>
       </c>
       <c r="K91" s="2" t="s">
@@ -5318,7 +5357,7 @@
       <c r="L91" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="M91" s="9" t="s">
+      <c r="M91" s="8" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5329,7 +5368,7 @@
       <c r="B92" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C92" s="9" t="s">
         <v>425</v>
       </c>
       <c r="D92" s="2" t="s">
@@ -5341,16 +5380,16 @@
       <c r="F92" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" s="6" t="s">
         <v>423</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="I92">
+      <c r="I92" s="6">
         <v>38.727029999999999</v>
       </c>
-      <c r="J92">
+      <c r="J92" s="6">
         <v>-77.130688000000006</v>
       </c>
       <c r="K92" s="2" t="s">
@@ -5359,8 +5398,172 @@
       <c r="L92" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="M92" s="9" t="s">
+      <c r="M92" s="8" t="s">
         <v>420</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
+      <c r="A93" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="I93" s="6">
+        <v>38.841723799999997</v>
+      </c>
+      <c r="J93" s="6">
+        <v>-77.308954900000003</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="L93" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="M93" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
+      <c r="A94" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L94" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="M94" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="41" x14ac:dyDescent="0.45">
+      <c r="A95" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L95" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="M95" s="6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="82" x14ac:dyDescent="0.45">
+      <c r="A96" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="I96" s="6">
+        <v>38.862159729003899</v>
+      </c>
+      <c r="J96" s="6">
+        <v>-77.332115173339801</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="L96" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="M96" s="7" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -5393,8 +5596,10 @@
     <hyperlink ref="M87" r:id="rId26" xr:uid="{F8107525-8BD8-4E17-8327-69D4372A675E}"/>
     <hyperlink ref="M88:M89" r:id="rId27" display="https://www.fairfaxcounty.gov/homeless/emergency-shelters" xr:uid="{3118F14B-4B01-42AE-BD3B-13E80435DD12}"/>
     <hyperlink ref="M90:M92" r:id="rId28" display="https://www.fairfaxcounty.gov/homeless/emergency-shelters" xr:uid="{FED8C5B7-572E-4144-8F75-650C52CEF26B}"/>
+    <hyperlink ref="M93" r:id="rId29" xr:uid="{4E2B6A62-A7E8-4369-831A-778871EEAA76}"/>
+    <hyperlink ref="M96" r:id="rId30" xr:uid="{528ED07F-7932-43EC-AC02-34CE91E57FBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Education program to combined excel sheet
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694ACB0B-C001-4006-8E92-46AA203C6D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A2373F-F4B0-4B5A-8563-975ABBEE0157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="450">
   <si>
     <t>County</t>
   </si>
@@ -1383,9 +1383,6 @@
     <t>https://www.fairfaxcounty.gov/housing/homeownership/wduhomebuyers</t>
   </si>
   <si>
-    <t>Participants  eceive assistance to rent privately-owned housing units</t>
-  </si>
-  <si>
     <t xml:space="preserve">Family’s total income must not exceed 50% of the Area Median Income, at least one member of the household must be a U.S. citizen or U.S. national or have eligible immigration status and all members of the household must provide a complete and accurate social security number (SSN). </t>
   </si>
   <si>
@@ -1393,6 +1390,21 @@
   </si>
   <si>
     <t>Housing Choice Voucher Program</t>
+  </si>
+  <si>
+    <t>Participants  receive assistance to rent privately-owned housing units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult and Community Education </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courses offered in ESOL, Business and IT and personal enrichnment as well as Apprenticeships and Trade classes offered </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairfax County Public Schools </t>
+  </si>
+  <si>
+    <t>https://aceclasses.fcps.edu/default.aspx</t>
   </si>
 </sst>
 </file>
@@ -1450,7 +1462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1464,6 +1476,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1788,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L101" sqref="L101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5122,7 +5138,7 @@
       <c r="B86" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="8" t="s">
         <v>407</v>
       </c>
       <c r="D86" s="2" t="s">
@@ -5152,7 +5168,7 @@
       <c r="L86" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="M86" s="7" t="s">
+      <c r="M86" s="9" t="s">
         <v>410</v>
       </c>
     </row>
@@ -5163,7 +5179,7 @@
       <c r="B87" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="8" t="s">
         <v>411</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -5175,25 +5191,25 @@
       <c r="F87" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G87" s="6" t="s">
+      <c r="G87" s="8" t="s">
         <v>414</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I87" s="6">
+      <c r="I87" s="8">
         <v>38.848489999999998</v>
       </c>
-      <c r="J87" s="6">
+      <c r="J87" s="8">
         <v>-77.128174999999999</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L87" s="6" t="s">
+      <c r="L87" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="M87" s="8" t="s">
+      <c r="M87" s="10" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5204,7 +5220,7 @@
       <c r="B88" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="11" t="s">
         <v>412</v>
       </c>
       <c r="D88" s="2" t="s">
@@ -5216,25 +5232,25 @@
       <c r="F88" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G88" s="6" t="s">
+      <c r="G88" s="8" t="s">
         <v>414</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I88" s="6">
+      <c r="I88" s="8">
         <v>38.709357400000002</v>
       </c>
-      <c r="J88" s="6">
+      <c r="J88" s="8">
         <v>-77.157447599999998</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="L88" s="6" t="s">
+      <c r="L88" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="M88" s="8" t="s">
+      <c r="M88" s="10" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5245,7 +5261,7 @@
       <c r="B89" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="8" t="s">
         <v>413</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -5257,25 +5273,25 @@
       <c r="F89" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G89" s="6" t="s">
+      <c r="G89" s="8" t="s">
         <v>424</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I89" s="6">
+      <c r="I89" s="8">
         <v>38.962038700000001</v>
       </c>
-      <c r="J89" s="6">
+      <c r="J89" s="8">
         <v>-77.3598353</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="L89" s="6" t="s">
+      <c r="L89" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="M89" s="8" t="s">
+      <c r="M89" s="10" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5286,7 +5302,7 @@
       <c r="B90" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="8" t="s">
         <v>421</v>
       </c>
       <c r="D90" s="2" t="s">
@@ -5298,25 +5314,25 @@
       <c r="F90" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G90" s="6" t="s">
+      <c r="G90" s="8" t="s">
         <v>423</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I90" s="6">
+      <c r="I90" s="8">
         <v>38.843446</v>
       </c>
-      <c r="J90" s="6">
+      <c r="J90" s="8">
         <v>-77.339151999999999</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="L90" s="6" t="s">
+      <c r="L90" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="M90" s="8" t="s">
+      <c r="M90" s="10" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5327,7 +5343,7 @@
       <c r="B91" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" s="8" t="s">
         <v>422</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -5339,25 +5355,25 @@
       <c r="F91" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G91" s="6" t="s">
+      <c r="G91" s="8" t="s">
         <v>423</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="I91" s="6">
+      <c r="I91" s="8">
         <v>38.867538452148402</v>
       </c>
-      <c r="J91" s="6">
+      <c r="J91" s="8">
         <v>-77.147491455078097</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L91" s="6" t="s">
+      <c r="L91" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="M91" s="8" t="s">
+      <c r="M91" s="10" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5368,7 +5384,7 @@
       <c r="B92" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C92" s="11" t="s">
         <v>425</v>
       </c>
       <c r="D92" s="2" t="s">
@@ -5380,25 +5396,25 @@
       <c r="F92" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G92" s="6" t="s">
+      <c r="G92" s="8" t="s">
         <v>423</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="I92" s="6">
+      <c r="I92" s="8">
         <v>38.727029999999999</v>
       </c>
-      <c r="J92" s="6">
+      <c r="J92" s="8">
         <v>-77.130688000000006</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L92" s="6" t="s">
+      <c r="L92" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="M92" s="8" t="s">
+      <c r="M92" s="10" t="s">
         <v>420</v>
       </c>
     </row>
@@ -5427,19 +5443,19 @@
       <c r="H93" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="I93" s="6">
+      <c r="I93" s="8">
         <v>38.841723799999997</v>
       </c>
-      <c r="J93" s="6">
+      <c r="J93" s="8">
         <v>-77.308954900000003</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="L93" s="6" t="s">
+      <c r="L93" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="M93" s="7" t="s">
+      <c r="M93" s="9" t="s">
         <v>432</v>
       </c>
     </row>
@@ -5450,7 +5466,7 @@
       <c r="B94" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="11" t="s">
         <v>433</v>
       </c>
       <c r="D94" s="2" t="s">
@@ -5465,7 +5481,7 @@
       <c r="G94" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="H94" s="6" t="s">
+      <c r="H94" s="8" t="s">
         <v>435</v>
       </c>
       <c r="I94" s="2" t="s">
@@ -5477,10 +5493,10 @@
       <c r="K94" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L94" s="6" t="s">
+      <c r="L94" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="M94" s="6" t="s">
+      <c r="M94" s="8" t="s">
         <v>437</v>
       </c>
     </row>
@@ -5491,7 +5507,7 @@
       <c r="B95" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C95" s="11" t="s">
         <v>438</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -5518,10 +5534,10 @@
       <c r="K95" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L95" s="6" t="s">
+      <c r="L95" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="M95" s="6" t="s">
+      <c r="M95" s="8" t="s">
         <v>441</v>
       </c>
     </row>
@@ -5532,8 +5548,8 @@
       <c r="B96" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>445</v>
+      <c r="C96" s="8" t="s">
+        <v>444</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>406</v>
@@ -5545,25 +5561,66 @@
         <v>284</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="H96" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="I96" s="6">
+      <c r="H96" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="I96" s="8">
         <v>38.862159729003899</v>
       </c>
-      <c r="J96" s="6">
+      <c r="J96" s="8">
         <v>-77.332115173339801</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="L96" s="6" t="s">
+      <c r="L96" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="M96" s="7" t="s">
-        <v>444</v>
+      <c r="M96" s="9" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A97" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I97">
+        <v>38.8068071</v>
+      </c>
+      <c r="J97">
+        <v>-77.181611500000002</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="L97" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="M97" s="6" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -5598,8 +5655,9 @@
     <hyperlink ref="M90:M92" r:id="rId28" display="https://www.fairfaxcounty.gov/homeless/emergency-shelters" xr:uid="{FED8C5B7-572E-4144-8F75-650C52CEF26B}"/>
     <hyperlink ref="M93" r:id="rId29" xr:uid="{4E2B6A62-A7E8-4369-831A-778871EEAA76}"/>
     <hyperlink ref="M96" r:id="rId30" xr:uid="{528ED07F-7932-43EC-AC02-34CE91E57FBE}"/>
+    <hyperlink ref="M97" r:id="rId31" xr:uid="{D868F7A1-2868-4114-A979-FBDA0AA08630}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i updated my information and changed the online coordinates to 0-0-online
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29163A6-EC22-194F-A1D6-5FD4C23E3190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666ECD58-7FC7-F543-B5F2-B6C99A7ACEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2860" yWindow="500" windowWidth="15920" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="428">
   <si>
     <t>County</t>
   </si>
@@ -1059,9 +1059,6 @@
   </si>
   <si>
     <t>Allegheny County PA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Online </t>
   </si>
   <si>
     <t>provides transportation to medical appointments for Medical Assistance recipients who do not have transportation available to them.</t>
@@ -1339,12 +1336,15 @@
   <si>
     <t xml:space="preserve">This program helps citizens find the right healthcare coverage for them. </t>
   </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Transportation/Behavioral-Health-Transportation-Program.aspx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1384,6 +1384,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1406,7 +1413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1424,12 +1431,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1747,11 +1755,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
@@ -1764,7 +1772,7 @@
     <col min="10" max="10" width="20.6640625" customWidth="1"/>
     <col min="11" max="11" width="51.5" customWidth="1"/>
     <col min="12" max="12" width="40" customWidth="1"/>
-    <col min="13" max="13" width="54" customWidth="1"/>
+    <col min="13" max="13" width="54" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="84" x14ac:dyDescent="0.2">
@@ -1940,7 +1948,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>33</v>
@@ -1981,7 +1989,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>33</v>
@@ -2022,7 +2030,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>33</v>
@@ -2063,7 +2071,7 @@
         <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>33</v>
@@ -2104,7 +2112,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
@@ -2145,7 +2153,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>33</v>
@@ -2186,7 +2194,7 @@
         <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>14</v>
@@ -2227,7 +2235,7 @@
         <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>14</v>
@@ -2274,10 +2282,10 @@
         <v>33</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>71</v>
@@ -2285,8 +2293,12 @@
       <c r="I13" s="2">
         <v>0</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
@@ -2307,10 +2319,10 @@
         <v>33</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>73</v>
@@ -2318,8 +2330,12 @@
       <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
@@ -2334,7 +2350,7 @@
         <v>74</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>33</v>
@@ -2375,7 +2391,7 @@
         <v>79</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>33</v>
@@ -2416,7 +2432,7 @@
         <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>33</v>
@@ -2446,7 +2462,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -2457,7 +2473,7 @@
         <v>89</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>33</v>
@@ -2498,7 +2514,7 @@
         <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>14</v>
@@ -2662,7 +2678,7 @@
         <v>112</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>14</v>
@@ -2783,7 +2799,7 @@
         <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
@@ -2824,7 +2840,7 @@
         <v>135</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>14</v>
@@ -2904,7 +2920,7 @@
         <v>148</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>14</v>
@@ -2945,7 +2961,7 @@
         <v>152</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>33</v>
@@ -3025,7 +3041,7 @@
         <v>156</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>33</v>
@@ -3039,15 +3055,23 @@
       <c r="H32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="I32" s="2">
+        <v>40.439188049999998</v>
+      </c>
+      <c r="J32" s="2">
+        <v>-80.001456360000006</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="L32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M32" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="M32" s="2"/>
-    </row>
-    <row r="33" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>263</v>
       </c>
@@ -3058,13 +3082,13 @@
         <v>160</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>161</v>
@@ -3072,11 +3096,21 @@
       <c r="H33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="3"/>
+      <c r="I33" s="2">
+        <v>40.437306100000001</v>
+      </c>
+      <c r="J33" s="2">
+        <v>-80.001021339999994</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -3089,25 +3123,33 @@
         <v>163</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="7" t="s">
+      <c r="I34" s="2">
+        <v>40.437306100000001</v>
+      </c>
+      <c r="J34" s="2">
+        <v>-80.001021339999994</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M34" s="8" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3122,24 +3164,32 @@
         <v>167</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="G35" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="M35" s="2" t="s">
         <v>168</v>
       </c>
@@ -3161,19 +3211,27 @@
         <v>33</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="7" t="s">
+      <c r="I36" s="2">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M36" s="8" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3194,7 +3252,7 @@
         <v>33</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>173</v>
@@ -3202,10 +3260,18 @@
       <c r="H37" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="M37" s="3" t="s">
         <v>169</v>
       </c>
@@ -3227,7 +3293,7 @@
         <v>33</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>173</v>
@@ -3235,13 +3301,21 @@
       <c r="H38" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="I38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="L38" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M38" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M38" s="2"/>
     </row>
     <row r="39" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
@@ -3350,11 +3424,11 @@
       <c r="H41" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>49</v>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>49</v>
@@ -3555,10 +3629,12 @@
       <c r="H46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J46" s="2"/>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0</v>
+      </c>
       <c r="K46" s="2" t="s">
         <v>49</v>
       </c>
@@ -3881,11 +3957,11 @@
       <c r="H54" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>49</v>
+      <c r="I54" s="2">
+        <v>0</v>
+      </c>
+      <c r="J54" s="2">
+        <v>0</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>256</v>
@@ -3922,10 +3998,12 @@
       <c r="H55" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J55" s="2"/>
+      <c r="I55" s="2">
+        <v>0</v>
+      </c>
+      <c r="J55" s="2">
+        <v>0</v>
+      </c>
       <c r="K55" s="2" t="s">
         <v>49</v>
       </c>
@@ -4002,11 +4080,11 @@
       <c r="H57" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>49</v>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2">
+        <v>0</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>49</v>
@@ -4043,11 +4121,11 @@
       <c r="H58" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>49</v>
+      <c r="I58" s="2">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2">
+        <v>0</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>49</v>
@@ -4084,11 +4162,11 @@
       <c r="H59" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>49</v>
+      <c r="I59" s="2">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2">
+        <v>0</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>49</v>
@@ -4125,11 +4203,11 @@
       <c r="H60" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>49</v>
+      <c r="I60" s="2">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2">
+        <v>0</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>49</v>
@@ -4166,11 +4244,15 @@
       <c r="H61" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2" t="s">
+      <c r="I61" s="2">
+        <v>0</v>
+      </c>
+      <c r="J61" s="2">
+        <v>0</v>
+      </c>
+      <c r="K61" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K61" s="2"/>
       <c r="L61" s="2" t="s">
         <v>278</v>
       </c>
@@ -4306,7 +4388,7 @@
         <v>263</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>312</v>
@@ -4321,16 +4403,16 @@
         <v>129</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>49</v>
+        <v>357</v>
+      </c>
+      <c r="I65" s="2">
+        <v>0</v>
+      </c>
+      <c r="J65" s="2">
+        <v>0</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>49</v>
@@ -4339,7 +4421,7 @@
         <v>338</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="63" x14ac:dyDescent="0.2">
@@ -4347,7 +4429,7 @@
         <v>263</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>313</v>
@@ -4365,7 +4447,7 @@
         <v>307</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I66" s="2">
         <v>40.427699869999998</v>
@@ -4377,10 +4459,10 @@
         <v>272</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -4388,7 +4470,7 @@
         <v>263</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>314</v>
@@ -4403,10 +4485,10 @@
         <v>34</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I67" s="2">
         <v>40.427699869999998</v>
@@ -4418,10 +4500,10 @@
         <v>272</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -4429,7 +4511,7 @@
         <v>263</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>315</v>
@@ -4447,7 +4529,7 @@
         <v>307</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I68" s="2">
         <v>40.427699869999998</v>
@@ -4459,10 +4541,10 @@
         <v>339</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -4470,7 +4552,7 @@
         <v>263</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>316</v>
@@ -4488,7 +4570,7 @@
         <v>307</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I69" s="2">
         <v>40.427699869999998</v>
@@ -4500,10 +4582,10 @@
         <v>339</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="21" x14ac:dyDescent="0.2">
@@ -4511,7 +4593,7 @@
         <v>263</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>317</v>
@@ -4529,20 +4611,20 @@
         <v>307</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>49</v>
+        <v>343</v>
+      </c>
+      <c r="I70" s="2">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2">
+        <v>0</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>339</v>
       </c>
       <c r="L70" s="2"/>
       <c r="M70" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -4550,7 +4632,7 @@
         <v>263</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>318</v>
@@ -4568,13 +4650,13 @@
         <v>307</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I71" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="J71" s="2" t="s">
-        <v>340</v>
+      <c r="I71" s="2">
+        <v>0</v>
+      </c>
+      <c r="J71" s="2">
+        <v>0</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>339</v>
@@ -4642,11 +4724,11 @@
       <c r="H73" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="I73" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>49</v>
+      <c r="I73" s="2">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2">
+        <v>0</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>49</v>
@@ -4707,7 +4789,7 @@
         <v>320</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>179</v>
@@ -4722,7 +4804,7 @@
         <v>328</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I75" s="2">
         <v>39.045227799999999</v>
@@ -4731,39 +4813,39 @@
         <v>-77.486494199999996</v>
       </c>
       <c r="K75" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="L75" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="L75" s="2" t="s">
+      <c r="M75" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="M75" s="2" t="s">
+    </row>
+    <row r="76" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" ht="84" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G76" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>369</v>
       </c>
       <c r="I76" s="2">
         <v>38.906303508879397</v>
@@ -4772,37 +4854,37 @@
         <v>-77.222641329237604</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L76" s="2"/>
       <c r="M76" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="H77" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="I77" s="2">
         <v>38.875816034503501</v>
@@ -4811,37 +4893,37 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L77" s="2"/>
       <c r="M77" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F78" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G78" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="G78" s="2" t="s">
-        <v>374</v>
-      </c>
       <c r="H78" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I78" s="2">
         <v>38.875816034503501</v>
@@ -4850,37 +4932,37 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="I79" s="2">
         <v>38.873610192974397</v>
@@ -4889,37 +4971,37 @@
         <v>-77.3055466310296</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>322</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>110</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I80" s="2">
         <v>38.868590773014198</v>
@@ -4928,22 +5010,22 @@
         <v>-77.224144877053305</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>322</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>13</v>
@@ -4952,13 +5034,13 @@
         <v>33</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G81" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="H81" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="I81" s="2">
         <v>38.774379099999997</v>
@@ -4970,35 +5052,35 @@
         <v>18</v>
       </c>
       <c r="L81" s="2"/>
-      <c r="M81" s="7" t="s">
-        <v>410</v>
+      <c r="M81" s="8" t="s">
+        <v>409</v>
       </c>
       <c r="N81" s="2"/>
     </row>
     <row r="82" spans="1:14" ht="168" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="H82" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>394</v>
       </c>
       <c r="I82" s="2">
         <v>38.8060490968736</v>
@@ -5007,37 +5089,37 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L82" s="2"/>
       <c r="M82" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I83" s="2">
         <v>38.8060490968736</v>
@@ -5046,37 +5128,37 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I84" s="2">
         <v>38.8553917225858</v>
@@ -5085,37 +5167,37 @@
         <v>-77.362718702194798</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="168" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="G85" s="2" t="s">
+      <c r="H85" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="I85" s="2">
         <v>38.854251580169802</v>
@@ -5124,22 +5206,22 @@
         <v>-77.356579302194902</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>13</v>
@@ -5148,13 +5230,13 @@
         <v>33</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G86" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="H86" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="I86" s="2">
         <v>38.8553408</v>
@@ -5163,24 +5245,24 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L86" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="M86" s="8" t="s">
         <v>414</v>
-      </c>
-      <c r="M86" s="7" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>13</v>
@@ -5189,13 +5271,13 @@
         <v>33</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G87" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>418</v>
       </c>
       <c r="I87" s="2">
         <v>38.8553408</v>
@@ -5204,24 +5286,24 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L87" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="M87" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="M87" s="7" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="105" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:14" ht="126" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>323</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>13</v>
@@ -5230,13 +5312,13 @@
         <v>33</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G88" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H88" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="I88" s="2">
         <v>38.8553408</v>
@@ -5245,12 +5327,12 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="M88" s="7"/>
+        <v>413</v>
+      </c>
+      <c r="M88" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5283,8 +5365,9 @@
     <hyperlink ref="M87" r:id="rId27" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
     <hyperlink ref="M34" r:id="rId28" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
     <hyperlink ref="M36" r:id="rId29" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
+    <hyperlink ref="M32" r:id="rId30" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a couple of housing services for loudoun
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666ECD58-7FC7-F543-B5F2-B6C99A7ACEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88132DC-CD7D-42BD-A796-F5E58E92E656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="500" windowWidth="15920" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="438">
   <si>
     <t>County</t>
   </si>
@@ -1339,12 +1339,42 @@
   <si>
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Transportation/Behavioral-Health-Transportation-Program.aspx</t>
   </si>
+  <si>
+    <t>Loudoun Abused Women’s Shelter</t>
+  </si>
+  <si>
+    <t>females who are victims of domestic violence and sexual assault who are fleeing abuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides Shelter to women who are fleeing domestic violence/sexual assualt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAWS </t>
+  </si>
+  <si>
+    <t>https://www.lcsj.org/services/</t>
+  </si>
+  <si>
+    <t>Mobile Hope</t>
+  </si>
+  <si>
+    <t>0-24</t>
+  </si>
+  <si>
+    <t>Loudoun County Youth Unstably Housed or Homeless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides basic needs to Loudoun County Youth (shelter, food, clothing, hygiene care) and prepares youth for independent lives such as paying SAT testing fees, providing classes in money management and securing employment if needed on an individual basis through case management </t>
+  </si>
+  <si>
+    <t>https://mobile-hope.org/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1391,6 +1421,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1413,7 +1450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1438,6 +1475,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1753,13 +1792,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
@@ -1775,7 +1814,7 @@
     <col min="13" max="13" width="54" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1816,7 +1855,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1857,7 +1896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1937,7 +1976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1978,7 +2017,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2019,7 +2058,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2060,7 +2099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2101,7 +2140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2142,7 +2181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2183,7 +2222,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2224,7 +2263,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2265,7 +2304,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -2302,7 +2341,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2339,7 +2378,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2380,7 +2419,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -2421,7 +2460,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -2462,7 +2501,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -2503,7 +2542,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2544,7 +2583,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -2585,7 +2624,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -2626,7 +2665,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -2667,7 +2706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -2706,7 +2745,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>263</v>
       </c>
@@ -2747,7 +2786,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>263</v>
       </c>
@@ -2788,7 +2827,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>263</v>
       </c>
@@ -2829,7 +2868,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>263</v>
       </c>
@@ -2870,7 +2909,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>263</v>
       </c>
@@ -2909,7 +2948,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>263</v>
       </c>
@@ -2950,7 +2989,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>263</v>
       </c>
@@ -2991,7 +3030,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>263</v>
       </c>
@@ -3030,7 +3069,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>263</v>
       </c>
@@ -3071,7 +3110,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>263</v>
       </c>
@@ -3112,7 +3151,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>263</v>
       </c>
@@ -3153,7 +3192,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>263</v>
       </c>
@@ -3194,7 +3233,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>263</v>
       </c>
@@ -3235,7 +3274,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>263</v>
       </c>
@@ -3276,7 +3315,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>263</v>
       </c>
@@ -3317,7 +3356,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
@@ -3358,7 +3397,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>10</v>
       </c>
@@ -3399,7 +3438,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
@@ -3440,7 +3479,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
@@ -3481,7 +3520,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -3522,7 +3561,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -3563,7 +3602,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -3604,7 +3643,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>10</v>
       </c>
@@ -3645,7 +3684,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>222</v>
       </c>
@@ -3686,7 +3725,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>222</v>
       </c>
@@ -3727,7 +3766,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -3768,7 +3807,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>10</v>
       </c>
@@ -3809,7 +3848,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>10</v>
       </c>
@@ -3850,7 +3889,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>10</v>
       </c>
@@ -3891,7 +3930,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>10</v>
       </c>
@@ -3932,7 +3971,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>10</v>
       </c>
@@ -3973,7 +4012,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>263</v>
       </c>
@@ -4014,7 +4053,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>263</v>
       </c>
@@ -4055,7 +4094,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>263</v>
       </c>
@@ -4096,7 +4135,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>263</v>
       </c>
@@ -4137,7 +4176,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>263</v>
       </c>
@@ -4178,7 +4217,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>263</v>
       </c>
@@ -4219,7 +4258,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>263</v>
       </c>
@@ -4260,7 +4299,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>263</v>
       </c>
@@ -4301,7 +4340,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>263</v>
       </c>
@@ -4342,7 +4381,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>263</v>
       </c>
@@ -4383,7 +4422,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>263</v>
       </c>
@@ -4424,7 +4463,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>263</v>
       </c>
@@ -4465,7 +4504,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>263</v>
       </c>
@@ -4506,7 +4545,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>263</v>
       </c>
@@ -4547,7 +4586,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>263</v>
       </c>
@@ -4588,7 +4627,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>263</v>
       </c>
@@ -4627,7 +4666,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>263</v>
       </c>
@@ -4668,7 +4707,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>263</v>
       </c>
@@ -4699,7 +4738,7 @@
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>263</v>
       </c>
@@ -4740,7 +4779,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" ht="41" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>10</v>
       </c>
@@ -4781,7 +4820,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>10</v>
       </c>
@@ -4822,7 +4861,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>399</v>
       </c>
@@ -4861,7 +4900,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" ht="82" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>399</v>
       </c>
@@ -4900,7 +4939,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" ht="102.5" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>399</v>
       </c>
@@ -4939,7 +4978,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>399</v>
       </c>
@@ -4978,7 +5017,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>399</v>
       </c>
@@ -5017,7 +5056,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>399</v>
       </c>
@@ -5057,7 +5096,7 @@
       </c>
       <c r="N81" s="2"/>
     </row>
-    <row r="82" spans="1:14" ht="168" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="143.5" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>399</v>
       </c>
@@ -5096,7 +5135,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>399</v>
       </c>
@@ -5135,7 +5174,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>399</v>
       </c>
@@ -5174,7 +5213,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="168" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" ht="164" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>399</v>
       </c>
@@ -5213,7 +5252,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
         <v>399</v>
       </c>
@@ -5254,7 +5293,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
         <v>399</v>
       </c>
@@ -5295,7 +5334,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="102.5" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
         <v>399</v>
       </c>
@@ -5333,6 +5372,88 @@
         <v>413</v>
       </c>
       <c r="M88" s="8"/>
+    </row>
+    <row r="89" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L89" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="M89" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" s="9" customFormat="1" ht="82" x14ac:dyDescent="0.45">
+      <c r="A90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="I90" s="9">
+        <v>39.110039999999998</v>
+      </c>
+      <c r="J90" s="9">
+        <v>-77.557019999999994</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L90" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="M90" s="11" t="s">
+        <v>437</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5366,8 +5487,10 @@
     <hyperlink ref="M34" r:id="rId28" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
     <hyperlink ref="M36" r:id="rId29" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
     <hyperlink ref="M32" r:id="rId30" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
+    <hyperlink ref="M89" r:id="rId31" xr:uid="{61331B93-B388-421E-BA89-53312F427E23}"/>
+    <hyperlink ref="M90" r:id="rId32" xr:uid="{55652876-144A-48FA-9BF6-C9358D435D0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the combined excel file, added folder for images
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666ECD58-7FC7-F543-B5F2-B6C99A7ACEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8E255A-C784-A645-B24B-8B26877F2091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="500" windowWidth="15920" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="2860" yWindow="500" windowWidth="25360" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="427">
   <si>
     <t>County</t>
   </si>
@@ -87,9 +87,6 @@
     <t> affiliated with the Virginia Foster Care System</t>
   </si>
   <si>
-    <t> Connecting them to community resources, scholarship opportunities and other support</t>
-  </si>
-  <si>
     <t>Alexandria</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>14-25</t>
   </si>
   <si>
-    <t>who either aged out of foster care or still in fsoter care;</t>
-  </si>
-  <si>
     <t> Funds can be applied toward, but not limited to, colleges, universities, community colleges, vocational programs, and one-year training institution</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>14-21</t>
   </si>
   <si>
-    <t> assists in developing the skills necessary to make the transition from foster care to independent living; Department of Social Services</t>
-  </si>
-  <si>
     <t>https://www.dss.virginia.gov/family/fc/independent.cgi</t>
   </si>
   <si>
@@ -201,9 +192,6 @@
     <t>TANF recipient</t>
   </si>
   <si>
-    <t>offers case management and support services to Loudoun County residents</t>
-  </si>
-  <si>
     <t>Leesburg</t>
   </si>
   <si>
@@ -222,9 +210,6 @@
     <t>Need IDs, past school records, Verification of Foster Care or receiving public assistance</t>
   </si>
   <si>
-    <t>Department of Labor; 1-on-1 training, resume building, interview prep, labor market review, etc. ; need verification of foster care or receiving public assistance </t>
-  </si>
-  <si>
     <t>Rachael Tichacek</t>
   </si>
   <si>
@@ -249,15 +234,9 @@
     <t>Housing Choice Voucher Program "Formerly Section 8</t>
   </si>
   <si>
-    <t>household income at or below 50 percent of the area median income $142,000; must apply and will be placed on waiting list that becomes open</t>
-  </si>
-  <si>
     <t>Affordable Dwelling Unit Program</t>
   </si>
   <si>
-    <t>affordable units for rent and sell for income-eligible citizen who live and work in the county;  must apply online and in person 10 days after online submission. The processor with take 2-3 weeks through through email</t>
-  </si>
-  <si>
     <t>Route 54 (Safe T-ride)</t>
   </si>
   <si>
@@ -279,9 +258,6 @@
     <t>Must have Medicaid number</t>
   </si>
   <si>
-    <t>non-emergency and urgent medical appointments; Must make requests 5 days early; Department of Medical Assistance Services </t>
-  </si>
-  <si>
     <t>Virginia Department of Medical Assistance Services</t>
   </si>
   <si>
@@ -312,9 +288,6 @@
     <t>under 19 years old, not insured and fall below family income of $2,201 monthly </t>
   </si>
   <si>
-    <t>covers all the medical care that growing children need to stay healthy and if they get sick or hurt; no enrollment costs or monthly premiums; no copays</t>
-  </si>
-  <si>
     <t>Local Department of Social Services</t>
   </si>
   <si>
@@ -330,9 +303,6 @@
     <t>if they were in foster care and had Medicaid in any state on their 18th birthday</t>
   </si>
   <si>
-    <t> no income limit for former foster care youths </t>
-  </si>
-  <si>
     <t>https://www.coverva.org/en/adults-19-64-years-old</t>
   </si>
   <si>
@@ -465,9 +435,6 @@
     <t>Involved in or transitioning from other Department of Human Service system; Diagnosed with serious mental illness, mental illness and substance abuse; Desires to live independently</t>
   </si>
   <si>
-    <t>make 24 units available annually for Office of Behavioral Health (OBH) priority transition-age youth, with psychiatric disabilities; connected to financial, advocacy and legal resources</t>
-  </si>
-  <si>
     <t>Mulitple locations </t>
   </si>
   <si>
@@ -510,9 +477,6 @@
     <t>Live in a household whose total income is no more than 200% of the federal Income Poverty Guidelines</t>
   </si>
   <si>
-    <t>This program has services that are for the TAY if they would have roadblocks keeping them from getting ahead or earn less than what they need to live. The services would help the TAY figure out their strengths and weakness, create a plan to reach their goals, and connect to those resources to help them achieve their goals</t>
-  </si>
-  <si>
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx</t>
   </si>
   <si>
@@ -522,15 +486,9 @@
     <t>Be receiving behavioral health services from a BHTP-participating, Department of Human services (DHS)- contracted provider. Live at least one-half mile from an eligible destination AND </t>
   </si>
   <si>
-    <t>This program helps citizens that need transportation due to a behavioral health condition. It is for any service that will help them be able to function as an individual while receiving care. </t>
-  </si>
-  <si>
     <t>Medicial Assistance Transportation Program</t>
   </si>
   <si>
-    <t>This program provides free public transportation (bus, subway and incline) ahead-of-time ticket, reimbursement for your use of public transportation or a private car, and free door-to-door service, when medically necessary, via shared-ride or ride-hailing service.</t>
-  </si>
-  <si>
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Transportation/Medical-Assistance-Transportation-Program.aspx</t>
   </si>
   <si>
@@ -597,9 +555,6 @@
     <t>Those currently homeless or at risk of becoming homeless</t>
   </si>
   <si>
-    <t>A coalition of services providing support for the homeless or those at risk of becoming homeless.</t>
-  </si>
-  <si>
     <t>Continuum of Care | Loudoun County, VA - Official Website</t>
   </si>
   <si>
@@ -610,9 +565,6 @@
   </si>
   <si>
     <t xml:space="preserve">Those recovering from drug and alcohol addiction aiming to prevent relapse </t>
-  </si>
-  <si>
-    <t>Democratically run housing for those recovering from substance abuse who wish to be drug free and support others in their efforts</t>
   </si>
   <si>
     <t>Oxford House World Services</t>
@@ -704,9 +656,6 @@
     <t>Work in Loudoun - Loudoun County Economic Development, VA</t>
   </si>
   <si>
-    <t>Northern Virginia</t>
-  </si>
-  <si>
     <t>OAR</t>
   </si>
   <si>
@@ -716,9 +665,6 @@
     <t>Those currently incarcerated or recently incarcerated</t>
   </si>
   <si>
-    <t>Works with those involved in the criminal justice system in Loudoun, Fairfax and Prince William County to provide employment assistance, post-release skill classes, community service substitutes for misdemeanor offers clothing, food, transportation, medication and violence prevention programs.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Leesburg, VA </t>
   </si>
   <si>
@@ -746,10 +692,6 @@
     <t xml:space="preserve">Those interested in continuing their education at a highschool level 18 and older </t>
   </si>
   <si>
-    <t xml:space="preserve">Provides education opportunities such as General Education Development and English as a Second Language programs as well as support services to adults 18 and older in Loudoun County.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Loudoun County Public Schools </t>
   </si>
   <si>
@@ -804,10 +746,6 @@
     <t>Must have Medicaid and associated Medicaid number</t>
   </si>
   <si>
-    <t xml:space="preserve">Offers free transportation for non-emergency and urgent medical appointments to those who have Medicaid.
-</t>
-  </si>
-  <si>
     <t>Loudoun County</t>
   </si>
   <si>
@@ -838,9 +776,6 @@
     <t>Pennsylvania youth aged 18-24 experiencing housing inequality in Allegheny, Armstrong and Westmoreland(16-24)</t>
   </si>
   <si>
-    <t>Home hosting programs for those aged 18-24 experiencing housing insecurity.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Valley Youth House </t>
   </si>
   <si>
@@ -871,9 +806,6 @@
     <t>18-24 year olds who are or have been involved in the justice system in Allegheny County</t>
   </si>
   <si>
-    <t>Provides paid vocational training opportunities, comprehensive career and education services and transportation funding to those aged 18-24 in Allegheny county who have past or present criminal justice system involvement</t>
-  </si>
-  <si>
     <t>Partner4Work</t>
   </si>
   <si>
@@ -881,9 +813,6 @@
   </si>
   <si>
     <t>STRIVE Program</t>
-  </si>
-  <si>
-    <t>Provides case management and career services, industry-recognized credentialing programs, hands-on job training, transitional jobs, and comprehensive supportive services for 18 to 24 year olds involved in the justice system in Allegheny County.</t>
   </si>
   <si>
     <t>Reentry Programs - Partner4Work</t>
@@ -1028,9 +957,6 @@
     <t>Those who are currently or are at risk of experiencing homelessness</t>
   </si>
   <si>
-    <t>provides extensive services to prevent, support and help end homelessness within Loudoun and surrounding counties</t>
-  </si>
-  <si>
     <t>https://www.voachesapeake.org/lhsc</t>
   </si>
   <si>
@@ -1079,9 +1005,6 @@
     <t> Community College of Allegheny County.</t>
   </si>
   <si>
-    <t>career services program</t>
-  </si>
-  <si>
     <t xml:space="preserve">Education </t>
   </si>
   <si>
@@ -1106,16 +1029,9 @@
     <t>https://www.ccac.edu/workforce/index.php</t>
   </si>
   <si>
-    <t xml:space="preserve">Programs designed to provide skills and knowledge needed to remain competitive in a variety of industries.
-</t>
-  </si>
-  <si>
     <t>https://www.alleghenycounty.us/Human-Services/Resources/Education/DHS-Methods.aspx</t>
   </si>
   <si>
-    <t>Individualized support for youth with educational barriers. The Liaison works within the framework of the Department of Human Services to coordinate continued education opportunities.</t>
-  </si>
-  <si>
     <t>Allegheny County youth with educational barriers</t>
   </si>
   <si>
@@ -1146,9 +1062,6 @@
     <t>Meet U.S. Department of Housing and Urban Development’s (HUD) definition of homelessness, meaning they are living in a homeless shelter, sleeping on the streets or another place not meant for human habitation, or fleeing domestic violence in Fairfax County, and be referred by a community provider</t>
   </si>
   <si>
-    <t>Long-term housing and support for youth aged 18-24 who are experiencing homelessness or living in an unsafe situation; Youth often come to us who have aged out of foster care, been kicked out of their parent or guardian’s home with insufficient resources, or have run away from an unsafe situation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dunn Loring </t>
   </si>
   <si>
@@ -1164,9 +1077,6 @@
     <t xml:space="preserve">Need a referral </t>
   </si>
   <si>
-    <t>focuses on providing: subsidized apartments that provide stable housing to homeless youth, viable vocational/career skills-building &amp; training, life skills prep, support services (including: shelter, food, clothing, medical assistance, crisis intervention, counseling, referrals &amp; aftercare services)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chantilly </t>
   </si>
   <si>
@@ -1188,9 +1098,6 @@
     <t xml:space="preserve">Referred by Fairfax County, working preference, earning 30% to 50% of area median income (AMI), living or working in Fairfax County, Not open referral </t>
   </si>
   <si>
-    <t>provides case management and supportive services like job training and financial education, depending on client needs, as well as rental assistance for up to 24 months</t>
-  </si>
-  <si>
     <t>Oakton</t>
   </si>
   <si>
@@ -1221,27 +1128,13 @@
     <t xml:space="preserve">Fairfax resident </t>
   </si>
   <si>
-    <t xml:space="preserve">Daytime: M-F (five days a week); five class periods lasting 75 minutes each and a 30 minute learning seminar; semester program
-Evening: Two 90 minute classes nightly M-W and/or T-Th; year-long classes
-Day program tuition is $80.00 per semester
-Evening program tuition is $160.00 per school year
-General Education students aged 18—19 do not pay tuition
-English Language Learners (ELLs) aged 18—21 do not pay tuition </t>
-  </si>
-  <si>
     <t xml:space="preserve">Springfield </t>
   </si>
   <si>
     <t>https://fairfaxadulths.fcps.edu/about</t>
   </si>
   <si>
-    <t>helps prepare *Fairfax County residents  to take the GED test</t>
-  </si>
-  <si>
     <t>Permanency and Life Skills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provides SAT prep, application fees, and dorm supplies, household items, moving fees and gift cards for gas, transportation, Department of Family Services </t>
   </si>
   <si>
     <t xml:space="preserve">Fairfax </t>
@@ -1260,84 +1153,178 @@
 annual income that meets the 225% federal poverty levels by household size</t>
   </si>
   <si>
-    <t>Options:
-Taxicabs
-Rideshare services (Uber and Lyft)
-Public Transportation: bus and rail via SmarTrip card
-Capital BikeShare rentals; 
+    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/tops</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>TIP- Transition to Independence Program</t>
+  </si>
+  <si>
+    <t>Must be enrolled at the Davis and Pulley Career Centers and have an IEP</t>
+  </si>
+  <si>
+    <t>https://www.fcps.edu/academics/academic-overview/special-education-instruction/career-and-transition-services/transition-to-independence</t>
+  </si>
+  <si>
+    <t>Taxi Access</t>
+  </si>
+  <si>
+    <t>Must be a resident of fairfax county or the City of Fairfax. Must be a registered user of Metro Access.</t>
+  </si>
+  <si>
+    <t>Department of Neighborhood and Community Services</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/taxi-voucherprogram</t>
+  </si>
+  <si>
+    <t>Dial-A_Ride</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must be a resident of Fairfax County or the City of Fairfax. Annual income must be 225% below Federal Poverty Guidelines. </t>
+  </si>
+  <si>
+    <t>Fairfax County Travel Training</t>
+  </si>
+  <si>
+    <t>Must be a resident of Fairfax county or the City of Fairfax.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must meet the income based requirements on the self-screening questionaire. This does require a criminal background check. </t>
+  </si>
+  <si>
+    <t>The household must make less than 50% of the Area Median Income (AMI) for the area where the voucher will be used (this is known as the income limit).</t>
+  </si>
+  <si>
+    <t>Must be eligbile for Medicaid and a resident of Allegheny</t>
+  </si>
+  <si>
+    <t>Medicaid became available to eligible adult Virginians ages 19 – 64 who live in households earning ≤138% of the Federal Poverty Level ($17,775 for an individual or $30,305 for a family of three in 2021)</t>
+  </si>
+  <si>
+    <t>19-24</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Transportation/Behavioral-Health-Transportation-Program.aspx</t>
+  </si>
+  <si>
+    <t>who either aged out of foster care or still in foster care</t>
+  </si>
+  <si>
+    <t>Connecting them to community resources, scholarship opportunities and other support</t>
+  </si>
+  <si>
+    <t> Assists in developing the skills necessary to make the transition from foster care to independent living; Department of Social Services</t>
+  </si>
+  <si>
+    <t>Offers case management and support services to Loudoun County residents</t>
+  </si>
+  <si>
+    <t>1-on-1 training, resume building, interview prep, labor market review, etc. ; need verification of foster care or receiving public assistance </t>
+  </si>
+  <si>
+    <t>must apply and will be placed on waiting list that becomes open</t>
+  </si>
+  <si>
+    <t>Affordable units for rent and sell for those who qualify in the county;  must apply online and in person 10 days after online submission, could take 2-3 weeks</t>
+  </si>
+  <si>
+    <t>Non-emergency and urgent medical appointments; Must make requests 5 days early; Department of Medical Assistance Services </t>
+  </si>
+  <si>
+    <t>Covers all the medical care that growing children need to stay healthy and if they get sick or hurt; no enrollment costs or monthly premiums; no copays</t>
+  </si>
+  <si>
+    <t> No income limit for former foster care youths </t>
+  </si>
+  <si>
+    <t>Make 24 units available annually for Office of Behavioral Health (OBH) priority transition-age youth, with psychiatric disabilities; connected to financial, advocacy and legal resources</t>
+  </si>
+  <si>
+    <t>For TAYs if they would have roadblocks keeping them from getting ahead or earn less than what they need to live, figure out their strengths and weakness, create a plan to reach their goals, and connect to those resources to help them achieve their goals</t>
+  </si>
+  <si>
+    <t>Helps citizens that need transportation due to a behavioral health condition; will help them be able to function as an individual while receiving care. </t>
+  </si>
+  <si>
+    <t>Provides free public transportation (bus, subway and incline) ahead-of-time ticket, reimbursement for your use of public transportation or a private car, and free door-to-door service, when medically necessary, via shared-ride or ride-hailing service.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Help citizens find the right healthcare coverage for them. </t>
+  </si>
+  <si>
+    <t>Support for the homeless or those at risk of becoming homeless.</t>
+  </si>
+  <si>
+    <t>Housing for those recovering from substance abuse who wish to be drug free and support others in their efforts</t>
+  </si>
+  <si>
+    <t>Works with those involved in the criminal justice system to provide employment assistance, post-release skill classes, community service substitutes for misdemeanor offers clothing, food, transportation, medication and violence prevention programs.</t>
+  </si>
+  <si>
+    <t>Provides education opportunities such as General Education Development and English as a Second Language programs as well as support services to adults 18 and older in Loudoun County</t>
+  </si>
+  <si>
+    <t>Offers free transportation for non-emergency and urgent medical appointments to those who have Medicaid</t>
+  </si>
+  <si>
+    <t>Home hosting programs for those aged 18-24 experiencing housing insecurity</t>
+  </si>
+  <si>
+    <t>Provides paid vocational training opportunities, comprehensive career and education services and transportation funding in Allegheny who have past or present criminal justice system involvement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides case management and career services, industry-recognized credentialing programs, hands-on job training, transitional jobs, and comprehensive supportive services for those involved in the justice system </t>
+  </si>
+  <si>
+    <t>Individualized support for youth with educational barriers</t>
+  </si>
+  <si>
+    <t>Programs designed to provide skills and knowledge needed to remain competitive in a variety of industries</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it is open for student travelers  who want to learn about the public transit system; help plan their trip, read bus and rail schedules, pay bus fares, transfer, reach specific destination, access local transportation resources</t>
+  </si>
+  <si>
+    <t>Travel affordable, safely, and independently with the purchase of a discounted taxicab coupon. Cost $10 per $33 coupon book. 16 coupon books per year (July 1- June 30)</t>
+  </si>
+  <si>
+    <t>Travel affordable, safely, and independently with the purchase of a discounted taxicab coupon. Cost $10 per $33 coupon book. 8 coupon books per year (July 1- June 30)</t>
+  </si>
+  <si>
+    <t>Options:Taxicabs, Rideshare services (Uber and Lyft), Public Transportation: bus and rail via SmarTrip card, Capital BikeShare rentals; 
 Apply online or send in application</t>
   </si>
   <si>
-    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/tops</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>TIP- Transition to Independence Program</t>
-  </si>
-  <si>
-    <t>Must be enrolled at the Davis and Pulley Career Centers and have an IEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This programs helps those students with IEP build employable skills at the local community colleges. It helps them have work-based learning, coordinate to postsecondary resources and services, provide an opportunity to experience post-secondary education and help them achieve their goals. </t>
-  </si>
-  <si>
-    <t>https://www.fcps.edu/academics/academic-overview/special-education-instruction/career-and-transition-services/transition-to-independence</t>
-  </si>
-  <si>
-    <t>Taxi Access</t>
-  </si>
-  <si>
-    <t>Must be a resident of fairfax county or the City of Fairfax. Must be a registered user of Metro Access.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> This program allows qualified users to travel affordable, safely, and independently with the purchase of a discounted taxicab coupon. Cost $10 per $33 coupon book. 8 coupon books per year (July 1- June 30)</t>
-  </si>
-  <si>
-    <t>Department of Neighborhood and Community Services</t>
-  </si>
-  <si>
-    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/taxi-voucherprogram</t>
-  </si>
-  <si>
-    <t>Dial-A_Ride</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must be a resident of Fairfax County or the City of Fairfax. Annual income must be 225% below Federal Poverty Guidelines. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> This program allows qualified users to travel affordable, safely, and independently with the purchase of a discounted taxicab coupon. Cost $10 per $33 coupon book. 16 coupon books per year (July 1- June 30)</t>
-  </si>
-  <si>
-    <t>Fairfax County Travel Training</t>
-  </si>
-  <si>
-    <t>Must be a resident of Fairfax county or the City of Fairfax.</t>
-  </si>
-  <si>
-    <t>This program is designed for independent senior services, but it is open for student travelers  who want to learn about the public transit system. This  course is designed to help citizens plan their trip, read bus and rail schedules, pay bus fares, transfer, reach specific destination, access local transportation resources. Call the Travel Training program at 703-877-5800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must meet the income based requirements on the self-screening questionaire. This does require a criminal background check. </t>
-  </si>
-  <si>
-    <t>The household must make less than 50% of the Area Median Income (AMI) for the area where the voucher will be used (this is known as the income limit).</t>
-  </si>
-  <si>
-    <t>Must be eligbile for Medicaid and a resident of Allegheny</t>
-  </si>
-  <si>
-    <t>Medicaid became available to eligible adult Virginians ages 19 – 64 who live in households earning ≤138% of the Federal Poverty Level ($17,775 for an individual or $30,305 for a family of three in 2021)</t>
-  </si>
-  <si>
-    <t>19-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This program helps citizens find the right healthcare coverage for them. </t>
-  </si>
-  <si>
-    <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Transportation/Behavioral-Health-Transportation-Program.aspx</t>
+    <t xml:space="preserve">Provides SAT prep, application fees, and dorm supplies, household items, moving fees and gift cards for gas, transportation, Department of Family Services </t>
+  </si>
+  <si>
+    <t>Helps prepare *Fairfax County residents  to take the GED test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daytime: M-F (five days a week): semester program; Evening: year-long classes; $80-$160 
+General Education students aged 18—19 do not pay tuition
+English Language Learners (ELLs) aged 18—21 do not pay tuition </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helps those students with IEP build employable skills at the local community colleges; helps them have work-based learning, coordinate to postsecondary resources and services, provide an opportunity to experience post-secondary education and help them achieve their goals. </t>
+  </si>
+  <si>
+    <t>Provides case management and supportive services like job training and financial education, depending on client needs, as well as rental assistance for up to 24 months</t>
+  </si>
+  <si>
+    <t>Focuses on providing: subsidized apartments that provide stable housing to homeless youth, viable vocational/career skills-building &amp; training, life skills prep, support services (including: shelter, food, clothing, medical assistance, crisis intervention, counseling, referrals &amp; aftercare services)</t>
+  </si>
+  <si>
+    <t>Long-term housing and support for youth who are experiencing homelessness or living in an unsafe situation; Youth often come to us who have aged out of foster care, or have run away from an unsafe situation</t>
+  </si>
+  <si>
+    <t>Provides extensive services to prevent, support and help end homelessness within Loudoun and surrounding counties</t>
+  </si>
+  <si>
+    <t>Career services program</t>
   </si>
 </sst>
 </file>
@@ -1755,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="G65" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1775,7 +1762,7 @@
     <col min="13" max="13" width="54" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1801,10 +1788,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
@@ -1813,7 +1800,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -1839,7 +1826,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>390</v>
       </c>
       <c r="I2" s="2">
         <v>38.840490000000003</v>
@@ -1848,13 +1835,13 @@
         <v>-77.115129999999994</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -1865,7 +1852,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -1874,13 +1861,13 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="I3" s="2">
         <v>37.538339999999998</v>
@@ -1889,13 +1876,13 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -1906,7 +1893,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -1915,11 +1902,13 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>389</v>
+      </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>391</v>
       </c>
       <c r="I4" s="2">
         <v>37.538339999999998</v>
@@ -1928,13 +1917,13 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.2">
@@ -1945,22 +1934,22 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="I5" s="2">
         <v>39.031359999999999</v>
@@ -1969,13 +1958,13 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -1986,22 +1975,22 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I6" s="2">
         <v>39.015009999999997</v>
@@ -2010,13 +1999,13 @@
         <v>-77.400989999999993</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2027,22 +2016,22 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="I7" s="2">
         <v>39.031359999999999</v>
@@ -2051,13 +2040,13 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="63" x14ac:dyDescent="0.2">
@@ -2068,22 +2057,22 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -2092,13 +2081,13 @@
         <v>0</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2109,22 +2098,22 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I9" s="2">
         <v>39.031359999999999</v>
@@ -2133,13 +2122,13 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2147,25 +2136,25 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>55</v>
+        <v>392</v>
       </c>
       <c r="I10" s="2">
         <v>39.114306589999998</v>
@@ -2174,39 +2163,39 @@
         <v>-77.539617179999993</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>62</v>
+        <v>393</v>
       </c>
       <c r="I11" s="2">
         <v>39.114306589999998</v>
@@ -2215,13 +2204,13 @@
         <v>-77.539617179999993</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2229,25 +2218,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I12" s="2">
         <v>38.917318170000001</v>
@@ -2256,13 +2245,13 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2270,25 +2259,25 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>422</v>
+        <v>384</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>71</v>
+        <v>394</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -2297,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -2307,25 +2296,25 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>421</v>
+        <v>383</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>73</v>
+        <v>395</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -2334,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -2344,25 +2333,25 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I15" s="2">
         <v>39.084557510000003</v>
@@ -2371,13 +2360,13 @@
         <v>-77.555403999999996</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2385,25 +2374,25 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>81</v>
+        <v>396</v>
       </c>
       <c r="I16" s="2">
         <v>37.61065696</v>
@@ -2412,13 +2401,13 @@
         <v>-77.340073020000005</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2426,25 +2415,25 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="I17" s="2">
         <v>39.114571660000003</v>
@@ -2453,39 +2442,39 @@
         <v>-77.540547570000001</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>92</v>
+        <v>397</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -2494,13 +2483,13 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2508,25 +2497,25 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>98</v>
+        <v>398</v>
       </c>
       <c r="I19" s="2">
         <v>0</v>
@@ -2535,13 +2524,13 @@
         <v>0</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -2549,25 +2538,25 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -2576,13 +2565,13 @@
         <v>0</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="63" x14ac:dyDescent="0.2">
@@ -2590,25 +2579,25 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -2617,13 +2606,13 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.2">
@@ -2631,10 +2620,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>13</v>
@@ -2643,13 +2632,13 @@
         <v>14</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -2658,13 +2647,13 @@
         <v>0</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="63" x14ac:dyDescent="0.2">
@@ -2672,25 +2661,25 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -2699,22 +2688,22 @@
         <v>0</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>13</v>
@@ -2723,13 +2712,13 @@
         <v>14</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="I24" s="2">
         <v>40.439188049999998</v>
@@ -2738,24 +2727,24 @@
         <v>-80.001456360000006</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>13</v>
@@ -2764,13 +2753,13 @@
         <v>14</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="I25" s="2">
         <v>40.437306100000001</v>
@@ -2779,39 +2768,39 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I26" s="2">
         <v>40.349269890000002</v>
@@ -2820,39 +2809,39 @@
         <v>-79.832162819999994</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="I27" s="2">
         <v>40.439132790000002</v>
@@ -2861,24 +2850,24 @@
         <v>-79.994721900000002</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>13</v>
@@ -2887,52 +2876,52 @@
         <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>143</v>
+        <v>399</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="I29" s="2">
         <v>40.40062056</v>
@@ -2941,39 +2930,39 @@
         <v>-79.8352431</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="I30" s="2">
         <v>40.40062056</v>
@@ -2982,24 +2971,24 @@
         <v>-79.8352431</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>13</v>
@@ -3008,10 +2997,10 @@
         <v>14</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2">
@@ -3021,39 +3010,39 @@
         <v>-79.8352431</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>158</v>
+        <v>400</v>
       </c>
       <c r="I32" s="2">
         <v>40.439188049999998</v>
@@ -3062,39 +3051,39 @@
         <v>-80.001456360000006</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>162</v>
+        <v>401</v>
       </c>
       <c r="I33" s="2">
         <v>40.437306100000001</v>
@@ -3103,39 +3092,39 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>427</v>
+        <v>388</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>423</v>
+        <v>385</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>164</v>
+        <v>402</v>
       </c>
       <c r="I34" s="2">
         <v>40.437306100000001</v>
@@ -3144,39 +3133,39 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>425</v>
+        <v>387</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>424</v>
+        <v>386</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -3185,39 +3174,39 @@
         <v>0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>423</v>
+        <v>385</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
@@ -3226,39 +3215,39 @@
         <v>0</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="I37" s="2">
         <v>0</v>
@@ -3267,39 +3256,39 @@
         <v>0</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -3308,13 +3297,13 @@
         <v>0</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3322,25 +3311,25 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="I39" s="2">
         <v>39.114409999999999</v>
@@ -3349,13 +3338,13 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3363,25 +3352,25 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>187</v>
+        <v>404</v>
       </c>
       <c r="I40" s="2">
         <v>39.114409999999999</v>
@@ -3390,13 +3379,13 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3404,25 +3393,25 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>192</v>
+        <v>405</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -3431,13 +3420,13 @@
         <v>0</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3445,25 +3434,25 @@
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="I42" s="2">
         <v>39.076819999999998</v>
@@ -3472,13 +3461,13 @@
         <v>-77.549896000000004</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3486,25 +3475,25 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="I43" s="2">
         <v>39.114409999999999</v>
@@ -3513,13 +3502,13 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3527,25 +3516,25 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="I44" s="2">
         <v>39.115279999999998</v>
@@ -3554,13 +3543,13 @@
         <v>-77.564430000000002</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3568,25 +3557,25 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="I45" s="2">
         <v>40.741895</v>
@@ -3595,13 +3584,13 @@
         <v>-73.989307999999994</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3609,25 +3598,25 @@
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="I46" s="2">
         <v>0</v>
@@ -3636,39 +3625,39 @@
         <v>0</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>222</v>
+        <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>226</v>
+        <v>406</v>
       </c>
       <c r="I47" s="2">
         <v>39.108399900000002</v>
@@ -3677,39 +3666,39 @@
         <v>-77.565337</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>222</v>
+        <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="I48" s="2">
         <v>39.114409999999999</v>
@@ -3718,16 +3707,16 @@
         <v>-77.540580000000006</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -3735,22 +3724,22 @@
         <v>11</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>236</v>
+        <v>407</v>
       </c>
       <c r="I49" s="2">
         <v>39.115943000000001</v>
@@ -3759,13 +3748,13 @@
         <v>-77.581795999999997</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3776,22 +3765,22 @@
         <v>11</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="I50" s="2">
         <v>39.114406199999998</v>
@@ -3800,13 +3789,13 @@
         <v>-77.567706299999998</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3814,25 +3803,25 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="I51" s="2">
         <v>37.542472099999998</v>
@@ -3841,13 +3830,13 @@
         <v>-77.435912200000004</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3855,25 +3844,25 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="I52" s="2">
         <v>39.117853099999998</v>
@@ -3882,39 +3871,39 @@
         <v>-77.568151900000004</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>255</v>
+        <v>408</v>
       </c>
       <c r="I53" s="2">
         <v>37.610656959136698</v>
@@ -3923,13 +3912,13 @@
         <v>-77.340073015724201</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3937,25 +3926,25 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="I54" s="2">
         <v>0</v>
@@ -3964,39 +3953,39 @@
         <v>0</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>266</v>
+        <v>409</v>
       </c>
       <c r="I55" s="2">
         <v>0</v>
@@ -4005,39 +3994,39 @@
         <v>0</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="I56" s="2">
         <v>40.439779999999999</v>
@@ -4046,39 +4035,39 @@
         <v>-79.998869999999997</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>277</v>
+        <v>410</v>
       </c>
       <c r="I57" s="2">
         <v>0</v>
@@ -4087,39 +4076,39 @@
         <v>0</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>281</v>
+        <v>411</v>
       </c>
       <c r="I58" s="2">
         <v>0</v>
@@ -4128,39 +4117,39 @@
         <v>0</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="I59" s="2">
         <v>0</v>
@@ -4169,39 +4158,39 @@
         <v>0</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="I60" s="2">
         <v>0</v>
@@ -4210,39 +4199,39 @@
         <v>0</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="I61" s="2">
         <v>0</v>
@@ -4251,39 +4240,39 @@
         <v>0</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="I62" s="2">
         <v>40.407960000000003</v>
@@ -4292,39 +4281,39 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="I63" s="2">
         <v>40.405259100000002</v>
@@ -4333,39 +4322,39 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="I64" s="2">
         <v>40.559510000000003</v>
@@ -4374,39 +4363,39 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>357</v>
+        <v>412</v>
       </c>
       <c r="I65" s="2">
         <v>0</v>
@@ -4415,39 +4404,39 @@
         <v>0</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>355</v>
+        <v>413</v>
       </c>
       <c r="I66" s="2">
         <v>40.427699869999998</v>
@@ -4456,39 +4445,39 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>353</v>
+        <v>328</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="I67" s="2">
         <v>40.427699869999998</v>
@@ -4497,39 +4486,39 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>349</v>
+        <v>324</v>
       </c>
       <c r="I68" s="2">
         <v>40.427699869999998</v>
@@ -4538,39 +4527,39 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>346</v>
+        <v>426</v>
       </c>
       <c r="I69" s="2">
         <v>40.427699869999998</v>
@@ -4579,39 +4568,39 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="I70" s="2">
         <v>0</v>
@@ -4620,37 +4609,37 @@
         <v>0</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="L70" s="2"/>
       <c r="M70" s="4" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="I71" s="2">
         <v>0</v>
@@ -4659,70 +4648,70 @@
         <v>0</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
     </row>
     <row r="73" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="I73" s="2">
         <v>0</v>
@@ -4731,13 +4720,13 @@
         <v>0</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -4745,25 +4734,25 @@
         <v>10</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>329</v>
+        <v>425</v>
       </c>
       <c r="I74" s="2">
         <v>39.078167000000001</v>
@@ -4772,13 +4761,13 @@
         <v>-77.550561000000002</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="21" x14ac:dyDescent="0.2">
@@ -4786,25 +4775,25 @@
         <v>10</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>360</v>
+        <v>333</v>
       </c>
       <c r="I75" s="2">
         <v>39.045227799999999</v>
@@ -4813,39 +4802,39 @@
         <v>-77.486494199999996</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>362</v>
+        <v>335</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>368</v>
+        <v>424</v>
       </c>
       <c r="I76" s="2">
         <v>38.906303508879397</v>
@@ -4854,37 +4843,37 @@
         <v>-77.222641329237604</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
       <c r="L76" s="2"/>
       <c r="M76" s="2" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>374</v>
+        <v>423</v>
       </c>
       <c r="I77" s="2">
         <v>38.875816034503501</v>
@@ -4893,37 +4882,37 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
       <c r="L77" s="2"/>
       <c r="M77" s="2" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>377</v>
+        <v>348</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="I78" s="2">
         <v>38.875816034503501</v>
@@ -4932,37 +4921,37 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>382</v>
+        <v>422</v>
       </c>
       <c r="I79" s="2">
         <v>38.873610192974397</v>
@@ -4971,37 +4960,37 @@
         <v>-77.3055466310296</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>383</v>
+        <v>353</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
       <c r="I80" s="2">
         <v>38.868590773014198</v>
@@ -5010,37 +4999,37 @@
         <v>-77.224144877053305</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>388</v>
+        <v>358</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2" t="s">
-        <v>389</v>
+        <v>359</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>406</v>
+        <v>372</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>407</v>
+        <v>373</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="I81" s="2">
         <v>38.774379099999997</v>
@@ -5049,38 +5038,38 @@
         <v>-77.074015599999996</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L81" s="2"/>
       <c r="M81" s="8" t="s">
-        <v>409</v>
+        <v>374</v>
       </c>
       <c r="N81" s="2"/>
     </row>
-    <row r="82" spans="1:14" ht="168" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>390</v>
+        <v>360</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>391</v>
+        <v>361</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>392</v>
+        <v>362</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="I82" s="2">
         <v>38.8060490968736</v>
@@ -5089,37 +5078,37 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="L82" s="2"/>
       <c r="M82" s="2" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>390</v>
+        <v>360</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>392</v>
+        <v>362</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>396</v>
+        <v>419</v>
       </c>
       <c r="I83" s="2">
         <v>38.8060490968736</v>
@@ -5128,37 +5117,37 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>397</v>
+        <v>365</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>392</v>
+        <v>362</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>398</v>
+        <v>418</v>
       </c>
       <c r="I84" s="2">
         <v>38.8553917225858</v>
@@ -5167,37 +5156,37 @@
         <v>-77.362718702194798</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" ht="168" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="126" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>401</v>
+        <v>368</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>402</v>
+        <v>369</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="I85" s="2">
         <v>38.854251580169802</v>
@@ -5206,37 +5195,37 @@
         <v>-77.356579302194902</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
-        <v>404</v>
+        <v>370</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>410</v>
+        <v>375</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>411</v>
+        <v>376</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="I86" s="2">
         <v>38.8553408</v>
@@ -5245,39 +5234,39 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>413</v>
+        <v>377</v>
       </c>
       <c r="M86" s="8" t="s">
-        <v>414</v>
+        <v>378</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>415</v>
+        <v>379</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F87" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="G87" s="2" t="s">
-        <v>416</v>
-      </c>
       <c r="H87" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I87" s="2">
         <v>38.8553408</v>
@@ -5286,39 +5275,39 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>413</v>
+        <v>377</v>
       </c>
       <c r="M87" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>419</v>
+        <v>382</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="I88" s="2">
         <v>38.8553408</v>
@@ -5327,10 +5316,10 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>413</v>
+        <v>377</v>
       </c>
       <c r="M88" s="8"/>
     </row>

</xml_diff>

<commit_message>
changed insurance to health services in app and excel. Added a second layer to excel for number codes for dendrogram???
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA39CB8F-D951-3045-AB68-83852F87BF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9A1F3C-D280-E344-B9D0-0A3EBCC1EEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="500" windowWidth="25360" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Services" sheetId="1" r:id="rId1"/>
+    <sheet name="number codes " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="415">
   <si>
     <t>County</t>
   </si>
@@ -492,9 +493,6 @@
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Transportation/Medical-Assistance-Transportation-Program.aspx</t>
   </si>
   <si>
-    <t>Insurance</t>
-  </si>
-  <si>
     <t>Health Insurance Marketplace</t>
   </si>
   <si>
@@ -582,10 +580,6 @@
     <t>Provides financial and case management resources to the homeless in Loudoun County</t>
   </si>
   <si>
-    <t>19520 Meadowview Court
-Leesburg, VA 20175</t>
-  </si>
-  <si>
     <t>Volunteers of America Chesapeake</t>
   </si>
   <si>
@@ -601,9 +595,6 @@
     <t>Provides free-of-charge guidance, equipment and resources to ex-offenders seeking jobs or ex-offenders with businesses.</t>
   </si>
   <si>
-    <t>Leesburg, VA</t>
-  </si>
-  <si>
     <t>Loudoun County Health and Human Services</t>
   </si>
   <si>
@@ -622,10 +613,6 @@
     <t>Free employment service that provides job search and placement services to Loudoun area adults</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Leesburg, VA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Crossroads Jobs Inc. </t>
   </si>
   <si>
@@ -665,39 +652,9 @@
     <t>Those currently incarcerated or recently incarcerated</t>
   </si>
   <si>
-    <t xml:space="preserve">Leesburg, VA </t>
-  </si>
-  <si>
     <t>Loudoun County (oarnova.org)</t>
   </si>
   <si>
-    <t>Youth WIOA Program</t>
-  </si>
-  <si>
-    <t>Those interested in gaining skills and education for success in the workforce</t>
-  </si>
-  <si>
-    <t>Provides job, internship and apprenticeship opportunities as well as career development programs and education educational support to those aged 17-24 in the Northern Virginia area.</t>
-  </si>
-  <si>
-    <t>Virginia Career Works Northern Region</t>
-  </si>
-  <si>
-    <t>Contact - Virginia Career Works Northern Region (vcwnorthern.com)</t>
-  </si>
-  <si>
-    <t>Loudoun County Public Schools Adult Education Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Those interested in continuing their education at a highschool level 18 and older </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loudoun County Public Schools </t>
-  </si>
-  <si>
-    <t>Instructional Programs / Adult Education (lcps.org)</t>
-  </si>
-  <si>
     <t>Loudoun Literacy Council</t>
   </si>
   <si>
@@ -713,18 +670,6 @@
     <t>19-64</t>
   </si>
   <si>
-    <t>Low-income adult aged 19-64 and not an inmate of a public institution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provides medical coverage to eligible people in need </t>
-  </si>
-  <si>
-    <t>Richmond, VA</t>
-  </si>
-  <si>
-    <t>https://www.dmas.virginia.gov/about-us/contact/our-location/</t>
-  </si>
-  <si>
     <t>Loudoun Free Clinic</t>
   </si>
   <si>
@@ -740,18 +685,9 @@
     <t>https://www.loudounfreeclinic.org/</t>
   </si>
   <si>
-    <t>Medicaid Transportation</t>
-  </si>
-  <si>
-    <t>Must have Medicaid and associated Medicaid number</t>
-  </si>
-  <si>
     <t>Loudoun County</t>
   </si>
   <si>
-    <t>http://transportation.dmas.virginia.gov/Contact-Us</t>
-  </si>
-  <si>
     <t>Care Mobile Tranportation</t>
   </si>
   <si>
@@ -791,9 +727,6 @@
     <t>Offers a variety of housing services to those at risk for homelessness</t>
   </si>
   <si>
-    <t>Pittsburgh, PA</t>
-  </si>
-  <si>
     <t>Allegheny County Department of Human Services</t>
   </si>
   <si>
@@ -860,9 +793,6 @@
     <t xml:space="preserve"> Provides assistance to those with criminal backgrounds searching for a job</t>
   </si>
   <si>
-    <t xml:space="preserve">Homestead, PA </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mon Valley Initiative </t>
   </si>
   <si>
@@ -878,9 +808,6 @@
     <t xml:space="preserve"> Individualized case management services in finance, employment, education and housing for adults making 200% of the federal poverty level or less.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Turtle Creek, PA</t>
-  </si>
-  <si>
     <t>Human Services Center Corporation</t>
   </si>
   <si>
@@ -896,10 +823,6 @@
     <t>Virtual career counseling, assessment and assistance through WorkAble for all Alleghany County residents</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Allison Park, PA </t>
-  </si>
-  <si>
     <t>North Hills Community Outreach</t>
   </si>
   <si>
@@ -972,9 +895,6 @@
     <t xml:space="preserve">Allegheny Couny residents who are or have applied to receive medicaid/third-party prescription coverage and make an adusted income of $500 dollars or less </t>
   </si>
   <si>
-    <t>Erie, PA</t>
-  </si>
-  <si>
     <t>A collection of programs available to Pennsylvania residents who recieve medicaid.</t>
   </si>
   <si>
@@ -984,9 +904,6 @@
     <t xml:space="preserve">Department of Human Services </t>
   </si>
   <si>
-    <t>Allegheny County PA</t>
-  </si>
-  <si>
     <t>provides transportation to medical appointments for Medical Assistance recipients who do not have transportation available to them.</t>
   </si>
   <si>
@@ -1039,9 +956,6 @@
   </si>
   <si>
     <t xml:space="preserve">Non-profit that offers homeless services and shelters </t>
-  </si>
-  <si>
-    <t>Ahsburn</t>
   </si>
   <si>
     <t xml:space="preserve">Good Sheppard Alliance </t>
@@ -1264,12 +1178,6 @@
     <t>Works with those involved in the criminal justice system to provide employment assistance, post-release skill classes, community service substitutes for misdemeanor offers clothing, food, transportation, medication and violence prevention programs.</t>
   </si>
   <si>
-    <t>Provides education opportunities such as General Education Development and English as a Second Language programs as well as support services to adults 18 and older in Loudoun County</t>
-  </si>
-  <si>
-    <t>Offers free transportation for non-emergency and urgent medical appointments to those who have Medicaid</t>
-  </si>
-  <si>
     <t>Home hosting programs for those aged 18-24 experiencing housing insecurity</t>
   </si>
   <si>
@@ -1325,13 +1233,68 @@
   </si>
   <si>
     <t>Career services program</t>
+  </si>
+  <si>
+    <t>Health Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualify for Medicaid </t>
+  </si>
+  <si>
+    <t>Allegheny County</t>
+  </si>
+  <si>
+    <t>Homestead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Turtle Creek</t>
+  </si>
+  <si>
+    <t>Erie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Allison Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number Codes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loudoun </t>
+  </si>
+  <si>
+    <t>Fairfax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pillars </t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subpopulation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Least Important </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Important </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used a lot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used not a lot </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1378,13 +1341,49 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDF1F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1400,7 +1399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1425,6 +1424,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1432,6 +1445,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFBDF1F6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1740,25 +1758,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:N84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="76" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="113" customWidth="1"/>
-    <col min="8" max="8" width="83.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="120.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51.5" customWidth="1"/>
-    <col min="12" max="12" width="40" customWidth="1"/>
+    <col min="12" max="12" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="54" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1788,10 +1806,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
@@ -1800,7 +1818,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -1826,7 +1844,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>390</v>
+        <v>362</v>
       </c>
       <c r="I2" s="2">
         <v>38.840490000000003</v>
@@ -1864,7 +1882,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>389</v>
+        <v>361</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
@@ -1905,10 +1923,10 @@
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>389</v>
+        <v>361</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>391</v>
+        <v>363</v>
       </c>
       <c r="I4" s="2">
         <v>37.538339999999998</v>
@@ -1937,7 +1955,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>30</v>
@@ -1978,7 +1996,7 @@
         <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>30</v>
@@ -2019,7 +2037,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>30</v>
@@ -2060,7 +2078,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>30</v>
@@ -2101,7 +2119,7 @@
         <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
@@ -2136,13 +2154,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>30</v>
@@ -2154,7 +2172,7 @@
         <v>51</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>392</v>
+        <v>364</v>
       </c>
       <c r="I10" s="2">
         <v>39.114306589999998</v>
@@ -2177,13 +2195,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>14</v>
@@ -2195,7 +2213,7 @@
         <v>57</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>393</v>
+        <v>365</v>
       </c>
       <c r="I11" s="2">
         <v>39.114306589999998</v>
@@ -2203,7 +2221,7 @@
       <c r="J11" s="2">
         <v>-77.539617179999993</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="10" t="s">
         <v>52</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -2218,13 +2236,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>14</v>
@@ -2259,7 +2277,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>65</v>
@@ -2271,13 +2289,13 @@
         <v>30</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>384</v>
+        <v>356</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>394</v>
+        <v>366</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -2296,7 +2314,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>66</v>
@@ -2308,13 +2326,13 @@
         <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>383</v>
+        <v>355</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>395</v>
+        <v>367</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -2333,13 +2351,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
@@ -2374,13 +2392,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>30</v>
@@ -2392,7 +2410,7 @@
         <v>73</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>396</v>
+        <v>368</v>
       </c>
       <c r="I16" s="2">
         <v>37.61065696</v>
@@ -2415,13 +2433,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>76</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>30</v>
@@ -2451,18 +2469,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>30</v>
@@ -2474,7 +2492,7 @@
         <v>83</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>397</v>
+        <v>369</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -2497,13 +2515,13 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>14</v>
@@ -2515,7 +2533,7 @@
         <v>88</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>398</v>
+        <v>370</v>
       </c>
       <c r="I19" s="2">
         <v>0</v>
@@ -2538,7 +2556,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>90</v>
@@ -2579,7 +2597,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>95</v>
@@ -2620,7 +2638,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>99</v>
@@ -2661,13 +2679,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>14</v>
@@ -2697,7 +2715,7 @@
     </row>
     <row r="24" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>11</v>
@@ -2738,10 +2756,10 @@
     </row>
     <row r="25" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>113</v>
@@ -2779,16 +2797,16 @@
     </row>
     <row r="26" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>118</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
@@ -2820,16 +2838,16 @@
     </row>
     <row r="27" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>14</v>
@@ -2861,10 +2879,10 @@
     </row>
     <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>130</v>
@@ -2882,7 +2900,7 @@
         <v>132</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>399</v>
+        <v>371</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>133</v>
@@ -2900,16 +2918,16 @@
     </row>
     <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>14</v>
@@ -2941,16 +2959,16 @@
     </row>
     <row r="30" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>141</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>30</v>
@@ -2982,10 +3000,10 @@
     </row>
     <row r="31" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>143</v>
@@ -3021,16 +3039,16 @@
     </row>
     <row r="32" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>145</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>30</v>
@@ -3042,7 +3060,7 @@
         <v>146</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>400</v>
+        <v>372</v>
       </c>
       <c r="I32" s="2">
         <v>40.439188049999998</v>
@@ -3062,28 +3080,28 @@
     </row>
     <row r="33" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>149</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
       <c r="I33" s="2">
         <v>40.437306100000001</v>
@@ -3098,33 +3116,33 @@
         <v>111</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>388</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>150</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>402</v>
+        <v>374</v>
       </c>
       <c r="I34" s="2">
         <v>40.437306100000001</v>
@@ -3144,28 +3162,28 @@
     </row>
     <row r="35" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>387</v>
+        <v>359</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>386</v>
+        <v>358</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>403</v>
+        <v>375</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -3180,18 +3198,18 @@
         <v>111</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>13</v>
@@ -3200,13 +3218,13 @@
         <v>30</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
@@ -3221,33 +3239,33 @@
         <v>111</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>13</v>
+        <v>343</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="G37" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="I37" s="2">
         <v>0</v>
@@ -3262,33 +3280,33 @@
         <v>111</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="84" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>397</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>13</v>
+        <v>343</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -3303,7 +3321,7 @@
         <v>111</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3311,13 +3329,13 @@
         <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>30</v>
@@ -3326,10 +3344,10 @@
         <v>31</v>
       </c>
       <c r="G39" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="I39" s="2">
         <v>39.114409999999999</v>
@@ -3341,10 +3359,10 @@
         <v>52</v>
       </c>
       <c r="L39" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M39" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3352,25 +3370,25 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="H40" s="2" t="s">
-        <v>404</v>
+        <v>376</v>
       </c>
       <c r="I40" s="2">
         <v>39.114409999999999</v>
@@ -3382,10 +3400,10 @@
         <v>52</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3393,25 +3411,25 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="H41" s="2" t="s">
-        <v>405</v>
+        <v>377</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -3423,10 +3441,10 @@
         <v>46</v>
       </c>
       <c r="L41" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="M41" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="M41" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3434,25 +3452,25 @@
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G42" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="I42" s="2">
         <v>39.076819999999998</v>
@@ -3461,13 +3479,13 @@
         <v>-77.549896000000004</v>
       </c>
       <c r="K42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M42" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="M42" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3475,25 +3493,25 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I43" s="2">
         <v>39.114409999999999</v>
@@ -3502,13 +3520,13 @@
         <v>-77.540581000000003</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3516,25 +3534,25 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I44" s="2">
         <v>39.115279999999998</v>
@@ -3543,13 +3561,13 @@
         <v>-77.564430000000002</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>195</v>
+        <v>52</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3557,25 +3575,25 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I45" s="2">
         <v>40.741895</v>
@@ -3584,13 +3602,13 @@
         <v>-73.989307999999994</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3598,25 +3616,25 @@
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G46" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="I46" s="2">
         <v>0</v>
@@ -3628,10 +3646,10 @@
         <v>46</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="84" x14ac:dyDescent="0.2">
@@ -3639,25 +3657,25 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>406</v>
+        <v>378</v>
       </c>
       <c r="I47" s="2">
         <v>39.108399900000002</v>
@@ -3666,95 +3684,95 @@
         <v>-77.565337</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>209</v>
+        <v>52</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>299</v>
+        <v>11</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="H48" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I48" s="2">
-        <v>39.114409999999999</v>
+        <v>39.114406199999998</v>
       </c>
       <c r="J48" s="2">
-        <v>-77.540580000000006</v>
+        <v>-77.567706299999998</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>11</v>
+        <v>397</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>407</v>
+        <v>213</v>
       </c>
       <c r="I49" s="2">
-        <v>39.115943000000001</v>
+        <v>39.117853099999998</v>
       </c>
       <c r="J49" s="2">
-        <v>-77.581795999999997</v>
+        <v>-77.568151900000004</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>195</v>
+        <v>52</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -3762,189 +3780,189 @@
         <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>11</v>
+        <v>275</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I50" s="2">
-        <v>39.114406199999998</v>
+        <v>0</v>
       </c>
       <c r="J50" s="2">
-        <v>-77.567706299999998</v>
+        <v>0</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>195</v>
+        <v>216</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="M50" s="4" t="s">
-        <v>223</v>
+      <c r="M50" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>10</v>
+        <v>222</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>152</v>
+        <v>272</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>86</v>
+        <v>223</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="F51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="H51" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L51" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="M51" s="4" t="s">
         <v>226</v>
-      </c>
-      <c r="I51" s="2">
-        <v>37.542472099999998</v>
-      </c>
-      <c r="J51" s="2">
-        <v>-77.435912200000004</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M51" s="4" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>10</v>
+        <v>222</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>152</v>
+        <v>272</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>224</v>
+        <v>170</v>
       </c>
       <c r="G52" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I52" s="2">
+        <v>40.439779999999999</v>
+      </c>
+      <c r="J52" s="2">
+        <v>-79.998869999999997</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L52" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="M52" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="I52" s="2">
-        <v>39.117853099999998</v>
-      </c>
-      <c r="J52" s="2">
-        <v>-77.568151900000004</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="L52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="M52" s="4" t="s">
+      <c r="D53" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="H53" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L53" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G53" s="2" t="s">
+      <c r="M53" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="I53" s="2">
-        <v>37.610656959136698</v>
-      </c>
-      <c r="J53" s="2">
-        <v>-77.340073015724201</v>
-      </c>
-      <c r="K53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L53" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="D54" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>240</v>
+        <v>381</v>
       </c>
       <c r="I54" s="2">
         <v>0</v>
@@ -3953,39 +3971,39 @@
         <v>0</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>236</v>
+        <v>46</v>
       </c>
       <c r="L54" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="I55" s="2">
         <v>0</v>
@@ -3997,77 +4015,77 @@
         <v>46</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="H56" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I56" s="2">
-        <v>40.439779999999999</v>
+        <v>0</v>
       </c>
       <c r="J56" s="2">
-        <v>-79.998869999999997</v>
+        <v>0</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>251</v>
+        <v>46</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>56</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>410</v>
+        <v>247</v>
       </c>
       <c r="I57" s="2">
         <v>0</v>
@@ -4079,159 +4097,159 @@
         <v>46</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>207</v>
+        <v>30</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>56</v>
+        <v>239</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>411</v>
+        <v>251</v>
       </c>
       <c r="I58" s="2">
-        <v>0</v>
+        <v>40.407960000000003</v>
       </c>
       <c r="J58" s="2">
-        <v>0</v>
+        <v>-79.909257999999994</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>46</v>
+        <v>400</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>207</v>
+        <v>30</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>261</v>
+        <v>31</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="I59" s="2">
-        <v>0</v>
+        <v>40.405259100000002</v>
       </c>
       <c r="J59" s="2">
-        <v>0</v>
+        <v>-79.829184400000003</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>46</v>
+        <v>401</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="I60" s="2">
+        <v>40.559510000000003</v>
+      </c>
+      <c r="J60" s="2">
+        <v>-79.958669999999998</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="I60" s="2">
-        <v>0</v>
-      </c>
-      <c r="J60" s="2">
-        <v>0</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="M60" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="D61" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>265</v>
+        <v>304</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>269</v>
+        <v>382</v>
       </c>
       <c r="I61" s="2">
         <v>0</v>
@@ -4243,65 +4261,65 @@
         <v>46</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>261</v>
+        <v>31</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>273</v>
+        <v>260</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>383</v>
       </c>
       <c r="I62" s="2">
-        <v>40.407960000000003</v>
+        <v>40.427699869999998</v>
       </c>
       <c r="J62" s="2">
-        <v>-79.909257999999994</v>
+        <v>-80.135979739999996</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>274</v>
+        <v>110</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>30</v>
@@ -4310,121 +4328,121 @@
         <v>31</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>279</v>
+        <v>300</v>
       </c>
       <c r="I63" s="2">
-        <v>40.405259100000002</v>
+        <v>40.427699869999998</v>
       </c>
       <c r="J63" s="2">
-        <v>-79.829184400000003</v>
+        <v>-80.135979739999996</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>280</v>
+        <v>110</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="M63" s="4" t="s">
-        <v>282</v>
+        <v>299</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="I64" s="2">
-        <v>40.559510000000003</v>
+        <v>40.427699869999998</v>
       </c>
       <c r="J64" s="2">
-        <v>-79.958669999999998</v>
+        <v>-80.135979739999996</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>286</v>
+        <v>399</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="M64" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>207</v>
+        <v>30</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>119</v>
+        <v>31</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>331</v>
+        <v>260</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="I65" s="2">
-        <v>0</v>
+        <v>40.427699869999998</v>
       </c>
       <c r="J65" s="2">
-        <v>0</v>
+        <v>-80.135979739999996</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>46</v>
+        <v>399</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>30</v>
@@ -4433,930 +4451,930 @@
         <v>31</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>413</v>
+        <v>260</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="I66" s="2">
-        <v>40.427699869999998</v>
+        <v>0</v>
       </c>
       <c r="J66" s="2">
-        <v>-80.135979739999996</v>
+        <v>0</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="L66" s="2"/>
       <c r="M66" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>31</v>
+        <v>170</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>328</v>
+        <v>260</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
       <c r="I67" s="2">
-        <v>40.427699869999998</v>
+        <v>0</v>
       </c>
       <c r="J67" s="2">
-        <v>-80.135979739999996</v>
+        <v>0</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>251</v>
+        <v>399</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>322</v>
+        <v>397</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>284</v>
+        <v>398</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="I68" s="2">
-        <v>40.427699869999998</v>
-      </c>
-      <c r="J68" s="2">
-        <v>-80.135979739999996</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
       <c r="K68" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="M68" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>322</v>
+        <v>397</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>293</v>
+        <v>157</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>31</v>
+        <v>170</v>
       </c>
       <c r="G69" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>426</v>
-      </c>
       <c r="I69" s="2">
-        <v>40.427699869999998</v>
+        <v>0</v>
       </c>
       <c r="J69" s="2">
-        <v>-80.135979739999996</v>
+        <v>0</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>315</v>
+        <v>46</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>243</v>
+        <v>10</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>317</v>
+        <v>272</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>31</v>
+        <v>239</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>319</v>
+        <v>395</v>
       </c>
       <c r="I70" s="2">
-        <v>0</v>
+        <v>39.078167000000001</v>
       </c>
       <c r="J70" s="2">
-        <v>0</v>
+        <v>-77.550561000000002</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="L70" s="2"/>
-      <c r="M70" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>243</v>
+        <v>10</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>317</v>
+        <v>272</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H71" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I71" s="2">
+        <v>39.045227799999999</v>
+      </c>
+      <c r="J71" s="2">
+        <v>-77.486494199999996</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="I72" s="2">
+        <v>38.906303508879397</v>
+      </c>
+      <c r="J72" s="2">
+        <v>-77.222641329237604</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="I71" s="2">
-        <v>0</v>
-      </c>
-      <c r="J71" s="2">
-        <v>0</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2" t="s">
+      <c r="G73" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="I73" s="2">
+        <v>38.875816034503501</v>
+      </c>
+      <c r="J73" s="2">
+        <v>-77.435718373358995</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="105" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="L72" s="2"/>
-      <c r="M72" s="2"/>
-    </row>
-    <row r="73" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="H73" s="2" t="s">
+      <c r="F74" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I74" s="2">
+        <v>38.875816034503501</v>
+      </c>
+      <c r="J74" s="2">
+        <v>-77.435718373358995</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I73" s="2">
-        <v>0</v>
-      </c>
-      <c r="J73" s="2">
-        <v>0</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="M73" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="I74" s="2">
-        <v>39.078167000000001</v>
-      </c>
-      <c r="J74" s="2">
-        <v>-77.550561000000002</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="C75" s="2" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>165</v>
+        <v>343</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>171</v>
+        <v>323</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>333</v>
+        <v>392</v>
       </c>
       <c r="I75" s="2">
-        <v>39.045227799999999</v>
+        <v>38.873610192974397</v>
       </c>
       <c r="J75" s="2">
-        <v>-77.486494199999996</v>
+        <v>-77.3055466310296</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>335</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="L75" s="2"/>
       <c r="M75" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>337</v>
+        <v>274</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>339</v>
+        <v>311</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>56</v>
+        <v>328</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>340</v>
+        <v>100</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>424</v>
+        <v>329</v>
       </c>
       <c r="I76" s="2">
-        <v>38.906303508879397</v>
+        <v>38.868590773014198</v>
       </c>
       <c r="J76" s="2">
-        <v>-77.222641329237604</v>
+        <v>-77.224144877053305</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="L76" s="2"/>
       <c r="M76" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>337</v>
+        <v>274</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>371</v>
+        <v>344</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>339</v>
+        <v>30</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>345</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="I77" s="2">
-        <v>38.875816034503501</v>
+        <v>38.774379099999997</v>
       </c>
       <c r="J77" s="2">
-        <v>-77.435718373358995</v>
+        <v>-77.074015599999996</v>
       </c>
       <c r="K77" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L77" s="2"/>
+      <c r="M77" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="105" x14ac:dyDescent="0.2">
+      <c r="N77" s="2"/>
+    </row>
+    <row r="78" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>337</v>
+        <v>11</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>13</v>
+        <v>343</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>339</v>
+        <v>311</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>349</v>
+        <v>390</v>
       </c>
       <c r="I78" s="2">
-        <v>38.875816034503501</v>
+        <v>38.8060490968736</v>
       </c>
       <c r="J78" s="2">
-        <v>-77.435718373358995</v>
+        <v>-77.181676502196197</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>337</v>
+        <v>11</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>30</v>
+        <v>311</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>351</v>
+        <v>31</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>422</v>
+        <v>389</v>
       </c>
       <c r="I79" s="2">
-        <v>38.873610192974397</v>
+        <v>38.8060490968736</v>
       </c>
       <c r="J79" s="2">
-        <v>-77.3055466310296</v>
+        <v>-77.181676502196197</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>299</v>
+        <v>11</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>339</v>
+        <v>311</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>356</v>
+        <v>27</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>100</v>
+        <v>334</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>357</v>
+        <v>388</v>
       </c>
       <c r="I80" s="2">
-        <v>38.868590773014198</v>
+        <v>38.8553917225858</v>
       </c>
       <c r="J80" s="2">
-        <v>-77.224144877053305</v>
+        <v>-77.362718702194798</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="126" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>13</v>
+        <v>340</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>356</v>
+        <v>323</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>373</v>
+        <v>341</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>421</v>
+        <v>387</v>
       </c>
       <c r="I81" s="2">
-        <v>38.774379099999997</v>
+        <v>38.854251580169802</v>
       </c>
       <c r="J81" s="2">
-        <v>-77.074015599999996</v>
+        <v>-77.356579302194902</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>17</v>
+        <v>338</v>
       </c>
       <c r="L81" s="2"/>
-      <c r="M81" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="N81" s="2"/>
-    </row>
-    <row r="82" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="M81" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>11</v>
+        <v>275</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>339</v>
+        <v>30</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>420</v>
+        <v>386</v>
       </c>
       <c r="I82" s="2">
-        <v>38.8060490968736</v>
+        <v>38.8553408</v>
       </c>
       <c r="J82" s="2">
-        <v>-77.181676502196197</v>
+        <v>-77.364854500000007</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M82" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>11</v>
+        <v>275</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>339</v>
+        <v>30</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>31</v>
+        <v>323</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>419</v>
+        <v>385</v>
       </c>
       <c r="I83" s="2">
-        <v>38.8060490968736</v>
+        <v>38.8553408</v>
       </c>
       <c r="J83" s="2">
-        <v>-77.181676502196197</v>
+        <v>-77.364854500000007</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="L83" s="2"/>
-      <c r="M83" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M83" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>11</v>
+        <v>275</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>339</v>
+        <v>30</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>27</v>
+        <v>323</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>418</v>
+        <v>384</v>
       </c>
       <c r="I84" s="2">
-        <v>38.8553917225858</v>
+        <v>38.8553408</v>
       </c>
       <c r="J84" s="2">
-        <v>-77.362718702194798</v>
+        <v>-77.364854500000007</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" ht="126" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I85" s="2">
-        <v>38.854251580169802</v>
-      </c>
-      <c r="J85" s="2">
-        <v>-77.356579302194902</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" ht="63" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="I86" s="2">
-        <v>38.8553408</v>
-      </c>
-      <c r="J86" s="2">
-        <v>-77.364854500000007</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="M86" s="8" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" ht="63" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="I87" s="2">
-        <v>38.8553408</v>
-      </c>
-      <c r="J87" s="2">
-        <v>-77.364854500000007</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="L87" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="M87" s="8" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="63" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="I88" s="2">
-        <v>38.8553408</v>
-      </c>
-      <c r="J88" s="2">
-        <v>-77.364854500000007</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="L88" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="M88" s="8"/>
+        <v>338</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="M84" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M53" r:id="rId1" xr:uid="{337874BF-AFEF-FF4C-91B8-75066397C911}"/>
-    <hyperlink ref="M52" r:id="rId2" xr:uid="{13FD1025-9919-E14D-A92B-00246A640824}"/>
-    <hyperlink ref="M39" r:id="rId3" xr:uid="{744E5DA9-18B1-1747-92BF-B5BB28046D72}"/>
-    <hyperlink ref="M41" r:id="rId4" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{6ED53666-C4AE-2E40-A60F-93C9F2AF47E8}"/>
-    <hyperlink ref="M40" r:id="rId5" display="https://www.loudoun.gov/CoC" xr:uid="{4122238C-598A-ED47-981E-4111B0118B0E}"/>
-    <hyperlink ref="M42" r:id="rId6" xr:uid="{7D4B8EF6-3883-A141-A8F0-C51B5B0CFCE3}"/>
-    <hyperlink ref="M43" r:id="rId7" display="https://www.loudoun.gov/1592/Workforce-Resource-Center" xr:uid="{94B820A0-D3F2-4840-9F07-CA5A487E6333}"/>
-    <hyperlink ref="M44" r:id="rId8" xr:uid="{1A4CA1E2-244B-2C40-8A40-EE156D467B01}"/>
-    <hyperlink ref="M45" r:id="rId9" xr:uid="{D64AF4FD-E657-684C-B86C-7619D977C987}"/>
-    <hyperlink ref="M46" r:id="rId10" display="https://biz.loudoun.gov/work-in-loudoun/" xr:uid="{4982EC8B-FAC5-5640-A062-CBB1672F3253}"/>
-    <hyperlink ref="M47" r:id="rId11" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{F2FBA2B3-8781-C147-9AA1-AEBC03ECB436}"/>
-    <hyperlink ref="M48" r:id="rId12" display="https://vcwnorthern.com/contact/" xr:uid="{6713DAB9-C47A-E746-ACC2-4AAE2BA73145}"/>
-    <hyperlink ref="M49" r:id="rId13" display="https://www.lcps.org/adulted" xr:uid="{2A378819-651D-3643-970D-A4D61984D906}"/>
-    <hyperlink ref="M50" r:id="rId14" display="https://loudounliteracy.org/" xr:uid="{9999DF84-E493-E44E-A3EE-CC9DCE69FA8F}"/>
-    <hyperlink ref="M55" r:id="rId15" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{15E0A920-6E95-7B4F-BB11-050D757A5EAB}"/>
-    <hyperlink ref="M57" r:id="rId16" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
-    <hyperlink ref="M58" r:id="rId17" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
-    <hyperlink ref="M60" r:id="rId18" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{6193B0D4-846D-4843-9837-B96F841B4261}"/>
-    <hyperlink ref="M59" r:id="rId19" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
-    <hyperlink ref="M61" r:id="rId20" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{D43D4075-EC70-464F-A85F-272BDC168DC4}"/>
-    <hyperlink ref="M62" r:id="rId21" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
-    <hyperlink ref="M63" r:id="rId22" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
-    <hyperlink ref="M64" r:id="rId23" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
-    <hyperlink ref="M56" r:id="rId24" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
-    <hyperlink ref="M81" r:id="rId25" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
-    <hyperlink ref="M86" r:id="rId26" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
-    <hyperlink ref="M87" r:id="rId27" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
-    <hyperlink ref="M34" r:id="rId28" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
-    <hyperlink ref="M36" r:id="rId29" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
-    <hyperlink ref="M32" r:id="rId30" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
+    <hyperlink ref="M49" r:id="rId1" xr:uid="{13FD1025-9919-E14D-A92B-00246A640824}"/>
+    <hyperlink ref="M39" r:id="rId2" xr:uid="{744E5DA9-18B1-1747-92BF-B5BB28046D72}"/>
+    <hyperlink ref="M41" r:id="rId3" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{6ED53666-C4AE-2E40-A60F-93C9F2AF47E8}"/>
+    <hyperlink ref="M40" r:id="rId4" display="https://www.loudoun.gov/CoC" xr:uid="{4122238C-598A-ED47-981E-4111B0118B0E}"/>
+    <hyperlink ref="M42" r:id="rId5" xr:uid="{7D4B8EF6-3883-A141-A8F0-C51B5B0CFCE3}"/>
+    <hyperlink ref="M43" r:id="rId6" display="https://www.loudoun.gov/1592/Workforce-Resource-Center" xr:uid="{94B820A0-D3F2-4840-9F07-CA5A487E6333}"/>
+    <hyperlink ref="M44" r:id="rId7" xr:uid="{1A4CA1E2-244B-2C40-8A40-EE156D467B01}"/>
+    <hyperlink ref="M45" r:id="rId8" xr:uid="{D64AF4FD-E657-684C-B86C-7619D977C987}"/>
+    <hyperlink ref="M46" r:id="rId9" display="https://biz.loudoun.gov/work-in-loudoun/" xr:uid="{4982EC8B-FAC5-5640-A062-CBB1672F3253}"/>
+    <hyperlink ref="M47" r:id="rId10" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{F2FBA2B3-8781-C147-9AA1-AEBC03ECB436}"/>
+    <hyperlink ref="M48" r:id="rId11" display="https://loudounliteracy.org/" xr:uid="{9999DF84-E493-E44E-A3EE-CC9DCE69FA8F}"/>
+    <hyperlink ref="M51" r:id="rId12" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{15E0A920-6E95-7B4F-BB11-050D757A5EAB}"/>
+    <hyperlink ref="M53" r:id="rId13" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
+    <hyperlink ref="M54" r:id="rId14" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
+    <hyperlink ref="M56" r:id="rId15" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{6193B0D4-846D-4843-9837-B96F841B4261}"/>
+    <hyperlink ref="M55" r:id="rId16" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
+    <hyperlink ref="M57" r:id="rId17" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{D43D4075-EC70-464F-A85F-272BDC168DC4}"/>
+    <hyperlink ref="M58" r:id="rId18" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
+    <hyperlink ref="M59" r:id="rId19" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
+    <hyperlink ref="M60" r:id="rId20" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
+    <hyperlink ref="M52" r:id="rId21" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
+    <hyperlink ref="M77" r:id="rId22" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
+    <hyperlink ref="M82" r:id="rId23" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
+    <hyperlink ref="M83" r:id="rId24" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
+    <hyperlink ref="M34" r:id="rId25" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
+    <hyperlink ref="M36" r:id="rId26" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
+    <hyperlink ref="M32" r:id="rId27" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E72460-2510-C043-8231-9B014E680B14}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B11" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="B12" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B18" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B20" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="B21" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="B23" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="B24" s="21">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created website, changed to individuals served, waiting on Kyle's data
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9A1F3C-D280-E344-B9D0-0A3EBCC1EEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9B236F-9000-C54B-B00A-AD76B691B165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="415">
   <si>
     <t>County</t>
   </si>
@@ -1758,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N84"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1821,7 +1821,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2309,7 +2309,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>222</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>222</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>222</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>222</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>222</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>222</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="63" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>222</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>222</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>222</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>222</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>222</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>222</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>338</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="105" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>338</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>338</v>
       </c>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="N77" s="2"/>
     </row>
-    <row r="78" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>338</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>338</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>338</v>
       </c>
@@ -5178,6 +5178,47 @@
         <v>349</v>
       </c>
       <c r="M84" s="8"/>
+    </row>
+    <row r="85" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I85" s="2">
+        <v>0</v>
+      </c>
+      <c r="J85" s="2">
+        <v>0</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added Yang's headshot, published website and added in Fairfax Health Services
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9B236F-9000-C54B-B00A-AD76B691B165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9EEBF-4CE4-004A-8B80-1FCC52ADB025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="454">
   <si>
     <t>County</t>
   </si>
@@ -1193,9 +1193,6 @@
     <t>Programs designed to provide skills and knowledge needed to remain competitive in a variety of industries</t>
   </si>
   <si>
-    <t xml:space="preserve"> it is open for student travelers  who want to learn about the public transit system; help plan their trip, read bus and rail schedules, pay bus fares, transfer, reach specific destination, access local transportation resources</t>
-  </si>
-  <si>
     <t>Travel affordable, safely, and independently with the purchase of a discounted taxicab coupon. Cost $10 per $33 coupon book. 16 coupon books per year (July 1- June 30)</t>
   </si>
   <si>
@@ -1288,13 +1285,133 @@
   </si>
   <si>
     <t xml:space="preserve">Used not a lot </t>
+  </si>
+  <si>
+    <t>Falls Church Health Clinic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All </t>
+  </si>
+  <si>
+    <t>Fees and eligibility vary by service. WIC services available here</t>
+  </si>
+  <si>
+    <t>https://fallschurchhealthcare.com/</t>
+  </si>
+  <si>
+    <t>Herndon/Reston Health Clinic</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/health/clinics/herndon-reston-district-office</t>
+  </si>
+  <si>
+    <t>Joseph Willard Health Center</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/health/clinics/joseph-willard-health-center</t>
+  </si>
+  <si>
+    <t>Community Health Care Network (CHCN)</t>
+  </si>
+  <si>
+    <t>Health services for low income and uninsured.</t>
+  </si>
+  <si>
+    <t>https://chcnetwork.org/</t>
+  </si>
+  <si>
+    <t>Community Health Care Network (CHCN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairfax  </t>
+  </si>
+  <si>
+    <t>Jeanie Schmidt Free Clinic</t>
+  </si>
+  <si>
+    <t>Serving NW FFX County</t>
+  </si>
+  <si>
+    <t>http://www.jsfreeclinic.org/</t>
+  </si>
+  <si>
+    <t>Mission Life Center Hope Clinic</t>
+  </si>
+  <si>
+    <t>Serving FFX County</t>
+  </si>
+  <si>
+    <t>https://seniornavigator.org/program/47239/mlc-hope-clinic</t>
+  </si>
+  <si>
+    <t>Culmore Clinic</t>
+  </si>
+  <si>
+    <t>https://www.culmoreclinic.org/</t>
+  </si>
+  <si>
+    <t>Northern Virginia Dental Society (NVDS)</t>
+  </si>
+  <si>
+    <t>Must be resident of Arlington, FFX, Loudoun Counties or City of Alexandria, FFX or Falls Church.</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>https://www.nvds.org/about-us</t>
+  </si>
+  <si>
+    <t>Northern Virginia Dental Clinic</t>
+  </si>
+  <si>
+    <t>18 +</t>
+  </si>
+  <si>
+    <t>https://www.novadentalclinic.org/</t>
+  </si>
+  <si>
+    <t>Reston</t>
+  </si>
+  <si>
+    <t>Herndon</t>
+  </si>
+  <si>
+    <t>Annadale</t>
+  </si>
+  <si>
+    <t>Funding and Policy</t>
+  </si>
+  <si>
+    <t>Accepts only individuals eligible through referral agency. Must be 18+ years and at or below 200% of fed. poverty guidelines.</t>
+  </si>
+  <si>
+    <t>Non-profit Medi-Cal managed care organization, providing business administrative support for community health centers to focus on what matters most–patients.</t>
+  </si>
+  <si>
+    <t>Christian free clinic offering medical and spiritual care to uninsured persons of all ages by connecting them to resources. </t>
+  </si>
+  <si>
+    <t>Non-profit healthcare clinic serving low-income adults in the Bailey’s Crossroads community at little to no cost.</t>
+  </si>
+  <si>
+    <t>Promote the ideals of the ​profession of Dentistry and to foster professional relationships among dentists; seeks to safeguard the interests and well-being of the public. </t>
+  </si>
+  <si>
+    <t>Private non-profit 501(c) (3) organization; wants to contribute a critically-needed service to the community while preserving the dignity of the underserved.</t>
+  </si>
+  <si>
+    <t>Values your decisions that will best nurture your future, your faith, and your family.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It is open for student travelers  who want to learn about the public transit system; help plan their trip, read bus and rail schedules, pay bus fares, transfer, reach specific destination, access local transportation resources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1344,6 +1461,12 @@
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF292929"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1399,7 +1522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1438,6 +1561,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1758,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="D51" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1773,14 +1899,14 @@
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="113" customWidth="1"/>
     <col min="8" max="8" width="120.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.83203125" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51.5" customWidth="1"/>
     <col min="12" max="12" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="54" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="42" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2474,7 +2600,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>81</v>
@@ -2515,7 +2641,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>86</v>
@@ -2556,7 +2682,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>273</v>
+        <v>445</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>90</v>
@@ -2597,7 +2723,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>273</v>
+        <v>445</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>95</v>
@@ -2638,7 +2764,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>273</v>
+        <v>445</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>99</v>
@@ -2679,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>273</v>
+        <v>445</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>102</v>
@@ -3165,7 +3291,7 @@
         <v>222</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>152</v>
@@ -3206,7 +3332,7 @@
         <v>222</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>155</v>
@@ -3247,7 +3373,7 @@
         <v>222</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>157</v>
@@ -3288,7 +3414,7 @@
         <v>222</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>160</v>
@@ -3739,7 +3865,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>211</v>
@@ -4135,7 +4261,7 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>252</v>
@@ -4176,7 +4302,7 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>257</v>
@@ -4217,7 +4343,7 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>262</v>
@@ -4381,7 +4507,7 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>294</v>
@@ -4413,7 +4539,7 @@
         <v>260</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I65" s="2">
         <v>40.427699869999998</v>
@@ -4422,7 +4548,7 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>294</v>
@@ -4463,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L66" s="2"/>
       <c r="M66" s="4" t="s">
@@ -4502,7 +4628,7 @@
         <v>0</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>288</v>
@@ -4516,7 +4642,7 @@
         <v>222</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>271</v>
@@ -4531,7 +4657,7 @@
         <v>210</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>286</v>
@@ -4539,7 +4665,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
@@ -4549,7 +4675,7 @@
         <v>222</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>157</v>
@@ -4608,7 +4734,7 @@
         <v>280</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I70" s="2">
         <v>39.078167000000001</v>
@@ -4690,7 +4816,7 @@
         <v>312</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I72" s="2">
         <v>38.906303508879397</v>
@@ -4729,7 +4855,7 @@
         <v>317</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I73" s="2">
         <v>38.875816034503501</v>
@@ -4807,7 +4933,7 @@
         <v>324</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I75" s="2">
         <v>38.873610192974397</v>
@@ -4885,7 +5011,7 @@
         <v>345</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I77" s="2">
         <v>38.774379099999997</v>
@@ -4925,7 +5051,7 @@
         <v>334</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I78" s="2">
         <v>38.8060490968736</v>
@@ -4964,7 +5090,7 @@
         <v>334</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I79" s="2">
         <v>38.8060490968736</v>
@@ -5003,7 +5129,7 @@
         <v>334</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I80" s="2">
         <v>38.8553917225858</v>
@@ -5042,7 +5168,7 @@
         <v>341</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I81" s="2">
         <v>38.854251580169802</v>
@@ -5081,7 +5207,7 @@
         <v>348</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I82" s="2">
         <v>38.8553408</v>
@@ -5122,7 +5248,7 @@
         <v>352</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I83" s="2">
         <v>38.8553408</v>
@@ -5163,7 +5289,7 @@
         <v>354</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>384</v>
+        <v>453</v>
       </c>
       <c r="I84" s="2">
         <v>38.8553408</v>
@@ -5184,7 +5310,7 @@
         <v>338</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>86</v>
@@ -5218,6 +5344,423 @@
       </c>
       <c r="M85" s="2" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="I86" s="2">
+        <v>38.886493000000002</v>
+      </c>
+      <c r="J86" s="2">
+        <v>-77.176064999999994</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2">
+        <v>38.965629999999997</v>
+      </c>
+      <c r="J87" s="2">
+        <v>-77.358909999999995</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2">
+        <v>38.850720000000003</v>
+      </c>
+      <c r="J88" s="2">
+        <v>-77.29956</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="I89" s="2">
+        <v>38.869669999999999</v>
+      </c>
+      <c r="J89" s="2">
+        <v>-77.147750000000002</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="I90" s="2">
+        <v>38.731589999999997</v>
+      </c>
+      <c r="J90" s="2">
+        <v>-77.104609999999994</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="I91" s="2">
+        <v>38.969389999999997</v>
+      </c>
+      <c r="J91" s="2">
+        <v>-77.342410000000001</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="H92" s="6"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="I93" s="2">
+        <v>38.849589999999999</v>
+      </c>
+      <c r="J93" s="2">
+        <v>-77.316599999999994</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="I94" s="2">
+        <v>38.831009999999999</v>
+      </c>
+      <c r="J94" s="2">
+        <v>-77.185820000000007</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H95" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -5271,13 +5814,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
@@ -5293,7 +5836,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4" s="13">
         <v>3</v>
@@ -5301,7 +5844,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B7" s="15"/>
     </row>
@@ -5315,7 +5858,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B9" s="15">
         <v>11</v>
@@ -5339,7 +5882,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B12" s="15">
         <v>14</v>
@@ -5355,7 +5898,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B15" s="17"/>
     </row>
@@ -5377,7 +5920,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B18" s="17">
         <v>22</v>
@@ -5385,7 +5928,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B20" s="19">
         <v>1</v>
@@ -5393,7 +5936,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B21" s="19">
         <v>10</v>
@@ -5401,7 +5944,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B23" s="21">
         <v>1</v>
@@ -5409,7 +5952,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B24" s="21">
         <v>5</v>

</xml_diff>

<commit_message>
changed column name on excel and added population density map
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2239EDE3-7090-9F46-8434-2188DA6F707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE3A8C6-A1A8-304F-A3D7-7A032EAC9DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="474">
   <si>
     <t>County</t>
   </si>
@@ -1398,9 +1398,6 @@
     <t xml:space="preserve"> It is open for student travelers  who want to learn about the public transit system; help plan their trip, read bus and rail schedules, pay bus fares, transfer, reach specific destination, access local transportation resources</t>
   </si>
   <si>
-    <t>Office_Location</t>
-  </si>
-  <si>
     <t>Counseling and referral, trauma empowerment and recovery programs, life skills and socialization groups, relapse prevention and substance abuse education</t>
   </si>
   <si>
@@ -1465,6 +1462,9 @@
   </si>
   <si>
     <t>Outpatient, MHSADS</t>
+  </si>
+  <si>
+    <t>Office</t>
   </si>
 </sst>
 </file>
@@ -1962,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -2016,7 +2016,7 @@
         <v>275</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>451</v>
+        <v>473</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>8</v>
@@ -5766,7 +5766,9 @@
       </c>
     </row>
     <row r="95" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
+      <c r="A95" s="2" t="s">
+        <v>337</v>
+      </c>
       <c r="B95" s="2" t="s">
         <v>394</v>
       </c>
@@ -5849,7 +5851,7 @@
         <v>394</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>4</v>
@@ -5864,7 +5866,7 @@
         <v>178</v>
       </c>
       <c r="H97" s="23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I97" s="2">
         <v>39.025618681403103</v>
@@ -5877,7 +5879,7 @@
       </c>
       <c r="L97" s="2"/>
       <c r="M97" s="24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -5888,7 +5890,7 @@
         <v>394</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>4</v>
@@ -5900,10 +5902,10 @@
         <v>55</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H98" s="23" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I98" s="2">
         <v>39.025618681403103</v>
@@ -5916,7 +5918,7 @@
       </c>
       <c r="L98" s="2"/>
       <c r="M98" s="25" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -5927,7 +5929,7 @@
         <v>271</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>4</v>
@@ -5942,7 +5944,7 @@
         <v>178</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I99" s="2">
         <v>39.097752638349299</v>
@@ -5955,7 +5957,7 @@
       </c>
       <c r="L99" s="2"/>
       <c r="M99" s="24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -5966,7 +5968,7 @@
         <v>394</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>4</v>
@@ -5981,7 +5983,7 @@
         <v>178</v>
       </c>
       <c r="H100" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I100" s="2">
         <v>39.114615286054203</v>
@@ -5994,7 +5996,7 @@
       </c>
       <c r="L100" s="2"/>
       <c r="M100" s="26" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -6005,7 +6007,7 @@
         <v>394</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>4</v>
@@ -6020,7 +6022,7 @@
         <v>178</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I101" s="2">
         <v>39.114615286054203</v>
@@ -6033,7 +6035,7 @@
       </c>
       <c r="L101" s="2"/>
       <c r="M101" s="25" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="42" x14ac:dyDescent="0.2">
@@ -6044,7 +6046,7 @@
         <v>273</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>4</v>
@@ -6059,7 +6061,7 @@
         <v>178</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I102" s="2">
         <v>39.097752638349299</v>
@@ -6083,7 +6085,7 @@
         <v>273</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>4</v>
@@ -6095,10 +6097,10 @@
         <v>55</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I103" s="2">
         <v>39.097752638349299</v>
@@ -6111,7 +6113,46 @@
       </c>
       <c r="L103" s="2"/>
       <c r="M103" s="25" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="H104" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="I104" s="2">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2">
+        <v>0</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L104" s="2"/>
+      <c r="M104" s="2" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
copied combined excel to try out some new comparing visuals, made a rmd for the list of the programs we need to contact for who they serve
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE3A8C6-A1A8-304F-A3D7-7A032EAC9DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA377C1-B057-C748-A119-125EFE91FE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -1964,8 +1964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added a comparison tree
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5EA22-ED88-1943-BEDA-EB9CBAE3C35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F3FBEB-CDFD-CF4A-B8BC-3AEB31927FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="840" windowWidth="30180" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="457">
   <si>
     <t>County</t>
   </si>
@@ -793,9 +793,6 @@
     <t>Port Authority Allegheny County</t>
   </si>
   <si>
-    <t>Medical Assistance Transportation Program</t>
-  </si>
-  <si>
     <t>Health Choices</t>
   </si>
   <si>
@@ -829,28 +826,10 @@
     <t>https://www.voachesapeake.org/lhsc</t>
   </si>
   <si>
-    <t>https://www.alleghenycounty.us/WorkArea/linkit.aspx?LinkIdentifier=id&amp;ItemID=2147486416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allegheny County Office of Behavioral Health </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free psychiatric prescription medication </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allegheny Couny residents who are or have applied to receive medicaid/third-party prescription coverage and make an adusted income of $500 dollars or less </t>
-  </si>
-  <si>
     <t>A collection of programs available to Pennsylvania residents who recieve medicaid.</t>
   </si>
   <si>
-    <t>http://matp.pa.gov/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Department of Human Services </t>
-  </si>
-  <si>
-    <t>provides transportation to medical appointments for Medical Assistance recipients who do not have transportation available to them.</t>
   </si>
   <si>
     <t>Transportation</t>
@@ -1260,9 +1239,6 @@
     <t>https://chcnetwork.org/</t>
   </si>
   <si>
-    <t>Community Health Care Network (CHCN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fairfax  </t>
   </si>
   <si>
@@ -1426,6 +1402,18 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>low-income residents</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Loudoun, Fairfax</t>
+  </si>
+  <si>
+    <t>Loudoun, Fairfax, Allegheny</t>
   </si>
 </sst>
 </file>
@@ -1536,9 +1524,29 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -1549,7 +1557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1604,6 +1612,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1924,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1944,9 +1958,10 @@
     <col min="11" max="11" width="51.5" customWidth="1"/>
     <col min="12" max="12" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="54" style="9" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1972,22 +1987,25 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="N1" s="28" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2010,7 +2028,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="I2" s="2">
         <v>38.840490000000003</v>
@@ -2027,8 +2045,11 @@
       <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N2" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2048,7 +2069,7 @@
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>20</v>
@@ -2068,8 +2089,11 @@
       <c r="M3" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N3" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2089,10 +2113,10 @@
         <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="I4" s="2">
         <v>37.538339999999998</v>
@@ -2109,8 +2133,11 @@
       <c r="M4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="N4" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2150,8 +2177,11 @@
       <c r="M5" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N5" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2191,8 +2221,11 @@
       <c r="M6" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N6" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2232,8 +2265,11 @@
       <c r="M7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N7" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2273,8 +2309,11 @@
       <c r="M8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N8" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2314,13 +2353,16 @@
       <c r="M9" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N9" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>47</v>
@@ -2338,7 +2380,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="I10" s="2">
         <v>39.114306589999998</v>
@@ -2355,13 +2397,16 @@
       <c r="M10" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N10" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>53</v>
@@ -2379,7 +2424,7 @@
         <v>55</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="I11" s="2">
         <v>39.114306589999998</v>
@@ -2396,13 +2441,16 @@
       <c r="M11" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N11" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>58</v>
@@ -2437,13 +2485,16 @@
       <c r="M12" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N12" s="28" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>63</v>
@@ -2455,13 +2506,13 @@
         <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -2474,13 +2525,16 @@
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N13" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>64</v>
@@ -2492,13 +2546,13 @@
         <v>28</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -2511,13 +2565,16 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N14" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>65</v>
@@ -2552,13 +2609,16 @@
       <c r="M15" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N15" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>70</v>
@@ -2576,7 +2636,7 @@
         <v>71</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="I16" s="2">
         <v>37.61065696</v>
@@ -2593,13 +2653,16 @@
       <c r="M16" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N16" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>74</v>
@@ -2634,13 +2697,16 @@
       <c r="M17" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N17" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>79</v>
@@ -2658,7 +2724,7 @@
         <v>81</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -2675,13 +2741,16 @@
       <c r="M18" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N18" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>84</v>
@@ -2699,7 +2768,7 @@
         <v>86</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="I19" s="2">
         <v>0</v>
@@ -2716,13 +2785,16 @@
       <c r="M19" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N19" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>88</v>
@@ -2757,13 +2829,16 @@
       <c r="M20" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N20" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>93</v>
@@ -2798,13 +2873,16 @@
       <c r="M21" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N21" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>97</v>
@@ -2839,13 +2917,16 @@
       <c r="M22" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N22" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>100</v>
@@ -2878,8 +2959,11 @@
       <c r="M23" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N23" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>204</v>
       </c>
@@ -2919,13 +3003,16 @@
       <c r="M24" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="N24" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>111</v>
@@ -2960,13 +3047,16 @@
       <c r="M25" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N25" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>116</v>
@@ -3001,13 +3091,16 @@
       <c r="M26" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N26" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>123</v>
@@ -3042,13 +3135,16 @@
       <c r="M27" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N27" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>128</v>
@@ -3066,7 +3162,7 @@
         <v>130</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>131</v>
@@ -3081,13 +3177,16 @@
       <c r="M28" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N28" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>135</v>
@@ -3122,13 +3221,16 @@
       <c r="M29" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N29" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>139</v>
@@ -3163,13 +3265,16 @@
       <c r="M30" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N30" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>141</v>
@@ -3202,13 +3307,16 @@
       <c r="M31" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+      <c r="N31" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>143</v>
@@ -3226,7 +3334,7 @@
         <v>144</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="I32" s="2">
         <v>40.439188049999998</v>
@@ -3243,13 +3351,16 @@
       <c r="M32" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+      <c r="N32" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>146</v>
@@ -3261,13 +3372,13 @@
         <v>28</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>147</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="I33" s="2">
         <v>40.437306100000001</v>
@@ -3282,15 +3393,18 @@
         <v>109</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+      <c r="N33" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>148</v>
@@ -3302,13 +3416,13 @@
         <v>28</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="I34" s="2">
         <v>40.437306100000001</v>
@@ -3325,13 +3439,16 @@
       <c r="M34" s="8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N34" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>150</v>
@@ -3343,13 +3460,13 @@
         <v>28</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -3366,13 +3483,16 @@
       <c r="M35" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N35" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>153</v>
@@ -3384,10 +3504,10 @@
         <v>28</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>154</v>
@@ -3407,13 +3527,16 @@
       <c r="M36" s="8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N36" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>155</v>
@@ -3425,7 +3548,7 @@
         <v>28</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>156</v>
@@ -3448,13 +3571,16 @@
       <c r="M37" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+      <c r="N37" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>158</v>
@@ -3466,10 +3592,10 @@
         <v>28</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>156</v>
+        <v>453</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>159</v>
@@ -3489,13 +3615,16 @@
       <c r="M38" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N38" s="28" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>163</v>
@@ -3513,7 +3642,7 @@
         <v>165</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="I39" s="2">
         <v>0</v>
@@ -3530,13 +3659,16 @@
       <c r="M39" s="4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N39" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>168</v>
@@ -3571,13 +3703,16 @@
       <c r="M40" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N40" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>173</v>
@@ -3612,13 +3747,16 @@
       <c r="M41" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N41" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>178</v>
@@ -3653,13 +3791,16 @@
       <c r="M42" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N42" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>186</v>
@@ -3694,13 +3835,16 @@
       <c r="M43" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N43" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>190</v>
@@ -3718,7 +3862,7 @@
         <v>192</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="I44" s="2">
         <v>39.108399900000002</v>
@@ -3735,8 +3879,11 @@
       <c r="M44" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="N44" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>8</v>
       </c>
@@ -3776,13 +3923,16 @@
       <c r="M45" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N45" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>199</v>
@@ -3817,13 +3967,16 @@
       <c r="M46" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N46" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>205</v>
@@ -3841,7 +3994,7 @@
         <v>206</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="I47" s="2">
         <v>0</v>
@@ -3858,13 +4011,16 @@
       <c r="M47" s="4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N47" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>209</v>
@@ -3899,13 +4055,16 @@
       <c r="M48" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N48" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>214</v>
@@ -3923,7 +4082,7 @@
         <v>215</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="I49" s="2">
         <v>0</v>
@@ -3940,13 +4099,16 @@
       <c r="M49" s="4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N49" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>218</v>
@@ -3964,7 +4126,7 @@
         <v>215</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="I50" s="2">
         <v>0</v>
@@ -3981,13 +4143,16 @@
       <c r="M50" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N50" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>220</v>
@@ -4022,13 +4187,16 @@
       <c r="M51" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N51" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>224</v>
@@ -4063,13 +4231,16 @@
       <c r="M52" s="4" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N52" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>228</v>
@@ -4104,13 +4275,16 @@
       <c r="M53" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+      <c r="N53" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>231</v>
@@ -4137,7 +4311,7 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>234</v>
@@ -4145,13 +4319,16 @@
       <c r="M54" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N54" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>236</v>
@@ -4178,7 +4355,7 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>239</v>
@@ -4186,13 +4363,16 @@
       <c r="M55" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N55" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>241</v>
@@ -4219,7 +4399,7 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>244</v>
@@ -4227,13 +4407,16 @@
       <c r="M56" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="N56" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>246</v>
@@ -4248,10 +4431,10 @@
         <v>117</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="I57" s="2">
         <v>0</v>
@@ -4263,18 +4446,21 @@
         <v>44</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+      <c r="N57" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>247</v>
@@ -4292,7 +4478,7 @@
         <v>242</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I58" s="2">
         <v>40.427699869999998</v>
@@ -4304,18 +4490,21 @@
         <v>108</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+      <c r="N58" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>248</v>
@@ -4330,10 +4519,10 @@
         <v>29</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="I59" s="2">
         <v>40.427699869999998</v>
@@ -4345,18 +4534,21 @@
         <v>108</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+      <c r="N59" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>249</v>
@@ -4374,7 +4566,7 @@
         <v>242</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="I60" s="2">
         <v>40.427699869999998</v>
@@ -4383,21 +4575,24 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+      <c r="N60" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>250</v>
@@ -4415,7 +4610,7 @@
         <v>242</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="I61" s="2">
         <v>40.427699869999998</v>
@@ -4424,21 +4619,24 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+      <c r="N61" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>251</v>
@@ -4456,7 +4654,7 @@
         <v>242</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -4465,19 +4663,22 @@
         <v>0</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="L62" s="2"/>
       <c r="M62" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+      <c r="N62" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>272</v>
+        <v>369</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>252</v>
@@ -4489,39 +4690,34 @@
         <v>28</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>242</v>
+        <v>370</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="I63" s="2">
-        <v>0</v>
-      </c>
-      <c r="J63" s="2">
-        <v>0</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
       <c r="K63" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>376</v>
+        <v>253</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>253</v>
+        <v>448</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>4</v>
@@ -4530,31 +4726,42 @@
         <v>28</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>198</v>
+        <v>388</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
+        <v>261</v>
+      </c>
+      <c r="H64" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2">
+        <v>0</v>
+      </c>
       <c r="K64" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="L64" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="N64" s="28" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="65" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>376</v>
+        <v>253</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>155</v>
+        <v>260</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>4</v>
@@ -4563,39 +4770,42 @@
         <v>28</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>266</v>
+        <v>367</v>
       </c>
       <c r="I65" s="2">
-        <v>0</v>
+        <v>39.078167000000001</v>
       </c>
       <c r="J65" s="2">
-        <v>0</v>
+        <v>-77.550561000000002</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="M65" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="N65" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>456</v>
+        <v>280</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>4</v>
@@ -4604,157 +4814,165 @@
         <v>28</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>395</v>
+        <v>162</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="H66" s="23" t="s">
-        <v>457</v>
+        <v>261</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="I66" s="2">
-        <v>0</v>
+        <v>39.045227799999999</v>
       </c>
       <c r="J66" s="2">
-        <v>0</v>
+        <v>-77.486494199999996</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L66" s="27" t="s">
-        <v>458</v>
+        <v>32</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>282</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+      <c r="N66" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>8</v>
+        <v>313</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>28</v>
+        <v>286</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>221</v>
+        <v>54</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>262</v>
+        <v>287</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="I67" s="2">
-        <v>39.078167000000001</v>
+        <v>38.906303508879397</v>
       </c>
       <c r="J67" s="2">
-        <v>-77.550561000000002</v>
+        <v>-77.222641329237604</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L67" s="2" t="s">
-        <v>261</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="L67" s="2"/>
       <c r="M67" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+      <c r="N67" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>8</v>
+        <v>313</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>28</v>
+        <v>286</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>162</v>
+        <v>291</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>262</v>
+        <v>292</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>288</v>
+        <v>365</v>
       </c>
       <c r="I68" s="2">
-        <v>39.045227799999999</v>
+        <v>38.875816034503501</v>
       </c>
       <c r="J68" s="2">
-        <v>-77.486494199999996</v>
+        <v>-77.435718373358995</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>289</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="L68" s="2"/>
       <c r="M68" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
+      </c>
+      <c r="N68" s="28" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="H69" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I69" s="2">
+        <v>38.875816034503501</v>
+      </c>
+      <c r="J69" s="2">
+        <v>-77.435718373358995</v>
+      </c>
+      <c r="K69" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="I69" s="2">
-        <v>38.906303508879397</v>
-      </c>
-      <c r="J69" s="2">
-        <v>-77.222641329237604</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="L69" s="2"/>
       <c r="M69" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+      <c r="N69" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>297</v>
@@ -4763,7 +4981,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>293</v>
+        <v>28</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>298</v>
@@ -4772,13 +4990,13 @@
         <v>299</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="I70" s="2">
-        <v>38.875816034503501</v>
+        <v>38.873610192974397</v>
       </c>
       <c r="J70" s="2">
-        <v>-77.435718373358995</v>
+        <v>-77.3055466310296</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>300</v>
@@ -4787,290 +5005,315 @@
       <c r="M70" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="N70" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>302</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>299</v>
+        <v>98</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I71" s="2">
-        <v>38.875816034503501</v>
+        <v>38.868590773014198</v>
       </c>
       <c r="J71" s="2">
-        <v>-77.435718373358995</v>
+        <v>-77.224144877053305</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="L71" s="2"/>
       <c r="M71" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+      <c r="N71" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>4</v>
+        <v>318</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="I72" s="2">
-        <v>38.873610192974397</v>
+        <v>38.774379099999997</v>
       </c>
       <c r="J72" s="2">
-        <v>-77.3055466310296</v>
+        <v>-77.074015599999996</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>307</v>
+        <v>15</v>
       </c>
       <c r="L72" s="2"/>
-      <c r="M72" s="2" t="s">
-        <v>308</v>
+      <c r="M72" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="N72" s="28" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>256</v>
+        <v>9</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F73" s="2" t="s">
+      <c r="H73" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I73" s="2">
+        <v>38.8060490968736</v>
+      </c>
+      <c r="J73" s="2">
+        <v>-77.181676502196197</v>
+      </c>
+      <c r="K73" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="I73" s="2">
-        <v>38.868590773014198</v>
-      </c>
-      <c r="J73" s="2">
-        <v>-77.224144877053305</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="L73" s="2"/>
       <c r="M73" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="N73" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="N73" s="2"/>
-    </row>
-    <row r="74" spans="1:14" ht="84" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>320</v>
-      </c>
       <c r="B74" s="2" t="s">
-        <v>256</v>
+        <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>11</v>
+        <v>307</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>28</v>
+        <v>286</v>
       </c>
       <c r="F74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I74" s="2">
+        <v>38.8060490968736</v>
+      </c>
+      <c r="J74" s="2">
+        <v>-77.181676502196197</v>
+      </c>
+      <c r="K74" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="G74" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="I74" s="2">
-        <v>38.774379099999997</v>
-      </c>
-      <c r="J74" s="2">
-        <v>-77.074015599999996</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="L74" s="2"/>
-      <c r="M74" s="8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="M74" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="N74" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>315</v>
+        <v>25</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="I75" s="2">
-        <v>38.8060490968736</v>
+        <v>38.8553917225858</v>
       </c>
       <c r="J75" s="2">
-        <v>-77.181676502196197</v>
+        <v>-77.362718702194798</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="L75" s="2"/>
       <c r="M75" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+      <c r="N75" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="126" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>9</v>
+        <v>256</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>293</v>
+        <v>28</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>29</v>
+        <v>298</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>316</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="I76" s="2">
-        <v>38.8060490968736</v>
+        <v>38.854251580169802</v>
       </c>
       <c r="J76" s="2">
-        <v>-77.181676502196197</v>
+        <v>-77.356579302194902</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="L76" s="2"/>
       <c r="M76" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+      <c r="N76" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>9</v>
+        <v>256</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>293</v>
+        <v>28</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>25</v>
+        <v>298</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="I77" s="2">
-        <v>38.8553917225858</v>
+        <v>38.8553408</v>
       </c>
       <c r="J77" s="2">
-        <v>-77.362718702194798</v>
+        <v>-77.364854500000007</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="M77" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="N77" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>4</v>
@@ -5079,37 +5322,42 @@
         <v>28</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G78" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I78" s="2">
+        <v>38.8553408</v>
+      </c>
+      <c r="J78" s="2">
+        <v>-77.364854500000007</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L78" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="I78" s="2">
-        <v>38.854251580169802</v>
-      </c>
-      <c r="J78" s="2">
-        <v>-77.356579302194902</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2" t="s">
+      <c r="M78" s="8" t="s">
         <v>324</v>
+      </c>
+      <c r="N78" s="28" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>4</v>
@@ -5118,13 +5366,13 @@
         <v>28</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>365</v>
+        <v>424</v>
       </c>
       <c r="I79" s="2">
         <v>38.8553408</v>
@@ -5133,24 +5381,25 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="M79" s="8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="M79" s="8"/>
+      <c r="N79" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>257</v>
+        <v>369</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>332</v>
+        <v>387</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>4</v>
@@ -5159,39 +5408,40 @@
         <v>28</v>
       </c>
       <c r="F80" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="I80" s="2">
+        <v>38.886493000000002</v>
+      </c>
+      <c r="J80" s="2">
+        <v>-77.176064999999994</v>
+      </c>
+      <c r="K80" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G80" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="I80" s="2">
-        <v>38.8553408</v>
-      </c>
-      <c r="J80" s="2">
-        <v>-77.364854500000007</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="L80" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="M80" s="8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="L80" s="2"/>
+      <c r="M80" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="N80" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>257</v>
+        <v>369</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>334</v>
+        <v>391</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>4</v>
@@ -5200,78 +5450,78 @@
         <v>28</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>305</v>
+        <v>388</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>432</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="H81" s="2"/>
       <c r="I81" s="2">
-        <v>38.8553408</v>
+        <v>38.965629999999997</v>
       </c>
       <c r="J81" s="2">
-        <v>-77.364854500000007</v>
+        <v>-77.358909999999995</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="L81" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="M81" s="8"/>
-    </row>
-    <row r="82" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="N81" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>84</v>
+        <v>393</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>85</v>
+        <v>388</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>351</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="H82" s="2"/>
       <c r="I82" s="2">
-        <v>0</v>
+        <v>38.850720000000003</v>
       </c>
       <c r="J82" s="2">
-        <v>0</v>
+        <v>-77.29956</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L82" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="L82" s="2"/>
       <c r="M82" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+      <c r="N82" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>4</v>
@@ -5280,37 +5530,40 @@
         <v>28</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>396</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="I83" s="2">
-        <v>38.886493000000002</v>
+        <v>38.869669999999999</v>
       </c>
       <c r="J83" s="2">
-        <v>-77.176064999999994</v>
+        <v>-77.147750000000002</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N83" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>320</v>
+        <v>398</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>4</v>
@@ -5319,35 +5572,34 @@
         <v>28</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2">
-        <v>38.965629999999997</v>
-      </c>
-      <c r="J84" s="2">
-        <v>-77.358909999999995</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="H84" s="6"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
       <c r="K84" s="2" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+      <c r="N84" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>4</v>
@@ -5356,35 +5608,40 @@
         <v>28</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="H85" s="2"/>
+        <v>403</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>419</v>
+      </c>
       <c r="I85" s="2">
-        <v>38.850720000000003</v>
+        <v>38.849589999999999</v>
       </c>
       <c r="J85" s="2">
-        <v>-77.29956</v>
+        <v>-77.316599999999994</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+      <c r="N85" s="29" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>4</v>
@@ -5393,37 +5650,40 @@
         <v>28</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>403</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="I86" s="2">
-        <v>38.869669999999999</v>
+        <v>38.831009999999999</v>
       </c>
       <c r="J86" s="2">
-        <v>-77.147750000000002</v>
+        <v>-77.185820000000007</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>312</v>
+        <v>415</v>
       </c>
       <c r="L86" s="2"/>
       <c r="M86" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+      <c r="N86" s="29" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>4</v>
@@ -5432,226 +5692,250 @@
         <v>28</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>426</v>
+        <v>408</v>
+      </c>
+      <c r="H87" s="22" t="s">
+        <v>421</v>
       </c>
       <c r="I87" s="2">
-        <v>38.731589999999997</v>
+        <v>0</v>
       </c>
       <c r="J87" s="2">
-        <v>-77.104609999999994</v>
+        <v>0</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="L87" s="2"/>
       <c r="M87" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+      <c r="N87" s="29" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>28</v>
+        <v>191</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>395</v>
+        <v>411</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="I88" s="2">
-        <v>38.969389999999997</v>
+        <v>0</v>
       </c>
       <c r="J88" s="2">
-        <v>-77.342410000000001</v>
+        <v>0</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>421</v>
+        <v>44</v>
       </c>
       <c r="L88" s="2"/>
       <c r="M88" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+      <c r="N88" s="29" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>406</v>
+        <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>407</v>
+        <v>446</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>28</v>
+        <v>191</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>395</v>
+        <v>54</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="H89" s="6"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
+        <v>169</v>
+      </c>
+      <c r="H89" s="23" t="s">
+        <v>425</v>
+      </c>
+      <c r="I89" s="2">
+        <v>39.025618681403103</v>
+      </c>
+      <c r="J89" s="2">
+        <v>-77.408055773543396</v>
+      </c>
       <c r="K89" s="2" t="s">
-        <v>422</v>
+        <v>50</v>
       </c>
       <c r="L89" s="2"/>
-      <c r="M89" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="M89" s="24" t="s">
+        <v>429</v>
+      </c>
+      <c r="N89" s="29" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>320</v>
+        <v>8</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>410</v>
+        <v>440</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>28</v>
+        <v>191</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>395</v>
+        <v>54</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="H90" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="H90" s="23" t="s">
+        <v>435</v>
+      </c>
+      <c r="I90" s="2">
+        <v>39.025618681403103</v>
+      </c>
+      <c r="J90" s="2">
+        <v>-77.408055773543396</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L90" s="2"/>
+      <c r="M90" s="25" t="s">
+        <v>430</v>
+      </c>
+      <c r="N90" s="29" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="I90" s="2">
-        <v>38.849589999999999</v>
-      </c>
-      <c r="J90" s="2">
-        <v>-77.316599999999994</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="L90" s="2"/>
-      <c r="M90" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="H91" s="6" t="s">
+      <c r="I91" s="2">
+        <v>39.097752638349299</v>
+      </c>
+      <c r="J91" s="2">
+        <v>-77.539036848396407</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L91" s="2"/>
+      <c r="M91" s="24" t="s">
         <v>428</v>
       </c>
-      <c r="I91" s="2">
-        <v>38.831009999999999</v>
-      </c>
-      <c r="J91" s="2">
-        <v>-77.185820000000007</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="L91" s="2"/>
-      <c r="M91" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="N91" s="29" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>320</v>
+        <v>8</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>415</v>
+        <v>442</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>28</v>
+        <v>191</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>395</v>
+        <v>54</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="H92" s="22" t="s">
-        <v>429</v>
+        <v>169</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>436</v>
       </c>
       <c r="I92" s="2">
-        <v>0</v>
+        <v>39.114615286054203</v>
       </c>
       <c r="J92" s="2">
-        <v>0</v>
+        <v>-77.540639660046097</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="L92" s="2"/>
-      <c r="M92" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="M92" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="N92" s="29" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>320</v>
+        <v>8</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>4</v>
@@ -5660,37 +5944,40 @@
         <v>191</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>419</v>
+        <v>54</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="H93" s="6" t="s">
-        <v>430</v>
+        <v>169</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>437</v>
       </c>
       <c r="I93" s="2">
-        <v>0</v>
+        <v>39.114615286054203</v>
       </c>
       <c r="J93" s="2">
-        <v>0</v>
+        <v>-77.540639660046097</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="L93" s="2"/>
-      <c r="M93" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="M93" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="N93" s="29" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>376</v>
+        <v>255</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>4</v>
@@ -5704,32 +5991,35 @@
       <c r="G94" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="H94" s="23" t="s">
-        <v>433</v>
+      <c r="H94" s="2" t="s">
+        <v>439</v>
       </c>
       <c r="I94" s="2">
-        <v>39.025618681403103</v>
+        <v>39.097752638349299</v>
       </c>
       <c r="J94" s="2">
-        <v>-77.408055773543396</v>
+        <v>-77.539036848396407</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>50</v>
       </c>
       <c r="L94" s="2"/>
-      <c r="M94" s="24" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="M94" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="N94" s="29" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>376</v>
+        <v>255</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>4</v>
@@ -5741,257 +6031,68 @@
         <v>54</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="H95" s="23" t="s">
-        <v>443</v>
+        <v>432</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>438</v>
       </c>
       <c r="I95" s="2">
-        <v>39.025618681403103</v>
+        <v>39.097752638349299</v>
       </c>
       <c r="J95" s="2">
-        <v>-77.408055773543396</v>
+        <v>-77.539036848396407</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>50</v>
       </c>
       <c r="L95" s="2"/>
       <c r="M95" s="25" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+      <c r="N95" s="29" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>254</v>
+        <v>369</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>449</v>
+        <v>407</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>191</v>
+        <v>28</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>54</v>
+        <v>388</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>435</v>
+        <v>408</v>
+      </c>
+      <c r="H96" s="22" t="s">
+        <v>421</v>
       </c>
       <c r="I96" s="2">
-        <v>39.097752638349299</v>
+        <v>0</v>
       </c>
       <c r="J96" s="2">
-        <v>-77.539036848396407</v>
+        <v>0</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L96" s="2"/>
-      <c r="M96" s="24" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H97" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="I97" s="2">
-        <v>39.114615286054203</v>
-      </c>
-      <c r="J97" s="2">
-        <v>-77.540639660046097</v>
-      </c>
-      <c r="K97" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L97" s="2"/>
-      <c r="M97" s="26" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="I98" s="2">
-        <v>39.114615286054203</v>
-      </c>
-      <c r="J98" s="2">
-        <v>-77.540639660046097</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L98" s="2"/>
-      <c r="M98" s="25" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="I99" s="2">
-        <v>39.097752638349299</v>
-      </c>
-      <c r="J99" s="2">
-        <v>-77.539036848396407</v>
-      </c>
-      <c r="K99" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L99" s="2"/>
-      <c r="M99" s="25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="I100" s="2">
-        <v>39.097752638349299</v>
-      </c>
-      <c r="J100" s="2">
-        <v>-77.539036848396407</v>
-      </c>
-      <c r="K100" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L100" s="2"/>
-      <c r="M100" s="25" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="H101" s="22" t="s">
-        <v>429</v>
-      </c>
-      <c r="I101" s="2">
-        <v>0</v>
-      </c>
-      <c r="J101" s="2">
-        <v>0</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L101" s="2"/>
-      <c r="M101" s="2" t="s">
-        <v>417</v>
+      <c r="M96" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="N96" s="29" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -6014,19 +6115,19 @@
     <hyperlink ref="M55" r:id="rId16" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
     <hyperlink ref="M56" r:id="rId17" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
     <hyperlink ref="M48" r:id="rId18" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
-    <hyperlink ref="M74" r:id="rId19" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
-    <hyperlink ref="M79" r:id="rId20" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
-    <hyperlink ref="M80" r:id="rId21" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
+    <hyperlink ref="M72" r:id="rId19" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
+    <hyperlink ref="M77" r:id="rId20" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
+    <hyperlink ref="M78" r:id="rId21" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
     <hyperlink ref="M34" r:id="rId22" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
     <hyperlink ref="M36" r:id="rId23" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
     <hyperlink ref="M32" r:id="rId24" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
-    <hyperlink ref="M96" r:id="rId25" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
-    <hyperlink ref="M94" r:id="rId26" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
-    <hyperlink ref="M95" r:id="rId27" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
-    <hyperlink ref="M100" r:id="rId28" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
-    <hyperlink ref="M99" r:id="rId29" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
-    <hyperlink ref="M98" r:id="rId30" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
-    <hyperlink ref="M97" r:id="rId31" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
+    <hyperlink ref="M91" r:id="rId25" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
+    <hyperlink ref="M89" r:id="rId26" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
+    <hyperlink ref="M90" r:id="rId27" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
+    <hyperlink ref="M95" r:id="rId28" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
+    <hyperlink ref="M94" r:id="rId29" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
+    <hyperlink ref="M93" r:id="rId30" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
+    <hyperlink ref="M92" r:id="rId31" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId32"/>
@@ -6049,13 +6150,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
@@ -6071,7 +6172,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B4" s="13">
         <v>3</v>
@@ -6079,7 +6180,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B7" s="15"/>
     </row>
@@ -6093,7 +6194,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B9" s="15">
         <v>11</v>
@@ -6101,7 +6202,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B10" s="15">
         <v>12</v>
@@ -6109,7 +6210,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B11" s="15">
         <v>13</v>
@@ -6117,7 +6218,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B12" s="15">
         <v>14</v>
@@ -6125,7 +6226,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B13" s="15">
         <v>15</v>
@@ -6133,7 +6234,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B15" s="17"/>
     </row>
@@ -6155,7 +6256,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B18" s="17">
         <v>22</v>
@@ -6163,7 +6264,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B20" s="19">
         <v>1</v>
@@ -6171,7 +6272,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B21" s="19">
         <v>10</v>
@@ -6179,7 +6280,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="B23" s="21">
         <v>1</v>
@@ -6187,7 +6288,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B24" s="21">
         <v>5</v>

</xml_diff>

<commit_message>
tried to source(theme.R), changed 2 locations on excel
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F3FBEB-CDFD-CF4A-B8BC-3AEB31927FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134EEB20-BE47-E646-A9B4-ECDE14009A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="456">
   <si>
     <t>County</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Loudoun County Local Bus Service; Free for all in the county; Runs every 20 mins at 10 stops </t>
   </si>
   <si>
-    <t>Loudoun County </t>
-  </si>
-  <si>
     <t>Loudoun County Department of Transit and Commuter Services </t>
   </si>
   <si>
@@ -431,9 +428,6 @@
   </si>
   <si>
     <t>Mulitple locations </t>
-  </si>
-  <si>
-    <t>Pittsburgh and McKeesport</t>
   </si>
   <si>
     <t>Community Care Behavioral Health Organization</t>
@@ -1157,9 +1151,6 @@
     <t xml:space="preserve">Qualify for Medicaid </t>
   </si>
   <si>
-    <t>Allegheny County</t>
-  </si>
-  <si>
     <t>Homestead</t>
   </si>
   <si>
@@ -1414,6 +1405,12 @@
   </si>
   <si>
     <t>Loudoun, Fairfax, Allegheny</t>
+  </si>
+  <si>
+    <t>Pittsburgh, McKeesport</t>
+  </si>
+  <si>
+    <t>Loudoun </t>
   </si>
 </sst>
 </file>
@@ -1940,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1987,22 +1984,22 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="N1" s="28" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
@@ -2028,7 +2025,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I2" s="2">
         <v>38.840490000000003</v>
@@ -2046,7 +2043,7 @@
         <v>17</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2069,7 +2066,7 @@
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>20</v>
@@ -2090,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2113,10 +2110,10 @@
         <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="I4" s="2">
         <v>37.538339999999998</v>
@@ -2134,7 +2131,7 @@
         <v>26</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
@@ -2178,7 +2175,7 @@
         <v>34</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2222,7 +2219,7 @@
         <v>34</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2266,7 +2263,7 @@
         <v>34</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2310,7 +2307,7 @@
         <v>34</v>
       </c>
       <c r="N8" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2354,7 +2351,7 @@
         <v>34</v>
       </c>
       <c r="N9" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2362,7 +2359,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>47</v>
@@ -2380,7 +2377,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I10" s="2">
         <v>39.114306589999998</v>
@@ -2398,7 +2395,7 @@
         <v>52</v>
       </c>
       <c r="N10" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2406,7 +2403,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>53</v>
@@ -2424,7 +2421,7 @@
         <v>55</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I11" s="2">
         <v>39.114306589999998</v>
@@ -2442,7 +2439,7 @@
         <v>57</v>
       </c>
       <c r="N11" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2450,7 +2447,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>58</v>
@@ -2486,7 +2483,7 @@
         <v>62</v>
       </c>
       <c r="N12" s="28" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2494,7 +2491,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>63</v>
@@ -2506,13 +2503,13 @@
         <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -2526,7 +2523,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2534,7 +2531,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>64</v>
@@ -2546,13 +2543,13 @@
         <v>28</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -2566,7 +2563,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2574,7 +2571,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>65</v>
@@ -2601,16 +2598,16 @@
         <v>-77.555403999999996</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="N15" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -2618,10 +2615,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
@@ -2633,10 +2630,10 @@
         <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I16" s="2">
         <v>37.61065696</v>
@@ -2645,16 +2642,16 @@
         <v>-77.340073020000005</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="L16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="N16" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2662,10 +2659,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>4</v>
@@ -2677,10 +2674,10 @@
         <v>39</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="I17" s="2">
         <v>39.114571660000003</v>
@@ -2689,16 +2686,16 @@
         <v>-77.540547570000001</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="L17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M17" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="N17" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2706,10 +2703,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>4</v>
@@ -2718,13 +2715,13 @@
         <v>28</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="H18" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -2736,13 +2733,13 @@
         <v>44</v>
       </c>
       <c r="L18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="N18" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2750,10 +2747,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>4</v>
@@ -2762,13 +2759,13 @@
         <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I19" s="2">
         <v>0</v>
@@ -2780,13 +2777,13 @@
         <v>44</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N19" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2794,10 +2791,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>11</v>
@@ -2809,10 +2806,10 @@
         <v>54</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -2824,13 +2821,13 @@
         <v>44</v>
       </c>
       <c r="L20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M20" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="N20" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2838,10 +2835,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -2856,7 +2853,7 @@
         <v>40</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -2868,13 +2865,13 @@
         <v>44</v>
       </c>
       <c r="L21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M21" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="N21" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -2882,10 +2879,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>11</v>
@@ -2897,10 +2894,10 @@
         <v>54</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -2918,7 +2915,7 @@
         <v>23</v>
       </c>
       <c r="N22" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="63" x14ac:dyDescent="0.2">
@@ -2926,10 +2923,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>4</v>
@@ -2938,13 +2935,13 @@
         <v>12</v>
       </c>
       <c r="F23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -2957,21 +2954,21 @@
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N23" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>11</v>
@@ -2980,13 +2977,13 @@
         <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="I24" s="2">
         <v>40.439188049999998</v>
@@ -2995,27 +2992,27 @@
         <v>-80.001456360000006</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M24" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="N24" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>11</v>
@@ -3024,13 +3021,13 @@
         <v>12</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="I25" s="2">
         <v>40.437306100000001</v>
@@ -3039,27 +3036,27 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="M25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N25" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
@@ -3068,13 +3065,13 @@
         <v>12</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="I26" s="2">
         <v>40.349269890000002</v>
@@ -3083,27 +3080,27 @@
         <v>-79.832162819999994</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="M26" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="N26" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>4</v>
@@ -3115,10 +3112,10 @@
         <v>54</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="I27" s="2">
         <v>40.439132790000002</v>
@@ -3127,27 +3124,27 @@
         <v>-79.994721900000002</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M27" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M27" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="N27" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>11</v>
@@ -3156,40 +3153,40 @@
         <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="N28" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>4</v>
@@ -3201,10 +3198,10 @@
         <v>54</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I29" s="2">
         <v>40.40062056</v>
@@ -3213,27 +3210,27 @@
         <v>-79.8352431</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N29" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>4</v>
@@ -3242,13 +3239,13 @@
         <v>28</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I30" s="2">
         <v>40.40062056</v>
@@ -3257,27 +3254,27 @@
         <v>-79.8352431</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>11</v>
@@ -3289,7 +3286,7 @@
         <v>29</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2">
@@ -3299,27 +3296,27 @@
         <v>-79.8352431</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N31" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>4</v>
@@ -3331,10 +3328,10 @@
         <v>29</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I32" s="2">
         <v>40.439188049999998</v>
@@ -3343,27 +3340,27 @@
         <v>-80.001456360000006</v>
       </c>
       <c r="K32" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="M32" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N32" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>4</v>
@@ -3372,13 +3369,13 @@
         <v>28</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="I33" s="2">
         <v>40.437306100000001</v>
@@ -3387,27 +3384,27 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="M33" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N33" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>4</v>
@@ -3416,13 +3413,13 @@
         <v>28</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I34" s="2">
         <v>40.437306100000001</v>
@@ -3431,27 +3428,27 @@
         <v>-80.001021339999994</v>
       </c>
       <c r="K34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L34" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="M34" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N34" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>4</v>
@@ -3460,13 +3457,13 @@
         <v>28</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -3478,24 +3475,24 @@
         <v>44</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N35" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>11</v>
@@ -3504,13 +3501,13 @@
         <v>28</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
@@ -3522,24 +3519,24 @@
         <v>44</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="N36" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>4</v>
@@ -3548,13 +3545,13 @@
         <v>28</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I37" s="2">
         <v>0</v>
@@ -3566,24 +3563,24 @@
         <v>44</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="N37" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>4</v>
@@ -3592,13 +3589,13 @@
         <v>28</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -3610,13 +3607,13 @@
         <v>44</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -3624,25 +3621,25 @@
         <v>8</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="I39" s="2">
         <v>0</v>
@@ -3654,13 +3651,13 @@
         <v>44</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -3668,10 +3665,10 @@
         <v>8</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>4</v>
@@ -3680,13 +3677,13 @@
         <v>28</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I40" s="2">
         <v>39.076819999999998</v>
@@ -3698,13 +3695,13 @@
         <v>50</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -3712,10 +3709,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>4</v>
@@ -3724,13 +3721,13 @@
         <v>28</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I41" s="2">
         <v>39.114409999999999</v>
@@ -3742,13 +3739,13 @@
         <v>50</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N41" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -3756,10 +3753,10 @@
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>4</v>
@@ -3768,13 +3765,13 @@
         <v>28</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="I42" s="2">
         <v>39.115279999999998</v>
@@ -3786,13 +3783,13 @@
         <v>50</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N42" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -3800,10 +3797,10 @@
         <v>8</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>4</v>
@@ -3812,13 +3809,13 @@
         <v>28</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I43" s="2">
         <v>0</v>
@@ -3830,13 +3827,13 @@
         <v>44</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N43" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="63" x14ac:dyDescent="0.2">
@@ -3844,25 +3841,25 @@
         <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I44" s="2">
         <v>39.108399900000002</v>
@@ -3874,13 +3871,13 @@
         <v>50</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N44" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="21" x14ac:dyDescent="0.2">
@@ -3891,7 +3888,7 @@
         <v>9</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>4</v>
@@ -3900,13 +3897,13 @@
         <v>28</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I45" s="2">
         <v>39.114406199999998</v>
@@ -3918,13 +3915,13 @@
         <v>50</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N45" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -3932,10 +3929,10 @@
         <v>8</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>4</v>
@@ -3944,13 +3941,13 @@
         <v>28</v>
       </c>
       <c r="F46" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="H46" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I46" s="2">
         <v>39.117853099999998</v>
@@ -3962,39 +3959,39 @@
         <v>50</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N46" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I47" s="2">
         <v>0</v>
@@ -4006,24 +4003,24 @@
         <v>44</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N47" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>4</v>
@@ -4032,13 +4029,13 @@
         <v>28</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I48" s="2">
         <v>40.439779999999999</v>
@@ -4047,42 +4044,42 @@
         <v>-79.998869999999997</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N48" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I49" s="2">
         <v>0</v>
@@ -4094,39 +4091,39 @@
         <v>44</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N49" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I50" s="2">
         <v>0</v>
@@ -4138,39 +4135,39 @@
         <v>44</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N50" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="I51" s="2">
         <v>0</v>
@@ -4182,39 +4179,39 @@
         <v>44</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N51" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I52" s="2">
         <v>0</v>
@@ -4226,39 +4223,39 @@
         <v>44</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N52" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I53" s="2">
         <v>0</v>
@@ -4270,24 +4267,24 @@
         <v>44</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="N53" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>4</v>
@@ -4296,13 +4293,13 @@
         <v>28</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I54" s="2">
         <v>40.407960000000003</v>
@@ -4311,27 +4308,27 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N54" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>4</v>
@@ -4343,10 +4340,10 @@
         <v>29</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I55" s="2">
         <v>40.405259100000002</v>
@@ -4355,27 +4352,27 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N55" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>4</v>
@@ -4384,13 +4381,13 @@
         <v>28</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I56" s="2">
         <v>40.559510000000003</v>
@@ -4399,42 +4396,42 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N56" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="I57" s="2">
         <v>0</v>
@@ -4446,24 +4443,24 @@
         <v>44</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N57" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>4</v>
@@ -4475,10 +4472,10 @@
         <v>29</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I58" s="2">
         <v>40.427699869999998</v>
@@ -4487,27 +4484,27 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N58" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>4</v>
@@ -4519,10 +4516,10 @@
         <v>29</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I59" s="2">
         <v>40.427699869999998</v>
@@ -4531,27 +4528,27 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N59" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>4</v>
@@ -4563,10 +4560,10 @@
         <v>29</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I60" s="2">
         <v>40.427699869999998</v>
@@ -4575,27 +4572,27 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>371</v>
+        <v>202</v>
       </c>
       <c r="L60" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="M60" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="M60" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="N60" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>4</v>
@@ -4607,10 +4604,10 @@
         <v>29</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I61" s="2">
         <v>40.427699869999998</v>
@@ -4619,27 +4616,27 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>371</v>
+        <v>202</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N61" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>4</v>
@@ -4651,10 +4648,10 @@
         <v>29</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -4663,25 +4660,25 @@
         <v>0</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>371</v>
+        <v>44</v>
       </c>
       <c r="L62" s="2"/>
       <c r="M62" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N62" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>4</v>
@@ -4690,23 +4687,23 @@
         <v>28</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -4714,10 +4711,10 @@
         <v>8</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>4</v>
@@ -4726,13 +4723,13 @@
         <v>28</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="I64" s="2">
         <v>0</v>
@@ -4741,16 +4738,16 @@
         <v>0</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>67</v>
+        <v>455</v>
       </c>
       <c r="L64" s="27" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="N64" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -4758,10 +4755,10 @@
         <v>8</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>4</v>
@@ -4770,13 +4767,13 @@
         <v>28</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I65" s="2">
         <v>39.078167000000001</v>
@@ -4788,13 +4785,13 @@
         <v>50</v>
       </c>
       <c r="L65" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="M65" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="M65" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="N65" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="21" x14ac:dyDescent="0.2">
@@ -4802,10 +4799,10 @@
         <v>8</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>4</v>
@@ -4814,13 +4811,13 @@
         <v>28</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I66" s="2">
         <v>39.045227799999999</v>
@@ -4832,39 +4829,39 @@
         <v>32</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N66" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I67" s="2">
         <v>38.906303508879397</v>
@@ -4873,40 +4870,40 @@
         <v>-77.222641329237604</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="L67" s="2"/>
       <c r="M67" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N67" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="F68" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="H68" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I68" s="2">
         <v>38.875816034503501</v>
@@ -4915,40 +4912,40 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L68" s="2"/>
       <c r="M68" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N68" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I69" s="2">
         <v>38.875816034503501</v>
@@ -4957,25 +4954,25 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L69" s="2"/>
       <c r="M69" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N69" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>4</v>
@@ -4984,13 +4981,13 @@
         <v>28</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I70" s="2">
         <v>38.873610192974397</v>
@@ -4999,40 +4996,40 @@
         <v>-77.3055466310296</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L70" s="2"/>
       <c r="M70" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="N70" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="I71" s="2">
         <v>38.868590773014198</v>
@@ -5041,25 +5038,25 @@
         <v>-77.224144877053305</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L71" s="2"/>
       <c r="M71" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="N71" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>11</v>
@@ -5068,13 +5065,13 @@
         <v>28</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I72" s="2">
         <v>38.774379099999997</v>
@@ -5087,36 +5084,36 @@
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N72" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="H73" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I73" s="2">
         <v>38.8060490968736</v>
@@ -5125,40 +5122,40 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L73" s="2"/>
       <c r="M73" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N73" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I74" s="2">
         <v>38.8060490968736</v>
@@ -5167,40 +5164,40 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L74" s="2"/>
       <c r="M74" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N74" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I75" s="2">
         <v>38.8553917225858</v>
@@ -5209,25 +5206,25 @@
         <v>-77.362718702194798</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L75" s="2"/>
       <c r="M75" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="N75" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="126" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>4</v>
@@ -5236,13 +5233,13 @@
         <v>28</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="I76" s="2">
         <v>38.854251580169802</v>
@@ -5251,25 +5248,25 @@
         <v>-77.356579302194902</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L76" s="2"/>
       <c r="M76" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N76" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>4</v>
@@ -5278,13 +5275,13 @@
         <v>28</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I77" s="2">
         <v>38.8553408</v>
@@ -5293,27 +5290,27 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M77" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N77" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>4</v>
@@ -5322,13 +5319,13 @@
         <v>28</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I78" s="2">
         <v>38.8553408</v>
@@ -5337,27 +5334,27 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M78" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N78" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>4</v>
@@ -5366,13 +5363,13 @@
         <v>28</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I79" s="2">
         <v>38.8553408</v>
@@ -5381,25 +5378,25 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M79" s="8"/>
       <c r="N79" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>4</v>
@@ -5408,13 +5405,13 @@
         <v>28</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="I80" s="2">
         <v>38.886493000000002</v>
@@ -5423,25 +5420,25 @@
         <v>-77.176064999999994</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="N80" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>4</v>
@@ -5450,10 +5447,10 @@
         <v>28</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="2">
@@ -5463,25 +5460,25 @@
         <v>-77.358909999999995</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="L81" s="2"/>
       <c r="M81" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="N81" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>4</v>
@@ -5490,10 +5487,10 @@
         <v>28</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2">
@@ -5503,25 +5500,25 @@
         <v>-77.29956</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L82" s="2"/>
       <c r="M82" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="N82" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>4</v>
@@ -5530,13 +5527,13 @@
         <v>28</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I83" s="2">
         <v>38.869669999999999</v>
@@ -5545,25 +5542,25 @@
         <v>-77.147750000000002</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="N83" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>4</v>
@@ -5572,34 +5569,34 @@
         <v>28</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H84" s="6"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="N84" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>4</v>
@@ -5608,13 +5605,13 @@
         <v>28</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I85" s="2">
         <v>38.849589999999999</v>
@@ -5623,25 +5620,25 @@
         <v>-77.316599999999994</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="N85" s="29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>4</v>
@@ -5650,13 +5647,13 @@
         <v>28</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I86" s="2">
         <v>38.831009999999999</v>
@@ -5665,25 +5662,25 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="L86" s="2"/>
       <c r="M86" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="N86" s="29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>4</v>
@@ -5692,13 +5689,13 @@
         <v>28</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H87" s="22" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="I87" s="2">
         <v>0</v>
@@ -5711,36 +5708,36 @@
       </c>
       <c r="L87" s="2"/>
       <c r="M87" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="N87" s="29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I88" s="2">
         <v>0</v>
@@ -5753,10 +5750,10 @@
       </c>
       <c r="L88" s="2"/>
       <c r="M88" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="N88" s="29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -5764,25 +5761,25 @@
         <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H89" s="23" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I89" s="2">
         <v>39.025618681403103</v>
@@ -5795,10 +5792,10 @@
       </c>
       <c r="L89" s="2"/>
       <c r="M89" s="24" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="N89" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -5806,25 +5803,25 @@
         <v>8</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H90" s="23" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I90" s="2">
         <v>39.025618681403103</v>
@@ -5837,10 +5834,10 @@
       </c>
       <c r="L90" s="2"/>
       <c r="M90" s="25" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="N90" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -5848,25 +5845,25 @@
         <v>8</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="I91" s="2">
         <v>39.097752638349299</v>
@@ -5879,10 +5876,10 @@
       </c>
       <c r="L91" s="2"/>
       <c r="M91" s="24" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="N91" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -5890,25 +5887,25 @@
         <v>8</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H92" s="10" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I92" s="2">
         <v>39.114615286054203</v>
@@ -5921,10 +5918,10 @@
       </c>
       <c r="L92" s="2"/>
       <c r="M92" s="26" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="N92" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -5932,25 +5929,25 @@
         <v>8</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I93" s="2">
         <v>39.114615286054203</v>
@@ -5963,10 +5960,10 @@
       </c>
       <c r="L93" s="2"/>
       <c r="M93" s="25" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="N93" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -5974,25 +5971,25 @@
         <v>8</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I94" s="2">
         <v>39.097752638349299</v>
@@ -6005,10 +6002,10 @@
       </c>
       <c r="L94" s="2"/>
       <c r="M94" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N94" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -6016,25 +6013,25 @@
         <v>8</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I95" s="2">
         <v>39.097752638349299</v>
@@ -6047,10 +6044,10 @@
       </c>
       <c r="L95" s="2"/>
       <c r="M95" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="N95" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -6058,10 +6055,10 @@
         <v>8</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>4</v>
@@ -6070,13 +6067,13 @@
         <v>28</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H96" s="22" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="I96" s="2">
         <v>0</v>
@@ -6089,10 +6086,10 @@
       </c>
       <c r="L96" s="2"/>
       <c r="M96" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="N96" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -6150,13 +6147,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
@@ -6164,7 +6161,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B3" s="13">
         <v>2</v>
@@ -6172,7 +6169,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B4" s="13">
         <v>3</v>
@@ -6180,7 +6177,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B7" s="15"/>
     </row>
@@ -6194,7 +6191,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B9" s="15">
         <v>11</v>
@@ -6202,7 +6199,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B10" s="15">
         <v>12</v>
@@ -6210,7 +6207,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B11" s="15">
         <v>13</v>
@@ -6218,7 +6215,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B12" s="15">
         <v>14</v>
@@ -6226,7 +6223,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B13" s="15">
         <v>15</v>
@@ -6234,7 +6231,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B15" s="17"/>
     </row>
@@ -6248,7 +6245,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B17" s="17">
         <v>21</v>
@@ -6256,7 +6253,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B18" s="17">
         <v>22</v>
@@ -6264,7 +6261,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B20" s="19">
         <v>1</v>
@@ -6272,7 +6269,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B21" s="19">
         <v>10</v>
@@ -6280,7 +6277,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B23" s="21">
         <v>1</v>
@@ -6288,7 +6285,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B24" s="21">
         <v>5</v>

</xml_diff>

<commit_message>
added availability of 32 programs in combined
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134EEB20-BE47-E646-A9B4-ECDE14009A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402DD690-C0A1-48B3-B2EA-D4C5D4156873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="460">
   <si>
     <t>County</t>
   </si>
@@ -1411,6 +1411,18 @@
   </si>
   <si>
     <t>Loudoun </t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In-Person &amp; Online </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online </t>
+  </si>
+  <si>
+    <t>In-Person</t>
   </si>
 </sst>
 </file>
@@ -1935,13 +1947,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N96"/>
+  <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -1956,9 +1968,10 @@
     <col min="12" max="12" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="54" style="9" customWidth="1"/>
     <col min="14" max="14" width="32.1640625" customWidth="1"/>
+    <col min="15" max="15" width="34.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2001,8 +2014,11 @@
       <c r="N1" s="28" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O1" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2045,8 +2061,11 @@
       <c r="N2" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O2" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2089,8 +2108,11 @@
       <c r="N3" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O3" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2133,8 +2155,11 @@
       <c r="N4" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O4" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2177,8 +2202,11 @@
       <c r="N5" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O5" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2221,8 +2249,11 @@
       <c r="N6" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O6" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2265,8 +2296,11 @@
       <c r="N7" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O7" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2309,8 +2343,11 @@
       <c r="N8" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O8" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2353,8 +2390,11 @@
       <c r="N9" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O9" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2397,8 +2437,11 @@
       <c r="N10" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O10" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2441,8 +2484,11 @@
       <c r="N11" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O11" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2486,7 +2532,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2525,8 +2571,11 @@
       <c r="N13" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O13" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2565,8 +2614,11 @@
       <c r="N14" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O14" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2609,8 +2661,11 @@
       <c r="N15" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O15" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2653,8 +2708,11 @@
       <c r="N16" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O16" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2697,8 +2755,11 @@
       <c r="N17" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O17" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2741,8 +2802,11 @@
       <c r="N18" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O18" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2785,8 +2849,11 @@
       <c r="N19" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O19" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -2829,8 +2896,11 @@
       <c r="N20" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O20" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -2873,8 +2943,11 @@
       <c r="N21" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O21" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2917,8 +2990,11 @@
       <c r="N22" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O22" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2959,8 +3035,11 @@
       <c r="N23" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O23" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>202</v>
       </c>
@@ -3003,8 +3082,11 @@
       <c r="N24" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O24" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>202</v>
       </c>
@@ -3047,8 +3129,11 @@
       <c r="N25" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O25" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>202</v>
       </c>
@@ -3091,8 +3176,11 @@
       <c r="N26" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O26" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>202</v>
       </c>
@@ -3135,8 +3223,11 @@
       <c r="N27" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O27" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>202</v>
       </c>
@@ -3177,8 +3268,11 @@
       <c r="N28" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O28" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>202</v>
       </c>
@@ -3221,8 +3315,11 @@
       <c r="N29" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O29" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
@@ -3265,8 +3362,11 @@
       <c r="N30" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O30" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="41" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>202</v>
       </c>
@@ -3307,8 +3407,11 @@
       <c r="N31" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="O31" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="82" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>202</v>
       </c>
@@ -3351,8 +3454,11 @@
       <c r="N32" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="O32" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>202</v>
       </c>
@@ -3396,7 +3502,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>202</v>
       </c>
@@ -3440,7 +3546,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>202</v>
       </c>
@@ -3484,7 +3590,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
@@ -3528,7 +3634,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>202</v>
       </c>
@@ -3572,7 +3678,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>202</v>
       </c>
@@ -3616,7 +3722,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
@@ -3660,7 +3766,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -3704,7 +3810,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
@@ -3748,7 +3854,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>8</v>
       </c>
@@ -3792,7 +3898,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
@@ -3836,7 +3942,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -3880,7 +3986,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>8</v>
       </c>
@@ -3924,7 +4030,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>8</v>
       </c>
@@ -3968,7 +4074,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>202</v>
       </c>
@@ -4012,7 +4118,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>202</v>
       </c>
@@ -4056,7 +4162,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>202</v>
       </c>
@@ -4100,7 +4206,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>202</v>
       </c>
@@ -4144,7 +4250,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>202</v>
       </c>
@@ -4188,7 +4294,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>202</v>
       </c>
@@ -4232,7 +4338,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>202</v>
       </c>
@@ -4276,7 +4382,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>202</v>
       </c>
@@ -4320,7 +4426,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>202</v>
       </c>
@@ -4364,7 +4470,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>202</v>
       </c>
@@ -4408,7 +4514,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>202</v>
       </c>
@@ -4452,7 +4558,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>202</v>
       </c>
@@ -4496,7 +4602,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>202</v>
       </c>
@@ -4540,7 +4646,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>202</v>
       </c>
@@ -4584,7 +4690,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>202</v>
       </c>
@@ -4628,7 +4734,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>202</v>
       </c>
@@ -4670,7 +4776,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>202</v>
       </c>
@@ -4706,7 +4812,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>8</v>
       </c>
@@ -4750,7 +4856,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>8</v>
       </c>
@@ -4794,7 +4900,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>8</v>
       </c>
@@ -4838,7 +4944,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>311</v>
       </c>
@@ -4880,7 +4986,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>311</v>
       </c>
@@ -4922,7 +5028,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>311</v>
       </c>
@@ -4964,7 +5070,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>311</v>
       </c>
@@ -5006,7 +5112,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>311</v>
       </c>
@@ -5048,7 +5154,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="82" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>311</v>
       </c>
@@ -5090,7 +5196,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>311</v>
       </c>
@@ -5132,7 +5238,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>311</v>
       </c>
@@ -5174,7 +5280,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>311</v>
       </c>
@@ -5216,7 +5322,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="123" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>311</v>
       </c>
@@ -5258,7 +5364,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>311</v>
       </c>
@@ -5302,7 +5408,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>311</v>
       </c>
@@ -5346,7 +5452,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>311</v>
       </c>
@@ -5388,7 +5494,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>311</v>
       </c>
@@ -5430,7 +5536,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>311</v>
       </c>
@@ -5470,7 +5576,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>311</v>
       </c>
@@ -5510,7 +5616,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>311</v>
       </c>
@@ -5552,7 +5658,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>395</v>
       </c>
@@ -5588,7 +5694,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>311</v>
       </c>
@@ -5630,7 +5736,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
         <v>311</v>
       </c>
@@ -5672,7 +5778,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
         <v>311</v>
       </c>
@@ -5714,7 +5820,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
         <v>311</v>
       </c>
@@ -5756,7 +5862,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
@@ -5798,7 +5904,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
         <v>8</v>
       </c>
@@ -5840,7 +5946,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5882,7 +5988,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
@@ -5924,7 +6030,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>8</v>
       </c>
@@ -5966,7 +6072,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
         <v>8</v>
       </c>
@@ -6008,7 +6114,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
         <v>8</v>
       </c>
@@ -6050,7 +6156,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="41" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
         <v>8</v>
       </c>
@@ -6139,19 +6245,19 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>373</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>374</v>
       </c>
@@ -6159,7 +6265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>202</v>
       </c>
@@ -6167,7 +6273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>375</v>
       </c>
@@ -6175,13 +6281,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>376</v>
       </c>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
@@ -6189,7 +6295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>377</v>
       </c>
@@ -6197,7 +6303,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>251</v>
       </c>
@@ -6205,7 +6311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>263</v>
       </c>
@@ -6213,7 +6319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>367</v>
       </c>
@@ -6221,7 +6327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>252</v>
       </c>
@@ -6229,13 +6335,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>378</v>
       </c>
       <c r="B15" s="17"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>11</v>
       </c>
@@ -6243,7 +6349,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>159</v>
       </c>
@@ -6251,7 +6357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>379</v>
       </c>
@@ -6259,7 +6365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>380</v>
       </c>
@@ -6267,7 +6373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>381</v>
       </c>
@@ -6275,7 +6381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>382</v>
       </c>
@@ -6283,7 +6389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>383</v>
       </c>

</xml_diff>

<commit_message>
I added the way to apply and I am going to do more.
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134EEB20-BE47-E646-A9B4-ECDE14009A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E5B011-A09E-CB43-AD7D-2A5B7CAF3B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="459">
   <si>
     <t>County</t>
   </si>
@@ -1411,6 +1411,15 @@
   </si>
   <si>
     <t>Loudoun </t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Online application for assessment and then contact Ziyoda Crew with additional documents.</t>
+  </si>
+  <si>
+    <t>Online, Allegheny</t>
   </si>
 </sst>
 </file>
@@ -1554,7 +1563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1614,6 +1623,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1935,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
-  <dimension ref="A1:N96"/>
+  <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+    <sheetView tabSelected="1" topLeftCell="L35" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1956,9 +1971,10 @@
     <col min="12" max="12" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="54" style="9" customWidth="1"/>
     <col min="14" max="14" width="32.1640625" customWidth="1"/>
+    <col min="15" max="15" width="56.33203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2001,8 +2017,11 @@
       <c r="N1" s="28" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O1" s="9" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2039,14 +2058,17 @@
       <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O2" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2083,14 +2105,17 @@
       <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="26" t="s">
         <v>23</v>
       </c>
       <c r="N3" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O3" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2133,8 +2158,11 @@
       <c r="N4" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O4" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2171,14 +2199,17 @@
       <c r="L5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="26" t="s">
         <v>34</v>
       </c>
       <c r="N5" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O5" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2221,8 +2252,11 @@
       <c r="N6" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O6" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2265,8 +2299,11 @@
       <c r="N7" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O7" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2309,8 +2346,11 @@
       <c r="N8" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O8" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2353,8 +2393,11 @@
       <c r="N9" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O9" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2391,14 +2434,17 @@
       <c r="L10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="26" t="s">
         <v>52</v>
       </c>
       <c r="N10" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O10" s="30" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2435,14 +2481,17 @@
       <c r="L11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="26" t="s">
         <v>57</v>
       </c>
       <c r="N11" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O11" s="31" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2479,14 +2528,17 @@
       <c r="L12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="26" t="s">
         <v>62</v>
       </c>
       <c r="N12" s="28" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O12" s="28" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2523,10 +2575,13 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="28" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+        <v>452</v>
+      </c>
+      <c r="O13" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2563,10 +2618,13 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="28" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+        <v>452</v>
+      </c>
+      <c r="O14" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2603,14 +2661,17 @@
       <c r="L15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="26" t="s">
         <v>68</v>
       </c>
       <c r="N15" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O15" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2647,14 +2708,17 @@
       <c r="L16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="26" t="s">
         <v>72</v>
       </c>
       <c r="N16" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O16" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2691,14 +2755,17 @@
       <c r="L17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="26" t="s">
         <v>77</v>
       </c>
       <c r="N17" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O17" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2735,14 +2802,17 @@
       <c r="L18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="26" t="s">
         <v>82</v>
       </c>
       <c r="N18" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O18" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2785,8 +2855,11 @@
       <c r="N19" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O19" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -2823,14 +2896,17 @@
       <c r="L20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="26" t="s">
         <v>91</v>
       </c>
       <c r="N20" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O20" s="9" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -2867,14 +2943,17 @@
       <c r="L21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="26" t="s">
         <v>95</v>
       </c>
       <c r="N21" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O21" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2917,8 +2996,11 @@
       <c r="N22" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O22" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2953,14 +3035,17 @@
         <v>44</v>
       </c>
       <c r="L23" s="2"/>
-      <c r="M23" s="2" t="s">
+      <c r="M23" s="26" t="s">
         <v>102</v>
       </c>
       <c r="N23" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O23" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>202</v>
       </c>
@@ -2997,14 +3082,17 @@
       <c r="L24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="26" t="s">
         <v>109</v>
       </c>
       <c r="N24" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O24" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>202</v>
       </c>
@@ -3047,8 +3135,11 @@
       <c r="N25" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O25" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="63" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>202</v>
       </c>
@@ -3085,14 +3176,17 @@
       <c r="L26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="M26" s="26" t="s">
         <v>121</v>
       </c>
       <c r="N26" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O26" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>202</v>
       </c>
@@ -3129,14 +3223,17 @@
       <c r="L27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="26" t="s">
         <v>126</v>
       </c>
       <c r="N27" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O27" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>202</v>
       </c>
@@ -3171,14 +3268,17 @@
       <c r="L28" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="M28" s="26" t="s">
         <v>132</v>
       </c>
       <c r="N28" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O28" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="63" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>202</v>
       </c>
@@ -3215,14 +3315,17 @@
       <c r="L29" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="M29" s="26" t="s">
         <v>136</v>
       </c>
       <c r="N29" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O29" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
@@ -3265,8 +3368,11 @@
       <c r="N30" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O30" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>202</v>
       </c>
@@ -3307,8 +3413,11 @@
       <c r="N31" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="O31" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>202</v>
       </c>
@@ -3351,8 +3460,11 @@
       <c r="N32" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="O32" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>202</v>
       </c>
@@ -3395,8 +3507,11 @@
       <c r="N33" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="O33" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>202</v>
       </c>
@@ -3439,8 +3554,11 @@
       <c r="N34" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O34" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="63" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>202</v>
       </c>
@@ -3483,8 +3601,11 @@
       <c r="N35" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O35" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="63" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
@@ -3527,8 +3648,11 @@
       <c r="N36" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O36" s="9" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="63" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>202</v>
       </c>
@@ -3571,8 +3695,11 @@
       <c r="N37" s="28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="O37" s="9" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>202</v>
       </c>
@@ -3609,14 +3736,17 @@
       <c r="L38" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M38" s="26" t="s">
         <v>158</v>
       </c>
       <c r="N38" s="28" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O38" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
@@ -3659,8 +3789,11 @@
       <c r="N39" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O39" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -3703,8 +3836,11 @@
       <c r="N40" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O40" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
@@ -3747,8 +3883,11 @@
       <c r="N41" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O41" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>8</v>
       </c>
@@ -3791,8 +3930,11 @@
       <c r="N42" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O42" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
@@ -3835,8 +3977,11 @@
       <c r="N43" s="28" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="O43" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="63" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -3879,8 +4024,11 @@
       <c r="N44" s="28" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O44" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>8</v>
       </c>
@@ -3924,7 +4072,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>8</v>
       </c>
@@ -3968,7 +4116,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>202</v>
       </c>
@@ -4012,7 +4160,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="42" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>202</v>
       </c>
@@ -6125,9 +6273,28 @@
     <hyperlink ref="M94" r:id="rId29" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
     <hyperlink ref="M93" r:id="rId30" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
     <hyperlink ref="M92" r:id="rId31" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
+    <hyperlink ref="M2" r:id="rId32" xr:uid="{E005716C-C6A0-E842-8114-F84C86DBBBC0}"/>
+    <hyperlink ref="M3" r:id="rId33" xr:uid="{8B847267-BF05-0A4A-97C6-E8462D113B75}"/>
+    <hyperlink ref="M5" r:id="rId34" xr:uid="{24323725-30A2-7840-88B2-F022B3E886B0}"/>
+    <hyperlink ref="M10" r:id="rId35" xr:uid="{3C1B9EA0-FE5B-1D4A-B0F4-25BF24B17A15}"/>
+    <hyperlink ref="M11" r:id="rId36" xr:uid="{4785B206-999E-554B-8C21-B6AED74E335C}"/>
+    <hyperlink ref="M12" r:id="rId37" xr:uid="{56D61543-AF5F-CE4C-B2BE-DB92AF5FD8B2}"/>
+    <hyperlink ref="M15" r:id="rId38" xr:uid="{009FF859-EB8A-6D42-B56A-BBD3AB85EA1D}"/>
+    <hyperlink ref="M16" r:id="rId39" xr:uid="{33658D4E-C47B-5647-8324-3ECF0F8E5C7F}"/>
+    <hyperlink ref="M17" r:id="rId40" xr:uid="{8703E5F8-CFAF-3042-854B-EC5BCE22E9E0}"/>
+    <hyperlink ref="M18" r:id="rId41" xr:uid="{19705E64-A978-0741-AC73-8F0318840D26}"/>
+    <hyperlink ref="M20" r:id="rId42" xr:uid="{3B29798F-D71E-DC40-9CB1-3A78EBB19A35}"/>
+    <hyperlink ref="M21" r:id="rId43" xr:uid="{63AB1D48-C1A2-6B46-AB45-2F02E7C215FF}"/>
+    <hyperlink ref="M23" r:id="rId44" xr:uid="{A6E5EE3E-9059-0646-9DA7-80F42FF92AB8}"/>
+    <hyperlink ref="M24" r:id="rId45" xr:uid="{71BFCB2C-4C4A-894A-A7E0-CC5793D459A0}"/>
+    <hyperlink ref="M26" r:id="rId46" xr:uid="{D5C23A14-1262-0E49-8E45-238FC333699C}"/>
+    <hyperlink ref="M27" r:id="rId47" xr:uid="{48F55102-5E5E-4846-931D-3C1345E815F8}"/>
+    <hyperlink ref="M28" r:id="rId48" xr:uid="{2C36D9E7-20CC-C046-8F37-B0335663708B}"/>
+    <hyperlink ref="M29" r:id="rId49" xr:uid="{9B456C34-A90A-4841-8D07-652EB0070D93}"/>
+    <hyperlink ref="M38" r:id="rId50" xr:uid="{FFFA7E44-A4C2-0B43-B181-D3CBD3860909}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
I finished the Apply
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024827D5-7E23-0D43-8CE4-CB9A56D6C6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF5DDE-1457-ED49-B7C7-EC72550A9C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="505">
   <si>
     <t>County</t>
   </si>
@@ -1426,9 +1426,6 @@
   </si>
   <si>
     <t>Offers case magement and support services to Loudoun County residents</t>
-  </si>
-  <si>
-    <t>Online application for assessment and then contact Ziyoda Crew with additiol documents.</t>
   </si>
   <si>
     <t>Shendoah Exxon, 984, Edwards Ferry Road Northeast, Edwards Landing, Leesburg, Loudoun County, Virginia, 20176, United States</t>
@@ -2096,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O81" sqref="O81"/>
+    <sheetView tabSelected="1" topLeftCell="I74" zoomScale="59" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O94" sqref="O94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -2638,13 +2635,13 @@
         <v>407</v>
       </c>
       <c r="O10" s="31" t="s">
-        <v>461</v>
+        <v>43</v>
       </c>
       <c r="P10" s="30" t="s">
         <v>415</v>
       </c>
       <c r="Q10" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2670,7 +2667,7 @@
         <v>56</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I11" s="2">
         <v>38.917318170000001</v>
@@ -2679,7 +2676,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>16</v>
@@ -2697,7 +2694,7 @@
         <v>415</v>
       </c>
       <c r="Q11" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2766,7 +2763,7 @@
         <v>268</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>309</v>
@@ -3000,7 +2997,7 @@
         <v>43</v>
       </c>
       <c r="Q17" s="32" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3126,7 +3123,7 @@
         <v>39</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -3161,7 +3158,7 @@
         <v>373</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -3176,7 +3173,7 @@
         <v>89</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -3226,7 +3223,7 @@
         <v>89</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -3239,7 +3236,7 @@
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N22" s="28" t="s">
         <v>407</v>
@@ -3324,7 +3321,7 @@
         <v>101</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I24" s="2">
         <v>40.437306100000001</v>
@@ -3427,7 +3424,7 @@
         <v>51</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>111</v>
@@ -3483,7 +3480,7 @@
         <v>116</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>117</v>
@@ -3496,7 +3493,7 @@
         <v>118</v>
       </c>
       <c r="M27" s="26" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="N27" s="28" t="s">
         <v>180</v>
@@ -3534,7 +3531,7 @@
         <v>89</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I28" s="2">
         <v>40.40062056</v>
@@ -3611,7 +3608,7 @@
         <v>415</v>
       </c>
       <c r="Q29" s="32" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3664,7 +3661,7 @@
         <v>414</v>
       </c>
       <c r="Q30" s="32" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="84" x14ac:dyDescent="0.2">
@@ -3705,7 +3702,7 @@
         <v>97</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N31" s="28" t="s">
         <v>180</v>
@@ -3717,7 +3714,7 @@
         <v>414</v>
       </c>
       <c r="Q31" s="32" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -3740,7 +3737,7 @@
         <v>268</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>314</v>
@@ -3902,7 +3899,7 @@
         <v>300</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -4102,7 +4099,7 @@
         <v>148</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I39" s="2">
         <v>39.076819999999998</v>
@@ -4117,7 +4114,7 @@
         <v>149</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N39" s="28" t="s">
         <v>407</v>
@@ -4230,7 +4227,7 @@
         <v>414</v>
       </c>
       <c r="Q41" s="32" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4281,7 +4278,7 @@
         <v>43</v>
       </c>
       <c r="Q42" s="32" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -4307,7 +4304,7 @@
         <v>168</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I43" s="2">
         <v>39.108399900000002</v>
@@ -4566,7 +4563,7 @@
         <v>191</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I48" s="2">
         <v>0</v>
@@ -4619,7 +4616,7 @@
         <v>191</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I49" s="2">
         <v>0</v>
@@ -4654,7 +4651,7 @@
         <v>228</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
@@ -4684,7 +4681,7 @@
         <v>192</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N50" s="28" t="s">
         <v>180</v>
@@ -4819,7 +4816,7 @@
         <v>207</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I53" s="2">
         <v>40.407960000000003</v>
@@ -4869,7 +4866,7 @@
         <v>211</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I54" s="2">
         <v>40.405259100000002</v>
@@ -4972,10 +4969,10 @@
         <v>104</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>491</v>
       </c>
       <c r="I56" s="2">
         <v>0</v>
@@ -4995,6 +4992,9 @@
       <c r="N56" s="28" t="s">
         <v>180</v>
       </c>
+      <c r="O56" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="P56" s="30" t="s">
         <v>415</v>
       </c>
@@ -5039,10 +5039,13 @@
       <c r="L57" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="M57" s="4" t="s">
+      <c r="M57" s="26" t="s">
         <v>249</v>
       </c>
       <c r="N57" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="O57" s="9" t="s">
         <v>180</v>
       </c>
       <c r="P57" s="30" t="s">
@@ -5092,6 +5095,9 @@
       <c r="N58" s="28" t="s">
         <v>180</v>
       </c>
+      <c r="O58" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="P58" s="30" t="s">
         <v>415</v>
       </c>
@@ -5122,7 +5128,7 @@
         <v>215</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I59" s="2">
         <v>40.427699869999998</v>
@@ -5142,6 +5148,9 @@
       <c r="N59" s="28" t="s">
         <v>180</v>
       </c>
+      <c r="O59" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="P59" s="30" t="s">
         <v>415</v>
       </c>
@@ -5190,6 +5199,9 @@
         <v>241</v>
       </c>
       <c r="N60" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="O60" s="9" t="s">
         <v>180</v>
       </c>
       <c r="P60" s="30" t="s">
@@ -5238,6 +5250,9 @@
         <v>239</v>
       </c>
       <c r="N61" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="O61" s="9" t="s">
         <v>180</v>
       </c>
       <c r="P61" s="30" t="s">
@@ -5282,6 +5297,9 @@
       <c r="N62" s="28" t="s">
         <v>180</v>
       </c>
+      <c r="O62" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="P62" s="30" t="s">
         <v>415</v>
       </c>
@@ -5329,6 +5347,9 @@
       <c r="N63" s="28" t="s">
         <v>407</v>
       </c>
+      <c r="O63" s="9" t="s">
+        <v>407</v>
+      </c>
       <c r="P63" s="30" t="s">
         <v>415</v>
       </c>
@@ -5376,6 +5397,9 @@
       <c r="N64" s="28" t="s">
         <v>336</v>
       </c>
+      <c r="O64" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P64" s="30" t="s">
         <v>415</v>
       </c>
@@ -5423,6 +5447,9 @@
       <c r="N65" s="28" t="s">
         <v>336</v>
       </c>
+      <c r="O65" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P65" s="30" t="s">
         <v>415</v>
       </c>
@@ -5471,6 +5498,9 @@
       <c r="N66" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O66" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P66" s="30" t="s">
         <v>415</v>
       </c>
@@ -5501,7 +5531,7 @@
         <v>263</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I67" s="2">
         <v>38.875816034503501</v>
@@ -5519,6 +5549,9 @@
       <c r="N67" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O67" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P67" s="30" t="s">
         <v>415</v>
       </c>
@@ -5549,7 +5582,7 @@
         <v>263</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I68" s="2">
         <v>38.875816034503501</v>
@@ -5567,6 +5600,9 @@
       <c r="N68" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O68" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P68" s="30" t="s">
         <v>415</v>
       </c>
@@ -5597,7 +5633,7 @@
         <v>269</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I69" s="2">
         <v>38.873610192974397</v>
@@ -5615,6 +5651,9 @@
       <c r="N69" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O69" s="9" t="s">
+        <v>504</v>
+      </c>
       <c r="P69" s="30" t="s">
         <v>414</v>
       </c>
@@ -5663,6 +5702,9 @@
       <c r="N70" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O70" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P70" s="30" t="s">
         <v>415</v>
       </c>
@@ -5693,7 +5735,7 @@
         <v>289</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I71" s="2">
         <v>38.774379099999997</v>
@@ -5711,6 +5753,9 @@
       <c r="N71" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O71" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P71" s="30" t="s">
         <v>415</v>
       </c>
@@ -5760,7 +5805,7 @@
         <v>337</v>
       </c>
       <c r="O72" s="9" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="P72" s="30" t="s">
         <v>415</v>
@@ -5811,7 +5856,7 @@
         <v>337</v>
       </c>
       <c r="O73" s="9" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="P73" s="30" t="s">
         <v>415</v>
@@ -5913,7 +5958,7 @@
         <v>337</v>
       </c>
       <c r="O75" s="9" t="s">
-        <v>505</v>
+        <v>337</v>
       </c>
       <c r="P75" s="30" t="s">
         <v>415</v>
@@ -5966,7 +6011,7 @@
         <v>337</v>
       </c>
       <c r="O76" s="9" t="s">
-        <v>505</v>
+        <v>337</v>
       </c>
       <c r="P76" s="30" t="s">
         <v>415</v>
@@ -6019,7 +6064,7 @@
         <v>337</v>
       </c>
       <c r="O77" s="9" t="s">
-        <v>505</v>
+        <v>337</v>
       </c>
       <c r="P77" s="30" t="s">
         <v>415</v>
@@ -6051,7 +6096,7 @@
         <v>298</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I78" s="2">
         <v>38.8553408</v>
@@ -6069,6 +6114,9 @@
       <c r="N78" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O78" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="Q78" s="32" t="s">
         <v>427</v>
       </c>
@@ -6114,6 +6162,9 @@
       <c r="N79" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O79" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P79" s="30" t="s">
         <v>415</v>
       </c>
@@ -6160,6 +6211,9 @@
       <c r="N80" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O80" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P80" s="30" t="s">
         <v>415</v>
       </c>
@@ -6206,6 +6260,9 @@
       <c r="N81" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O81" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P81" s="30" t="s">
         <v>415</v>
       </c>
@@ -6236,7 +6293,7 @@
         <v>355</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I82" s="2">
         <v>38.869669999999999</v>
@@ -6252,6 +6309,9 @@
         <v>356</v>
       </c>
       <c r="N82" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="O82" s="9" t="s">
         <v>337</v>
       </c>
       <c r="P82" s="30" t="s">
@@ -6296,6 +6356,9 @@
       <c r="N83" s="28" t="s">
         <v>337</v>
       </c>
+      <c r="O83" s="9" t="s">
+        <v>337</v>
+      </c>
       <c r="P83" s="30" t="s">
         <v>415</v>
       </c>
@@ -6339,9 +6402,12 @@
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="N84" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="O84" s="9" t="s">
         <v>407</v>
       </c>
       <c r="P84" s="30" t="s">
@@ -6380,7 +6446,7 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
@@ -6389,6 +6455,9 @@
       <c r="N85" s="29" t="s">
         <v>407</v>
       </c>
+      <c r="O85" s="9" t="s">
+        <v>407</v>
+      </c>
       <c r="P85" s="30" t="s">
         <v>415</v>
       </c>
@@ -6419,7 +6488,7 @@
         <v>366</v>
       </c>
       <c r="H86" s="22" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I86" s="2">
         <v>0</v>
@@ -6437,11 +6506,14 @@
       <c r="N86" s="29" t="s">
         <v>407</v>
       </c>
+      <c r="O86" s="9" t="s">
+        <v>407</v>
+      </c>
       <c r="P86" s="30" t="s">
         <v>415</v>
       </c>
       <c r="Q86" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6485,6 +6557,9 @@
       <c r="N87" s="29" t="s">
         <v>407</v>
       </c>
+      <c r="O87" s="9" t="s">
+        <v>407</v>
+      </c>
       <c r="P87" s="30" t="s">
         <v>415</v>
       </c>
@@ -6530,6 +6605,9 @@
       <c r="N88" s="29" t="s">
         <v>336</v>
       </c>
+      <c r="O88" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P88" s="30" t="s">
         <v>415</v>
       </c>
@@ -6542,7 +6620,7 @@
         <v>329</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>4</v>
@@ -6570,10 +6648,13 @@
       </c>
       <c r="L89" s="2"/>
       <c r="M89" s="25" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="N89" s="29" t="s">
         <v>336</v>
+      </c>
+      <c r="O89" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="P89" s="30" t="s">
         <v>415</v>
@@ -6623,6 +6704,9 @@
       <c r="N90" s="29" t="s">
         <v>336</v>
       </c>
+      <c r="O90" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P90" s="30" t="s">
         <v>415</v>
       </c>
@@ -6671,6 +6755,9 @@
       <c r="N91" s="29" t="s">
         <v>336</v>
       </c>
+      <c r="O91" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P91" s="30" t="s">
         <v>415</v>
       </c>
@@ -6719,11 +6806,14 @@
       <c r="N92" s="29" t="s">
         <v>336</v>
       </c>
+      <c r="O92" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P92" s="30" t="s">
         <v>415</v>
       </c>
       <c r="Q92" s="32" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6767,11 +6857,14 @@
       <c r="N93" s="29" t="s">
         <v>336</v>
       </c>
+      <c r="O93" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P93" s="30" t="s">
         <v>415</v>
       </c>
       <c r="Q93" s="32" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6815,6 +6908,9 @@
       <c r="N94" s="29" t="s">
         <v>336</v>
       </c>
+      <c r="O94" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P94" s="30" t="s">
         <v>415</v>
       </c>
@@ -6845,7 +6941,7 @@
         <v>366</v>
       </c>
       <c r="H95" s="22" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I95" s="2">
         <v>0</v>
@@ -6857,11 +6953,17 @@
         <v>43</v>
       </c>
       <c r="L95" s="2"/>
-      <c r="M95" s="2" t="s">
+      <c r="M95" s="26" t="s">
         <v>367</v>
       </c>
       <c r="N95" s="29" t="s">
         <v>336</v>
+      </c>
+      <c r="O95" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="P95" s="30" t="s">
+        <v>415</v>
       </c>
       <c r="Q95" s="32" t="s">
         <v>420</v>
@@ -6925,9 +7027,11 @@
     <hyperlink ref="M32" r:id="rId54" xr:uid="{B6BCA1D7-7506-4CE1-9D15-8D927D6913EA}"/>
     <hyperlink ref="M56" r:id="rId55" xr:uid="{EDFE2AA0-FB0F-7D4A-B94C-3655942F41D3}"/>
     <hyperlink ref="M69" r:id="rId56" xr:uid="{08DD2E30-6D9F-E448-B23B-C201DE5632C2}"/>
+    <hyperlink ref="M57" r:id="rId57" xr:uid="{ED202AB3-1CAE-7A40-8605-6C07A07B887B}"/>
+    <hyperlink ref="M95" r:id="rId58" xr:uid="{C30B469B-CEFC-2C48-818B-E30D93C9DA2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId57"/>
+  <pageSetup orientation="portrait" r:id="rId59"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
filled in some missing information
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF5DDE-1457-ED49-B7C7-EC72550A9C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E43439B-C4A1-4F45-AE4D-881A669ECBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="508">
   <si>
     <t>County</t>
   </si>
@@ -1416,9 +1416,6 @@
     <t>Wytestone Plaza, South 8th Street, Shockoe Slip, Richmond, Virginia, 23298, United States</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>Dold L. Bisdorf Building (AA), Netherton Drive, John Adams, Washington Forest, Alexandria, Virginia, 22311, United States</t>
   </si>
   <si>
@@ -1558,6 +1555,18 @@
   </si>
   <si>
     <t>Online, Fairfax</t>
+  </si>
+  <si>
+    <t>Loudoun County Department of Family Services</t>
+  </si>
+  <si>
+    <t>https://www.loudoun.gov/1816/Housing-Choice-Voucher-Program</t>
+  </si>
+  <si>
+    <t>Virginia Community Colleges</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1767,9 +1776,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2093,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I74" zoomScale="59" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O94" sqref="O94"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -2114,7 +2120,7 @@
     <col min="14" max="14" width="32.1640625" customWidth="1"/>
     <col min="15" max="15" width="56.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.1640625" customWidth="1"/>
-    <col min="17" max="17" width="78.5" style="32" customWidth="1"/>
+    <col min="17" max="17" width="78.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.2">
@@ -2166,11 +2172,11 @@
       <c r="P1" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="Q1" s="32" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q1" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2219,8 +2225,8 @@
       <c r="P2" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q2" s="32" t="s">
-        <v>458</v>
+      <c r="Q2" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2246,7 +2252,7 @@
         <v>304</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I3" s="2">
         <v>37.538339999999998</v>
@@ -2272,7 +2278,7 @@
       <c r="P3" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="32" t="s">
+      <c r="Q3" s="2" t="s">
         <v>456</v>
       </c>
     </row>
@@ -2325,11 +2331,11 @@
       <c r="P4" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q4" s="32" t="s">
+      <c r="Q4" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2378,7 +2384,7 @@
       <c r="P5" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="2" t="s">
         <v>454</v>
       </c>
     </row>
@@ -2431,7 +2437,7 @@
       <c r="P6" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="2" t="s">
         <v>455</v>
       </c>
     </row>
@@ -2484,7 +2490,7 @@
       <c r="P7" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q7" s="32" t="s">
+      <c r="Q7" s="2" t="s">
         <v>454</v>
       </c>
     </row>
@@ -2538,7 +2544,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I9" s="2">
         <v>39.114306589999998</v>
@@ -2587,7 +2593,7 @@
       <c r="P9" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q9" s="32" t="s">
+      <c r="Q9" s="2" t="s">
         <v>454</v>
       </c>
     </row>
@@ -2640,8 +2646,8 @@
       <c r="P10" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q10" s="32" t="s">
-        <v>461</v>
+      <c r="Q10" s="2" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2667,7 +2673,7 @@
         <v>56</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I11" s="2">
         <v>38.917318170000001</v>
@@ -2676,7 +2682,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>16</v>
@@ -2693,8 +2699,8 @@
       <c r="P11" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q11" s="32" t="s">
-        <v>461</v>
+      <c r="Q11" s="2" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2731,15 +2737,22 @@
       <c r="K12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="L12" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>505</v>
+      </c>
       <c r="N12" s="28" t="s">
         <v>407</v>
       </c>
       <c r="O12" s="28" t="s">
         <v>407</v>
       </c>
-      <c r="Q12" s="32" t="s">
+      <c r="P12" s="30" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>453</v>
       </c>
     </row>
@@ -2763,7 +2776,7 @@
         <v>268</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>309</v>
@@ -2777,7 +2790,9 @@
       <c r="K13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>504</v>
+      </c>
       <c r="M13" s="26" t="s">
         <v>416</v>
       </c>
@@ -2890,7 +2905,7 @@
       <c r="P15" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q15" s="32" t="s">
+      <c r="Q15" s="2" t="s">
         <v>452</v>
       </c>
     </row>
@@ -2943,11 +2958,11 @@
       <c r="P16" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q16" s="32" t="s">
+      <c r="Q16" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2996,8 +3011,8 @@
       <c r="P17" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q17" s="32" t="s">
-        <v>465</v>
+      <c r="Q17" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3123,7 +3138,7 @@
         <v>39</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -3158,7 +3173,7 @@
         <v>373</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -3173,7 +3188,7 @@
         <v>89</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -3223,7 +3238,7 @@
         <v>89</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -3234,9 +3249,11 @@
       <c r="K22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L22" s="2"/>
+      <c r="L22" s="2" t="s">
+        <v>506</v>
+      </c>
       <c r="M22" s="26" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N22" s="28" t="s">
         <v>407</v>
@@ -3298,7 +3315,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>180</v>
       </c>
@@ -3321,7 +3338,7 @@
         <v>101</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I24" s="2">
         <v>40.437306100000001</v>
@@ -3347,7 +3364,7 @@
       <c r="P24" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q24" s="32" t="s">
+      <c r="Q24" s="2" t="s">
         <v>448</v>
       </c>
     </row>
@@ -3400,7 +3417,7 @@
       <c r="P25" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q25" s="32" t="s">
+      <c r="Q25" s="2" t="s">
         <v>447</v>
       </c>
     </row>
@@ -3424,7 +3441,7 @@
         <v>51</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>111</v>
@@ -3453,7 +3470,7 @@
       <c r="P26" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q26" s="32" t="s">
+      <c r="Q26" s="2" t="s">
         <v>450</v>
       </c>
     </row>
@@ -3480,7 +3497,7 @@
         <v>116</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>117</v>
@@ -3493,7 +3510,7 @@
         <v>118</v>
       </c>
       <c r="M27" s="26" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N27" s="28" t="s">
         <v>180</v>
@@ -3504,7 +3521,7 @@
       <c r="P27" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q27" s="32" t="s">
+      <c r="Q27" s="2" t="s">
         <v>449</v>
       </c>
     </row>
@@ -3531,7 +3548,7 @@
         <v>89</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I28" s="2">
         <v>40.40062056</v>
@@ -3607,8 +3624,8 @@
       <c r="P29" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q29" s="32" t="s">
-        <v>476</v>
+      <c r="Q29" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3660,8 +3677,8 @@
       <c r="P30" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q30" s="32" t="s">
-        <v>476</v>
+      <c r="Q30" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="84" x14ac:dyDescent="0.2">
@@ -3702,7 +3719,7 @@
         <v>97</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N31" s="28" t="s">
         <v>180</v>
@@ -3713,8 +3730,8 @@
       <c r="P31" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q31" s="32" t="s">
-        <v>476</v>
+      <c r="Q31" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -3737,7 +3754,7 @@
         <v>268</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>314</v>
@@ -3766,7 +3783,7 @@
       <c r="P32" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q32" s="32" t="s">
+      <c r="Q32" s="2" t="s">
         <v>448</v>
       </c>
     </row>
@@ -3819,7 +3836,7 @@
       <c r="P33" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q33" s="32" t="s">
+      <c r="Q33" s="2" t="s">
         <v>447</v>
       </c>
     </row>
@@ -3872,7 +3889,7 @@
       <c r="P34" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q34" s="32" t="s">
+      <c r="Q34" s="2" t="s">
         <v>447</v>
       </c>
     </row>
@@ -3899,7 +3916,7 @@
         <v>300</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -4099,7 +4116,7 @@
         <v>148</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I39" s="2">
         <v>39.076819999999998</v>
@@ -4114,7 +4131,7 @@
         <v>149</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N39" s="28" t="s">
         <v>407</v>
@@ -4126,7 +4143,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -4175,11 +4192,11 @@
       <c r="P40" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q40" s="32" t="s">
+      <c r="Q40" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
@@ -4226,8 +4243,8 @@
       <c r="P41" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q41" s="32" t="s">
-        <v>465</v>
+      <c r="Q41" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4277,8 +4294,8 @@
       <c r="P42" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q42" s="32" t="s">
-        <v>482</v>
+      <c r="Q42" s="2" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -4304,7 +4321,7 @@
         <v>168</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I43" s="2">
         <v>39.108399900000002</v>
@@ -4331,7 +4348,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -4380,7 +4397,7 @@
       <c r="P44" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q44" s="32" t="s">
+      <c r="Q44" s="2" t="s">
         <v>445</v>
       </c>
     </row>
@@ -4433,7 +4450,7 @@
       <c r="P45" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q45" s="32" t="s">
+      <c r="Q45" s="2" t="s">
         <v>444</v>
       </c>
     </row>
@@ -4486,7 +4503,7 @@
       <c r="P46" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q46" s="32" t="s">
+      <c r="Q46" s="2" t="s">
         <v>443</v>
       </c>
     </row>
@@ -4563,7 +4580,7 @@
         <v>191</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I48" s="2">
         <v>0</v>
@@ -4589,7 +4606,7 @@
       <c r="P48" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q48" s="32" t="s">
+      <c r="Q48" s="2" t="s">
         <v>442</v>
       </c>
     </row>
@@ -4616,7 +4633,7 @@
         <v>191</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I49" s="2">
         <v>0</v>
@@ -4651,7 +4668,7 @@
         <v>228</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
@@ -4681,7 +4698,7 @@
         <v>192</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N50" s="28" t="s">
         <v>180</v>
@@ -4816,7 +4833,7 @@
         <v>207</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I53" s="2">
         <v>40.407960000000003</v>
@@ -4866,7 +4883,7 @@
         <v>211</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I54" s="2">
         <v>40.405259100000002</v>
@@ -4892,7 +4909,7 @@
       <c r="P54" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q54" s="32" t="s">
+      <c r="Q54" s="2" t="s">
         <v>441</v>
       </c>
     </row>
@@ -4945,11 +4962,11 @@
       <c r="P55" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q55" s="32" t="s">
+      <c r="Q55" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>180</v>
       </c>
@@ -4969,10 +4986,10 @@
         <v>104</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>489</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>490</v>
       </c>
       <c r="I56" s="2">
         <v>0</v>
@@ -4998,7 +5015,7 @@
       <c r="P56" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q56" s="32" t="s">
+      <c r="Q56" s="2" t="s">
         <v>439</v>
       </c>
     </row>
@@ -5101,7 +5118,7 @@
       <c r="P58" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q58" s="32" t="s">
+      <c r="Q58" s="2" t="s">
         <v>438</v>
       </c>
     </row>
@@ -5128,7 +5145,7 @@
         <v>215</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I59" s="2">
         <v>40.427699869999998</v>
@@ -5154,7 +5171,7 @@
       <c r="P59" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q59" s="32" t="s">
+      <c r="Q59" s="2" t="s">
         <v>438</v>
       </c>
     </row>
@@ -5207,11 +5224,11 @@
       <c r="P60" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q60" s="32" t="s">
+      <c r="Q60" s="2" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>180</v>
       </c>
@@ -5258,7 +5275,7 @@
       <c r="P61" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q61" s="32" t="s">
+      <c r="Q61" s="2" t="s">
         <v>438</v>
       </c>
     </row>
@@ -5404,7 +5421,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>8</v>
       </c>
@@ -5453,7 +5470,7 @@
       <c r="P65" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q65" s="32" t="s">
+      <c r="Q65" s="2" t="s">
         <v>437</v>
       </c>
     </row>
@@ -5504,7 +5521,7 @@
       <c r="P66" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q66" s="32" t="s">
+      <c r="Q66" s="2" t="s">
         <v>436</v>
       </c>
     </row>
@@ -5531,7 +5548,7 @@
         <v>263</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I67" s="2">
         <v>38.875816034503501</v>
@@ -5555,7 +5572,7 @@
       <c r="P67" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q67" s="32" t="s">
+      <c r="Q67" s="2" t="s">
         <v>435</v>
       </c>
     </row>
@@ -5582,7 +5599,7 @@
         <v>263</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I68" s="2">
         <v>38.875816034503501</v>
@@ -5606,7 +5623,7 @@
       <c r="P68" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q68" s="32" t="s">
+      <c r="Q68" s="2" t="s">
         <v>434</v>
       </c>
     </row>
@@ -5633,7 +5650,7 @@
         <v>269</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I69" s="2">
         <v>38.873610192974397</v>
@@ -5652,12 +5669,12 @@
         <v>337</v>
       </c>
       <c r="O69" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="P69" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="Q69" s="32" t="s">
+      <c r="Q69" s="2" t="s">
         <v>434</v>
       </c>
     </row>
@@ -5708,7 +5725,7 @@
       <c r="P70" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q70" s="32" t="s">
+      <c r="Q70" s="2" t="s">
         <v>433</v>
       </c>
     </row>
@@ -5735,7 +5752,7 @@
         <v>289</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I71" s="2">
         <v>38.774379099999997</v>
@@ -5759,7 +5776,7 @@
       <c r="P71" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q71" s="32" t="s">
+      <c r="Q71" s="2" t="s">
         <v>432</v>
       </c>
     </row>
@@ -5810,11 +5827,11 @@
       <c r="P72" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q72" s="32" t="s">
+      <c r="Q72" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>283</v>
       </c>
@@ -5861,7 +5878,7 @@
       <c r="P73" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q73" s="32" t="s">
+      <c r="Q73" s="2" t="s">
         <v>430</v>
       </c>
     </row>
@@ -5912,7 +5929,7 @@
       <c r="P74" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q74" s="32" t="s">
+      <c r="Q74" s="2" t="s">
         <v>430</v>
       </c>
     </row>
@@ -5963,7 +5980,7 @@
       <c r="P75" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q75" s="32" t="s">
+      <c r="Q75" s="2" t="s">
         <v>429</v>
       </c>
     </row>
@@ -6016,7 +6033,7 @@
       <c r="P76" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q76" s="32" t="s">
+      <c r="Q76" s="2" t="s">
         <v>428</v>
       </c>
     </row>
@@ -6069,7 +6086,7 @@
       <c r="P77" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q77" s="32" t="s">
+      <c r="Q77" s="2" t="s">
         <v>427</v>
       </c>
     </row>
@@ -6096,7 +6113,7 @@
         <v>298</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I78" s="2">
         <v>38.8553408</v>
@@ -6117,11 +6134,11 @@
       <c r="O78" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="Q78" s="32" t="s">
+      <c r="Q78" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>283</v>
       </c>
@@ -6168,7 +6185,7 @@
       <c r="P79" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q79" s="32" t="s">
+      <c r="Q79" s="2" t="s">
         <v>427</v>
       </c>
     </row>
@@ -6217,7 +6234,7 @@
       <c r="P80" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q80" s="32" t="s">
+      <c r="Q80" s="2" t="s">
         <v>426</v>
       </c>
     </row>
@@ -6266,7 +6283,7 @@
       <c r="P81" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q81" s="32" t="s">
+      <c r="Q81" s="2" t="s">
         <v>425</v>
       </c>
     </row>
@@ -6293,7 +6310,7 @@
         <v>355</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I82" s="2">
         <v>38.869669999999999</v>
@@ -6317,11 +6334,11 @@
       <c r="P82" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q82" s="32" t="s">
+      <c r="Q82" s="2" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>357</v>
       </c>
@@ -6362,7 +6379,7 @@
       <c r="P83" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q83" s="32" t="s">
+      <c r="Q83" s="2" t="s">
         <v>423</v>
       </c>
     </row>
@@ -6402,7 +6419,7 @@
       </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="N84" s="29" t="s">
         <v>407</v>
@@ -6446,7 +6463,7 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2" t="s">
@@ -6461,7 +6478,7 @@
       <c r="P85" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q85" s="32" t="s">
+      <c r="Q85" s="2" t="s">
         <v>422</v>
       </c>
     </row>
@@ -6488,7 +6505,7 @@
         <v>366</v>
       </c>
       <c r="H86" s="22" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I86" s="2">
         <v>0</v>
@@ -6512,8 +6529,8 @@
       <c r="P86" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q86" s="32" t="s">
-        <v>501</v>
+      <c r="Q86" s="2" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6620,7 +6637,7 @@
         <v>329</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>4</v>
@@ -6648,7 +6665,7 @@
       </c>
       <c r="L89" s="2"/>
       <c r="M89" s="25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N89" s="29" t="s">
         <v>336</v>
@@ -6659,7 +6676,7 @@
       <c r="P89" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q89" s="32" t="s">
+      <c r="Q89" s="2" t="s">
         <v>421</v>
       </c>
     </row>
@@ -6710,7 +6727,7 @@
       <c r="P90" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q90" s="32" t="s">
+      <c r="Q90" s="2" t="s">
         <v>421</v>
       </c>
     </row>
@@ -6761,11 +6778,11 @@
       <c r="P91" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q91" s="32" t="s">
+      <c r="Q91" s="2" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
@@ -6812,11 +6829,11 @@
       <c r="P92" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q92" s="32" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+      <c r="Q92" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>8</v>
       </c>
@@ -6863,8 +6880,8 @@
       <c r="P93" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q93" s="32" t="s">
-        <v>465</v>
+      <c r="Q93" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6914,7 +6931,7 @@
       <c r="P94" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q94" s="32" t="s">
+      <c r="Q94" s="2" t="s">
         <v>420</v>
       </c>
     </row>
@@ -6941,7 +6958,7 @@
         <v>366</v>
       </c>
       <c r="H95" s="22" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I95" s="2">
         <v>0</v>
@@ -6965,7 +6982,7 @@
       <c r="P95" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="Q95" s="32" t="s">
+      <c r="Q95" s="2" t="s">
         <v>420</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished filling in the blanks. it was a few websites that do not work.
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E43439B-C4A1-4F45-AE4D-881A669ECBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98464B3D-CFDB-D044-8578-8EA558100C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="-1940" yWindow="2540" windowWidth="28800" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="519">
   <si>
     <t>County</t>
   </si>
@@ -757,13 +757,7 @@
     <t>PortAuthority.org</t>
   </si>
   <si>
-    <t>Public transit agency in Alleghany Count</t>
-  </si>
-  <si>
     <t>https://www.ccac.edu/academics/apprenticeship.php</t>
-  </si>
-  <si>
-    <t> Community College of Allegheny County.</t>
   </si>
   <si>
     <t xml:space="preserve">Education </t>
@@ -1125,9 +1119,6 @@
     <t>Serving NW FFX County</t>
   </si>
   <si>
-    <t>http://www.jsfreeclinic.org/</t>
-  </si>
-  <si>
     <t>Mission Life Center Hope Clinic</t>
   </si>
   <si>
@@ -1296,9 +1287,6 @@
     <t>https://www.loudoun.gov/1813/Affordable-Dwelling-Unit-Program</t>
   </si>
   <si>
-    <t>Loudoun County Human and Health Services</t>
-  </si>
-  <si>
     <t xml:space="preserve">Allows eligible youth to apply for apartments in Allegheny. </t>
   </si>
   <si>
@@ -1536,9 +1524,6 @@
     <t>Non-profit Medi-Cal maged care organization, providing business administrative support for community health centers to focus on what matters most–patients.</t>
   </si>
   <si>
-    <t>https://seniorvigator.org/program/47239/mlc-hope-clinic</t>
-  </si>
-  <si>
     <t>Andale</t>
   </si>
   <si>
@@ -1567,6 +1552,54 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Public transit agency in Alleghany County</t>
+  </si>
+  <si>
+    <t>Port Authority of Allegheny County</t>
+  </si>
+  <si>
+    <t>Pennsylvania Department of Human Services</t>
+  </si>
+  <si>
+    <t>https://www.dhs.pa.gov/HealthChoices/Pages/HealthChoices.aspx</t>
+  </si>
+  <si>
+    <t>Second Story</t>
+  </si>
+  <si>
+    <t>Choice. Respect. Independence.</t>
+  </si>
+  <si>
+    <t>Fairfax County Public Schools</t>
+  </si>
+  <si>
+    <t>Fairfax County Department of Family Services</t>
+  </si>
+  <si>
+    <t>Fairfax County Human Services Transportation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falls Church Health Care </t>
+  </si>
+  <si>
+    <t>Fairfax Health Department</t>
+  </si>
+  <si>
+    <t>Community Health Center Network</t>
+  </si>
+  <si>
+    <t>http://www.jsfreeclinic.org/ (DOES NOT WORK</t>
+  </si>
+  <si>
+    <t>https://seniorvigator.org/program/47239/mlc-hope-clinic (does not work)</t>
+  </si>
+  <si>
+    <t>Northern Virginia Dental Society</t>
+  </si>
+  <si>
+    <t>Community College of Allegheny County.</t>
   </si>
 </sst>
 </file>
@@ -2100,7 +2133,7 @@
   <dimension ref="A1:Q95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -2155,25 +2188,25 @@
         <v>230</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>232</v>
       </c>
       <c r="N1" s="28" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="P1" s="30" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2199,7 +2232,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I2" s="2">
         <v>38.840490000000003</v>
@@ -2217,16 +2250,16 @@
         <v>17</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O2" s="30" t="s">
         <v>43</v>
       </c>
       <c r="P2" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2249,10 +2282,10 @@
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I3" s="2">
         <v>37.538339999999998</v>
@@ -2270,7 +2303,7 @@
         <v>22</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O3" s="30" t="s">
         <v>43</v>
@@ -2279,7 +2312,7 @@
         <v>43</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2302,10 +2335,10 @@
         <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="I4" s="2">
         <v>37.538339999999998</v>
@@ -2323,16 +2356,16 @@
         <v>25</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O4" s="30" t="s">
         <v>43</v>
       </c>
       <c r="P4" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2376,16 +2409,16 @@
         <v>33</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O5" s="30" t="s">
         <v>43</v>
       </c>
       <c r="P5" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2429,7 +2462,7 @@
         <v>33</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O6" s="30" t="s">
         <v>43</v>
@@ -2438,7 +2471,7 @@
         <v>43</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2482,16 +2515,16 @@
         <v>33</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O7" s="30" t="s">
         <v>43</v>
       </c>
       <c r="P7" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2535,7 +2568,7 @@
         <v>33</v>
       </c>
       <c r="N8" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O8" s="30" t="s">
         <v>43</v>
@@ -2567,7 +2600,7 @@
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="I9" s="2">
         <v>39.114306589999998</v>
@@ -2585,16 +2618,16 @@
         <v>49</v>
       </c>
       <c r="N9" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O9" s="30" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P9" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.2">
@@ -2620,7 +2653,7 @@
         <v>52</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I10" s="2">
         <v>39.114306589999998</v>
@@ -2638,16 +2671,16 @@
         <v>54</v>
       </c>
       <c r="N10" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O10" s="31" t="s">
         <v>43</v>
       </c>
       <c r="P10" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2673,7 +2706,7 @@
         <v>56</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="I11" s="2">
         <v>38.917318170000001</v>
@@ -2682,7 +2715,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>16</v>
@@ -2691,16 +2724,16 @@
         <v>57</v>
       </c>
       <c r="N11" s="28" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="O11" s="28" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="P11" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2720,13 +2753,13 @@
         <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I12" s="2">
         <v>0</v>
@@ -2738,22 +2771,22 @@
         <v>43</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="N12" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O12" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P12" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2773,13 +2806,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -2791,19 +2824,19 @@
         <v>43</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="M13" s="26" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="N13" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O13" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P13" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2847,13 +2880,13 @@
         <v>63</v>
       </c>
       <c r="N14" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P14" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -2879,7 +2912,7 @@
         <v>65</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I15" s="2">
         <v>37.61065696</v>
@@ -2897,16 +2930,16 @@
         <v>67</v>
       </c>
       <c r="N15" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="P15" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -2950,16 +2983,16 @@
         <v>72</v>
       </c>
       <c r="N16" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -2967,7 +3000,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>73</v>
@@ -2985,7 +3018,7 @@
         <v>75</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -3003,7 +3036,7 @@
         <v>77</v>
       </c>
       <c r="N17" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O17" s="9" t="s">
         <v>43</v>
@@ -3012,7 +3045,7 @@
         <v>43</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3020,7 +3053,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>78</v>
@@ -3038,7 +3071,7 @@
         <v>80</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -3056,7 +3089,7 @@
         <v>81</v>
       </c>
       <c r="N18" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O18" s="9" t="s">
         <v>43</v>
@@ -3070,7 +3103,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>82</v>
@@ -3100,19 +3133,19 @@
         <v>43</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>417</v>
+        <v>153</v>
       </c>
       <c r="M19" s="26" t="s">
         <v>85</v>
       </c>
       <c r="N19" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P19" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3120,7 +3153,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>86</v>
@@ -3138,7 +3171,7 @@
         <v>39</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -3156,7 +3189,7 @@
         <v>88</v>
       </c>
       <c r="N20" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O20" s="9" t="s">
         <v>43</v>
@@ -3170,10 +3203,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -3188,7 +3221,7 @@
         <v>89</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -3206,7 +3239,7 @@
         <v>22</v>
       </c>
       <c r="N21" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O21" s="9" t="s">
         <v>43</v>
@@ -3220,7 +3253,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>90</v>
@@ -3238,7 +3271,7 @@
         <v>89</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -3250,13 +3283,13 @@
         <v>43</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="M22" s="26" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="N22" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O22" s="9" t="s">
         <v>43</v>
@@ -3312,7 +3345,7 @@
         <v>180</v>
       </c>
       <c r="P23" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3338,7 +3371,7 @@
         <v>101</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="I24" s="2">
         <v>40.437306100000001</v>
@@ -3362,10 +3395,10 @@
         <v>180</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -3415,10 +3448,10 @@
         <v>43</v>
       </c>
       <c r="P25" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3441,7 +3474,7 @@
         <v>51</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>111</v>
@@ -3468,10 +3501,10 @@
         <v>180</v>
       </c>
       <c r="P26" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3497,20 +3530,20 @@
         <v>116</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>117</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>118</v>
       </c>
       <c r="M27" s="26" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="N27" s="28" t="s">
         <v>180</v>
@@ -3519,10 +3552,10 @@
         <v>180</v>
       </c>
       <c r="P27" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -3548,7 +3581,7 @@
         <v>89</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="I28" s="2">
         <v>40.40062056</v>
@@ -3572,7 +3605,7 @@
         <v>180</v>
       </c>
       <c r="P28" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3622,10 +3655,10 @@
         <v>180</v>
       </c>
       <c r="P29" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -3651,7 +3684,7 @@
         <v>125</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="I30" s="2">
         <v>40.40062056</v>
@@ -3675,10 +3708,10 @@
         <v>180</v>
       </c>
       <c r="P30" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="84" x14ac:dyDescent="0.2">
@@ -3689,7 +3722,7 @@
         <v>229</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>4</v>
@@ -3704,7 +3737,7 @@
         <v>126</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I31" s="2">
         <v>40.439188049999998</v>
@@ -3719,7 +3752,7 @@
         <v>97</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="N31" s="28" t="s">
         <v>180</v>
@@ -3728,10 +3761,10 @@
         <v>180</v>
       </c>
       <c r="P31" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
@@ -3751,13 +3784,13 @@
         <v>27</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I32" s="2">
         <v>40.437306100000001</v>
@@ -3772,7 +3805,7 @@
         <v>97</v>
       </c>
       <c r="M32" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N32" s="28" t="s">
         <v>180</v>
@@ -3781,10 +3814,10 @@
         <v>180</v>
       </c>
       <c r="P32" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="84" x14ac:dyDescent="0.2">
@@ -3804,13 +3837,13 @@
         <v>27</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I33" s="2">
         <v>40.437306100000001</v>
@@ -3834,10 +3867,10 @@
         <v>180</v>
       </c>
       <c r="P33" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -3845,7 +3878,7 @@
         <v>180</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>130</v>
@@ -3857,13 +3890,13 @@
         <v>27</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I34" s="2">
         <v>0</v>
@@ -3890,7 +3923,7 @@
         <v>43</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -3898,7 +3931,7 @@
         <v>180</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>133</v>
@@ -3910,13 +3943,13 @@
         <v>27</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -3937,7 +3970,7 @@
         <v>180</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="P35" s="30" t="s">
         <v>43</v>
@@ -3948,7 +3981,7 @@
         <v>180</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>134</v>
@@ -3960,7 +3993,7 @@
         <v>27</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>135</v>
@@ -3987,7 +4020,7 @@
         <v>180</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="P36" s="30" t="s">
         <v>43</v>
@@ -3998,7 +4031,7 @@
         <v>180</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>137</v>
@@ -4010,10 +4043,10 @@
         <v>27</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>138</v>
@@ -4034,7 +4067,7 @@
         <v>139</v>
       </c>
       <c r="N37" s="28" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="O37" s="9" t="s">
         <v>43</v>
@@ -4066,7 +4099,7 @@
         <v>144</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -4084,13 +4117,13 @@
         <v>146</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O38" s="9" t="s">
         <v>43</v>
       </c>
       <c r="P38" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4116,7 +4149,7 @@
         <v>148</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="I39" s="2">
         <v>39.076819999999998</v>
@@ -4131,16 +4164,16 @@
         <v>149</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O39" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P39" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -4184,16 +4217,16 @@
         <v>154</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O40" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P40" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -4235,16 +4268,16 @@
         <v>159</v>
       </c>
       <c r="N41" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O41" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P41" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4286,7 +4319,7 @@
         <v>165</v>
       </c>
       <c r="N42" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O42" s="9" t="s">
         <v>43</v>
@@ -4295,7 +4328,7 @@
         <v>43</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -4321,7 +4354,7 @@
         <v>168</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="I43" s="2">
         <v>39.108399900000002</v>
@@ -4339,13 +4372,13 @@
         <v>169</v>
       </c>
       <c r="N43" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O43" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P43" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4389,16 +4422,16 @@
         <v>173</v>
       </c>
       <c r="N44" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O44" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P44" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4406,7 +4439,7 @@
         <v>8</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>175</v>
@@ -4442,16 +4475,16 @@
         <v>179</v>
       </c>
       <c r="N45" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O45" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P45" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4477,7 +4510,7 @@
         <v>182</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I46" s="2">
         <v>0</v>
@@ -4498,13 +4531,13 @@
         <v>180</v>
       </c>
       <c r="O46" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4551,10 +4584,10 @@
         <v>180</v>
       </c>
       <c r="O47" s="9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="P47" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -4580,7 +4613,7 @@
         <v>191</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="I48" s="2">
         <v>0</v>
@@ -4601,13 +4634,13 @@
         <v>180</v>
       </c>
       <c r="O48" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="P48" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="P48" s="30" t="s">
-        <v>415</v>
-      </c>
       <c r="Q48" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -4633,7 +4666,7 @@
         <v>191</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="I49" s="2">
         <v>0</v>
@@ -4654,10 +4687,10 @@
         <v>180</v>
       </c>
       <c r="O49" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="P49" s="30" t="s">
         <v>412</v>
-      </c>
-      <c r="P49" s="30" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4668,7 +4701,7 @@
         <v>228</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
@@ -4698,16 +4731,16 @@
         <v>192</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="N50" s="28" t="s">
         <v>180</v>
       </c>
       <c r="O50" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="P50" s="30" t="s">
         <v>412</v>
-      </c>
-      <c r="P50" s="30" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4754,10 +4787,10 @@
         <v>180</v>
       </c>
       <c r="O51" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="P51" s="30" t="s">
         <v>412</v>
-      </c>
-      <c r="P51" s="30" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4804,10 +4837,10 @@
         <v>180</v>
       </c>
       <c r="O52" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="P52" s="30" t="s">
         <v>412</v>
-      </c>
-      <c r="P52" s="30" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="21" x14ac:dyDescent="0.2">
@@ -4833,7 +4866,7 @@
         <v>207</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="I53" s="2">
         <v>40.407960000000003</v>
@@ -4842,7 +4875,7 @@
         <v>-79.909257999999994</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>208</v>
@@ -4883,7 +4916,7 @@
         <v>211</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="I54" s="2">
         <v>40.405259100000002</v>
@@ -4892,7 +4925,7 @@
         <v>-79.829184400000003</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>212</v>
@@ -4907,10 +4940,10 @@
         <v>43</v>
       </c>
       <c r="P54" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4945,7 +4978,7 @@
         <v>-79.958669999999998</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>217</v>
@@ -4963,7 +4996,7 @@
         <v>43</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -4971,7 +5004,7 @@
         <v>180</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>219</v>
@@ -4986,10 +5019,10 @@
         <v>104</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="I56" s="2">
         <v>0</v>
@@ -5004,7 +5037,7 @@
         <v>237</v>
       </c>
       <c r="M56" s="26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N56" s="28" t="s">
         <v>180</v>
@@ -5013,10 +5046,10 @@
         <v>43</v>
       </c>
       <c r="P56" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5024,7 +5057,7 @@
         <v>180</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>220</v>
@@ -5042,7 +5075,7 @@
         <v>215</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I57" s="2">
         <v>40.427699869999998</v>
@@ -5054,10 +5087,10 @@
         <v>96</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M57" s="26" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="N57" s="28" t="s">
         <v>180</v>
@@ -5066,7 +5099,7 @@
         <v>180</v>
       </c>
       <c r="P57" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5074,7 +5107,7 @@
         <v>180</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>221</v>
@@ -5089,10 +5122,10 @@
         <v>28</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I58" s="2">
         <v>40.427699869999998</v>
@@ -5104,10 +5137,10 @@
         <v>96</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N58" s="28" t="s">
         <v>180</v>
@@ -5116,10 +5149,10 @@
         <v>180</v>
       </c>
       <c r="P58" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5127,7 +5160,7 @@
         <v>180</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>222</v>
@@ -5145,7 +5178,7 @@
         <v>215</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="I59" s="2">
         <v>40.427699869999998</v>
@@ -5157,11 +5190,11 @@
         <v>180</v>
       </c>
       <c r="L59" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="M59" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="M59" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="N59" s="28" t="s">
         <v>180</v>
       </c>
@@ -5169,10 +5202,10 @@
         <v>180</v>
       </c>
       <c r="P59" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5180,7 +5213,7 @@
         <v>180</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>223</v>
@@ -5198,7 +5231,7 @@
         <v>215</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I60" s="2">
         <v>40.427699869999998</v>
@@ -5210,10 +5243,10 @@
         <v>180</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>242</v>
+        <v>518</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N60" s="28" t="s">
         <v>180</v>
@@ -5222,10 +5255,10 @@
         <v>180</v>
       </c>
       <c r="P60" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q60" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5251,7 +5284,7 @@
         <v>215</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>240</v>
+        <v>503</v>
       </c>
       <c r="I61" s="2">
         <v>0</v>
@@ -5262,7 +5295,9 @@
       <c r="K61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L61" s="2"/>
+      <c r="L61" s="2" t="s">
+        <v>504</v>
+      </c>
       <c r="M61" s="4" t="s">
         <v>239</v>
       </c>
@@ -5273,10 +5308,10 @@
         <v>180</v>
       </c>
       <c r="P61" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q61" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="21" x14ac:dyDescent="0.2">
@@ -5284,7 +5319,7 @@
         <v>180</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>225</v>
@@ -5299,7 +5334,7 @@
         <v>174</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>236</v>
@@ -5307,10 +5342,14 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
+        <v>331</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>506</v>
+      </c>
       <c r="N62" s="28" t="s">
         <v>180</v>
       </c>
@@ -5318,7 +5357,7 @@
         <v>180</v>
       </c>
       <c r="P62" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5329,7 +5368,7 @@
         <v>226</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>4</v>
@@ -5338,13 +5377,13 @@
         <v>27</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>234</v>
       </c>
       <c r="H63" s="23" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I63" s="2">
         <v>0</v>
@@ -5353,22 +5392,22 @@
         <v>0</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="L63" s="27" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="N63" s="28" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O63" s="9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P63" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5394,7 +5433,7 @@
         <v>234</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I64" s="2">
         <v>39.078167000000001</v>
@@ -5412,13 +5451,13 @@
         <v>235</v>
       </c>
       <c r="N64" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O64" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P64" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -5429,7 +5468,7 @@
         <v>226</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>4</v>
@@ -5444,7 +5483,7 @@
         <v>234</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I65" s="2">
         <v>39.045227799999999</v>
@@ -5456,48 +5495,48 @@
         <v>31</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N65" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O65" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P65" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="84" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I66" s="2">
         <v>38.906303508879397</v>
@@ -5506,49 +5545,51 @@
         <v>-77.222641329237604</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="M66" s="26" t="s">
+        <v>258</v>
       </c>
       <c r="N66" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O66" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P66" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q66" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="84" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="F67" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="H67" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="I67" s="2">
         <v>38.875816034503501</v>
@@ -5557,49 +5598,51 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="M67" s="26" t="s">
+        <v>263</v>
       </c>
       <c r="N67" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O67" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P67" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q67" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="84" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I68" s="2">
         <v>38.875816034503501</v>
@@ -5608,34 +5651,36 @@
         <v>-77.435718373358995</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="L68" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>508</v>
+      </c>
       <c r="M68" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N68" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O68" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P68" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>4</v>
@@ -5644,13 +5689,13 @@
         <v>27</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="I69" s="2">
         <v>38.873610192974397</v>
@@ -5659,49 +5704,51 @@
         <v>-77.3055466310296</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="L69" s="2"/>
+        <v>268</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="M69" s="26" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N69" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O69" s="9" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="P69" s="30" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q69" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>228</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>89</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I70" s="2">
         <v>38.868590773014198</v>
@@ -5710,34 +5757,36 @@
         <v>-77.224144877053305</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="L70" s="2"/>
+        <v>273</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="M70" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="N70" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O70" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P70" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="84" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>228</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>11</v>
@@ -5746,13 +5795,13 @@
         <v>27</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="I71" s="2">
         <v>38.774379099999997</v>
@@ -5763,47 +5812,49 @@
       <c r="K71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L71" s="2"/>
+      <c r="L71" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="M71" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="N71" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O71" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P71" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="H72" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I72" s="2">
         <v>38.8060490968736</v>
@@ -5812,49 +5863,51 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L72" s="2"/>
-      <c r="M72" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="M72" s="26" t="s">
+        <v>279</v>
       </c>
       <c r="N72" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O72" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P72" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q72" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="73" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I73" s="2">
         <v>38.8060490968736</v>
@@ -5863,49 +5916,51 @@
         <v>-77.181676502196197</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L73" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="M73" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="N73" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O73" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P73" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I74" s="2">
         <v>38.8553917225858</v>
@@ -5914,14 +5969,16 @@
         <v>-77.362718702194798</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="M74" s="26" t="s">
+        <v>282</v>
       </c>
       <c r="N74" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O74" s="9" t="s">
         <v>43</v>
@@ -5930,18 +5987,18 @@
         <v>43</v>
       </c>
       <c r="Q74" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="126" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>4</v>
@@ -5950,13 +6007,13 @@
         <v>27</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I75" s="2">
         <v>38.854251580169802</v>
@@ -5965,34 +6022,36 @@
         <v>-77.356579302194902</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L75" s="2"/>
-      <c r="M75" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="M75" s="26" t="s">
+        <v>285</v>
       </c>
       <c r="N75" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O75" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P75" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>4</v>
@@ -6001,13 +6060,13 @@
         <v>27</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I76" s="2">
         <v>38.8553408</v>
@@ -6016,36 +6075,36 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M76" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N76" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O76" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P76" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q76" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>4</v>
@@ -6054,13 +6113,13 @@
         <v>27</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I77" s="2">
         <v>38.8553408</v>
@@ -6069,36 +6128,36 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M77" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N77" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O77" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P77" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q77" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="78" spans="1:17" ht="63" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>4</v>
@@ -6107,13 +6166,13 @@
         <v>27</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="I78" s="2">
         <v>38.8553408</v>
@@ -6122,31 +6181,31 @@
         <v>-77.364854500000007</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M78" s="8"/>
       <c r="N78" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O78" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="Q78" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="79" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>4</v>
@@ -6155,13 +6214,13 @@
         <v>27</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="I79" s="2">
         <v>38.886493000000002</v>
@@ -6170,34 +6229,36 @@
         <v>-77.176064999999994</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2" t="s">
-        <v>349</v>
+        <v>273</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="M79" s="26" t="s">
+        <v>347</v>
       </c>
       <c r="N79" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O79" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P79" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q79" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>4</v>
@@ -6206,10 +6267,10 @@
         <v>27</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2">
@@ -6219,34 +6280,36 @@
         <v>-77.358909999999995</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2" t="s">
-        <v>351</v>
+        <v>368</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="M80" s="26" t="s">
+        <v>349</v>
       </c>
       <c r="N80" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O80" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P80" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q80" s="2" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>4</v>
@@ -6255,10 +6318,10 @@
         <v>27</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="2">
@@ -6268,34 +6331,36 @@
         <v>-77.29956</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L81" s="2"/>
-      <c r="M81" s="2" t="s">
-        <v>353</v>
+        <v>281</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="M81" s="26" t="s">
+        <v>351</v>
       </c>
       <c r="N81" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O81" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P81" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q81" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>4</v>
@@ -6304,13 +6369,13 @@
         <v>27</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="I82" s="2">
         <v>38.869669999999999</v>
@@ -6319,34 +6384,36 @@
         <v>-77.147750000000002</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2" t="s">
-        <v>356</v>
+        <v>273</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="M82" s="26" t="s">
+        <v>354</v>
       </c>
       <c r="N82" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O82" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P82" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>4</v>
@@ -6355,43 +6422,43 @@
         <v>27</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H83" s="6"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="L83" s="2"/>
-      <c r="M83" s="2" t="s">
-        <v>360</v>
+      <c r="M83" s="26" t="s">
+        <v>515</v>
       </c>
       <c r="N83" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O83" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P83" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q83" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>4</v>
@@ -6400,13 +6467,13 @@
         <v>27</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I84" s="2">
         <v>38.849589999999999</v>
@@ -6415,31 +6482,30 @@
         <v>-77.316599999999994</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2" t="s">
-        <v>497</v>
+        <v>281</v>
+      </c>
+      <c r="M84" s="26" t="s">
+        <v>516</v>
       </c>
       <c r="N84" s="29" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O84" s="9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P84" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>4</v>
@@ -6448,13 +6514,13 @@
         <v>27</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="I85" s="2">
         <v>38.831009999999999</v>
@@ -6463,34 +6529,36 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2" t="s">
-        <v>364</v>
+        <v>493</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="M85" s="26" t="s">
+        <v>361</v>
       </c>
       <c r="N85" s="29" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O85" s="9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P85" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q85" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>4</v>
@@ -6499,13 +6567,13 @@
         <v>27</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="H86" s="22" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="I86" s="2">
         <v>0</v>
@@ -6516,32 +6584,34 @@
       <c r="K86" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2" t="s">
-        <v>367</v>
+      <c r="L86" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="M86" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="N86" s="29" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O86" s="9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P86" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q86" s="2" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="42" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>4</v>
@@ -6550,13 +6620,13 @@
         <v>167</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G87" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H87" s="6" t="s">
         <v>374</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>377</v>
       </c>
       <c r="I87" s="2">
         <v>0</v>
@@ -6567,18 +6637,20 @@
       <c r="K87" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L87" s="2"/>
-      <c r="M87" s="2" t="s">
-        <v>370</v>
+      <c r="L87" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="M87" s="26" t="s">
+        <v>367</v>
       </c>
       <c r="N87" s="29" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="O87" s="9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="P87" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6586,10 +6658,10 @@
         <v>8</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>4</v>
@@ -6604,7 +6676,7 @@
         <v>148</v>
       </c>
       <c r="H88" s="23" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I88" s="2">
         <v>39.025618681403103</v>
@@ -6615,18 +6687,20 @@
       <c r="K88" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L88" s="2"/>
+      <c r="L88" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="M88" s="24" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="N88" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O88" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P88" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="89" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6634,10 +6708,10 @@
         <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>4</v>
@@ -6649,10 +6723,10 @@
         <v>51</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H89" s="23" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I89" s="2">
         <v>39.025618681403103</v>
@@ -6663,21 +6737,23 @@
       <c r="K89" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L89" s="2"/>
+      <c r="L89" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="M89" s="25" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="N89" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O89" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P89" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q89" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6688,7 +6764,7 @@
         <v>226</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>4</v>
@@ -6703,7 +6779,7 @@
         <v>148</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I90" s="2">
         <v>39.097752638349299</v>
@@ -6714,21 +6790,23 @@
       <c r="K90" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L90" s="2"/>
+      <c r="L90" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="M90" s="24" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="N90" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O90" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P90" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6736,10 +6814,10 @@
         <v>8</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>4</v>
@@ -6754,7 +6832,7 @@
         <v>148</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I91" s="2">
         <v>39.114615286054203</v>
@@ -6765,21 +6843,23 @@
       <c r="K91" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L91" s="2"/>
+      <c r="L91" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="M91" s="26" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="N91" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O91" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P91" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -6787,10 +6867,10 @@
         <v>8</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>4</v>
@@ -6805,7 +6885,7 @@
         <v>148</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I92" s="2">
         <v>39.114615286054203</v>
@@ -6816,21 +6896,23 @@
       <c r="K92" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L92" s="2"/>
+      <c r="L92" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="M92" s="25" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="N92" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O92" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P92" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q92" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="63" x14ac:dyDescent="0.2">
@@ -6841,7 +6923,7 @@
         <v>228</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>4</v>
@@ -6856,7 +6938,7 @@
         <v>148</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I93" s="2">
         <v>39.097752638349299</v>
@@ -6867,21 +6949,23 @@
       <c r="K93" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L93" s="2"/>
+      <c r="L93" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="M93" s="25" t="s">
         <v>161</v>
       </c>
       <c r="N93" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O93" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P93" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q93" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6892,7 +6976,7 @@
         <v>228</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>4</v>
@@ -6904,10 +6988,10 @@
         <v>51</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="I94" s="2">
         <v>39.097752638349299</v>
@@ -6918,21 +7002,23 @@
       <c r="K94" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L94" s="2"/>
+      <c r="L94" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="M94" s="25" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="N94" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O94" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P94" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q94" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="42" x14ac:dyDescent="0.2">
@@ -6940,10 +7026,10 @@
         <v>8</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>4</v>
@@ -6952,13 +7038,13 @@
         <v>27</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="H95" s="22" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="I95" s="2">
         <v>0</v>
@@ -6969,21 +7055,23 @@
       <c r="K95" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L95" s="2"/>
+      <c r="L95" s="2" t="s">
+        <v>517</v>
+      </c>
       <c r="M95" s="26" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="N95" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O95" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P95" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Q95" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -7046,9 +7134,23 @@
     <hyperlink ref="M69" r:id="rId56" xr:uid="{08DD2E30-6D9F-E448-B23B-C201DE5632C2}"/>
     <hyperlink ref="M57" r:id="rId57" xr:uid="{ED202AB3-1CAE-7A40-8605-6C07A07B887B}"/>
     <hyperlink ref="M95" r:id="rId58" xr:uid="{C30B469B-CEFC-2C48-818B-E30D93C9DA2C}"/>
+    <hyperlink ref="M66" r:id="rId59" xr:uid="{D47D5AEF-E1AD-DB42-9E73-177F1DFD9B5F}"/>
+    <hyperlink ref="M67" r:id="rId60" xr:uid="{74F35D5C-B8E2-7946-991F-AF0EB1C77C3A}"/>
+    <hyperlink ref="M72" r:id="rId61" xr:uid="{D234A5E8-C231-CB46-83EA-768401B84DCE}"/>
+    <hyperlink ref="M74" r:id="rId62" xr:uid="{96CB652D-CD1D-9240-9215-431BCE317721}"/>
+    <hyperlink ref="M75" r:id="rId63" xr:uid="{E05BDA41-39DE-E541-A650-FEFB2247F423}"/>
+    <hyperlink ref="M79" r:id="rId64" xr:uid="{02D418A8-483E-F34A-AABD-9BBC33136D93}"/>
+    <hyperlink ref="M80" r:id="rId65" xr:uid="{36A33342-D8A5-CD43-9CA0-0F47D53CAABD}"/>
+    <hyperlink ref="M81" r:id="rId66" xr:uid="{366630D1-2D8D-EE46-9369-BB0EAF04F2DC}"/>
+    <hyperlink ref="M82" r:id="rId67" xr:uid="{6CD8CE33-B2A3-0F43-BE9F-2712DDE7002C}"/>
+    <hyperlink ref="M83" r:id="rId68" xr:uid="{43F35154-B2E7-424D-8904-7897204C168D}"/>
+    <hyperlink ref="M84" r:id="rId69" xr:uid="{D64B06C0-9B20-7547-BE0E-F4223F14C588}"/>
+    <hyperlink ref="M85" r:id="rId70" xr:uid="{2B260585-39CA-7A45-A7F3-F2374875A6E4}"/>
+    <hyperlink ref="M86" r:id="rId71" xr:uid="{5F5D5005-9EEA-2C4C-BD43-FECDEB8C681D}"/>
+    <hyperlink ref="M87" r:id="rId72" xr:uid="{C8025F34-6251-4E48-B559-C4B3A0F3957E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId59"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
 
@@ -7068,13 +7170,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
@@ -7090,7 +7192,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B4" s="13">
         <v>3</v>
@@ -7098,7 +7200,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B7" s="15"/>
     </row>
@@ -7112,7 +7214,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B9" s="15">
         <v>11</v>
@@ -7136,7 +7238,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B12" s="15">
         <v>14</v>
@@ -7152,7 +7254,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B15" s="17"/>
     </row>
@@ -7174,7 +7276,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B18" s="17">
         <v>22</v>
@@ -7182,7 +7284,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B20" s="19">
         <v>1</v>
@@ -7190,7 +7292,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B21" s="19">
         <v>10</v>
@@ -7198,7 +7300,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B23" s="21">
         <v>1</v>
@@ -7206,7 +7308,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B24" s="21">
         <v>5</v>

</xml_diff>

<commit_message>
Changed mixed to both in combined programs
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77A94A4-F41F-CF46-927E-07207E4664C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629D9619-ACAB-417B-BC3A-39EB7F714031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1560" windowWidth="28800" windowHeight="16440" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -1278,9 +1278,6 @@
     <t xml:space="preserve">Delivery </t>
   </si>
   <si>
-    <t>Mixed</t>
-  </si>
-  <si>
     <t>In-Person</t>
   </si>
   <si>
@@ -1600,6 +1597,9 @@
   </si>
   <si>
     <t>Community College of Allegheny County.</t>
+  </si>
+  <si>
+    <t>Both</t>
   </si>
 </sst>
 </file>
@@ -2132,11 +2132,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -2156,7 +2156,7 @@
     <col min="17" max="17" width="78.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2206,10 +2206,10 @@
         <v>410</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2256,13 +2256,13 @@
         <v>43</v>
       </c>
       <c r="P2" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>302</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I3" s="2">
         <v>37.538339999999998</v>
@@ -2312,10 +2312,10 @@
         <v>43</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2362,13 +2362,13 @@
         <v>43</v>
       </c>
       <c r="P4" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2415,13 +2415,13 @@
         <v>43</v>
       </c>
       <c r="P5" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2471,10 +2471,10 @@
         <v>43</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2521,13 +2521,13 @@
         <v>43</v>
       </c>
       <c r="P7" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I9" s="2">
         <v>39.114306589999998</v>
@@ -2624,13 +2624,13 @@
         <v>404</v>
       </c>
       <c r="P9" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2677,13 +2677,13 @@
         <v>43</v>
       </c>
       <c r="P10" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>56</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I11" s="2">
         <v>38.917318170000001</v>
@@ -2715,7 +2715,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>16</v>
@@ -2730,13 +2730,13 @@
         <v>405</v>
       </c>
       <c r="P11" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2771,10 +2771,10 @@
         <v>43</v>
       </c>
       <c r="L12" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>499</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>500</v>
       </c>
       <c r="N12" s="28" t="s">
         <v>404</v>
@@ -2783,13 +2783,13 @@
         <v>404</v>
       </c>
       <c r="P12" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>266</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>307</v>
@@ -2824,10 +2824,10 @@
         <v>43</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M13" s="26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N13" s="28" t="s">
         <v>404</v>
@@ -2836,10 +2836,10 @@
         <v>404</v>
       </c>
       <c r="P13" s="30" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2886,10 +2886,10 @@
         <v>8</v>
       </c>
       <c r="P14" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2936,13 +2936,13 @@
         <v>43</v>
       </c>
       <c r="P15" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2989,13 +2989,13 @@
         <v>8</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -3045,10 +3045,10 @@
         <v>43</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -3145,10 +3145,10 @@
         <v>404</v>
       </c>
       <c r="P19" s="30" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>39</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -3198,7 +3198,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>370</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -3221,7 +3221,7 @@
         <v>89</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -3248,7 +3248,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>89</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -3283,10 +3283,10 @@
         <v>43</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="M22" s="26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="N22" s="28" t="s">
         <v>404</v>
@@ -3298,7 +3298,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>180</v>
       </c>
@@ -3345,10 +3345,10 @@
         <v>180</v>
       </c>
       <c r="P23" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>180</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>101</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I24" s="2">
         <v>40.437306100000001</v>
@@ -3395,13 +3395,13 @@
         <v>180</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>180</v>
       </c>
@@ -3448,13 +3448,13 @@
         <v>43</v>
       </c>
       <c r="P25" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>180</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>51</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>111</v>
@@ -3501,13 +3501,13 @@
         <v>180</v>
       </c>
       <c r="P26" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>180</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>116</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>117</v>
@@ -3543,7 +3543,7 @@
         <v>118</v>
       </c>
       <c r="M27" s="26" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="N27" s="28" t="s">
         <v>180</v>
@@ -3552,13 +3552,13 @@
         <v>180</v>
       </c>
       <c r="P27" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>180</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>89</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I28" s="2">
         <v>40.40062056</v>
@@ -3605,10 +3605,10 @@
         <v>180</v>
       </c>
       <c r="P28" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>180</v>
       </c>
@@ -3655,13 +3655,13 @@
         <v>180</v>
       </c>
       <c r="P29" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>180</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>125</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I30" s="2">
         <v>40.40062056</v>
@@ -3708,13 +3708,13 @@
         <v>180</v>
       </c>
       <c r="P30" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="84" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="82" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>180</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>229</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>4</v>
@@ -3752,7 +3752,7 @@
         <v>97</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N31" s="28" t="s">
         <v>180</v>
@@ -3761,13 +3761,13 @@
         <v>180</v>
       </c>
       <c r="P31" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="47.5" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>180</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>266</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>312</v>
@@ -3814,13 +3814,13 @@
         <v>180</v>
       </c>
       <c r="P32" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="84" x14ac:dyDescent="0.2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="82" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>180</v>
       </c>
@@ -3867,13 +3867,13 @@
         <v>180</v>
       </c>
       <c r="P33" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>180</v>
       </c>
@@ -3923,10 +3923,10 @@
         <v>43</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>180</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>298</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -3976,7 +3976,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>180</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="84" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="82" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>180</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>8</v>
       </c>
@@ -4123,10 +4123,10 @@
         <v>43</v>
       </c>
       <c r="P38" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>148</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I39" s="2">
         <v>39.076819999999998</v>
@@ -4164,7 +4164,7 @@
         <v>149</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="N39" s="28" t="s">
         <v>404</v>
@@ -4173,10 +4173,10 @@
         <v>8</v>
       </c>
       <c r="P39" s="30" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -4223,13 +4223,13 @@
         <v>8</v>
       </c>
       <c r="P40" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
@@ -4274,13 +4274,13 @@
         <v>8</v>
       </c>
       <c r="P41" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>8</v>
       </c>
@@ -4328,10 +4328,10 @@
         <v>43</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>168</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I43" s="2">
         <v>39.108399900000002</v>
@@ -4378,10 +4378,10 @@
         <v>8</v>
       </c>
       <c r="P43" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -4428,13 +4428,13 @@
         <v>8</v>
       </c>
       <c r="P44" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>8</v>
       </c>
@@ -4481,13 +4481,13 @@
         <v>8</v>
       </c>
       <c r="P45" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>180</v>
       </c>
@@ -4534,13 +4534,13 @@
         <v>409</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>180</v>
       </c>
@@ -4587,10 +4587,10 @@
         <v>409</v>
       </c>
       <c r="P47" s="30" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>180</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>191</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I48" s="2">
         <v>0</v>
@@ -4637,13 +4637,13 @@
         <v>409</v>
       </c>
       <c r="P48" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>180</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>191</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I49" s="2">
         <v>0</v>
@@ -4690,10 +4690,10 @@
         <v>409</v>
       </c>
       <c r="P49" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>180</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>228</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
@@ -4731,7 +4731,7 @@
         <v>192</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N50" s="28" t="s">
         <v>180</v>
@@ -4740,10 +4740,10 @@
         <v>409</v>
       </c>
       <c r="P50" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
@@ -4790,10 +4790,10 @@
         <v>409</v>
       </c>
       <c r="P51" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>180</v>
       </c>
@@ -4840,10 +4840,10 @@
         <v>409</v>
       </c>
       <c r="P52" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" ht="21" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>180</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>207</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I53" s="2">
         <v>40.407960000000003</v>
@@ -4893,7 +4893,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>180</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>211</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I54" s="2">
         <v>40.405259100000002</v>
@@ -4940,13 +4940,13 @@
         <v>43</v>
       </c>
       <c r="P54" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>180</v>
       </c>
@@ -4996,10 +4996,10 @@
         <v>43</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>180</v>
       </c>
@@ -5019,10 +5019,10 @@
         <v>104</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="I56" s="2">
         <v>0</v>
@@ -5046,13 +5046,13 @@
         <v>43</v>
       </c>
       <c r="P56" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>180</v>
       </c>
@@ -5099,10 +5099,10 @@
         <v>180</v>
       </c>
       <c r="P57" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>180</v>
       </c>
@@ -5149,13 +5149,13 @@
         <v>180</v>
       </c>
       <c r="P58" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>180</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>215</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I59" s="2">
         <v>40.427699869999998</v>
@@ -5190,7 +5190,7 @@
         <v>180</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>242</v>
@@ -5202,13 +5202,13 @@
         <v>180</v>
       </c>
       <c r="P59" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>180</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>180</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>240</v>
@@ -5255,13 +5255,13 @@
         <v>180</v>
       </c>
       <c r="P60" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q60" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>180</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>215</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I61" s="2">
         <v>0</v>
@@ -5296,7 +5296,7 @@
         <v>43</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="M61" s="4" t="s">
         <v>239</v>
@@ -5308,13 +5308,13 @@
         <v>180</v>
       </c>
       <c r="P61" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q61" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>180</v>
       </c>
@@ -5345,11 +5345,11 @@
         <v>331</v>
       </c>
       <c r="L62" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="M62" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="M62" s="2" t="s">
-        <v>506</v>
-      </c>
       <c r="N62" s="28" t="s">
         <v>180</v>
       </c>
@@ -5357,10 +5357,10 @@
         <v>180</v>
       </c>
       <c r="P62" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>8</v>
       </c>
@@ -5407,10 +5407,10 @@
         <v>404</v>
       </c>
       <c r="P63" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>8</v>
       </c>
@@ -5457,10 +5457,10 @@
         <v>8</v>
       </c>
       <c r="P64" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>8</v>
       </c>
@@ -5507,13 +5507,13 @@
         <v>8</v>
       </c>
       <c r="P65" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" ht="84" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="82" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>281</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>257</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M66" s="26" t="s">
         <v>258</v>
@@ -5560,13 +5560,13 @@
         <v>335</v>
       </c>
       <c r="P66" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q66" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" ht="84" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="82" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>281</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>261</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I67" s="2">
         <v>38.875816034503501</v>
@@ -5601,7 +5601,7 @@
         <v>262</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M67" s="26" t="s">
         <v>263</v>
@@ -5613,13 +5613,13 @@
         <v>335</v>
       </c>
       <c r="P67" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q67" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" ht="84" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="82" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>281</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>261</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I68" s="2">
         <v>38.875816034503501</v>
@@ -5654,7 +5654,7 @@
         <v>262</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M68" s="2" t="s">
         <v>263</v>
@@ -5666,13 +5666,13 @@
         <v>335</v>
       </c>
       <c r="P68" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>281</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>267</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I69" s="2">
         <v>38.873610192974397</v>
@@ -5716,16 +5716,16 @@
         <v>335</v>
       </c>
       <c r="O69" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P69" s="30" t="s">
-        <v>411</v>
+        <v>518</v>
       </c>
       <c r="Q69" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>281</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>273</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="M70" s="2" t="s">
         <v>274</v>
@@ -5772,13 +5772,13 @@
         <v>335</v>
       </c>
       <c r="P70" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" ht="84" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" ht="82" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>281</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>287</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I71" s="2">
         <v>38.774379099999997</v>
@@ -5813,7 +5813,7 @@
         <v>15</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="M71" s="8" t="s">
         <v>288</v>
@@ -5825,13 +5825,13 @@
         <v>335</v>
       </c>
       <c r="P71" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>281</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>278</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="M72" s="26" t="s">
         <v>279</v>
@@ -5878,13 +5878,13 @@
         <v>335</v>
       </c>
       <c r="P72" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q72" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>281</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>278</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="M73" s="2" t="s">
         <v>279</v>
@@ -5931,13 +5931,13 @@
         <v>335</v>
       </c>
       <c r="P73" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>281</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>281</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="M74" s="26" t="s">
         <v>282</v>
@@ -5987,10 +5987,10 @@
         <v>43</v>
       </c>
       <c r="Q74" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" ht="126" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" ht="123" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>281</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>281</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="M75" s="26" t="s">
         <v>285</v>
@@ -6037,13 +6037,13 @@
         <v>335</v>
       </c>
       <c r="P75" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>281</v>
       </c>
@@ -6090,13 +6090,13 @@
         <v>335</v>
       </c>
       <c r="P76" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q76" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>281</v>
       </c>
@@ -6143,13 +6143,13 @@
         <v>335</v>
       </c>
       <c r="P77" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q77" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>281</v>
       </c>
@@ -6172,7 +6172,7 @@
         <v>296</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I78" s="2">
         <v>38.8553408</v>
@@ -6194,10 +6194,10 @@
         <v>335</v>
       </c>
       <c r="Q78" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>281</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>273</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="M79" s="26" t="s">
         <v>347</v>
@@ -6244,13 +6244,13 @@
         <v>335</v>
       </c>
       <c r="P79" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q79" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>281</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>368</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M80" s="26" t="s">
         <v>349</v>
@@ -6295,13 +6295,13 @@
         <v>335</v>
       </c>
       <c r="P80" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q80" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>281</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>281</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M81" s="26" t="s">
         <v>351</v>
@@ -6346,13 +6346,13 @@
         <v>335</v>
       </c>
       <c r="P81" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q81" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>281</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>353</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I82" s="2">
         <v>38.869669999999999</v>
@@ -6387,7 +6387,7 @@
         <v>273</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M82" s="26" t="s">
         <v>354</v>
@@ -6399,13 +6399,13 @@
         <v>335</v>
       </c>
       <c r="P82" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>355</v>
       </c>
@@ -6435,7 +6435,7 @@
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="26" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="N83" s="28" t="s">
         <v>335</v>
@@ -6444,13 +6444,13 @@
         <v>335</v>
       </c>
       <c r="P83" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q83" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>281</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>281</v>
       </c>
       <c r="M84" s="26" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N84" s="29" t="s">
         <v>404</v>
@@ -6494,10 +6494,10 @@
         <v>404</v>
       </c>
       <c r="P84" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>281</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>360</v>
@@ -6544,13 +6544,13 @@
         <v>404</v>
       </c>
       <c r="P85" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q85" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
         <v>281</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>363</v>
       </c>
       <c r="H86" s="22" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I86" s="2">
         <v>0</v>
@@ -6585,7 +6585,7 @@
         <v>43</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M86" s="26" t="s">
         <v>364</v>
@@ -6597,13 +6597,13 @@
         <v>404</v>
       </c>
       <c r="P86" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q86" s="2" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
         <v>281</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>43</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M87" s="26" t="s">
         <v>367</v>
@@ -6650,10 +6650,10 @@
         <v>404</v>
       </c>
       <c r="P87" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
         <v>8</v>
       </c>
@@ -6700,10 +6700,10 @@
         <v>8</v>
       </c>
       <c r="P88" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>327</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>4</v>
@@ -6741,7 +6741,7 @@
         <v>153</v>
       </c>
       <c r="M89" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="N89" s="29" t="s">
         <v>334</v>
@@ -6750,13 +6750,13 @@
         <v>8</v>
       </c>
       <c r="P89" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q89" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
         <v>8</v>
       </c>
@@ -6803,13 +6803,13 @@
         <v>8</v>
       </c>
       <c r="P90" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -6856,13 +6856,13 @@
         <v>8</v>
       </c>
       <c r="P91" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
@@ -6909,13 +6909,13 @@
         <v>8</v>
       </c>
       <c r="P92" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q92" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" ht="63" x14ac:dyDescent="0.2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>8</v>
       </c>
@@ -6962,13 +6962,13 @@
         <v>8</v>
       </c>
       <c r="P93" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q93" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
         <v>8</v>
       </c>
@@ -7015,13 +7015,13 @@
         <v>8</v>
       </c>
       <c r="P94" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q94" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" ht="42" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" ht="41" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
         <v>8</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>363</v>
       </c>
       <c r="H95" s="22" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I95" s="2">
         <v>0</v>
@@ -7056,7 +7056,7 @@
         <v>43</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M95" s="26" t="s">
         <v>364</v>
@@ -7068,10 +7068,10 @@
         <v>8</v>
       </c>
       <c r="P95" s="30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q95" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -7162,19 +7162,19 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>333</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>334</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>180</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>335</v>
       </c>
@@ -7198,13 +7198,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>336</v>
       </c>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>337</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>226</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>238</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>327</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>227</v>
       </c>
@@ -7252,13 +7252,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>338</v>
       </c>
       <c r="B15" s="17"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>11</v>
       </c>
@@ -7266,7 +7266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>140</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>339</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>340</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>341</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>342</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>343</v>
       </c>

</xml_diff>

<commit_message>
Changed delivery both to hybrid
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629D9619-ACAB-417B-BC3A-39EB7F714031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE77BC57-273A-4207-B21E-1098551AB45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -1599,7 +1599,7 @@
     <t>Community College of Allegheny County.</t>
   </si>
   <si>
-    <t>Both</t>
+    <t>Hybrid</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2133,7 @@
   <dimension ref="A1:Q95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
fix some of the trees
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F003F6-99D1-9042-AF93-E9C1DDA1BF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3102C57-6EBE-5742-BBD1-75888A758893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -2179,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
@@ -2423,7 +2423,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -2432,28 +2432,28 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>253</v>
+        <v>480</v>
       </c>
       <c r="I5" s="2">
-        <v>38.840490000000003</v>
+        <v>37.538339999999998</v>
       </c>
       <c r="J5" s="2">
-        <v>-77.115129999999994</v>
+        <v>-77.437179999999998</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>15</v>
+        <v>481</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N5" s="26" t="s">
         <v>345</v>
@@ -2462,10 +2462,10 @@
         <v>38</v>
       </c>
       <c r="P5" s="28" t="s">
-        <v>429</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="43">
@@ -2476,7 +2476,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>432</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -2485,28 +2485,28 @@
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>480</v>
+        <v>253</v>
       </c>
       <c r="I6" s="2">
-        <v>37.538339999999998</v>
+        <v>38.840490000000003</v>
       </c>
       <c r="J6" s="2">
-        <v>-77.437179999999998</v>
+        <v>-77.115129999999994</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>481</v>
+        <v>15</v>
       </c>
       <c r="M6" s="33" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N6" s="26" t="s">
         <v>345</v>
@@ -2515,10 +2515,10 @@
         <v>38</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>38</v>
+        <v>429</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="44">
@@ -3969,7 +3969,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="64">
+    <row r="35" spans="1:17" ht="42">
       <c r="A35" s="2" t="s">
         <v>143</v>
       </c>
@@ -3977,49 +3977,46 @@
         <v>188</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>79</v>
+        <v>165</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="I35" s="2">
-        <v>40.349269890000002</v>
+        <v>0</v>
       </c>
       <c r="J35" s="2">
-        <v>-79.832162819999994</v>
+        <v>0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M35" s="33" t="s">
-        <v>85</v>
+        <v>154</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="N35" s="26" t="s">
         <v>143</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>38</v>
+        <v>350</v>
       </c>
       <c r="P35" s="28" t="s">
         <v>352</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="43">
@@ -4126,7 +4123,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="64">
+    <row r="38" spans="1:17" ht="42">
       <c r="A38" s="2" t="s">
         <v>143</v>
       </c>
@@ -4134,22 +4131,22 @@
         <v>186</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>493</v>
+        <v>96</v>
       </c>
       <c r="I38" s="2">
         <v>40.40062056</v>
@@ -4163,7 +4160,7 @@
       <c r="L38" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M38" s="33" t="s">
+      <c r="M38" s="2" t="s">
         <v>94</v>
       </c>
       <c r="N38" s="26" t="s">
@@ -4175,8 +4172,11 @@
       <c r="P38" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" ht="42">
+      <c r="Q38" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="64">
       <c r="A39" s="2" t="s">
         <v>143</v>
       </c>
@@ -4184,22 +4184,22 @@
         <v>186</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>96</v>
+        <v>493</v>
       </c>
       <c r="I39" s="2">
         <v>40.40062056</v>
@@ -4213,7 +4213,7 @@
       <c r="L39" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="M39" s="33" t="s">
         <v>94</v>
       </c>
       <c r="N39" s="26" t="s">
@@ -4224,9 +4224,6 @@
       </c>
       <c r="P39" s="28" t="s">
         <v>352</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="44">
@@ -5262,7 +5259,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="63">
+    <row r="60" spans="1:17" ht="42">
       <c r="A60" s="2" t="s">
         <v>143</v>
       </c>
@@ -5270,22 +5267,22 @@
         <v>188</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>474</v>
+        <v>162</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>500</v>
+        <v>163</v>
       </c>
       <c r="I60" s="2">
         <v>0</v>
@@ -5300,7 +5297,7 @@
         <v>154</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="N60" s="26" t="s">
         <v>143</v>
@@ -5311,11 +5308,8 @@
       <c r="P60" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q60" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" ht="63">
+    </row>
+    <row r="61" spans="1:17" ht="64">
       <c r="A61" s="2" t="s">
         <v>143</v>
       </c>
@@ -5323,49 +5317,52 @@
         <v>188</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>156</v>
+        <v>79</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>474</v>
+        <v>81</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>501</v>
+        <v>82</v>
       </c>
       <c r="I61" s="2">
-        <v>0</v>
+        <v>40.349269890000002</v>
       </c>
       <c r="J61" s="2">
-        <v>0</v>
+        <v>-79.832162819999994</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M61" s="4" t="s">
-        <v>157</v>
+        <v>84</v>
+      </c>
+      <c r="M61" s="33" t="s">
+        <v>85</v>
       </c>
       <c r="N61" s="26" t="s">
         <v>143</v>
       </c>
       <c r="O61" s="8" t="s">
-        <v>350</v>
+        <v>38</v>
       </c>
       <c r="P61" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" ht="42">
+      <c r="Q61" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="63">
       <c r="A62" s="2" t="s">
         <v>143</v>
       </c>
@@ -5373,22 +5370,22 @@
         <v>188</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>502</v>
+        <v>153</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>159</v>
+        <v>474</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>160</v>
+        <v>500</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -5403,7 +5400,7 @@
         <v>154</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>502</v>
+        <v>155</v>
       </c>
       <c r="N62" s="26" t="s">
         <v>143</v>
@@ -5414,8 +5411,11 @@
       <c r="P62" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" ht="42">
+      <c r="Q62" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="63">
       <c r="A63" s="2" t="s">
         <v>143</v>
       </c>
@@ -5423,22 +5423,22 @@
         <v>188</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>132</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>162</v>
+        <v>474</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>163</v>
+        <v>501</v>
       </c>
       <c r="I63" s="2">
         <v>0</v>
@@ -5453,7 +5453,7 @@
         <v>154</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="N63" s="26" t="s">
         <v>143</v>
@@ -5473,7 +5473,7 @@
         <v>188</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>165</v>
+        <v>502</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>4</v>
@@ -5482,13 +5482,13 @@
         <v>132</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="I64" s="2">
         <v>0</v>
@@ -5503,7 +5503,7 @@
         <v>154</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>167</v>
+        <v>502</v>
       </c>
       <c r="N64" s="26" t="s">
         <v>143</v>
@@ -5671,7 +5671,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="66">
+    <row r="68" spans="1:17" ht="42">
       <c r="A68" s="2" t="s">
         <v>143</v>
       </c>
@@ -5679,52 +5679,49 @@
         <v>200</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>132</v>
+        <v>24</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>506</v>
+        <v>177</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>266</v>
       </c>
       <c r="I68" s="2">
-        <v>0</v>
+        <v>40.427699869999998</v>
       </c>
       <c r="J68" s="2">
-        <v>0</v>
+        <v>-80.135979739999996</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="M68" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N68" s="26" t="s">
         <v>143</v>
       </c>
       <c r="O68" s="8" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="P68" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q68" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" ht="42">
+    </row>
+    <row r="69" spans="1:17" ht="66">
       <c r="A69" s="2" t="s">
         <v>143</v>
       </c>
@@ -5732,46 +5729,49 @@
         <v>200</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>266</v>
+        <v>475</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>506</v>
       </c>
       <c r="I69" s="2">
-        <v>40.427699869999998</v>
+        <v>0</v>
       </c>
       <c r="J69" s="2">
-        <v>-80.135979739999996</v>
+        <v>0</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="M69" s="33" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N69" s="26" t="s">
         <v>143</v>
       </c>
       <c r="O69" s="8" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="P69" s="28" t="s">
         <v>352</v>
+      </c>
+      <c r="Q69" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="42">
@@ -5782,7 +5782,7 @@
         <v>200</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>4</v>
@@ -5794,10 +5794,10 @@
         <v>25</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>204</v>
+        <v>402</v>
       </c>
       <c r="I70" s="2">
         <v>40.427699869999998</v>
@@ -5806,13 +5806,13 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>203</v>
+        <v>428</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N70" s="26" t="s">
         <v>143</v>
@@ -5835,7 +5835,7 @@
         <v>200</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>4</v>
@@ -5847,10 +5847,10 @@
         <v>25</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>402</v>
+        <v>204</v>
       </c>
       <c r="I71" s="2">
         <v>40.427699869999998</v>
@@ -5859,13 +5859,13 @@
         <v>-80.135979739999996</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>428</v>
+        <v>203</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N71" s="26" t="s">
         <v>143</v>
@@ -6606,7 +6606,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="42">
+    <row r="86" spans="1:17" ht="44">
       <c r="A86" s="2" t="s">
         <v>238</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>9</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>446</v>
+        <v>237</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>4</v>
@@ -6623,43 +6623,43 @@
         <v>214</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>234</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I86" s="2">
-        <v>38.8060490968736</v>
+        <v>38.8553917225858</v>
       </c>
       <c r="J86" s="2">
-        <v>-77.181676502196197</v>
+        <v>-77.362718702194798</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="M86" s="2" t="s">
-        <v>236</v>
+        <v>420</v>
+      </c>
+      <c r="M86" s="33" t="s">
+        <v>239</v>
       </c>
       <c r="N86" s="26" t="s">
         <v>283</v>
       </c>
       <c r="O86" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="P86" s="28" t="s">
-        <v>352</v>
+        <v>38</v>
+      </c>
+      <c r="P86" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="Q86" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="44">
+    <row r="87" spans="1:17" ht="42">
       <c r="A87" s="2" t="s">
         <v>238</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>9</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>237</v>
+        <v>446</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>4</v>
@@ -6676,37 +6676,37 @@
         <v>214</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>234</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I87" s="2">
-        <v>38.8553917225858</v>
+        <v>38.8060490968736</v>
       </c>
       <c r="J87" s="2">
-        <v>-77.362718702194798</v>
+        <v>-77.181676502196197</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="M87" s="33" t="s">
-        <v>239</v>
+        <v>419</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="N87" s="26" t="s">
         <v>283</v>
       </c>
       <c r="O87" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="P87" s="8" t="s">
-        <v>38</v>
+        <v>283</v>
+      </c>
+      <c r="P87" s="28" t="s">
+        <v>352</v>
       </c>
       <c r="Q87" s="2" t="s">
         <v>365</v>
@@ -8228,80 +8228,80 @@
     <hyperlink ref="M55" r:id="rId7" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{F2FBA2B3-8781-C147-9AA1-AEBC03ECB436}"/>
     <hyperlink ref="M56" r:id="rId8" display="https://loudounliteracy.org/" xr:uid="{9999DF84-E493-E44E-A3EE-CC9DCE69FA8F}"/>
     <hyperlink ref="M58" r:id="rId9" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{15E0A920-6E95-7B4F-BB11-050D757A5EAB}"/>
-    <hyperlink ref="M60" r:id="rId10" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
-    <hyperlink ref="M61" r:id="rId11" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
-    <hyperlink ref="M63" r:id="rId12" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{6193B0D4-846D-4843-9837-B96F841B4261}"/>
-    <hyperlink ref="M62" r:id="rId13" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
-    <hyperlink ref="M64" r:id="rId14" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{D43D4075-EC70-464F-A85F-272BDC168DC4}"/>
-    <hyperlink ref="M65" r:id="rId15" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
-    <hyperlink ref="M66" r:id="rId16" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
-    <hyperlink ref="M67" r:id="rId17" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
-    <hyperlink ref="M59" r:id="rId18" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
-    <hyperlink ref="M84" r:id="rId19" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
-    <hyperlink ref="M89" r:id="rId20" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
-    <hyperlink ref="M90" r:id="rId21" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
-    <hyperlink ref="M43" r:id="rId22" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
-    <hyperlink ref="M45" r:id="rId23" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
-    <hyperlink ref="M41" r:id="rId24" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
-    <hyperlink ref="M107" r:id="rId25" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
-    <hyperlink ref="M105" r:id="rId26" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
-    <hyperlink ref="M106" r:id="rId27" display="https://www.loudoun.gov/1336/Case-Management-Support-Coordination" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
-    <hyperlink ref="M111" r:id="rId28" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
-    <hyperlink ref="M110" r:id="rId29" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
-    <hyperlink ref="M109" r:id="rId30" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
-    <hyperlink ref="M108" r:id="rId31" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
-    <hyperlink ref="M5" r:id="rId32" xr:uid="{E005716C-C6A0-E842-8114-F84C86DBBBC0}"/>
-    <hyperlink ref="M6" r:id="rId33" xr:uid="{8B847267-BF05-0A4A-97C6-E8462D113B75}"/>
-    <hyperlink ref="M8" r:id="rId34" xr:uid="{24323725-30A2-7840-88B2-F022B3E886B0}"/>
-    <hyperlink ref="M15" r:id="rId35" xr:uid="{4785B206-999E-554B-8C21-B6AED74E335C}"/>
-    <hyperlink ref="M18" r:id="rId36" xr:uid="{009FF859-EB8A-6D42-B56A-BBD3AB85EA1D}"/>
-    <hyperlink ref="M20" r:id="rId37" xr:uid="{33658D4E-C47B-5647-8324-3ECF0F8E5C7F}"/>
-    <hyperlink ref="M21" r:id="rId38" xr:uid="{8703E5F8-CFAF-3042-854B-EC5BCE22E9E0}"/>
-    <hyperlink ref="M27" r:id="rId39" xr:uid="{19705E64-A978-0741-AC73-8F0318840D26}"/>
-    <hyperlink ref="M30" r:id="rId40" xr:uid="{63AB1D48-C1A2-6B46-AB45-2F02E7C215FF}"/>
-    <hyperlink ref="M32" r:id="rId41" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{A6E5EE3E-9059-0646-9DA7-80F42FF92AB8}"/>
-    <hyperlink ref="M33" r:id="rId42" xr:uid="{71BFCB2C-4C4A-894A-A7E0-CC5793D459A0}"/>
-    <hyperlink ref="M35" r:id="rId43" xr:uid="{D5C23A14-1262-0E49-8E45-238FC333699C}"/>
-    <hyperlink ref="M36" r:id="rId44" xr:uid="{48F55102-5E5E-4846-931D-3C1345E815F8}"/>
-    <hyperlink ref="M37" r:id="rId45" display="https://www.transitionalservices.org/programs/psychiatric-disabilities/transition-age-youth-tay" xr:uid="{2C36D9E7-20CC-C046-8F37-B0335663708B}"/>
-    <hyperlink ref="M38" r:id="rId46" xr:uid="{9B456C34-A90A-4841-8D07-652EB0070D93}"/>
-    <hyperlink ref="M7" r:id="rId47" xr:uid="{F55E9326-7175-4BF4-B2D8-CD58AF42F319}"/>
-    <hyperlink ref="M40" r:id="rId48" xr:uid="{94D3612A-7340-4BE3-ACF9-1758DC167AD4}"/>
-    <hyperlink ref="M42" r:id="rId49" xr:uid="{B6BCA1D7-7506-4CE1-9D15-8D927D6913EA}"/>
-    <hyperlink ref="M68" r:id="rId50" xr:uid="{EDFE2AA0-FB0F-7D4A-B94C-3655942F41D3}"/>
-    <hyperlink ref="M82" r:id="rId51" xr:uid="{08DD2E30-6D9F-E448-B23B-C201DE5632C2}"/>
-    <hyperlink ref="M69" r:id="rId52" xr:uid="{ED202AB3-1CAE-7A40-8605-6C07A07B887B}"/>
-    <hyperlink ref="M79" r:id="rId53" xr:uid="{D47D5AEF-E1AD-DB42-9E73-177F1DFD9B5F}"/>
-    <hyperlink ref="M80" r:id="rId54" xr:uid="{74F35D5C-B8E2-7946-991F-AF0EB1C77C3A}"/>
-    <hyperlink ref="M85" r:id="rId55" xr:uid="{D234A5E8-C231-CB46-83EA-768401B84DCE}"/>
-    <hyperlink ref="M87" r:id="rId56" xr:uid="{96CB652D-CD1D-9240-9215-431BCE317721}"/>
-    <hyperlink ref="M88" r:id="rId57" xr:uid="{E05BDA41-39DE-E541-A650-FEFB2247F423}"/>
-    <hyperlink ref="M92" r:id="rId58" xr:uid="{02D418A8-483E-F34A-AABD-9BBC33136D93}"/>
-    <hyperlink ref="M93" r:id="rId59" xr:uid="{36A33342-D8A5-CD43-9CA0-0F47D53CAABD}"/>
-    <hyperlink ref="M94" r:id="rId60" xr:uid="{366630D1-2D8D-EE46-9369-BB0EAF04F2DC}"/>
-    <hyperlink ref="M95" r:id="rId61" xr:uid="{6CD8CE33-B2A3-0F43-BE9F-2712DDE7002C}"/>
-    <hyperlink ref="M96" r:id="rId62" xr:uid="{43F35154-B2E7-424D-8904-7897204C168D}"/>
-    <hyperlink ref="M101" r:id="rId63" xr:uid="{D64B06C0-9B20-7547-BE0E-F4223F14C588}"/>
-    <hyperlink ref="M102" r:id="rId64" xr:uid="{2B260585-39CA-7A45-A7F3-F2374875A6E4}"/>
-    <hyperlink ref="M103" r:id="rId65" xr:uid="{5F5D5005-9EEA-2C4C-BD43-FECDEB8C681D}"/>
-    <hyperlink ref="M104" r:id="rId66" xr:uid="{C8025F34-6251-4E48-B559-C4B3A0F3957E}"/>
-    <hyperlink ref="M4" r:id="rId67" xr:uid="{4A0865FD-526B-2444-B026-7CB2FDE4A41B}"/>
-    <hyperlink ref="M12" r:id="rId68" xr:uid="{9B598B0F-66CE-EC45-8022-4A1D6AE6D051}"/>
-    <hyperlink ref="M13" r:id="rId69" xr:uid="{CAF9F199-60F2-664A-A81A-4AB8FE496566}"/>
-    <hyperlink ref="M16" r:id="rId70" xr:uid="{EB8575A9-3C4C-794C-92BD-38FAF9AB99EE}"/>
-    <hyperlink ref="M19" r:id="rId71" xr:uid="{4A41C897-257A-B342-972F-9DD944FE1C97}"/>
-    <hyperlink ref="M22" r:id="rId72" xr:uid="{BFF792ED-FD9C-B142-B875-600AA753D811}"/>
-    <hyperlink ref="M24" r:id="rId73" xr:uid="{64709C7F-2530-CD4B-A678-651174F58B61}"/>
-    <hyperlink ref="M26" r:id="rId74" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{B0F8649D-9B55-3046-A585-14D2AF1D1862}"/>
-    <hyperlink ref="M47" r:id="rId75" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{09CED698-6AB2-D647-9EBC-592C28C734CD}"/>
-    <hyperlink ref="M48" r:id="rId76" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{B7C6202C-DF68-7D4F-8492-0B66B0D3AA47}"/>
-    <hyperlink ref="M54" r:id="rId77" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{262A22CE-A7A2-B949-9752-EEC16517F35A}"/>
-    <hyperlink ref="M97" r:id="rId78" xr:uid="{11D63D27-1546-AA43-853A-B814B607AEC7}"/>
-    <hyperlink ref="M98" r:id="rId79" xr:uid="{64219F6B-917E-264F-832D-0F8C9F3960AF}"/>
-    <hyperlink ref="M99" r:id="rId80" xr:uid="{0ED172BB-0B06-2346-ABA5-50BB328FEF9E}"/>
-    <hyperlink ref="M100" r:id="rId81" xr:uid="{C4C09A72-EE5E-3E45-8186-ED1764C727B3}"/>
-    <hyperlink ref="M3" r:id="rId82" xr:uid="{608DDFB8-CB8A-9645-819E-D96E5B1DB4F5}"/>
-    <hyperlink ref="M2" r:id="rId83" xr:uid="{9EB0AB2E-3B32-624A-912B-53537091A11D}"/>
+    <hyperlink ref="M62" r:id="rId10" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
+    <hyperlink ref="M63" r:id="rId11" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
+    <hyperlink ref="M64" r:id="rId12" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
+    <hyperlink ref="M65" r:id="rId13" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
+    <hyperlink ref="M66" r:id="rId14" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
+    <hyperlink ref="M67" r:id="rId15" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
+    <hyperlink ref="M59" r:id="rId16" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
+    <hyperlink ref="M84" r:id="rId17" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
+    <hyperlink ref="M89" r:id="rId18" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
+    <hyperlink ref="M90" r:id="rId19" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
+    <hyperlink ref="M43" r:id="rId20" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
+    <hyperlink ref="M45" r:id="rId21" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
+    <hyperlink ref="M41" r:id="rId22" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
+    <hyperlink ref="M107" r:id="rId23" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
+    <hyperlink ref="M105" r:id="rId24" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
+    <hyperlink ref="M106" r:id="rId25" display="https://www.loudoun.gov/1336/Case-Management-Support-Coordination" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
+    <hyperlink ref="M111" r:id="rId26" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
+    <hyperlink ref="M110" r:id="rId27" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
+    <hyperlink ref="M109" r:id="rId28" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
+    <hyperlink ref="M108" r:id="rId29" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
+    <hyperlink ref="M6" r:id="rId30" xr:uid="{E005716C-C6A0-E842-8114-F84C86DBBBC0}"/>
+    <hyperlink ref="M8" r:id="rId31" xr:uid="{24323725-30A2-7840-88B2-F022B3E886B0}"/>
+    <hyperlink ref="M15" r:id="rId32" xr:uid="{4785B206-999E-554B-8C21-B6AED74E335C}"/>
+    <hyperlink ref="M18" r:id="rId33" xr:uid="{009FF859-EB8A-6D42-B56A-BBD3AB85EA1D}"/>
+    <hyperlink ref="M20" r:id="rId34" xr:uid="{33658D4E-C47B-5647-8324-3ECF0F8E5C7F}"/>
+    <hyperlink ref="M21" r:id="rId35" xr:uid="{8703E5F8-CFAF-3042-854B-EC5BCE22E9E0}"/>
+    <hyperlink ref="M27" r:id="rId36" xr:uid="{19705E64-A978-0741-AC73-8F0318840D26}"/>
+    <hyperlink ref="M30" r:id="rId37" xr:uid="{63AB1D48-C1A2-6B46-AB45-2F02E7C215FF}"/>
+    <hyperlink ref="M32" r:id="rId38" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{A6E5EE3E-9059-0646-9DA7-80F42FF92AB8}"/>
+    <hyperlink ref="M33" r:id="rId39" xr:uid="{71BFCB2C-4C4A-894A-A7E0-CC5793D459A0}"/>
+    <hyperlink ref="M36" r:id="rId40" xr:uid="{48F55102-5E5E-4846-931D-3C1345E815F8}"/>
+    <hyperlink ref="M37" r:id="rId41" display="https://www.transitionalservices.org/programs/psychiatric-disabilities/transition-age-youth-tay" xr:uid="{2C36D9E7-20CC-C046-8F37-B0335663708B}"/>
+    <hyperlink ref="M7" r:id="rId42" xr:uid="{F55E9326-7175-4BF4-B2D8-CD58AF42F319}"/>
+    <hyperlink ref="M40" r:id="rId43" xr:uid="{94D3612A-7340-4BE3-ACF9-1758DC167AD4}"/>
+    <hyperlink ref="M42" r:id="rId44" xr:uid="{B6BCA1D7-7506-4CE1-9D15-8D927D6913EA}"/>
+    <hyperlink ref="M82" r:id="rId45" xr:uid="{08DD2E30-6D9F-E448-B23B-C201DE5632C2}"/>
+    <hyperlink ref="M79" r:id="rId46" xr:uid="{D47D5AEF-E1AD-DB42-9E73-177F1DFD9B5F}"/>
+    <hyperlink ref="M80" r:id="rId47" xr:uid="{74F35D5C-B8E2-7946-991F-AF0EB1C77C3A}"/>
+    <hyperlink ref="M85" r:id="rId48" xr:uid="{D234A5E8-C231-CB46-83EA-768401B84DCE}"/>
+    <hyperlink ref="M88" r:id="rId49" xr:uid="{E05BDA41-39DE-E541-A650-FEFB2247F423}"/>
+    <hyperlink ref="M92" r:id="rId50" xr:uid="{02D418A8-483E-F34A-AABD-9BBC33136D93}"/>
+    <hyperlink ref="M93" r:id="rId51" xr:uid="{36A33342-D8A5-CD43-9CA0-0F47D53CAABD}"/>
+    <hyperlink ref="M94" r:id="rId52" xr:uid="{366630D1-2D8D-EE46-9369-BB0EAF04F2DC}"/>
+    <hyperlink ref="M95" r:id="rId53" xr:uid="{6CD8CE33-B2A3-0F43-BE9F-2712DDE7002C}"/>
+    <hyperlink ref="M96" r:id="rId54" xr:uid="{43F35154-B2E7-424D-8904-7897204C168D}"/>
+    <hyperlink ref="M101" r:id="rId55" xr:uid="{D64B06C0-9B20-7547-BE0E-F4223F14C588}"/>
+    <hyperlink ref="M102" r:id="rId56" xr:uid="{2B260585-39CA-7A45-A7F3-F2374875A6E4}"/>
+    <hyperlink ref="M103" r:id="rId57" xr:uid="{5F5D5005-9EEA-2C4C-BD43-FECDEB8C681D}"/>
+    <hyperlink ref="M104" r:id="rId58" xr:uid="{C8025F34-6251-4E48-B559-C4B3A0F3957E}"/>
+    <hyperlink ref="M4" r:id="rId59" xr:uid="{4A0865FD-526B-2444-B026-7CB2FDE4A41B}"/>
+    <hyperlink ref="M12" r:id="rId60" xr:uid="{9B598B0F-66CE-EC45-8022-4A1D6AE6D051}"/>
+    <hyperlink ref="M13" r:id="rId61" xr:uid="{CAF9F199-60F2-664A-A81A-4AB8FE496566}"/>
+    <hyperlink ref="M16" r:id="rId62" xr:uid="{EB8575A9-3C4C-794C-92BD-38FAF9AB99EE}"/>
+    <hyperlink ref="M19" r:id="rId63" xr:uid="{4A41C897-257A-B342-972F-9DD944FE1C97}"/>
+    <hyperlink ref="M22" r:id="rId64" xr:uid="{BFF792ED-FD9C-B142-B875-600AA753D811}"/>
+    <hyperlink ref="M24" r:id="rId65" xr:uid="{64709C7F-2530-CD4B-A678-651174F58B61}"/>
+    <hyperlink ref="M26" r:id="rId66" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{B0F8649D-9B55-3046-A585-14D2AF1D1862}"/>
+    <hyperlink ref="M47" r:id="rId67" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{09CED698-6AB2-D647-9EBC-592C28C734CD}"/>
+    <hyperlink ref="M48" r:id="rId68" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{B7C6202C-DF68-7D4F-8492-0B66B0D3AA47}"/>
+    <hyperlink ref="M54" r:id="rId69" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{262A22CE-A7A2-B949-9752-EEC16517F35A}"/>
+    <hyperlink ref="M97" r:id="rId70" xr:uid="{11D63D27-1546-AA43-853A-B814B607AEC7}"/>
+    <hyperlink ref="M98" r:id="rId71" xr:uid="{64219F6B-917E-264F-832D-0F8C9F3960AF}"/>
+    <hyperlink ref="M99" r:id="rId72" xr:uid="{0ED172BB-0B06-2346-ABA5-50BB328FEF9E}"/>
+    <hyperlink ref="M100" r:id="rId73" xr:uid="{C4C09A72-EE5E-3E45-8186-ED1764C727B3}"/>
+    <hyperlink ref="M3" r:id="rId74" xr:uid="{608DDFB8-CB8A-9645-819E-D96E5B1DB4F5}"/>
+    <hyperlink ref="M2" r:id="rId75" xr:uid="{9EB0AB2E-3B32-624A-912B-53537091A11D}"/>
+    <hyperlink ref="M60" r:id="rId76" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{AC946866-D12C-4141-A0F5-356929FEF69C}"/>
+    <hyperlink ref="M35" r:id="rId77" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{AD08644F-6242-C246-A29F-DBA9063E9589}"/>
+    <hyperlink ref="M61" r:id="rId78" xr:uid="{2FE450C9-711D-0540-8D45-12EBCAF17988}"/>
+    <hyperlink ref="M68" r:id="rId79" xr:uid="{1922F5D6-649B-DC40-AEEA-7B7C357B837C}"/>
+    <hyperlink ref="M69" r:id="rId80" xr:uid="{3B025EDF-A3E9-DE40-9A96-4037D5031AFE}"/>
+    <hyperlink ref="M39" r:id="rId81" xr:uid="{A355E03C-9AB0-364C-9B42-22A3AD341E4C}"/>
+    <hyperlink ref="M5" r:id="rId82" xr:uid="{95701045-E657-1644-A0F0-C8AA1A1648AA}"/>
+    <hyperlink ref="M86" r:id="rId83" xr:uid="{67ABFA7A-7DB4-9848-AC22-2A760D037AEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId84"/>

</xml_diff>

<commit_message>
Fixed Adresses and added text from Bradburn/Holmes
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3102C57-6EBE-5742-BBD1-75888A758893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC1088-8479-4AC7-BA65-2586008E9267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="524">
   <si>
     <t>County</t>
   </si>
@@ -1109,126 +1109,6 @@
     <t>Self Sufficiency Programs</t>
   </si>
   <si>
-    <t>Trailview Boulevard Southeast, Leesburg, Loudoun County, Virginia, 20175-4795, United States</t>
-  </si>
-  <si>
-    <t>George Mason University Loudoun, Ridgetop Circle, Dulles Town Center, Loudoun County, Virginia, 20164-6607, United States</t>
-  </si>
-  <si>
-    <t>10721, Main Street, Ardmore, Fairfax, Fairfax (city), Virginia, 22030, United States</t>
-  </si>
-  <si>
-    <t>Dollar City, Arlington Boulevard, Lee Boulevard Heights, Seven Corners, Fairfax County, Virginia, 22044, United States</t>
-  </si>
-  <si>
-    <t>Cue, Old Lee Highway, Fairview, Fairfax, Fairfax (city), Virginia, 22030-2508, United States</t>
-  </si>
-  <si>
-    <t>1850, Cameron Glen Drive, Reston, Fairfax County, Virginia, 20190, United States</t>
-  </si>
-  <si>
-    <t>419-???, Park Avenue, Offutt Village, Falls Church, Arlington, Fairfax (city), Virginia, 22046, United States</t>
-  </si>
-  <si>
-    <t>12122, Pine Forest Circle, Dixie Hill, Fair Oaks, Fairfax County, Virginia, 22030, United States</t>
-  </si>
-  <si>
-    <t>Fairfax County Government Center, 12000, Government Center Parkway, Dixie Hill, Fair Oaks, Fairfax County, Virginia, 22035, United States</t>
-  </si>
-  <si>
-    <t>Pennino Building, 12011, Government Center Parkway, Fairfax County Government Center, Dixie Hill, Fair Oaks, Fairfax County, Virginia, 22035, United States</t>
-  </si>
-  <si>
-    <t>Edsall Park Center, Edsall Road, Edsall Park, Springfield, Fairfax County, Virginia, 22151, United States</t>
-  </si>
-  <si>
-    <t>West Potomac High School, Dawn Drive, Belle Haven, Fairfax County, Virginia, 22306, United States</t>
-  </si>
-  <si>
-    <t>Merrifield, Fairfax County, Virginia, 22031, United States</t>
-  </si>
-  <si>
-    <t>10453, White Granite Drive, Fairfax County, Virginia, 22124, United States</t>
-  </si>
-  <si>
-    <t>Newbrook Drive, Centreville, Fairfax County, Virginia, 20120, United States</t>
-  </si>
-  <si>
-    <t>8098, Merry Oaks Court, Madrillon Farms, Tysons, Fairfax County, Virginia, 22182, United States</t>
-  </si>
-  <si>
-    <t>Good Shepherd Alliance, 20684, Ashburn Road, Ashburn, Loudoun County, Virginia, 20147, United States</t>
-  </si>
-  <si>
-    <t>19598, Meadowview Court, Loudoun County, Virginia, 20175, United States</t>
-  </si>
-  <si>
-    <t>665, Ridge Road, Collier Township, Allegheny County, Pennsylvania, 15205, United States</t>
-  </si>
-  <si>
-    <t>William Flinn Highway, Allison Park, Hampton Township, Allegheny County, Pennsylvania, 15101, United States</t>
-  </si>
-  <si>
-    <t>519, Penn Avenue, Turtle Creek, Allegheny County, Pennsylvania, 15145, United States</t>
-  </si>
-  <si>
-    <t>East 8th Avenue at Ann, Ann Street, Homestead Park, Homestead, Allegheny County, Pennsylvania, 15120, United States</t>
-  </si>
-  <si>
-    <t>Sbarro, 441, Smithfield Street, Downtown, Pittsburgh, Allegheny County, Pennsylvania, 15222, United States</t>
-  </si>
-  <si>
-    <t>216, Cornwall Street Northwest, Leesburg, Loudoun County, Virginia, 20176, United States</t>
-  </si>
-  <si>
-    <t>199, Liberty Street Southwest, Leesburg, Loudoun County, Virginia, 20176, United States</t>
-  </si>
-  <si>
-    <t>26, Fairfax Street Southeast, Leesburg, Loudoun County, Virginia, 20175, United States</t>
-  </si>
-  <si>
-    <t>LOUDOUN CO. JUVENILE DETENTION HOME, 16400, Meadowview Court, Leesburg, Loudoun County, Virginia, 20175, United States</t>
-  </si>
-  <si>
-    <t>Allegheny County Department of Human Services, 1, Smithfield Street, Downtown, Pittsburgh, Allegheny County, Pennsylvania, 15222, United States</t>
-  </si>
-  <si>
-    <t>Point Park University, Smithfield Street, Downtown, Pittsburgh, Allegheny County, Pennsylvania, 15222, United States</t>
-  </si>
-  <si>
-    <t>BNY Mellon Client Service Center, 500, Ross Street, Downtown, Pittsburgh, Allegheny County, Pennsylvania, 15219, United States</t>
-  </si>
-  <si>
-    <t>Auberle, Myrtle Street, McKeesport, Allegheny County, Pennsylvania, 15132, United States</t>
-  </si>
-  <si>
-    <t>7053, Mechanicsville Turnpike, Spring Meadows, Mechanicsville, Hanover County, Virginia, 23111, United States</t>
-  </si>
-  <si>
-    <t>193, Blue Seal Drive Southeast, Leesburg, Loudoun County, Virginia, 20175, United States</t>
-  </si>
-  <si>
-    <t>1834, Howard Avenue, Howard, Tysons, Fairfax County, Virginia, 22182, United States</t>
-  </si>
-  <si>
-    <t>21000, Education Court, Broadlands, Loudoun County, Virginia, 20148, United States</t>
-  </si>
-  <si>
-    <t>Park View High School, Old Vestal's Gap Road, Sterling, Loudoun County, Virginia, 20164-6607, United States</t>
-  </si>
-  <si>
-    <t>Wytestone Plaza, South 8th Street, Shockoe Slip, Richmond, Virginia, 23298, United States</t>
-  </si>
-  <si>
-    <t>Dold L. Bisdorf Building (AA), Netherton Drive, John Adams, Washington Forest, Alexandria, Virginia, 22311, United States</t>
-  </si>
-  <si>
-    <t>Shendoah Exxon, 984, Edwards Ferry Road Northeast, Edwards Landing, Leesburg, Loudoun County, Virginia, 20176, United States</t>
-  </si>
-  <si>
-    <t>Loudoun County Family Services Department, Edwards Ferry Road Northeast, Shendoah Square, Leesburg, Loudoun County, Virginia, 20176, United States</t>
-  </si>
-  <si>
     <t>Virginia Department of Social Services through the federal government; Provides  fincial assistance of up to $5,000 per year for up to five years for college, career school, or training </t>
   </si>
   <si>
@@ -1238,18 +1118,12 @@
     <t>https://www.transitiolservices.org/programs/psychiatric-disabilities/transition-age-youth-tay</t>
   </si>
   <si>
-    <t>East Pittsburgh City Hall, Dymo Alley, East Pittsburgh, Allegheny County, Pennsylvania, 15112, United States</t>
-  </si>
-  <si>
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Magement,-Training,-and-Job-Placement.aspx</t>
   </si>
   <si>
     <t>https://veteransvigator.org/program/74824/loudoun-county-rapid-re-housing-program</t>
   </si>
   <si>
-    <t>So Bank, South King Street, Leesburg, Loudoun County, Virginia, 20175, United States</t>
-  </si>
-  <si>
     <t>KEYS is for Temporary Assistance for Needy Families (TANF) cash assistance and some SP recipients in Pennsylvania.</t>
   </si>
   <si>
@@ -1259,9 +1133,6 @@
     <t>Andale</t>
   </si>
   <si>
-    <t>4364, Evergreen Lane, Alpine, Anndale, Fairfax County, Virginia, 22003, United States</t>
-  </si>
-  <si>
     <t>Case Magement, MHSADS</t>
   </si>
   <si>
@@ -1394,9 +1265,6 @@
     <t>Provides support and emergency shelter to youth up to age 24 who are at-risk, precariously housed or homeless and empowers them to become self-sufficient</t>
   </si>
   <si>
-    <t>302 Parker Court SE, Leesburg, VA 20175</t>
-  </si>
-  <si>
     <t xml:space="preserve">Loudoun, Online </t>
   </si>
   <si>
@@ -1419,9 +1287,6 @@
   </si>
   <si>
     <t>https://www.loudouncares.org/</t>
-  </si>
-  <si>
-    <t>8 S St SW, Leesburg, VA 20175</t>
   </si>
   <si>
     <t>Mixed</t>
@@ -1609,6 +1474,147 @@
   </si>
   <si>
     <t>Receive housing, vocational and educational services, life skills training, therapeutic services (counseling, therapy and/or substance abuse education), and the development of a network of support services in the community; apartment-based Independent Living and Support Services to help foster care youth</t>
+  </si>
+  <si>
+    <t>801 E Main St, Richmond, VA 23219, USA</t>
+  </si>
+  <si>
+    <t>3001 N Beauregard St, Alexandria, VA 22311, USA</t>
+  </si>
+  <si>
+    <t>21167 Stonewheel Way, Broadlands, VA 20148, USA</t>
+  </si>
+  <si>
+    <t>400 W Laurel Ave, Sterling, VA 20164, USA</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>984 Edwards Ferry Rd NE, Leesburg, VA 20176, USA</t>
+  </si>
+  <si>
+    <t>8300 Boone Blvd, Vienna, VA 22182, USA</t>
+  </si>
+  <si>
+    <t>101 Blue Seal Dr SE, Leesburg, VA 20175, USA</t>
+  </si>
+  <si>
+    <t>7443 Lee Davis Rd, Mechanicsville, VA 23111, USA</t>
+  </si>
+  <si>
+    <t>958 Edwards Ferry Rd NE, Leesburg, VA 20176, USA</t>
+  </si>
+  <si>
+    <t>Wood St + Third Ave FS, Pittsburgh, PA 15222, USA</t>
+  </si>
+  <si>
+    <t>1 Smithfield St, Pittsburgh, PA 15222, USA</t>
+  </si>
+  <si>
+    <t>500 Ross St, Pittsburgh, PA 15262, USA</t>
+  </si>
+  <si>
+    <t>813 E Pittsburgh Mall, East Pittsburgh, PA 15112, USA</t>
+  </si>
+  <si>
+    <t>16400 Meadowview Ct, Leesburg, VA 20175, USA</t>
+  </si>
+  <si>
+    <t>102 Heritage Way NE UNIT 103, Leesburg, VA 20176, USA</t>
+  </si>
+  <si>
+    <t>1 VA-7 BUS, Leesburg, VA 20176, USA</t>
+  </si>
+  <si>
+    <t>26 Fairfax St SE, Leesburg, VA 20175, USA</t>
+  </si>
+  <si>
+    <t>199 Liberty St SW, Leesburg, VA 20175, USA</t>
+  </si>
+  <si>
+    <t>217 Cornwall St NW, Leesburg, VA 20176, USA</t>
+  </si>
+  <si>
+    <t>1101 Hartman St, McKeesport, PA 15132, USA</t>
+  </si>
+  <si>
+    <t>8th Ave + Ann, Homestead, PA 15120, USA</t>
+  </si>
+  <si>
+    <t>501 Penn Ave, Turtle Creek, PA 15145, USA</t>
+  </si>
+  <si>
+    <t>3916 William Flinn Hwy, Allison Park, PA 15101, USA</t>
+  </si>
+  <si>
+    <t>652 Ridge Rd, Pittsburgh, PA 15205, USA</t>
+  </si>
+  <si>
+    <t>16451 Meadowview Ct, Leesburg, VA 20175, USA</t>
+  </si>
+  <si>
+    <t>20684 Ashburn Rd, Ashburn, VA 20147, USA</t>
+  </si>
+  <si>
+    <t>8021 Merry Oaks Ct, Vienna, VA 22182, USA</t>
+  </si>
+  <si>
+    <t>14160 Newbrook Dr, Chantilly, VA 20151, USA</t>
+  </si>
+  <si>
+    <t>10455 White Granite Dr, Oakton, VA 22124, USA</t>
+  </si>
+  <si>
+    <t>8115 Gatehouse Rd, Falls Church, VA 22042, USA</t>
+  </si>
+  <si>
+    <t>2411 Belle Haven Meadows Ct, Alexandria, VA 22306, USA</t>
+  </si>
+  <si>
+    <t>6815 Edsall Rd, Springfield, VA 22151, USA</t>
+  </si>
+  <si>
+    <t>12011 Government Center Pkwy, Fairfax, VA 22035, USA</t>
+  </si>
+  <si>
+    <t>12000 Government Center Pkwy, Fairfax, VA 22035, USA</t>
+  </si>
+  <si>
+    <t>12103 Pine Forest Cir, Fairfax, VA 22030, USA</t>
+  </si>
+  <si>
+    <t>427 Park Ave, Falls Church, VA 22046, USA</t>
+  </si>
+  <si>
+    <t>1850 Cameron Glen Dr, Reston, VA 20190, USA</t>
+  </si>
+  <si>
+    <t>3750 Old Lee Hwy, Fairfax, VA 22030, USA</t>
+  </si>
+  <si>
+    <t>6198 a Arlington Blvd, Seven Corners, VA 22044, USA</t>
+  </si>
+  <si>
+    <t>10734 Main St, Fairfax, VA 22030, USA</t>
+  </si>
+  <si>
+    <t>4328e Evergreen Ln, Annandale, VA 22003, USA</t>
+  </si>
+  <si>
+    <t>21641 Ridgetop Cir, Sterling, VA 20166, USA</t>
+  </si>
+  <si>
+    <t>904 Trailview Blvd SE, Leesburg, VA 20175, USA</t>
+  </si>
+  <si>
+    <t>102 Heritage Way NE, Leesburg, VA 20176, USA</t>
+  </si>
+  <si>
+    <t>304 Parker Ct SE, Leesburg, VA 20175, USA</t>
+  </si>
+  <si>
+    <t>5 Royal St SW, Leesburg, VA 20175, USA</t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1848,7 +1854,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2179,11 +2184,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="N8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20.5"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -2200,10 +2205,10 @@
     <col min="14" max="14" width="32.1640625" customWidth="1"/>
     <col min="15" max="15" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.1640625" customWidth="1"/>
-    <col min="17" max="17" width="78.5" style="2" customWidth="1"/>
+    <col min="17" max="17" width="80.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2252,11 +2257,11 @@
       <c r="P1" s="28" t="s">
         <v>351</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="43">
+      <c r="Q1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="41.5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2264,7 +2269,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>432</v>
+        <v>389</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -2276,10 +2281,10 @@
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>464</v>
+        <v>419</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>520</v>
+        <v>475</v>
       </c>
       <c r="I2" s="2">
         <v>37.538339999999998</v>
@@ -2291,7 +2296,7 @@
         <v>18</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>19</v>
@@ -2305,11 +2310,11 @@
       <c r="P2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="43">
+      <c r="Q2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="21">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2329,7 +2334,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>463</v>
+        <v>418</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>253</v>
@@ -2356,13 +2361,13 @@
         <v>38</v>
       </c>
       <c r="P3" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="44">
+        <v>386</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="42">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2382,7 +2387,7 @@
         <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>464</v>
+        <v>419</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>254</v>
@@ -2397,7 +2402,7 @@
         <v>18</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>22</v>
@@ -2409,13 +2414,13 @@
         <v>38</v>
       </c>
       <c r="P4" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="43">
+        <v>386</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="41.5">
       <c r="A5" s="2" t="s">
         <v>283</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>432</v>
+        <v>389</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -2435,10 +2440,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>464</v>
+        <v>419</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>480</v>
+        <v>435</v>
       </c>
       <c r="I5" s="2">
         <v>37.538339999999998</v>
@@ -2450,7 +2455,7 @@
         <v>18</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="M5" s="33" t="s">
         <v>19</v>
@@ -2464,11 +2469,11 @@
       <c r="P5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="43">
+      <c r="Q5" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="21">
       <c r="A6" s="2" t="s">
         <v>283</v>
       </c>
@@ -2488,7 +2493,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>463</v>
+        <v>418</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>253</v>
@@ -2515,13 +2520,13 @@
         <v>38</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="44">
+        <v>386</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="42">
       <c r="A7" s="2" t="s">
         <v>283</v>
       </c>
@@ -2541,7 +2546,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>464</v>
+        <v>419</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>254</v>
@@ -2556,7 +2561,7 @@
         <v>18</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="M7" s="33" t="s">
         <v>22</v>
@@ -2568,13 +2573,13 @@
         <v>38</v>
       </c>
       <c r="P7" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="43">
+        <v>386</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="21">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2594,7 +2599,7 @@
         <v>25</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>465</v>
+        <v>420</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>26</v>
@@ -2623,11 +2628,11 @@
       <c r="P8" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="42">
+      <c r="Q8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="41">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2676,11 +2681,11 @@
       <c r="P9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="42">
+      <c r="Q9" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="41">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2688,7 +2693,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>433</v>
+        <v>390</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -2727,13 +2732,13 @@
         <v>38</v>
       </c>
       <c r="P10" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="42">
+        <v>386</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="41">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2781,6 +2786,9 @@
       </c>
       <c r="P11" s="28" t="s">
         <v>38</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="44" customHeight="1">
@@ -2832,11 +2840,11 @@
       <c r="P12" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q12" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="43">
+      <c r="Q12" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="41.5">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2844,7 +2852,7 @@
         <v>188</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>434</v>
+        <v>391</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>4</v>
@@ -2859,7 +2867,7 @@
         <v>46</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>482</v>
+        <v>437</v>
       </c>
       <c r="I13" s="2">
         <v>38.917318170000001</v>
@@ -2868,7 +2876,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>483</v>
+        <v>438</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>15</v>
@@ -2885,11 +2893,11 @@
       <c r="P13" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q13" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="42">
+      <c r="Q13" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="41">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2897,7 +2905,7 @@
         <v>186</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>435</v>
+        <v>392</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
@@ -2909,7 +2917,7 @@
         <v>224</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>466</v>
+        <v>421</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>256</v>
@@ -2924,10 +2932,10 @@
         <v>38</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>409</v>
+        <v>366</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>410</v>
+        <v>367</v>
       </c>
       <c r="N14" s="26" t="s">
         <v>345</v>
@@ -2936,10 +2944,10 @@
         <v>345</v>
       </c>
       <c r="P14" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="44" customHeight="1">
@@ -2991,11 +2999,11 @@
       <c r="P15" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q15" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="43">
+      <c r="Q15" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="41.5">
       <c r="A16" s="2" t="s">
         <v>283</v>
       </c>
@@ -3003,7 +3011,7 @@
         <v>188</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>434</v>
+        <v>391</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
@@ -3018,7 +3026,7 @@
         <v>46</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>482</v>
+        <v>437</v>
       </c>
       <c r="I16" s="2">
         <v>38.917318170000001</v>
@@ -3027,7 +3035,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>483</v>
+        <v>438</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>15</v>
@@ -3044,11 +3052,11 @@
       <c r="P16" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q16" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="42">
+      <c r="Q16" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="41">
       <c r="A17" s="2" t="s">
         <v>283</v>
       </c>
@@ -3056,7 +3064,7 @@
         <v>186</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>435</v>
+        <v>392</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>11</v>
@@ -3068,7 +3076,7 @@
         <v>224</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>466</v>
+        <v>421</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>256</v>
@@ -3083,10 +3091,10 @@
         <v>38</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>409</v>
+        <v>366</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>410</v>
+        <v>367</v>
       </c>
       <c r="N17" s="26" t="s">
         <v>345</v>
@@ -3095,13 +3103,13 @@
         <v>345</v>
       </c>
       <c r="P17" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="43">
+        <v>386</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="41.5">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -3109,7 +3117,7 @@
         <v>189</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>436</v>
+        <v>393</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>4</v>
@@ -3149,6 +3157,9 @@
       </c>
       <c r="P18" s="28" t="s">
         <v>352</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="36" customHeight="1">
@@ -3159,7 +3170,7 @@
         <v>189</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>437</v>
+        <v>394</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>4</v>
@@ -3200,8 +3211,8 @@
       <c r="P19" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q19" s="2" t="s">
-        <v>387</v>
+      <c r="Q19" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="36" customHeight="1">
@@ -3212,7 +3223,7 @@
         <v>189</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>437</v>
+        <v>394</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>4</v>
@@ -3253,11 +3264,11 @@
       <c r="P20" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q20" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="44">
+      <c r="Q20" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="42">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3306,11 +3317,11 @@
       <c r="P21" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q21" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="64">
+      <c r="Q21" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="41.5">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -3330,7 +3341,7 @@
         <v>60</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>467</v>
+        <v>422</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>258</v>
@@ -3359,11 +3370,11 @@
       <c r="P22" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q22" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="21">
+      <c r="Q22" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -3371,7 +3382,7 @@
         <v>275</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>4</v>
@@ -3383,7 +3394,7 @@
         <v>63</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>468</v>
+        <v>423</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>259</v>
@@ -3401,7 +3412,7 @@
         <v>61</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>431</v>
+        <v>388</v>
       </c>
       <c r="N23" s="26" t="s">
         <v>345</v>
@@ -3412,8 +3423,11 @@
       <c r="P23" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" ht="43">
+      <c r="Q23" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="41.5">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -3436,7 +3450,7 @@
         <v>34</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>484</v>
+        <v>439</v>
       </c>
       <c r="I24" s="2">
         <v>0</v>
@@ -3462,8 +3476,11 @@
       <c r="P24" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" ht="42">
+      <c r="Q24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="41">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -3471,7 +3488,7 @@
         <v>315</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>485</v>
+        <v>440</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>11</v>
@@ -3486,7 +3503,7 @@
         <v>67</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
       <c r="I25" s="2">
         <v>0</v>
@@ -3498,7 +3515,7 @@
         <v>38</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>19</v>
@@ -3512,8 +3529,11 @@
       <c r="P25" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" ht="66">
+      <c r="Q25" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="63">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -3536,7 +3556,7 @@
         <v>67</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>486</v>
+        <v>441</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -3548,10 +3568,10 @@
         <v>38</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>411</v>
+        <v>368</v>
       </c>
       <c r="M26" s="33" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="N26" s="26" t="s">
         <v>345</v>
@@ -3562,8 +3582,11 @@
       <c r="P26" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" ht="64">
+      <c r="Q26" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="41.5">
       <c r="A27" s="2" t="s">
         <v>283</v>
       </c>
@@ -3583,7 +3606,7 @@
         <v>60</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>467</v>
+        <v>422</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>258</v>
@@ -3612,11 +3635,11 @@
       <c r="P27" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q27" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="21">
+      <c r="Q27" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="2" t="s">
         <v>283</v>
       </c>
@@ -3624,7 +3647,7 @@
         <v>275</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>4</v>
@@ -3636,7 +3659,7 @@
         <v>63</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>468</v>
+        <v>423</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>259</v>
@@ -3654,7 +3677,7 @@
         <v>61</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>431</v>
+        <v>388</v>
       </c>
       <c r="N28" s="26" t="s">
         <v>345</v>
@@ -3665,8 +3688,11 @@
       <c r="P28" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" ht="21">
+      <c r="Q28" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="2" t="s">
         <v>143</v>
       </c>
@@ -3674,7 +3700,7 @@
         <v>275</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>4</v>
@@ -3686,7 +3712,7 @@
         <v>63</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>468</v>
+        <v>423</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>259</v>
@@ -3704,7 +3730,7 @@
         <v>61</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>431</v>
+        <v>388</v>
       </c>
       <c r="N29" s="26" t="s">
         <v>345</v>
@@ -3715,8 +3741,11 @@
       <c r="P29" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" ht="43">
+      <c r="Q29" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="41.5">
       <c r="A30" s="2" t="s">
         <v>283</v>
       </c>
@@ -3739,7 +3768,7 @@
         <v>34</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>484</v>
+        <v>439</v>
       </c>
       <c r="I30" s="2">
         <v>0</v>
@@ -3765,8 +3794,11 @@
       <c r="P30" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" ht="42">
+      <c r="Q30" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="41">
       <c r="A31" s="2" t="s">
         <v>283</v>
       </c>
@@ -3774,7 +3806,7 @@
         <v>315</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>485</v>
+        <v>440</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>11</v>
@@ -3789,7 +3821,7 @@
         <v>67</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>487</v>
+        <v>442</v>
       </c>
       <c r="I31" s="2">
         <v>0</v>
@@ -3801,7 +3833,7 @@
         <v>38</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>19</v>
@@ -3815,8 +3847,11 @@
       <c r="P31" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="66">
+      <c r="Q31" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="63">
       <c r="A32" s="2" t="s">
         <v>283</v>
       </c>
@@ -3839,7 +3874,7 @@
         <v>67</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>486</v>
+        <v>441</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -3851,10 +3886,10 @@
         <v>38</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>411</v>
+        <v>368</v>
       </c>
       <c r="M32" s="33" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="N32" s="26" t="s">
         <v>345</v>
@@ -3865,8 +3900,11 @@
       <c r="P32" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" ht="66">
+      <c r="Q32" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="63">
       <c r="A33" s="2" t="s">
         <v>143</v>
       </c>
@@ -3886,7 +3924,7 @@
         <v>71</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>469</v>
+        <v>424</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>72</v>
@@ -3915,8 +3953,11 @@
       <c r="P33" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" ht="42">
+      <c r="Q33" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" s="2" t="s">
         <v>143</v>
       </c>
@@ -3936,10 +3977,10 @@
         <v>77</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>470</v>
+        <v>425</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>488</v>
+        <v>443</v>
       </c>
       <c r="I34" s="2">
         <v>40.437306100000001</v>
@@ -3963,13 +4004,13 @@
         <v>143</v>
       </c>
       <c r="P34" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="42">
+        <v>386</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="41">
       <c r="A35" s="2" t="s">
         <v>143</v>
       </c>
@@ -4018,8 +4059,11 @@
       <c r="P35" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" ht="43">
+      <c r="Q35" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="41.5">
       <c r="A36" s="2" t="s">
         <v>143</v>
       </c>
@@ -4039,7 +4083,7 @@
         <v>42</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>489</v>
+        <v>444</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>87</v>
@@ -4054,7 +4098,7 @@
         <v>73</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>490</v>
+        <v>445</v>
       </c>
       <c r="M36" s="33" t="s">
         <v>88</v>
@@ -4068,11 +4112,11 @@
       <c r="P36" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q36" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="44">
+      <c r="Q36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="42">
       <c r="A37" s="2" t="s">
         <v>143</v>
       </c>
@@ -4080,7 +4124,7 @@
         <v>186</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>439</v>
+        <v>396</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>11</v>
@@ -4095,10 +4139,10 @@
         <v>90</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>491</v>
+        <v>446</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>492</v>
+        <v>447</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2" t="s">
@@ -4108,7 +4152,7 @@
         <v>91</v>
       </c>
       <c r="M37" s="33" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="N37" s="26" t="s">
         <v>143</v>
@@ -4119,11 +4163,11 @@
       <c r="P37" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q37" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="42">
+      <c r="Q37" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="41">
       <c r="A38" s="2" t="s">
         <v>143</v>
       </c>
@@ -4172,11 +4216,11 @@
       <c r="P38" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q38" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="64">
+      <c r="Q38" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="62">
       <c r="A39" s="2" t="s">
         <v>143</v>
       </c>
@@ -4199,7 +4243,7 @@
         <v>67</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>493</v>
+        <v>448</v>
       </c>
       <c r="I39" s="2">
         <v>40.40062056</v>
@@ -4225,8 +4269,11 @@
       <c r="P39" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" ht="44">
+      <c r="Q39" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="42">
       <c r="A40" s="2" t="s">
         <v>143</v>
       </c>
@@ -4273,13 +4320,13 @@
         <v>143</v>
       </c>
       <c r="P40" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="84">
+        <v>386</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="82">
       <c r="A41" s="2" t="s">
         <v>143</v>
       </c>
@@ -4317,7 +4364,7 @@
         <v>74</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>399</v>
+        <v>358</v>
       </c>
       <c r="N41" s="26" t="s">
         <v>143</v>
@@ -4326,13 +4373,13 @@
         <v>143</v>
       </c>
       <c r="P41" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="88">
+        <v>386</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="84">
       <c r="A42" s="2" t="s">
         <v>143</v>
       </c>
@@ -4352,7 +4399,7 @@
         <v>224</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>494</v>
+        <v>449</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>261</v>
@@ -4381,11 +4428,11 @@
       <c r="P42" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q42" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="84">
+      <c r="Q42" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="82">
       <c r="A43" s="2" t="s">
         <v>143</v>
       </c>
@@ -4393,7 +4440,7 @@
         <v>189</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>495</v>
+        <v>450</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>4</v>
@@ -4405,7 +4452,7 @@
         <v>224</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>496</v>
+        <v>451</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>262</v>
@@ -4434,11 +4481,11 @@
       <c r="P43" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q43" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="63">
+      <c r="Q43" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44" s="2" t="s">
         <v>143</v>
       </c>
@@ -4460,7 +4507,7 @@
       <c r="G44" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H44" s="39" t="s">
+      <c r="H44" s="38" t="s">
         <v>263</v>
       </c>
       <c r="I44" s="2">
@@ -4487,11 +4534,11 @@
       <c r="P44" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q44" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="63">
+      <c r="Q44" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="61.5">
       <c r="A45" s="2" t="s">
         <v>143</v>
       </c>
@@ -4499,7 +4546,7 @@
         <v>275</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>445</v>
+        <v>402</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>11</v>
@@ -4511,10 +4558,10 @@
         <v>224</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>496</v>
+        <v>451</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>497</v>
+        <v>452</v>
       </c>
       <c r="I45" s="2">
         <v>0</v>
@@ -4540,8 +4587,11 @@
       <c r="P45" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" ht="63">
+      <c r="Q45" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="61.5">
       <c r="A46" s="2" t="s">
         <v>143</v>
       </c>
@@ -4590,8 +4640,11 @@
       <c r="P46" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" ht="42">
+      <c r="Q46" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="41">
       <c r="A47" s="2" t="s">
         <v>8</v>
       </c>
@@ -4640,8 +4693,11 @@
       <c r="P47" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" ht="42">
+      <c r="Q47" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="41">
       <c r="A48" s="2" t="s">
         <v>8</v>
       </c>
@@ -4664,7 +4720,7 @@
         <v>115</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>498</v>
+        <v>453</v>
       </c>
       <c r="I48" s="2">
         <v>39.076819999999998</v>
@@ -4679,7 +4735,7 @@
         <v>116</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>400</v>
+        <v>359</v>
       </c>
       <c r="N48" s="26" t="s">
         <v>345</v>
@@ -4688,10 +4744,13 @@
         <v>8</v>
       </c>
       <c r="P48" s="28" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" ht="42">
+        <v>386</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="41">
       <c r="A49" s="2" t="s">
         <v>283</v>
       </c>
@@ -4740,8 +4799,11 @@
       <c r="P49" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" ht="42">
+      <c r="Q49" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="41">
       <c r="A50" s="2" t="s">
         <v>283</v>
       </c>
@@ -4764,7 +4826,7 @@
         <v>115</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>498</v>
+        <v>453</v>
       </c>
       <c r="I50" s="2">
         <v>39.076819999999998</v>
@@ -4779,7 +4841,7 @@
         <v>116</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>400</v>
+        <v>359</v>
       </c>
       <c r="N50" s="26" t="s">
         <v>345</v>
@@ -4788,10 +4850,13 @@
         <v>8</v>
       </c>
       <c r="P50" s="28" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" ht="63">
+        <v>386</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="41">
       <c r="A51" s="2" t="s">
         <v>8</v>
       </c>
@@ -4811,7 +4876,7 @@
         <v>33</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>471</v>
+        <v>426</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>118</v>
@@ -4838,13 +4903,13 @@
         <v>8</v>
       </c>
       <c r="P51" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q51" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="63">
+        <v>386</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="41">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4891,13 +4956,13 @@
         <v>8</v>
       </c>
       <c r="P52" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q52" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" ht="42">
+        <v>386</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="41">
       <c r="A53" s="2" t="s">
         <v>8</v>
       </c>
@@ -4917,7 +4982,7 @@
         <v>33</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>472</v>
+        <v>427</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>128</v>
@@ -4946,11 +5011,11 @@
       <c r="P53" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q53" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" ht="63">
+      <c r="Q53" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="61.5">
       <c r="A54" s="2" t="s">
         <v>8</v>
       </c>
@@ -4970,10 +5035,10 @@
         <v>25</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>471</v>
+        <v>426</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>473</v>
+        <v>428</v>
       </c>
       <c r="I54" s="2">
         <v>39.108399900000002</v>
@@ -4999,8 +5064,11 @@
       <c r="P54" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" ht="63">
+      <c r="Q54" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="61.5">
       <c r="A55" s="2" t="s">
         <v>283</v>
       </c>
@@ -5020,10 +5088,10 @@
         <v>25</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>471</v>
+        <v>426</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>473</v>
+        <v>428</v>
       </c>
       <c r="I55" s="2">
         <v>39.108399900000002</v>
@@ -5049,8 +5117,11 @@
       <c r="P55" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" ht="42">
+      <c r="Q55" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
       <c r="A56" s="2" t="s">
         <v>8</v>
       </c>
@@ -5058,7 +5129,7 @@
         <v>9</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>447</v>
+        <v>404</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>4</v>
@@ -5099,11 +5170,11 @@
       <c r="P56" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q56" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="42">
+      <c r="Q56" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="41">
       <c r="A57" s="2" t="s">
         <v>8</v>
       </c>
@@ -5123,7 +5194,7 @@
         <v>138</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>499</v>
+        <v>454</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>140</v>
@@ -5152,11 +5223,11 @@
       <c r="P57" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q57" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" ht="42">
+      <c r="Q57" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="41">
       <c r="A58" s="2" t="s">
         <v>143</v>
       </c>
@@ -5203,13 +5274,13 @@
         <v>350</v>
       </c>
       <c r="P58" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q58" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="42">
+        <v>386</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="41">
       <c r="A59" s="2" t="s">
         <v>143</v>
       </c>
@@ -5256,10 +5327,13 @@
         <v>350</v>
       </c>
       <c r="P59" s="28" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" ht="42">
+        <v>386</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="41">
       <c r="A60" s="2" t="s">
         <v>143</v>
       </c>
@@ -5308,8 +5382,11 @@
       <c r="P60" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" ht="64">
+      <c r="Q60" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="62">
       <c r="A61" s="2" t="s">
         <v>143</v>
       </c>
@@ -5358,11 +5435,11 @@
       <c r="P61" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q61" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" ht="63">
+      <c r="Q61" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="61.5">
       <c r="A62" s="2" t="s">
         <v>143</v>
       </c>
@@ -5382,10 +5459,10 @@
         <v>42</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>474</v>
+        <v>429</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>500</v>
+        <v>455</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -5411,11 +5488,11 @@
       <c r="P62" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q62" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" ht="63">
+      <c r="Q62" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="61.5">
       <c r="A63" s="2" t="s">
         <v>143</v>
       </c>
@@ -5435,10 +5512,10 @@
         <v>42</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>474</v>
+        <v>429</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>501</v>
+        <v>456</v>
       </c>
       <c r="I63" s="2">
         <v>0</v>
@@ -5464,8 +5541,11 @@
       <c r="P63" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" ht="42">
+      <c r="Q63" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="41">
       <c r="A64" s="2" t="s">
         <v>143</v>
       </c>
@@ -5473,7 +5553,7 @@
         <v>188</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>502</v>
+        <v>457</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>4</v>
@@ -5503,7 +5583,7 @@
         <v>154</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>502</v>
+        <v>457</v>
       </c>
       <c r="N64" s="26" t="s">
         <v>143</v>
@@ -5514,8 +5594,11 @@
       <c r="P64" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" ht="21">
+      <c r="Q64" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65" s="2" t="s">
         <v>143</v>
       </c>
@@ -5538,7 +5621,7 @@
         <v>169</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>503</v>
+        <v>458</v>
       </c>
       <c r="I65" s="2">
         <v>40.407960000000003</v>
@@ -5564,8 +5647,11 @@
       <c r="P65" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" ht="42">
+      <c r="Q65" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="41">
       <c r="A66" s="2" t="s">
         <v>143</v>
       </c>
@@ -5588,7 +5674,7 @@
         <v>173</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>504</v>
+        <v>459</v>
       </c>
       <c r="I66" s="2">
         <v>40.405259100000002</v>
@@ -5612,13 +5698,13 @@
         <v>38</v>
       </c>
       <c r="P66" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q66" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" ht="42">
+        <v>386</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="41">
       <c r="A67" s="2" t="s">
         <v>143</v>
       </c>
@@ -5641,7 +5727,7 @@
         <v>177</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>505</v>
+        <v>460</v>
       </c>
       <c r="I67" s="2">
         <v>40.559510000000003</v>
@@ -5667,11 +5753,11 @@
       <c r="P67" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q67" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" ht="42">
+      <c r="Q67" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="41">
       <c r="A68" s="2" t="s">
         <v>143</v>
       </c>
@@ -5720,8 +5806,11 @@
       <c r="P68" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" ht="66">
+      <c r="Q68" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="63">
       <c r="A69" s="2" t="s">
         <v>143</v>
       </c>
@@ -5741,10 +5830,10 @@
         <v>80</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>475</v>
+        <v>430</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>506</v>
+        <v>461</v>
       </c>
       <c r="I69" s="2">
         <v>0</v>
@@ -5770,11 +5859,11 @@
       <c r="P69" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q69" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" ht="42">
+      <c r="Q69" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" ht="41">
       <c r="A70" s="2" t="s">
         <v>143</v>
       </c>
@@ -5797,7 +5886,7 @@
         <v>177</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>402</v>
+        <v>360</v>
       </c>
       <c r="I70" s="2">
         <v>40.427699869999998</v>
@@ -5809,7 +5898,7 @@
         <v>143</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>428</v>
+        <v>385</v>
       </c>
       <c r="M70" s="2" t="s">
         <v>201</v>
@@ -5823,11 +5912,11 @@
       <c r="P70" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q70" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" ht="42">
+      <c r="Q70" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" ht="41">
       <c r="A71" s="2" t="s">
         <v>143</v>
       </c>
@@ -5876,11 +5965,11 @@
       <c r="P71" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q71" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" ht="42">
+      <c r="Q71" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="41">
       <c r="A72" s="2" t="s">
         <v>143</v>
       </c>
@@ -5915,7 +6004,7 @@
         <v>143</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>428</v>
+        <v>385</v>
       </c>
       <c r="M72" s="4" t="s">
         <v>199</v>
@@ -5929,11 +6018,11 @@
       <c r="P72" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q72" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" ht="42">
+      <c r="Q72" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
       <c r="A73" s="2" t="s">
         <v>143</v>
       </c>
@@ -5941,7 +6030,7 @@
         <v>197</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>444</v>
+        <v>401</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>4</v>
@@ -5956,7 +6045,7 @@
         <v>177</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>413</v>
+        <v>370</v>
       </c>
       <c r="I73" s="2">
         <v>0</v>
@@ -5968,7 +6057,7 @@
         <v>38</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>414</v>
+        <v>371</v>
       </c>
       <c r="M73" s="4" t="s">
         <v>198</v>
@@ -5982,11 +6071,11 @@
       <c r="P73" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q73" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" ht="42">
+      <c r="Q73" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" ht="41">
       <c r="A74" s="2" t="s">
         <v>143</v>
       </c>
@@ -6009,7 +6098,7 @@
         <v>276</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>507</v>
+        <v>462</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
@@ -6017,10 +6106,10 @@
         <v>279</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>415</v>
+        <v>372</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>416</v>
+        <v>373</v>
       </c>
       <c r="N74" s="26" t="s">
         <v>143</v>
@@ -6031,8 +6120,11 @@
       <c r="P74" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" ht="42">
+      <c r="Q74" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" ht="41">
       <c r="A75" s="2" t="s">
         <v>8</v>
       </c>
@@ -6040,7 +6132,7 @@
         <v>186</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>508</v>
+        <v>463</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>4</v>
@@ -6081,8 +6173,11 @@
       <c r="P75" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" ht="42">
+      <c r="Q75" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" ht="41">
       <c r="A76" s="2" t="s">
         <v>283</v>
       </c>
@@ -6090,7 +6185,7 @@
         <v>186</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>438</v>
+        <v>395</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>4</v>
@@ -6131,8 +6226,11 @@
       <c r="P76" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" ht="42">
+      <c r="Q76" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" ht="41">
       <c r="A77" s="2" t="s">
         <v>8</v>
       </c>
@@ -6181,8 +6279,11 @@
       <c r="P77" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" ht="42">
+      <c r="Q77" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
       <c r="A78" s="2" t="s">
         <v>8</v>
       </c>
@@ -6231,11 +6332,11 @@
       <c r="P78" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q78" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" ht="64">
+      <c r="Q78" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="62">
       <c r="A79" s="2" t="s">
         <v>238</v>
       </c>
@@ -6255,7 +6356,7 @@
         <v>42</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>476</v>
+        <v>431</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>272</v>
@@ -6270,7 +6371,7 @@
         <v>215</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>417</v>
+        <v>374</v>
       </c>
       <c r="M79" s="33" t="s">
         <v>216</v>
@@ -6284,11 +6385,11 @@
       <c r="P79" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q79" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" ht="85">
+      <c r="Q79" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" ht="82.5">
       <c r="A80" s="2" t="s">
         <v>238</v>
       </c>
@@ -6311,7 +6412,7 @@
         <v>219</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="I80" s="2">
         <v>38.875816034503501</v>
@@ -6323,7 +6424,7 @@
         <v>220</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>418</v>
+        <v>375</v>
       </c>
       <c r="M80" s="33" t="s">
         <v>221</v>
@@ -6337,11 +6438,11 @@
       <c r="P80" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q80" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" ht="84">
+      <c r="Q80" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="82">
       <c r="A81" s="2" t="s">
         <v>238</v>
       </c>
@@ -6364,7 +6465,7 @@
         <v>219</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>521</v>
+        <v>476</v>
       </c>
       <c r="I81" s="2">
         <v>38.875816034503501</v>
@@ -6376,7 +6477,7 @@
         <v>220</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>418</v>
+        <v>375</v>
       </c>
       <c r="M81" s="2" t="s">
         <v>221</v>
@@ -6390,11 +6491,11 @@
       <c r="P81" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q81" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" ht="44">
+      <c r="Q81" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" ht="42">
       <c r="A82" s="2" t="s">
         <v>238</v>
       </c>
@@ -6417,7 +6518,7 @@
         <v>225</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>509</v>
+        <v>464</v>
       </c>
       <c r="I82" s="2">
         <v>38.873610192974397</v>
@@ -6438,16 +6539,16 @@
         <v>283</v>
       </c>
       <c r="O82" s="8" t="s">
-        <v>408</v>
+        <v>365</v>
       </c>
       <c r="P82" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q82" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" ht="63">
+        <v>386</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" ht="61.5">
       <c r="A83" s="2" t="s">
         <v>238</v>
       </c>
@@ -6455,7 +6556,7 @@
         <v>188</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>443</v>
+        <v>400</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>4</v>
@@ -6482,7 +6583,7 @@
         <v>230</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="M83" s="2" t="s">
         <v>231</v>
@@ -6496,11 +6597,11 @@
       <c r="P83" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q83" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" ht="84">
+      <c r="Q83" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" ht="82">
       <c r="A84" s="2" t="s">
         <v>238</v>
       </c>
@@ -6508,7 +6609,7 @@
         <v>188</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>442</v>
+        <v>399</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>11</v>
@@ -6523,7 +6624,7 @@
         <v>242</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>510</v>
+        <v>465</v>
       </c>
       <c r="I84" s="2">
         <v>38.774379099999997</v>
@@ -6535,7 +6636,7 @@
         <v>14</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="M84" s="7" t="s">
         <v>243</v>
@@ -6549,11 +6650,11 @@
       <c r="P84" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q84" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" ht="64">
+      <c r="Q84" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" ht="62">
       <c r="A85" s="2" t="s">
         <v>238</v>
       </c>
@@ -6588,7 +6689,7 @@
         <v>235</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="M85" s="33" t="s">
         <v>236</v>
@@ -6602,11 +6703,11 @@
       <c r="P85" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q85" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" ht="44">
+      <c r="Q85" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" ht="42">
       <c r="A86" s="2" t="s">
         <v>238</v>
       </c>
@@ -6641,7 +6742,7 @@
         <v>238</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>420</v>
+        <v>377</v>
       </c>
       <c r="M86" s="33" t="s">
         <v>239</v>
@@ -6655,11 +6756,11 @@
       <c r="P86" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q86" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" ht="42">
+      <c r="Q86" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
       <c r="A87" s="2" t="s">
         <v>238</v>
       </c>
@@ -6667,7 +6768,7 @@
         <v>9</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>446</v>
+        <v>403</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>4</v>
@@ -6694,7 +6795,7 @@
         <v>235</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="M87" s="2" t="s">
         <v>236</v>
@@ -6708,11 +6809,11 @@
       <c r="P87" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q87" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" ht="127">
+      <c r="Q87" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" ht="123.5">
       <c r="A88" s="2" t="s">
         <v>238</v>
       </c>
@@ -6720,7 +6821,7 @@
         <v>189</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>441</v>
+        <v>398</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>4</v>
@@ -6735,7 +6836,7 @@
         <v>240</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>511</v>
+        <v>466</v>
       </c>
       <c r="I88" s="2">
         <v>38.854251580169802</v>
@@ -6747,7 +6848,7 @@
         <v>238</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>421</v>
+        <v>378</v>
       </c>
       <c r="M88" s="33" t="s">
         <v>241</v>
@@ -6761,11 +6862,11 @@
       <c r="P88" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q88" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" ht="63">
+      <c r="Q88" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="61.5">
       <c r="A89" s="2" t="s">
         <v>238</v>
       </c>
@@ -6785,7 +6886,7 @@
         <v>224</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>512</v>
+        <v>467</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>268</v>
@@ -6814,11 +6915,11 @@
       <c r="P89" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q89" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" ht="63">
+      <c r="Q89" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" ht="61.5">
       <c r="A90" s="2" t="s">
         <v>238</v>
       </c>
@@ -6867,11 +6968,11 @@
       <c r="P90" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q90" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" ht="64">
+      <c r="Q90" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" ht="62">
       <c r="A91" s="2" t="s">
         <v>238</v>
       </c>
@@ -6894,7 +6995,7 @@
         <v>250</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>513</v>
+        <v>468</v>
       </c>
       <c r="I91" s="2">
         <v>38.8553408</v>
@@ -6916,11 +7017,11 @@
         <v>283</v>
       </c>
       <c r="P91" s="34"/>
-      <c r="Q91" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" ht="43">
+      <c r="Q91" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" ht="21">
       <c r="A92" s="2" t="s">
         <v>238</v>
       </c>
@@ -6955,7 +7056,7 @@
         <v>230</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>422</v>
+        <v>379</v>
       </c>
       <c r="M92" s="33" t="s">
         <v>294</v>
@@ -6969,11 +7070,11 @@
       <c r="P92" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q92" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" ht="44">
+      <c r="Q92" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" ht="42">
       <c r="A93" s="2" t="s">
         <v>238</v>
       </c>
@@ -7006,7 +7107,7 @@
         <v>313</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>423</v>
+        <v>380</v>
       </c>
       <c r="M93" s="33" t="s">
         <v>296</v>
@@ -7020,11 +7121,11 @@
       <c r="P93" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q93" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" ht="44">
+      <c r="Q93" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" ht="42">
       <c r="A94" s="2" t="s">
         <v>238</v>
       </c>
@@ -7057,7 +7158,7 @@
         <v>238</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>423</v>
+        <v>380</v>
       </c>
       <c r="M94" s="33" t="s">
         <v>298</v>
@@ -7071,11 +7172,11 @@
       <c r="P94" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q94" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" ht="43">
+      <c r="Q94" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" ht="41.5">
       <c r="A95" s="2" t="s">
         <v>238</v>
       </c>
@@ -7083,7 +7184,7 @@
         <v>275</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>440</v>
+        <v>397</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>4</v>
@@ -7098,7 +7199,7 @@
         <v>299</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>514</v>
+        <v>469</v>
       </c>
       <c r="I95" s="2">
         <v>38.869669999999999</v>
@@ -7110,7 +7211,7 @@
         <v>230</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
       <c r="M95" s="33" t="s">
         <v>300</v>
@@ -7124,11 +7225,11 @@
       <c r="P95" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q95" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" ht="43">
+      <c r="Q95" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" ht="21">
       <c r="A96" s="2" t="s">
         <v>301</v>
       </c>
@@ -7158,7 +7259,7 @@
       </c>
       <c r="L96" s="2"/>
       <c r="M96" s="33" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="N96" s="26" t="s">
         <v>283</v>
@@ -7169,11 +7270,11 @@
       <c r="P96" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q96" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" ht="44">
+      <c r="Q96" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" ht="42">
       <c r="A97" s="2" t="s">
         <v>238</v>
       </c>
@@ -7209,7 +7310,7 @@
       </c>
       <c r="L97" s="34"/>
       <c r="M97" s="33" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="N97" s="27" t="s">
         <v>345</v>
@@ -7220,8 +7321,11 @@
       <c r="P97" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" ht="43">
+      <c r="Q97" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" ht="41.5">
       <c r="A98" s="2" t="s">
         <v>238</v>
       </c>
@@ -7253,7 +7357,7 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>404</v>
+        <v>362</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>306</v>
@@ -7270,11 +7374,11 @@
       <c r="P98" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q98" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" ht="43">
+      <c r="Q98" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" ht="41.5">
       <c r="A99" s="2" t="s">
         <v>238</v>
       </c>
@@ -7282,7 +7386,7 @@
         <v>275</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>4</v>
@@ -7297,7 +7401,7 @@
         <v>308</v>
       </c>
       <c r="H99" s="21" t="s">
-        <v>515</v>
+        <v>470</v>
       </c>
       <c r="I99" s="2">
         <v>0</v>
@@ -7309,7 +7413,7 @@
         <v>38</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
       <c r="M99" s="33" t="s">
         <v>309</v>
@@ -7323,11 +7427,11 @@
       <c r="P99" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q99" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" ht="43">
+      <c r="Q99" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" ht="41.5">
       <c r="A100" s="2" t="s">
         <v>238</v>
       </c>
@@ -7347,7 +7451,7 @@
         <v>311</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>477</v>
+        <v>432</v>
       </c>
       <c r="H100" s="6" t="s">
         <v>318</v>
@@ -7362,7 +7466,7 @@
         <v>38</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
       <c r="M100" s="33" t="s">
         <v>312</v>
@@ -7376,8 +7480,11 @@
       <c r="P100" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="101" spans="1:17" ht="44">
+      <c r="Q100" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" ht="42">
       <c r="A101" s="2" t="s">
         <v>8</v>
       </c>
@@ -7413,7 +7520,7 @@
       </c>
       <c r="L101" s="34"/>
       <c r="M101" s="33" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="N101" s="27" t="s">
         <v>345</v>
@@ -7424,8 +7531,11 @@
       <c r="P101" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="102" spans="1:17" ht="43">
+      <c r="Q101" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" ht="41.5">
       <c r="A102" s="2" t="s">
         <v>8</v>
       </c>
@@ -7457,7 +7567,7 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>404</v>
+        <v>362</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>306</v>
@@ -7474,11 +7584,11 @@
       <c r="P102" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q102" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" ht="43">
+      <c r="Q102" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" ht="41.5">
       <c r="A103" s="2" t="s">
         <v>8</v>
       </c>
@@ -7486,7 +7596,7 @@
         <v>275</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>4</v>
@@ -7501,7 +7611,7 @@
         <v>308</v>
       </c>
       <c r="H103" s="21" t="s">
-        <v>515</v>
+        <v>470</v>
       </c>
       <c r="I103" s="2">
         <v>0</v>
@@ -7513,7 +7623,7 @@
         <v>38</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
       <c r="M103" s="33" t="s">
         <v>309</v>
@@ -7527,11 +7637,11 @@
       <c r="P103" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q103" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" ht="43">
+      <c r="Q103" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" ht="41.5">
       <c r="A104" s="2" t="s">
         <v>8</v>
       </c>
@@ -7551,7 +7661,7 @@
         <v>311</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>477</v>
+        <v>432</v>
       </c>
       <c r="H104" s="6" t="s">
         <v>318</v>
@@ -7566,7 +7676,7 @@
         <v>38</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
       <c r="M104" s="33" t="s">
         <v>312</v>
@@ -7580,8 +7690,11 @@
       <c r="P104" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="105" spans="1:17" ht="42">
+      <c r="Q104" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" ht="41">
       <c r="A105" s="2" t="s">
         <v>8</v>
       </c>
@@ -7630,8 +7743,11 @@
       <c r="P105" s="28" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="106" spans="1:17" ht="42">
+      <c r="Q105" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" ht="41">
       <c r="A106" s="2" t="s">
         <v>8</v>
       </c>
@@ -7639,7 +7755,7 @@
         <v>275</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>406</v>
+        <v>363</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>4</v>
@@ -7669,7 +7785,7 @@
         <v>119</v>
       </c>
       <c r="M106" s="24" t="s">
-        <v>407</v>
+        <v>364</v>
       </c>
       <c r="N106" s="27" t="s">
         <v>282</v>
@@ -7680,11 +7796,11 @@
       <c r="P106" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q106" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" ht="42">
+      <c r="Q106" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" ht="41">
       <c r="A107" s="2" t="s">
         <v>8</v>
       </c>
@@ -7692,7 +7808,7 @@
         <v>186</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>516</v>
+        <v>471</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>4</v>
@@ -7733,11 +7849,11 @@
       <c r="P107" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q107" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="108" spans="1:17" ht="44">
+      <c r="Q107" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" ht="42">
       <c r="A108" s="2" t="s">
         <v>8</v>
       </c>
@@ -7786,11 +7902,11 @@
       <c r="P108" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q108" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" ht="63">
+      <c r="Q108" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" ht="41">
       <c r="A109" s="2" t="s">
         <v>8</v>
       </c>
@@ -7839,11 +7955,11 @@
       <c r="P109" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q109" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="110" spans="1:17" ht="63">
+      <c r="Q109" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" ht="41">
       <c r="A110" s="2" t="s">
         <v>8</v>
       </c>
@@ -7892,11 +8008,11 @@
       <c r="P110" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q110" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="111" spans="1:17" ht="42">
+      <c r="Q110" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" ht="41">
       <c r="A111" s="2" t="s">
         <v>8</v>
       </c>
@@ -7945,11 +8061,11 @@
       <c r="P111" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q111" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="112" spans="1:17" ht="43">
+      <c r="Q111" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" ht="41.5">
       <c r="A112" s="2" t="s">
         <v>8</v>
       </c>
@@ -7957,7 +8073,7 @@
         <v>186</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>448</v>
+        <v>405</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>4</v>
@@ -7966,13 +8082,13 @@
         <v>132</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>453</v>
+        <v>409</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>517</v>
+        <v>472</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>449</v>
+        <v>406</v>
       </c>
       <c r="I112" s="34">
         <v>39.110308750134202</v>
@@ -7984,25 +8100,25 @@
         <v>39</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>448</v>
+        <v>405</v>
       </c>
       <c r="M112" s="8" t="s">
-        <v>452</v>
+        <v>408</v>
       </c>
       <c r="N112" s="27" t="s">
         <v>282</v>
       </c>
       <c r="O112" s="8" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="P112" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q112" s="35" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="113" spans="1:17" ht="43">
+      <c r="Q112" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" ht="41.5">
       <c r="A113" s="2" t="s">
         <v>8</v>
       </c>
@@ -8010,7 +8126,7 @@
         <v>9</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>518</v>
+        <v>473</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>4</v>
@@ -8019,13 +8135,13 @@
         <v>132</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>453</v>
+        <v>409</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>517</v>
+        <v>472</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>454</v>
+        <v>410</v>
       </c>
       <c r="I113" s="34">
         <v>39.110308750134202</v>
@@ -8037,25 +8153,25 @@
         <v>39</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>448</v>
+        <v>405</v>
       </c>
       <c r="M113" s="8" t="s">
-        <v>452</v>
+        <v>408</v>
       </c>
       <c r="N113" s="27" t="s">
         <v>282</v>
       </c>
       <c r="O113" s="8" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="P113" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q113" s="37" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="114" spans="1:17" ht="22">
+      <c r="Q113" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" ht="21">
       <c r="A114" s="2" t="s">
         <v>8</v>
       </c>
@@ -8063,7 +8179,7 @@
         <v>186</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>455</v>
+        <v>411</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>4</v>
@@ -8074,11 +8190,11 @@
       <c r="F114" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G114" s="36" t="s">
-        <v>479</v>
+      <c r="G114" s="35" t="s">
+        <v>434</v>
       </c>
       <c r="H114" s="31" t="s">
-        <v>519</v>
+        <v>474</v>
       </c>
       <c r="I114" s="34">
         <v>39.113335992329198</v>
@@ -8090,25 +8206,25 @@
         <v>39</v>
       </c>
       <c r="L114" s="34" t="s">
-        <v>457</v>
+        <v>413</v>
       </c>
       <c r="M114" s="8" t="s">
-        <v>458</v>
+        <v>414</v>
       </c>
       <c r="N114" s="27" t="s">
         <v>282</v>
       </c>
       <c r="O114" s="8" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="P114" s="34" t="s">
-        <v>460</v>
-      </c>
-      <c r="Q114" s="36" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="115" spans="1:17" ht="22">
+        <v>415</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" ht="21">
       <c r="A115" s="2" t="s">
         <v>8</v>
       </c>
@@ -8116,7 +8232,7 @@
         <v>188</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>455</v>
+        <v>411</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>4</v>
@@ -8127,11 +8243,11 @@
       <c r="F115" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G115" s="36" t="s">
-        <v>479</v>
+      <c r="G115" s="35" t="s">
+        <v>434</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>456</v>
+        <v>412</v>
       </c>
       <c r="I115" s="34">
         <v>39.113335992329198</v>
@@ -8143,25 +8259,25 @@
         <v>39</v>
       </c>
       <c r="L115" s="34" t="s">
-        <v>457</v>
+        <v>413</v>
       </c>
       <c r="M115" s="8" t="s">
-        <v>458</v>
+        <v>414</v>
       </c>
       <c r="N115" s="27" t="s">
         <v>282</v>
       </c>
       <c r="O115" s="8" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="P115" s="34" t="s">
-        <v>460</v>
-      </c>
-      <c r="Q115" s="36" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="116" spans="1:17" ht="43">
+        <v>415</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" ht="41">
       <c r="A116" s="2" t="s">
         <v>8</v>
       </c>
@@ -8169,7 +8285,7 @@
         <v>188</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>461</v>
+        <v>416</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>108</v>
@@ -8180,11 +8296,11 @@
       <c r="F116" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G116" s="37" t="s">
-        <v>478</v>
-      </c>
-      <c r="H116" s="38" t="s">
-        <v>462</v>
+      <c r="G116" s="36" t="s">
+        <v>433</v>
+      </c>
+      <c r="H116" s="37" t="s">
+        <v>417</v>
       </c>
       <c r="I116" s="34">
         <v>39.110308750134202</v>
@@ -8196,22 +8312,22 @@
         <v>39</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>448</v>
+        <v>405</v>
       </c>
       <c r="M116" s="8" t="s">
-        <v>452</v>
+        <v>408</v>
       </c>
       <c r="N116" s="27" t="s">
         <v>282</v>
       </c>
       <c r="O116" s="8" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="P116" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="Q116" s="37" t="s">
-        <v>450</v>
+      <c r="Q116" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="117" spans="1:17" ht="21">
@@ -8316,7 +8432,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="10" customWidth="1"/>

</xml_diff>

<commit_message>
Removed skillsource, reclassified foster care as TAY for those erroneously labeled
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\ShinyApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B8343A-2ABE-4D7F-A2BF-F1FA3A5350F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEE7F26-E26A-4DC1-B1B8-17E721951B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -2137,7 +2137,7 @@
   <dimension ref="A1:Q113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20.5"/>
@@ -8075,88 +8075,88 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M53" r:id="rId1" xr:uid="{13FD1025-9919-E14D-A92B-00246A640824}"/>
-    <hyperlink ref="M45" r:id="rId2" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{6ED53666-C4AE-2E40-A60F-93C9F2AF47E8}"/>
-    <hyperlink ref="M46" r:id="rId3" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{7D4B8EF6-3883-A141-A8F0-C51B5B0CFCE3}"/>
-    <hyperlink ref="M47" r:id="rId4" display="https://www.loudoun.gov/1592/Workforce-Resource-Center" xr:uid="{94B820A0-D3F2-4840-9F07-CA5A487E6333}"/>
-    <hyperlink ref="M48" r:id="rId5" xr:uid="{1A4CA1E2-244B-2C40-8A40-EE156D467B01}"/>
-    <hyperlink ref="M49" r:id="rId6" display="https://biz.loudoun.gov/work-in-loudoun/" xr:uid="{4982EC8B-FAC5-5640-A062-CBB1672F3253}"/>
-    <hyperlink ref="M51" r:id="rId7" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{F2FBA2B3-8781-C147-9AA1-AEBC03ECB436}"/>
-    <hyperlink ref="M52" r:id="rId8" display="https://loudounliteracy.org/" xr:uid="{9999DF84-E493-E44E-A3EE-CC9DCE69FA8F}"/>
-    <hyperlink ref="M54" r:id="rId9" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{15E0A920-6E95-7B4F-BB11-050D757A5EAB}"/>
-    <hyperlink ref="M58" r:id="rId10" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
-    <hyperlink ref="M59" r:id="rId11" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
-    <hyperlink ref="M60" r:id="rId12" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
-    <hyperlink ref="M61" r:id="rId13" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
-    <hyperlink ref="M62" r:id="rId14" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
-    <hyperlink ref="M63" r:id="rId15" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
-    <hyperlink ref="M55" r:id="rId16" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
-    <hyperlink ref="M80" r:id="rId17" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
-    <hyperlink ref="M85" r:id="rId18" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
-    <hyperlink ref="M86" r:id="rId19" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
-    <hyperlink ref="M39" r:id="rId20" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
-    <hyperlink ref="M41" r:id="rId21" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
-    <hyperlink ref="M37" r:id="rId22" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
-    <hyperlink ref="M103" r:id="rId23" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
-    <hyperlink ref="M101" r:id="rId24" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
-    <hyperlink ref="M102" r:id="rId25" display="https://www.loudoun.gov/1336/Case-Management-Support-Coordination" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
-    <hyperlink ref="M107" r:id="rId26" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
-    <hyperlink ref="M106" r:id="rId27" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
-    <hyperlink ref="M105" r:id="rId28" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
-    <hyperlink ref="M104" r:id="rId29" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
-    <hyperlink ref="M6" r:id="rId30" xr:uid="{E005716C-C6A0-E842-8114-F84C86DBBBC0}"/>
-    <hyperlink ref="M8" r:id="rId31" xr:uid="{24323725-30A2-7840-88B2-F022B3E886B0}"/>
-    <hyperlink ref="M15" r:id="rId32" xr:uid="{4785B206-999E-554B-8C21-B6AED74E335C}"/>
-    <hyperlink ref="M18" r:id="rId33" xr:uid="{009FF859-EB8A-6D42-B56A-BBD3AB85EA1D}"/>
-    <hyperlink ref="M20" r:id="rId34" xr:uid="{33658D4E-C47B-5647-8324-3ECF0F8E5C7F}"/>
-    <hyperlink ref="M21" r:id="rId35" xr:uid="{8703E5F8-CFAF-3042-854B-EC5BCE22E9E0}"/>
-    <hyperlink ref="M25" r:id="rId36" xr:uid="{19705E64-A978-0741-AC73-8F0318840D26}"/>
-    <hyperlink ref="M29" r:id="rId37" xr:uid="{71BFCB2C-4C4A-894A-A7E0-CC5793D459A0}"/>
-    <hyperlink ref="M32" r:id="rId38" xr:uid="{48F55102-5E5E-4846-931D-3C1345E815F8}"/>
-    <hyperlink ref="M33" r:id="rId39" display="https://www.transitionalservices.org/programs/psychiatric-disabilities/transition-age-youth-tay" xr:uid="{2C36D9E7-20CC-C046-8F37-B0335663708B}"/>
-    <hyperlink ref="M7" r:id="rId40" xr:uid="{F55E9326-7175-4BF4-B2D8-CD58AF42F319}"/>
-    <hyperlink ref="M36" r:id="rId41" xr:uid="{94D3612A-7340-4BE3-ACF9-1758DC167AD4}"/>
-    <hyperlink ref="M38" r:id="rId42" xr:uid="{B6BCA1D7-7506-4CE1-9D15-8D927D6913EA}"/>
-    <hyperlink ref="M78" r:id="rId43" xr:uid="{08DD2E30-6D9F-E448-B23B-C201DE5632C2}"/>
-    <hyperlink ref="M75" r:id="rId44" xr:uid="{D47D5AEF-E1AD-DB42-9E73-177F1DFD9B5F}"/>
-    <hyperlink ref="M76" r:id="rId45" xr:uid="{74F35D5C-B8E2-7946-991F-AF0EB1C77C3A}"/>
-    <hyperlink ref="M81" r:id="rId46" xr:uid="{D234A5E8-C231-CB46-83EA-768401B84DCE}"/>
-    <hyperlink ref="M84" r:id="rId47" xr:uid="{E05BDA41-39DE-E541-A650-FEFB2247F423}"/>
-    <hyperlink ref="M88" r:id="rId48" xr:uid="{02D418A8-483E-F34A-AABD-9BBC33136D93}"/>
-    <hyperlink ref="M89" r:id="rId49" xr:uid="{36A33342-D8A5-CD43-9CA0-0F47D53CAABD}"/>
-    <hyperlink ref="M90" r:id="rId50" xr:uid="{366630D1-2D8D-EE46-9369-BB0EAF04F2DC}"/>
-    <hyperlink ref="M91" r:id="rId51" xr:uid="{6CD8CE33-B2A3-0F43-BE9F-2712DDE7002C}"/>
-    <hyperlink ref="M92" r:id="rId52" xr:uid="{43F35154-B2E7-424D-8904-7897204C168D}"/>
-    <hyperlink ref="M97" r:id="rId53" xr:uid="{D64B06C0-9B20-7547-BE0E-F4223F14C588}"/>
-    <hyperlink ref="M98" r:id="rId54" xr:uid="{2B260585-39CA-7A45-A7F3-F2374875A6E4}"/>
-    <hyperlink ref="M99" r:id="rId55" xr:uid="{5F5D5005-9EEA-2C4C-BD43-FECDEB8C681D}"/>
-    <hyperlink ref="M100" r:id="rId56" xr:uid="{C8025F34-6251-4E48-B559-C4B3A0F3957E}"/>
-    <hyperlink ref="M3" r:id="rId57" xr:uid="{4A0865FD-526B-2444-B026-7CB2FDE4A41B}"/>
-    <hyperlink ref="M12" r:id="rId58" xr:uid="{9B598B0F-66CE-EC45-8022-4A1D6AE6D051}"/>
-    <hyperlink ref="M13" r:id="rId59" xr:uid="{CAF9F199-60F2-664A-A81A-4AB8FE496566}"/>
-    <hyperlink ref="M16" r:id="rId60" xr:uid="{EB8575A9-3C4C-794C-92BD-38FAF9AB99EE}"/>
-    <hyperlink ref="M19" r:id="rId61" xr:uid="{4A41C897-257A-B342-972F-9DD944FE1C97}"/>
-    <hyperlink ref="M22" r:id="rId62" xr:uid="{BFF792ED-FD9C-B142-B875-600AA753D811}"/>
-    <hyperlink ref="M24" r:id="rId63" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{B0F8649D-9B55-3046-A585-14D2AF1D1862}"/>
-    <hyperlink ref="M43" r:id="rId64" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{09CED698-6AB2-D647-9EBC-592C28C734CD}"/>
-    <hyperlink ref="M44" r:id="rId65" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{B7C6202C-DF68-7D4F-8492-0B66B0D3AA47}"/>
-    <hyperlink ref="M50" r:id="rId66" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{262A22CE-A7A2-B949-9752-EEC16517F35A}"/>
-    <hyperlink ref="M93" r:id="rId67" xr:uid="{11D63D27-1546-AA43-853A-B814B607AEC7}"/>
-    <hyperlink ref="M94" r:id="rId68" xr:uid="{64219F6B-917E-264F-832D-0F8C9F3960AF}"/>
-    <hyperlink ref="M95" r:id="rId69" xr:uid="{0ED172BB-0B06-2346-ABA5-50BB328FEF9E}"/>
-    <hyperlink ref="M96" r:id="rId70" xr:uid="{C4C09A72-EE5E-3E45-8186-ED1764C727B3}"/>
-    <hyperlink ref="M56" r:id="rId71" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{AC946866-D12C-4141-A0F5-356929FEF69C}"/>
-    <hyperlink ref="M31" r:id="rId72" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{AD08644F-6242-C246-A29F-DBA9063E9589}"/>
-    <hyperlink ref="M57" r:id="rId73" xr:uid="{2FE450C9-711D-0540-8D45-12EBCAF17988}"/>
-    <hyperlink ref="M64" r:id="rId74" xr:uid="{1922F5D6-649B-DC40-AEEA-7B7C357B837C}"/>
-    <hyperlink ref="M65" r:id="rId75" xr:uid="{3B025EDF-A3E9-DE40-9A96-4037D5031AFE}"/>
-    <hyperlink ref="M35" r:id="rId76" xr:uid="{A355E03C-9AB0-364C-9B42-22A3AD341E4C}"/>
-    <hyperlink ref="M82" r:id="rId77" xr:uid="{67ABFA7A-7DB4-9848-AC22-2A760D037AEE}"/>
-    <hyperlink ref="M79" r:id="rId78" xr:uid="{02E84075-DB95-444A-8C2E-3EDD3AE99B90}"/>
-    <hyperlink ref="M28" r:id="rId79" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{A6E5EE3E-9059-0646-9DA7-80F42FF92AB8}"/>
-    <hyperlink ref="M5" r:id="rId80" xr:uid="{DA6D7009-460A-40EC-BAB5-D7141DD363C8}"/>
-    <hyperlink ref="M2" r:id="rId81" xr:uid="{5C1DFE40-E41A-4935-AEA4-E0B8F74AEEF5}"/>
-    <hyperlink ref="M4" r:id="rId82" xr:uid="{445C7AEA-96E6-4311-8054-74DEDACE7125}"/>
+    <hyperlink ref="M4" r:id="rId1" xr:uid="{445C7AEA-96E6-4311-8054-74DEDACE7125}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{5C1DFE40-E41A-4935-AEA4-E0B8F74AEEF5}"/>
+    <hyperlink ref="M5" r:id="rId3" xr:uid="{DA6D7009-460A-40EC-BAB5-D7141DD363C8}"/>
+    <hyperlink ref="M28" r:id="rId4" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{A6E5EE3E-9059-0646-9DA7-80F42FF92AB8}"/>
+    <hyperlink ref="M79" r:id="rId5" xr:uid="{02E84075-DB95-444A-8C2E-3EDD3AE99B90}"/>
+    <hyperlink ref="M82" r:id="rId6" xr:uid="{67ABFA7A-7DB4-9848-AC22-2A760D037AEE}"/>
+    <hyperlink ref="M35" r:id="rId7" xr:uid="{A355E03C-9AB0-364C-9B42-22A3AD341E4C}"/>
+    <hyperlink ref="M65" r:id="rId8" xr:uid="{3B025EDF-A3E9-DE40-9A96-4037D5031AFE}"/>
+    <hyperlink ref="M64" r:id="rId9" xr:uid="{1922F5D6-649B-DC40-AEEA-7B7C357B837C}"/>
+    <hyperlink ref="M57" r:id="rId10" xr:uid="{2FE450C9-711D-0540-8D45-12EBCAF17988}"/>
+    <hyperlink ref="M31" r:id="rId11" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{AD08644F-6242-C246-A29F-DBA9063E9589}"/>
+    <hyperlink ref="M56" r:id="rId12" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{AC946866-D12C-4141-A0F5-356929FEF69C}"/>
+    <hyperlink ref="M96" r:id="rId13" xr:uid="{C4C09A72-EE5E-3E45-8186-ED1764C727B3}"/>
+    <hyperlink ref="M95" r:id="rId14" xr:uid="{0ED172BB-0B06-2346-ABA5-50BB328FEF9E}"/>
+    <hyperlink ref="M94" r:id="rId15" xr:uid="{64219F6B-917E-264F-832D-0F8C9F3960AF}"/>
+    <hyperlink ref="M93" r:id="rId16" xr:uid="{11D63D27-1546-AA43-853A-B814B607AEC7}"/>
+    <hyperlink ref="M50" r:id="rId17" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{262A22CE-A7A2-B949-9752-EEC16517F35A}"/>
+    <hyperlink ref="M44" r:id="rId18" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{B7C6202C-DF68-7D4F-8492-0B66B0D3AA47}"/>
+    <hyperlink ref="M43" r:id="rId19" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{09CED698-6AB2-D647-9EBC-592C28C734CD}"/>
+    <hyperlink ref="M24" r:id="rId20" display="https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf" xr:uid="{B0F8649D-9B55-3046-A585-14D2AF1D1862}"/>
+    <hyperlink ref="M22" r:id="rId21" xr:uid="{BFF792ED-FD9C-B142-B875-600AA753D811}"/>
+    <hyperlink ref="M19" r:id="rId22" xr:uid="{4A41C897-257A-B342-972F-9DD944FE1C97}"/>
+    <hyperlink ref="M16" r:id="rId23" xr:uid="{EB8575A9-3C4C-794C-92BD-38FAF9AB99EE}"/>
+    <hyperlink ref="M13" r:id="rId24" xr:uid="{CAF9F199-60F2-664A-A81A-4AB8FE496566}"/>
+    <hyperlink ref="M12" r:id="rId25" xr:uid="{9B598B0F-66CE-EC45-8022-4A1D6AE6D051}"/>
+    <hyperlink ref="M3" r:id="rId26" xr:uid="{4A0865FD-526B-2444-B026-7CB2FDE4A41B}"/>
+    <hyperlink ref="M100" r:id="rId27" xr:uid="{C8025F34-6251-4E48-B559-C4B3A0F3957E}"/>
+    <hyperlink ref="M99" r:id="rId28" xr:uid="{5F5D5005-9EEA-2C4C-BD43-FECDEB8C681D}"/>
+    <hyperlink ref="M98" r:id="rId29" xr:uid="{2B260585-39CA-7A45-A7F3-F2374875A6E4}"/>
+    <hyperlink ref="M97" r:id="rId30" xr:uid="{D64B06C0-9B20-7547-BE0E-F4223F14C588}"/>
+    <hyperlink ref="M92" r:id="rId31" xr:uid="{43F35154-B2E7-424D-8904-7897204C168D}"/>
+    <hyperlink ref="M91" r:id="rId32" xr:uid="{6CD8CE33-B2A3-0F43-BE9F-2712DDE7002C}"/>
+    <hyperlink ref="M90" r:id="rId33" xr:uid="{366630D1-2D8D-EE46-9369-BB0EAF04F2DC}"/>
+    <hyperlink ref="M89" r:id="rId34" xr:uid="{36A33342-D8A5-CD43-9CA0-0F47D53CAABD}"/>
+    <hyperlink ref="M88" r:id="rId35" xr:uid="{02D418A8-483E-F34A-AABD-9BBC33136D93}"/>
+    <hyperlink ref="M84" r:id="rId36" xr:uid="{E05BDA41-39DE-E541-A650-FEFB2247F423}"/>
+    <hyperlink ref="M81" r:id="rId37" xr:uid="{D234A5E8-C231-CB46-83EA-768401B84DCE}"/>
+    <hyperlink ref="M76" r:id="rId38" xr:uid="{74F35D5C-B8E2-7946-991F-AF0EB1C77C3A}"/>
+    <hyperlink ref="M75" r:id="rId39" xr:uid="{D47D5AEF-E1AD-DB42-9E73-177F1DFD9B5F}"/>
+    <hyperlink ref="M78" r:id="rId40" xr:uid="{08DD2E30-6D9F-E448-B23B-C201DE5632C2}"/>
+    <hyperlink ref="M38" r:id="rId41" xr:uid="{B6BCA1D7-7506-4CE1-9D15-8D927D6913EA}"/>
+    <hyperlink ref="M36" r:id="rId42" xr:uid="{94D3612A-7340-4BE3-ACF9-1758DC167AD4}"/>
+    <hyperlink ref="M7" r:id="rId43" xr:uid="{F55E9326-7175-4BF4-B2D8-CD58AF42F319}"/>
+    <hyperlink ref="M33" r:id="rId44" display="https://www.transitionalservices.org/programs/psychiatric-disabilities/transition-age-youth-tay" xr:uid="{2C36D9E7-20CC-C046-8F37-B0335663708B}"/>
+    <hyperlink ref="M32" r:id="rId45" xr:uid="{48F55102-5E5E-4846-931D-3C1345E815F8}"/>
+    <hyperlink ref="M29" r:id="rId46" xr:uid="{71BFCB2C-4C4A-894A-A7E0-CC5793D459A0}"/>
+    <hyperlink ref="M25" r:id="rId47" xr:uid="{19705E64-A978-0741-AC73-8F0318840D26}"/>
+    <hyperlink ref="M21" r:id="rId48" xr:uid="{8703E5F8-CFAF-3042-854B-EC5BCE22E9E0}"/>
+    <hyperlink ref="M20" r:id="rId49" xr:uid="{33658D4E-C47B-5647-8324-3ECF0F8E5C7F}"/>
+    <hyperlink ref="M18" r:id="rId50" xr:uid="{009FF859-EB8A-6D42-B56A-BBD3AB85EA1D}"/>
+    <hyperlink ref="M15" r:id="rId51" xr:uid="{4785B206-999E-554B-8C21-B6AED74E335C}"/>
+    <hyperlink ref="M8" r:id="rId52" xr:uid="{24323725-30A2-7840-88B2-F022B3E886B0}"/>
+    <hyperlink ref="M6" r:id="rId53" xr:uid="{E005716C-C6A0-E842-8114-F84C86DBBBC0}"/>
+    <hyperlink ref="M104" r:id="rId54" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
+    <hyperlink ref="M105" r:id="rId55" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
+    <hyperlink ref="M106" r:id="rId56" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
+    <hyperlink ref="M107" r:id="rId57" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
+    <hyperlink ref="M102" r:id="rId58" display="https://www.loudoun.gov/1336/Case-Management-Support-Coordination" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
+    <hyperlink ref="M101" r:id="rId59" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
+    <hyperlink ref="M103" r:id="rId60" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
+    <hyperlink ref="M37" r:id="rId61" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
+    <hyperlink ref="M41" r:id="rId62" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
+    <hyperlink ref="M39" r:id="rId63" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
+    <hyperlink ref="M86" r:id="rId64" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
+    <hyperlink ref="M85" r:id="rId65" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
+    <hyperlink ref="M80" r:id="rId66" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
+    <hyperlink ref="M55" r:id="rId67" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
+    <hyperlink ref="M63" r:id="rId68" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
+    <hyperlink ref="M62" r:id="rId69" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
+    <hyperlink ref="M61" r:id="rId70" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
+    <hyperlink ref="M60" r:id="rId71" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
+    <hyperlink ref="M59" r:id="rId72" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
+    <hyperlink ref="M58" r:id="rId73" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
+    <hyperlink ref="M54" r:id="rId74" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{15E0A920-6E95-7B4F-BB11-050D757A5EAB}"/>
+    <hyperlink ref="M52" r:id="rId75" display="https://loudounliteracy.org/" xr:uid="{9999DF84-E493-E44E-A3EE-CC9DCE69FA8F}"/>
+    <hyperlink ref="M51" r:id="rId76" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{F2FBA2B3-8781-C147-9AA1-AEBC03ECB436}"/>
+    <hyperlink ref="M49" r:id="rId77" display="https://biz.loudoun.gov/work-in-loudoun/" xr:uid="{4982EC8B-FAC5-5640-A062-CBB1672F3253}"/>
+    <hyperlink ref="M48" r:id="rId78" xr:uid="{1A4CA1E2-244B-2C40-8A40-EE156D467B01}"/>
+    <hyperlink ref="M47" r:id="rId79" display="https://www.loudoun.gov/1592/Workforce-Resource-Center" xr:uid="{94B820A0-D3F2-4840-9F07-CA5A487E6333}"/>
+    <hyperlink ref="M46" r:id="rId80" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{7D4B8EF6-3883-A141-A8F0-C51B5B0CFCE3}"/>
+    <hyperlink ref="M45" r:id="rId81" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{6ED53666-C4AE-2E40-A60F-93C9F2AF47E8}"/>
+    <hyperlink ref="M53" r:id="rId82" xr:uid="{13FD1025-9919-E14D-A92B-00246A640824}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId83"/>

</xml_diff>

<commit_message>
new layout with Services tab
</commit_message>
<xml_diff>
--- a/ShinyApp/data/combined-programs.xlsx
+++ b/ShinyApp/data/combined-programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8D812B-2C21-CD45-9832-888C42606078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFC0320-98CF-4848-B410-0F850F6C5DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="16840" xr2:uid="{4632C4BB-D241-C74A-8837-66435AB2A0CF}"/>
   </bookViews>
@@ -1067,9 +1067,6 @@
     <t>https://www.vccs.edu/wp-content/uploads/2020/04/FINCIAL-AID-PROGRAMS-revised-100719.pdf</t>
   </si>
   <si>
-    <t>https://www.transitiolservices.org/programs/psychiatric-disabilities/transition-age-youth-tay</t>
-  </si>
-  <si>
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Magement,-Training,-and-Job-Placement.aspx</t>
   </si>
   <si>
@@ -1236,9 +1233,6 @@
   </si>
   <si>
     <t>Must take TEAS exam prior </t>
-  </si>
-  <si>
-    <t>Household must make less than 50% of the Area Median Income (AMI) for the area where the voucher will be used (this is known as the income limit).</t>
   </si>
   <si>
     <t>Under 19 years old, not insured and fall below family income of $2,201 monthly </t>
@@ -1600,13 +1594,19 @@
   </si>
   <si>
     <t>TOPS</t>
+  </si>
+  <si>
+    <t>Have a household income at or below 50 percent of the area median income as determined by the U.S. Department of Housing and Urban Development (HUD); Be a United States citizen, or a non-citizen with "eligible immigration status.”</t>
+  </si>
+  <si>
+    <t>https://www.transitionalservices.org/programs/psychiatric-disabilities/transition-age-youth-tay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1672,6 +1672,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="21"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1745,7 +1751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1805,6 +1811,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2127,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A57FC4F-EB06-AA42-A723-3E738AABF9A5}">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="19" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="59" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
@@ -2201,7 +2211,7 @@
         <v>336</v>
       </c>
       <c r="Q1" s="28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="21" customFormat="1">
@@ -2212,7 +2222,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>4</v>
@@ -2224,10 +2234,10 @@
         <v>17</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I2" s="15">
         <v>37.538339999999998</v>
@@ -2239,7 +2249,7 @@
         <v>18</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>19</v>
@@ -2254,7 +2264,7 @@
         <v>38</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="44">
@@ -2277,7 +2287,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>245</v>
@@ -2292,7 +2302,7 @@
         <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="M3" s="24" t="s">
         <v>22</v>
@@ -2304,10 +2314,10 @@
         <v>38</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q3" s="28" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="21" customFormat="1">
@@ -2318,7 +2328,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>4</v>
@@ -2330,10 +2340,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I4" s="15">
         <v>37.538339999999998</v>
@@ -2345,7 +2355,7 @@
         <v>18</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>19</v>
@@ -2360,7 +2370,7 @@
         <v>38</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="64">
@@ -2383,10 +2393,10 @@
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I5" s="2">
         <v>39.028318303137603</v>
@@ -2410,10 +2420,10 @@
         <v>38</v>
       </c>
       <c r="P5" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="64">
@@ -2436,10 +2446,10 @@
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I6" s="2">
         <v>39.028318303137603</v>
@@ -2463,10 +2473,10 @@
         <v>38</v>
       </c>
       <c r="P6" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="44">
@@ -2489,7 +2499,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>245</v>
@@ -2504,7 +2514,7 @@
         <v>18</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="M7" s="24" t="s">
         <v>22</v>
@@ -2516,10 +2526,10 @@
         <v>38</v>
       </c>
       <c r="P7" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q7" s="28" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="22">
@@ -2542,7 +2552,7 @@
         <v>25</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>26</v>
@@ -2572,7 +2582,7 @@
         <v>337</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="43">
@@ -2625,7 +2635,7 @@
         <v>38</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="43">
@@ -2636,7 +2646,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -2675,10 +2685,10 @@
         <v>38</v>
       </c>
       <c r="P10" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="43">
@@ -2731,7 +2741,7 @@
         <v>38</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="44" customHeight="1">
@@ -2742,7 +2752,7 @@
         <v>180</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>4</v>
@@ -2757,7 +2767,7 @@
         <v>42</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I12" s="2">
         <v>39.114306589999998</v>
@@ -2784,7 +2794,7 @@
         <v>337</v>
       </c>
       <c r="Q12" s="28" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="43">
@@ -2795,7 +2805,7 @@
         <v>180</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>4</v>
@@ -2810,7 +2820,7 @@
         <v>45</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I13" s="2">
         <v>38.917318170000001</v>
@@ -2819,7 +2829,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>15</v>
@@ -2828,19 +2838,19 @@
         <v>46</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P13" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q13" s="28" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="43">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="44">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2848,7 +2858,7 @@
         <v>178</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>4</v>
@@ -2859,8 +2869,8 @@
       <c r="F14" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>398</v>
+      <c r="G14" s="35" t="s">
+        <v>517</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>247</v>
@@ -2875,10 +2885,10 @@
         <v>38</v>
       </c>
       <c r="L14" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="N14" s="22" t="s">
         <v>332</v>
@@ -2887,10 +2897,10 @@
         <v>332</v>
       </c>
       <c r="P14" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q14" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="44" customHeight="1">
@@ -2901,7 +2911,7 @@
         <v>180</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>4</v>
@@ -2943,7 +2953,7 @@
         <v>337</v>
       </c>
       <c r="Q15" s="28" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="43">
@@ -2954,7 +2964,7 @@
         <v>180</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
@@ -2969,7 +2979,7 @@
         <v>45</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I16" s="2">
         <v>38.917318170000001</v>
@@ -2978,7 +2988,7 @@
         <v>-77.231870560000004</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>15</v>
@@ -2987,19 +2997,19 @@
         <v>46</v>
       </c>
       <c r="N16" s="22" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="O16" s="22" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P16" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q16" s="28" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="43">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="44">
       <c r="A17" s="2" t="s">
         <v>274</v>
       </c>
@@ -3007,7 +3017,7 @@
         <v>178</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>4</v>
@@ -3018,8 +3028,8 @@
       <c r="F17" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>398</v>
+      <c r="G17" s="35" t="s">
+        <v>517</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>247</v>
@@ -3034,10 +3044,10 @@
         <v>38</v>
       </c>
       <c r="L17" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="N17" s="22" t="s">
         <v>332</v>
@@ -3046,10 +3056,10 @@
         <v>332</v>
       </c>
       <c r="P17" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q17" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="43">
@@ -3060,7 +3070,7 @@
         <v>181</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>4</v>
@@ -3102,7 +3112,7 @@
         <v>337</v>
       </c>
       <c r="Q18" s="28" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="36" customHeight="1">
@@ -3113,7 +3123,7 @@
         <v>181</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>4</v>
@@ -3155,7 +3165,7 @@
         <v>337</v>
       </c>
       <c r="Q19" s="28" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="36" customHeight="1">
@@ -3166,7 +3176,7 @@
         <v>181</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>4</v>
@@ -3208,7 +3218,7 @@
         <v>337</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="44">
@@ -3219,7 +3229,7 @@
         <v>181</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>4</v>
@@ -3234,7 +3244,7 @@
         <v>53</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I21" s="2">
         <v>39.114571660000003</v>
@@ -3261,7 +3271,7 @@
         <v>337</v>
       </c>
       <c r="Q21" s="28" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="43">
@@ -3272,7 +3282,7 @@
         <v>266</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>4</v>
@@ -3284,7 +3294,7 @@
         <v>56</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>249</v>
@@ -3314,7 +3324,7 @@
         <v>38</v>
       </c>
       <c r="Q22" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="22">
@@ -3325,7 +3335,7 @@
         <v>266</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>4</v>
@@ -3337,7 +3347,7 @@
         <v>59</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>250</v>
@@ -3355,7 +3365,7 @@
         <v>57</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N23" s="22" t="s">
         <v>332</v>
@@ -3367,7 +3377,7 @@
         <v>38</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="66">
@@ -3393,7 +3403,7 @@
         <v>60</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I24" s="2">
         <v>0</v>
@@ -3405,7 +3415,7 @@
         <v>38</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M24" s="24" t="s">
         <v>340</v>
@@ -3420,7 +3430,7 @@
         <v>38</v>
       </c>
       <c r="Q24" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="22">
@@ -3431,7 +3441,7 @@
         <v>266</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>4</v>
@@ -3443,7 +3453,7 @@
         <v>59</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>250</v>
@@ -3461,7 +3471,7 @@
         <v>57</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N25" s="22" t="s">
         <v>332</v>
@@ -3473,18 +3483,18 @@
         <v>38</v>
       </c>
       <c r="Q25" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="22">
       <c r="A26" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
@@ -3496,7 +3506,7 @@
         <v>59</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>250</v>
@@ -3514,7 +3524,7 @@
         <v>57</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N26" s="22" t="s">
         <v>332</v>
@@ -3526,7 +3536,7 @@
         <v>38</v>
       </c>
       <c r="Q26" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="64">
@@ -3564,7 +3574,7 @@
         <v>227</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M27" s="24" t="s">
         <v>228</v>
@@ -3579,12 +3589,12 @@
         <v>337</v>
       </c>
       <c r="Q27" s="28" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="66">
       <c r="A28" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>9</v>
@@ -3602,7 +3612,7 @@
         <v>64</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>65</v>
@@ -3623,21 +3633,21 @@
         <v>68</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O28" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P28" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q28" s="28" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="22">
       <c r="A29" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>180</v>
@@ -3655,10 +3665,10 @@
         <v>70</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I29" s="2">
         <v>40.437306100000001</v>
@@ -3676,21 +3686,21 @@
         <v>71</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O29" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P29" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q29" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="43">
       <c r="A30" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>180</v>
@@ -3729,21 +3739,21 @@
         <v>159</v>
       </c>
       <c r="N30" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O30" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="O30" s="15" t="s">
-        <v>511</v>
       </c>
       <c r="P30" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q30" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="43">
       <c r="A31" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>178</v>
@@ -3761,7 +3771,7 @@
         <v>41</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>80</v>
@@ -3776,33 +3786,33 @@
         <v>66</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M31" s="24" t="s">
         <v>81</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O31" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P31" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q31" s="28" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="44">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="43">
       <c r="A32" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>11</v>
@@ -3817,10 +3827,10 @@
         <v>83</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
@@ -3829,25 +3839,25 @@
       <c r="L32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M32" s="24" t="s">
-        <v>341</v>
+      <c r="M32" s="36" t="s">
+        <v>518</v>
       </c>
       <c r="N32" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O32" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P32" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q32" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="43">
       <c r="A33" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>178</v>
@@ -3886,21 +3896,21 @@
         <v>87</v>
       </c>
       <c r="N33" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O33" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P33" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q33" s="28" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="64">
       <c r="A34" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>178</v>
@@ -3921,7 +3931,7 @@
         <v>60</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I34" s="2">
         <v>40.40062056</v>
@@ -3939,21 +3949,21 @@
         <v>87</v>
       </c>
       <c r="N34" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O34" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P34" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q34" s="28" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="44">
       <c r="A35" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>178</v>
@@ -3992,21 +4002,21 @@
         <v>87</v>
       </c>
       <c r="N35" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O35" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P35" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q35" s="28" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="85">
       <c r="A36" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>181</v>
@@ -4042,24 +4052,24 @@
         <v>67</v>
       </c>
       <c r="M36" s="26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N36" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O36" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P36" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q36" s="28" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="88">
       <c r="A37" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>181</v>
@@ -4077,7 +4087,7 @@
         <v>216</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>252</v>
@@ -4098,27 +4108,27 @@
         <v>244</v>
       </c>
       <c r="N37" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O37" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P37" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q37" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="85">
       <c r="A38" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>4</v>
@@ -4130,7 +4140,7 @@
         <v>216</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>253</v>
@@ -4151,21 +4161,21 @@
         <v>94</v>
       </c>
       <c r="N38" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O38" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P38" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q38" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="22">
       <c r="A39" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>266</v>
@@ -4204,7 +4214,7 @@
         <v>96</v>
       </c>
       <c r="N39" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O39" s="15" t="s">
         <v>38</v>
@@ -4213,21 +4223,21 @@
         <v>38</v>
       </c>
       <c r="Q39" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="64">
       <c r="A40" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>24</v>
@@ -4236,10 +4246,10 @@
         <v>216</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I40" s="2">
         <v>0</v>
@@ -4257,21 +4267,21 @@
         <v>97</v>
       </c>
       <c r="N40" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O40" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="O40" s="15" t="s">
-        <v>511</v>
       </c>
       <c r="P40" s="23" t="s">
         <v>38</v>
       </c>
       <c r="Q40" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="64">
       <c r="A41" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>266</v>
@@ -4310,16 +4320,16 @@
         <v>97</v>
       </c>
       <c r="N41" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O41" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="O41" s="15" t="s">
-        <v>511</v>
       </c>
       <c r="P41" s="23" t="s">
         <v>38</v>
       </c>
       <c r="Q41" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="43">
@@ -4372,7 +4382,7 @@
         <v>337</v>
       </c>
       <c r="Q42" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="43">
@@ -4398,7 +4408,7 @@
         <v>108</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I43" s="2">
         <v>39.076819999999998</v>
@@ -4413,7 +4423,7 @@
         <v>109</v>
       </c>
       <c r="M43" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N43" s="22" t="s">
         <v>332</v>
@@ -4422,10 +4432,10 @@
         <v>8</v>
       </c>
       <c r="P43" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q43" s="28" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="43">
@@ -4478,7 +4488,7 @@
         <v>337</v>
       </c>
       <c r="Q44" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="43">
@@ -4504,7 +4514,7 @@
         <v>108</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I45" s="2">
         <v>39.076819999999998</v>
@@ -4519,7 +4529,7 @@
         <v>109</v>
       </c>
       <c r="M45" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N45" s="22" t="s">
         <v>332</v>
@@ -4528,10 +4538,10 @@
         <v>8</v>
       </c>
       <c r="P45" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q45" s="28" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="43">
@@ -4554,7 +4564,7 @@
         <v>33</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>111</v>
@@ -4581,10 +4591,10 @@
         <v>8</v>
       </c>
       <c r="P46" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q46" s="28" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="43">
@@ -4634,10 +4644,10 @@
         <v>8</v>
       </c>
       <c r="P47" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q47" s="28" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="43">
@@ -4660,7 +4670,7 @@
         <v>33</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>121</v>
@@ -4690,7 +4700,7 @@
         <v>38</v>
       </c>
       <c r="Q48" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="22">
@@ -4713,10 +4723,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I49" s="2">
         <v>39.108399900000002</v>
@@ -4743,7 +4753,7 @@
         <v>337</v>
       </c>
       <c r="Q49" s="28" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="64">
@@ -4766,10 +4776,10 @@
         <v>25</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="I50" s="2">
         <v>39.108399900000002</v>
@@ -4796,7 +4806,7 @@
         <v>337</v>
       </c>
       <c r="Q50" s="28" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="22">
@@ -4807,7 +4817,7 @@
         <v>9</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>4</v>
@@ -4822,7 +4832,7 @@
         <v>128</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I51" s="2">
         <v>39.114406199999998</v>
@@ -4849,7 +4859,7 @@
         <v>337</v>
       </c>
       <c r="Q51" s="28" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="43">
@@ -4872,7 +4882,7 @@
         <v>130</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>132</v>
@@ -4902,12 +4912,12 @@
         <v>337</v>
       </c>
       <c r="Q52" s="28" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="43">
       <c r="A53" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>178</v>
@@ -4946,21 +4956,21 @@
         <v>139</v>
       </c>
       <c r="N53" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O53" s="15" t="s">
         <v>509</v>
       </c>
-      <c r="O53" s="15" t="s">
-        <v>511</v>
-      </c>
       <c r="P53" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q53" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="43">
       <c r="A54" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>178</v>
@@ -4999,21 +5009,21 @@
         <v>144</v>
       </c>
       <c r="N54" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O54" s="15" t="s">
         <v>509</v>
       </c>
-      <c r="O54" s="15" t="s">
-        <v>511</v>
-      </c>
       <c r="P54" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q54" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="43">
       <c r="A55" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>180</v>
@@ -5052,21 +5062,21 @@
         <v>156</v>
       </c>
       <c r="N55" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O55" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="O55" s="15" t="s">
-        <v>511</v>
       </c>
       <c r="P55" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q55" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="64">
       <c r="A56" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>180</v>
@@ -5105,7 +5115,7 @@
         <v>78</v>
       </c>
       <c r="N56" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O56" s="15" t="s">
         <v>38</v>
@@ -5114,12 +5124,12 @@
         <v>337</v>
       </c>
       <c r="Q56" s="28" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="64">
       <c r="A57" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>180</v>
@@ -5137,10 +5147,10 @@
         <v>41</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I57" s="2">
         <v>0</v>
@@ -5158,21 +5168,21 @@
         <v>147</v>
       </c>
       <c r="N57" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O57" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="O57" s="15" t="s">
-        <v>511</v>
       </c>
       <c r="P57" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q57" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="64">
       <c r="A58" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>180</v>
@@ -5190,10 +5200,10 @@
         <v>41</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I58" s="2">
         <v>0</v>
@@ -5211,27 +5221,27 @@
         <v>149</v>
       </c>
       <c r="N58" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O58" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="O58" s="15" t="s">
-        <v>511</v>
       </c>
       <c r="P58" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q58" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="43">
       <c r="A59" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>4</v>
@@ -5261,24 +5271,24 @@
         <v>146</v>
       </c>
       <c r="M59" s="26" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="N59" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O59" s="15" t="s">
         <v>509</v>
-      </c>
-      <c r="O59" s="15" t="s">
-        <v>511</v>
       </c>
       <c r="P59" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q59" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="22">
       <c r="A60" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>180</v>
@@ -5299,7 +5309,7 @@
         <v>161</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I60" s="2">
         <v>40.407960000000003</v>
@@ -5317,7 +5327,7 @@
         <v>163</v>
       </c>
       <c r="N60" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O60" s="15" t="s">
         <v>38</v>
@@ -5326,12 +5336,12 @@
         <v>38</v>
       </c>
       <c r="Q60" s="28" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="43">
       <c r="A61" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>180</v>
@@ -5352,7 +5362,7 @@
         <v>165</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I61" s="2">
         <v>40.405259100000002</v>
@@ -5370,21 +5380,21 @@
         <v>167</v>
       </c>
       <c r="N61" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O61" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P61" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q61" s="28" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="43">
       <c r="A62" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>180</v>
@@ -5405,7 +5415,7 @@
         <v>169</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I62" s="2">
         <v>40.559510000000003</v>
@@ -5423,7 +5433,7 @@
         <v>171</v>
       </c>
       <c r="N62" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O62" s="15" t="s">
         <v>38</v>
@@ -5432,12 +5442,12 @@
         <v>38</v>
       </c>
       <c r="Q62" s="28" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="42">
       <c r="A63" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>192</v>
@@ -5476,21 +5486,21 @@
         <v>198</v>
       </c>
       <c r="N63" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O63" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P63" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q63" s="28" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="66">
       <c r="A64" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>192</v>
@@ -5508,10 +5518,10 @@
         <v>73</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I64" s="2">
         <v>0</v>
@@ -5529,7 +5539,7 @@
         <v>199</v>
       </c>
       <c r="N64" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O64" s="15" t="s">
         <v>38</v>
@@ -5538,12 +5548,12 @@
         <v>337</v>
       </c>
       <c r="Q64" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="43">
       <c r="A65" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>192</v>
@@ -5564,7 +5574,7 @@
         <v>169</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I65" s="2">
         <v>40.427699869999998</v>
@@ -5576,27 +5586,27 @@
         <v>135</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M65" s="2" t="s">
         <v>193</v>
       </c>
       <c r="N65" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O65" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P65" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q65" s="28" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="43">
       <c r="A66" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>192</v>
@@ -5635,21 +5645,21 @@
         <v>194</v>
       </c>
       <c r="N66" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O66" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P66" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q66" s="28" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="43">
       <c r="A67" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>192</v>
@@ -5682,33 +5692,33 @@
         <v>135</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M67" s="26" t="s">
         <v>191</v>
       </c>
       <c r="N67" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O67" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P67" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q67" s="28" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="22">
       <c r="A68" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>4</v>
@@ -5723,7 +5733,7 @@
         <v>169</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I68" s="2">
         <v>0</v>
@@ -5735,27 +5745,27 @@
         <v>38</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M68" s="26" t="s">
         <v>190</v>
       </c>
       <c r="N68" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O68" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P68" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q68" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="43">
       <c r="A69" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>266</v>
@@ -5776,7 +5786,7 @@
         <v>267</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
@@ -5784,22 +5794,22 @@
         <v>270</v>
       </c>
       <c r="L69" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M69" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="M69" s="2" t="s">
-        <v>356</v>
-      </c>
       <c r="N69" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="O69" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P69" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q69" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="43">
@@ -5810,7 +5820,7 @@
         <v>178</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>4</v>
@@ -5852,7 +5862,7 @@
         <v>337</v>
       </c>
       <c r="Q70" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="43">
@@ -5863,7 +5873,7 @@
         <v>178</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>4</v>
@@ -5905,7 +5915,7 @@
         <v>337</v>
       </c>
       <c r="Q71" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="43">
@@ -5958,7 +5968,7 @@
         <v>337</v>
       </c>
       <c r="Q72" s="28" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="73" spans="1:17" ht="22">
@@ -6011,7 +6021,7 @@
         <v>337</v>
       </c>
       <c r="Q73" s="28" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="64">
@@ -6034,7 +6044,7 @@
         <v>41</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>263</v>
@@ -6049,7 +6059,7 @@
         <v>207</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M74" s="24" t="s">
         <v>208</v>
@@ -6064,7 +6074,7 @@
         <v>337</v>
       </c>
       <c r="Q74" s="28" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="85">
@@ -6090,7 +6100,7 @@
         <v>211</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I75" s="2">
         <v>38.875816034503501</v>
@@ -6102,7 +6112,7 @@
         <v>212</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M75" s="24" t="s">
         <v>213</v>
@@ -6117,7 +6127,7 @@
         <v>337</v>
       </c>
       <c r="Q75" s="28" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="85">
@@ -6143,7 +6153,7 @@
         <v>211</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I76" s="2">
         <v>38.875816034503501</v>
@@ -6155,7 +6165,7 @@
         <v>212</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M76" s="2" t="s">
         <v>213</v>
@@ -6170,7 +6180,7 @@
         <v>337</v>
       </c>
       <c r="Q76" s="28" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="77" spans="1:17" ht="44">
@@ -6196,7 +6206,7 @@
         <v>217</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I77" s="2">
         <v>38.873610192974397</v>
@@ -6217,13 +6227,13 @@
         <v>274</v>
       </c>
       <c r="O77" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P77" s="23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q77" s="28" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="78" spans="1:17" ht="66">
@@ -6234,7 +6244,7 @@
         <v>180</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>4</v>
@@ -6261,7 +6271,7 @@
         <v>222</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M78" s="24" t="s">
         <v>223</v>
@@ -6276,7 +6286,7 @@
         <v>337</v>
       </c>
       <c r="Q78" s="28" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="79" spans="1:17" ht="85">
@@ -6287,7 +6297,7 @@
         <v>180</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>4</v>
@@ -6302,7 +6312,7 @@
         <v>234</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I79" s="2">
         <v>38.774379099999997</v>
@@ -6314,7 +6324,7 @@
         <v>14</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M79" s="26" t="s">
         <v>235</v>
@@ -6329,7 +6339,7 @@
         <v>337</v>
       </c>
       <c r="Q79" s="28" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="66">
@@ -6355,7 +6365,7 @@
         <v>60</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I80" s="2">
         <v>0</v>
@@ -6367,7 +6377,7 @@
         <v>38</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M80" s="24" t="s">
         <v>340</v>
@@ -6382,7 +6392,7 @@
         <v>38</v>
       </c>
       <c r="Q80" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="44">
@@ -6420,7 +6430,7 @@
         <v>230</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="M81" s="24" t="s">
         <v>231</v>
@@ -6435,7 +6445,7 @@
         <v>38</v>
       </c>
       <c r="Q81" s="28" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="22">
@@ -6446,7 +6456,7 @@
         <v>9</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>4</v>
@@ -6473,7 +6483,7 @@
         <v>227</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M82" s="2" t="s">
         <v>228</v>
@@ -6488,7 +6498,7 @@
         <v>337</v>
       </c>
       <c r="Q82" s="28" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="127">
@@ -6499,7 +6509,7 @@
         <v>181</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>4</v>
@@ -6514,7 +6524,7 @@
         <v>232</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I83" s="2">
         <v>38.854251580169802</v>
@@ -6526,7 +6536,7 @@
         <v>230</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M83" s="24" t="s">
         <v>233</v>
@@ -6541,7 +6551,7 @@
         <v>337</v>
       </c>
       <c r="Q83" s="28" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="64">
@@ -6564,7 +6574,7 @@
         <v>216</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>259</v>
@@ -6594,7 +6604,7 @@
         <v>337</v>
       </c>
       <c r="Q84" s="28" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="64">
@@ -6647,7 +6657,7 @@
         <v>337</v>
       </c>
       <c r="Q85" s="28" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="64">
@@ -6673,7 +6683,7 @@
         <v>242</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I86" s="2">
         <v>38.8553408</v>
@@ -6696,7 +6706,7 @@
       </c>
       <c r="P86" s="28"/>
       <c r="Q86" s="28" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="22">
@@ -6734,7 +6744,7 @@
         <v>222</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M87" s="24" t="s">
         <v>285</v>
@@ -6749,7 +6759,7 @@
         <v>337</v>
       </c>
       <c r="Q87" s="28" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="44">
@@ -6785,7 +6795,7 @@
         <v>302</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M88" s="24" t="s">
         <v>287</v>
@@ -6800,7 +6810,7 @@
         <v>337</v>
       </c>
       <c r="Q88" s="28" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="89" spans="1:17" ht="44">
@@ -6836,7 +6846,7 @@
         <v>230</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M89" s="24" t="s">
         <v>289</v>
@@ -6851,7 +6861,7 @@
         <v>337</v>
       </c>
       <c r="Q89" s="28" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="43">
@@ -6862,7 +6872,7 @@
         <v>266</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>4</v>
@@ -6877,7 +6887,7 @@
         <v>290</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I90" s="2">
         <v>38.869669999999999</v>
@@ -6889,7 +6899,7 @@
         <v>222</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M90" s="24" t="s">
         <v>291</v>
@@ -6904,7 +6914,7 @@
         <v>337</v>
       </c>
       <c r="Q90" s="28" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="22">
@@ -6937,7 +6947,7 @@
       </c>
       <c r="L91" s="2"/>
       <c r="M91" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N91" s="22" t="s">
         <v>274</v>
@@ -6949,7 +6959,7 @@
         <v>337</v>
       </c>
       <c r="Q91" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="44">
@@ -6988,7 +6998,7 @@
       </c>
       <c r="L92" s="28"/>
       <c r="M92" s="24" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="N92" s="29" t="s">
         <v>332</v>
@@ -7000,7 +7010,7 @@
         <v>337</v>
       </c>
       <c r="Q92" s="28" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="43">
@@ -7035,7 +7045,7 @@
         <v>-77.150020760575501</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>297</v>
@@ -7053,7 +7063,7 @@
         <v>337</v>
       </c>
       <c r="Q93" s="28" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="43">
@@ -7076,7 +7086,7 @@
         <v>300</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>306</v>
@@ -7091,7 +7101,7 @@
         <v>38</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M94" s="24" t="s">
         <v>301</v>
@@ -7106,7 +7116,7 @@
         <v>337</v>
       </c>
       <c r="Q94" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="44">
@@ -7145,7 +7155,7 @@
       </c>
       <c r="L95" s="28"/>
       <c r="M95" s="24" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="N95" s="29" t="s">
         <v>332</v>
@@ -7157,7 +7167,7 @@
         <v>337</v>
       </c>
       <c r="Q95" s="28" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="43">
@@ -7192,7 +7202,7 @@
         <v>-77.185820000000007</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>297</v>
@@ -7210,7 +7220,7 @@
         <v>337</v>
       </c>
       <c r="Q96" s="28" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="97" spans="1:17" ht="43">
@@ -7233,7 +7243,7 @@
         <v>300</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>306</v>
@@ -7248,7 +7258,7 @@
         <v>38</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M97" s="24" t="s">
         <v>301</v>
@@ -7263,7 +7273,7 @@
         <v>337</v>
       </c>
       <c r="Q97" s="28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="98" spans="1:17" ht="43">
@@ -7316,7 +7326,7 @@
         <v>337</v>
       </c>
       <c r="Q98" s="28" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="99" spans="1:17" ht="43">
@@ -7327,7 +7337,7 @@
         <v>266</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>4</v>
@@ -7357,7 +7367,7 @@
         <v>112</v>
       </c>
       <c r="M99" s="31" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N99" s="29" t="s">
         <v>273</v>
@@ -7369,7 +7379,7 @@
         <v>337</v>
       </c>
       <c r="Q99" s="28" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="100" spans="1:17" ht="85">
@@ -7380,7 +7390,7 @@
         <v>178</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>4</v>
@@ -7395,7 +7405,7 @@
         <v>108</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I100" s="2">
         <v>39.099651906603597</v>
@@ -7422,7 +7432,7 @@
         <v>337</v>
       </c>
       <c r="Q100" s="28" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="101" spans="1:17" ht="44">
@@ -7475,7 +7485,7 @@
         <v>337</v>
       </c>
       <c r="Q101" s="28" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="102" spans="1:17" ht="43">
@@ -7528,7 +7538,7 @@
         <v>337</v>
       </c>
       <c r="Q102" s="28" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="103" spans="1:17" ht="42">
@@ -7581,7 +7591,7 @@
         <v>337</v>
       </c>
       <c r="Q103" s="28" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="43">
@@ -7634,7 +7644,7 @@
         <v>337</v>
       </c>
       <c r="Q104" s="28" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="105" spans="1:17" ht="22">
@@ -7645,7 +7655,7 @@
         <v>178</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>4</v>
@@ -7654,13 +7664,13 @@
         <v>125</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I105" s="28">
         <v>39.110308750134202</v>
@@ -7672,22 +7682,22 @@
         <v>39</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M105" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N105" s="29" t="s">
         <v>273</v>
       </c>
       <c r="O105" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="P105" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q105" s="28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="106" spans="1:17" ht="43">
@@ -7698,7 +7708,7 @@
         <v>9</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>4</v>
@@ -7707,13 +7717,13 @@
         <v>125</v>
       </c>
       <c r="F106" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="H106" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="I106" s="28">
         <v>39.110308750134202</v>
@@ -7725,22 +7735,22 @@
         <v>39</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M106" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N106" s="29" t="s">
         <v>273</v>
       </c>
       <c r="O106" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="P106" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q106" s="28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="107" spans="1:17" ht="22">
@@ -7751,7 +7761,7 @@
         <v>178</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>4</v>
@@ -7763,10 +7773,10 @@
         <v>216</v>
       </c>
       <c r="G107" s="18" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H107" s="16" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I107" s="28">
         <v>39.113335992329198</v>
@@ -7778,22 +7788,22 @@
         <v>39</v>
       </c>
       <c r="L107" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="M107" s="15" t="s">
         <v>391</v>
-      </c>
-      <c r="M107" s="15" t="s">
-        <v>392</v>
       </c>
       <c r="N107" s="29" t="s">
         <v>273</v>
       </c>
       <c r="O107" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="P107" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q107" s="28" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="108" spans="1:17" ht="22">
@@ -7804,7 +7814,7 @@
         <v>180</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>4</v>
@@ -7816,10 +7826,10 @@
         <v>216</v>
       </c>
       <c r="G108" s="18" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I108" s="28">
         <v>39.113335992329198</v>
@@ -7831,22 +7841,22 @@
         <v>39</v>
       </c>
       <c r="L108" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="M108" s="15" t="s">
         <v>391</v>
-      </c>
-      <c r="M108" s="15" t="s">
-        <v>392</v>
       </c>
       <c r="N108" s="29" t="s">
         <v>273</v>
       </c>
       <c r="O108" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="P108" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q108" s="28" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="109" spans="1:17" ht="43">
@@ -7857,7 +7867,7 @@
         <v>180</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>101</v>
@@ -7869,10 +7879,10 @@
         <v>41</v>
       </c>
       <c r="G109" s="19" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H109" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I109" s="28">
         <v>39.110308750134202</v>
@@ -7884,22 +7894,22 @@
         <v>39</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M109" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N109" s="29" t="s">
         <v>273</v>
       </c>
       <c r="O109" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="P109" s="23" t="s">
         <v>337</v>
       </c>
       <c r="Q109" s="28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="110" spans="1:17" ht="21">
@@ -7945,47 +7955,47 @@
     <hyperlink ref="M37" r:id="rId36" xr:uid="{B6BCA1D7-7506-4CE1-9D15-8D927D6913EA}"/>
     <hyperlink ref="M35" r:id="rId37" xr:uid="{94D3612A-7340-4BE3-ACF9-1758DC167AD4}"/>
     <hyperlink ref="M7" r:id="rId38" xr:uid="{F55E9326-7175-4BF4-B2D8-CD58AF42F319}"/>
-    <hyperlink ref="M32" r:id="rId39" display="https://www.transitionalservices.org/programs/psychiatric-disabilities/transition-age-youth-tay" xr:uid="{2C36D9E7-20CC-C046-8F37-B0335663708B}"/>
-    <hyperlink ref="M31" r:id="rId40" xr:uid="{48F55102-5E5E-4846-931D-3C1345E815F8}"/>
-    <hyperlink ref="M28" r:id="rId41" xr:uid="{71BFCB2C-4C4A-894A-A7E0-CC5793D459A0}"/>
-    <hyperlink ref="M21" r:id="rId42" xr:uid="{8703E5F8-CFAF-3042-854B-EC5BCE22E9E0}"/>
-    <hyperlink ref="M20" r:id="rId43" xr:uid="{33658D4E-C47B-5647-8324-3ECF0F8E5C7F}"/>
-    <hyperlink ref="M18" r:id="rId44" xr:uid="{009FF859-EB8A-6D42-B56A-BBD3AB85EA1D}"/>
-    <hyperlink ref="M15" r:id="rId45" xr:uid="{4785B206-999E-554B-8C21-B6AED74E335C}"/>
-    <hyperlink ref="M8" r:id="rId46" xr:uid="{24323725-30A2-7840-88B2-F022B3E886B0}"/>
-    <hyperlink ref="M6" r:id="rId47" xr:uid="{E005716C-C6A0-E842-8114-F84C86DBBBC0}"/>
-    <hyperlink ref="M101" r:id="rId48" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
-    <hyperlink ref="M102" r:id="rId49" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
-    <hyperlink ref="M103" r:id="rId50" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
-    <hyperlink ref="M104" r:id="rId51" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
-    <hyperlink ref="M99" r:id="rId52" display="https://www.loudoun.gov/1336/Case-Management-Support-Coordination" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
-    <hyperlink ref="M98" r:id="rId53" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
-    <hyperlink ref="M100" r:id="rId54" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
-    <hyperlink ref="M36" r:id="rId55" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
-    <hyperlink ref="M40" r:id="rId56" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
-    <hyperlink ref="M38" r:id="rId57" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
-    <hyperlink ref="M85" r:id="rId58" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
-    <hyperlink ref="M84" r:id="rId59" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
-    <hyperlink ref="M79" r:id="rId60" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
-    <hyperlink ref="M54" r:id="rId61" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
-    <hyperlink ref="M62" r:id="rId62" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
-    <hyperlink ref="M61" r:id="rId63" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
-    <hyperlink ref="M60" r:id="rId64" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
-    <hyperlink ref="M59" r:id="rId65" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
-    <hyperlink ref="M58" r:id="rId66" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
-    <hyperlink ref="M57" r:id="rId67" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
-    <hyperlink ref="M53" r:id="rId68" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{15E0A920-6E95-7B4F-BB11-050D757A5EAB}"/>
-    <hyperlink ref="M51" r:id="rId69" display="https://loudounliteracy.org/" xr:uid="{9999DF84-E493-E44E-A3EE-CC9DCE69FA8F}"/>
-    <hyperlink ref="M50" r:id="rId70" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{F2FBA2B3-8781-C147-9AA1-AEBC03ECB436}"/>
-    <hyperlink ref="M48" r:id="rId71" display="https://biz.loudoun.gov/work-in-loudoun/" xr:uid="{4982EC8B-FAC5-5640-A062-CBB1672F3253}"/>
-    <hyperlink ref="M47" r:id="rId72" xr:uid="{1A4CA1E2-244B-2C40-8A40-EE156D467B01}"/>
-    <hyperlink ref="M46" r:id="rId73" display="https://www.loudoun.gov/1592/Workforce-Resource-Center" xr:uid="{94B820A0-D3F2-4840-9F07-CA5A487E6333}"/>
-    <hyperlink ref="M45" r:id="rId74" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{7D4B8EF6-3883-A141-A8F0-C51B5B0CFCE3}"/>
-    <hyperlink ref="M44" r:id="rId75" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{6ED53666-C4AE-2E40-A60F-93C9F2AF47E8}"/>
-    <hyperlink ref="M52" r:id="rId76" xr:uid="{13FD1025-9919-E14D-A92B-00246A640824}"/>
-    <hyperlink ref="M55" r:id="rId77" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{AC946866-D12C-4141-A0F5-356929FEF69C}"/>
-    <hyperlink ref="M30" r:id="rId78" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{AD08644F-6242-C246-A29F-DBA9063E9589}"/>
-    <hyperlink ref="M27" r:id="rId79" xr:uid="{BA803B63-C457-1646-B625-49C3B0B95A83}"/>
+    <hyperlink ref="M31" r:id="rId39" xr:uid="{48F55102-5E5E-4846-931D-3C1345E815F8}"/>
+    <hyperlink ref="M28" r:id="rId40" xr:uid="{71BFCB2C-4C4A-894A-A7E0-CC5793D459A0}"/>
+    <hyperlink ref="M21" r:id="rId41" xr:uid="{8703E5F8-CFAF-3042-854B-EC5BCE22E9E0}"/>
+    <hyperlink ref="M20" r:id="rId42" xr:uid="{33658D4E-C47B-5647-8324-3ECF0F8E5C7F}"/>
+    <hyperlink ref="M18" r:id="rId43" xr:uid="{009FF859-EB8A-6D42-B56A-BBD3AB85EA1D}"/>
+    <hyperlink ref="M15" r:id="rId44" xr:uid="{4785B206-999E-554B-8C21-B6AED74E335C}"/>
+    <hyperlink ref="M8" r:id="rId45" xr:uid="{24323725-30A2-7840-88B2-F022B3E886B0}"/>
+    <hyperlink ref="M6" r:id="rId46" xr:uid="{E005716C-C6A0-E842-8114-F84C86DBBBC0}"/>
+    <hyperlink ref="M101" r:id="rId47" xr:uid="{4587D793-653C-6948-B395-2B7F7B1203E2}"/>
+    <hyperlink ref="M102" r:id="rId48" xr:uid="{0ABFCA0D-341D-6A49-94F7-25238C73854B}"/>
+    <hyperlink ref="M103" r:id="rId49" xr:uid="{76D68E60-31F6-C64B-A244-7730C39832B1}"/>
+    <hyperlink ref="M104" r:id="rId50" xr:uid="{CB9764A9-BF71-2E49-9BF0-A4576657AB40}"/>
+    <hyperlink ref="M99" r:id="rId51" display="https://www.loudoun.gov/1336/Case-Management-Support-Coordination" xr:uid="{25F3554C-16DF-BE4B-B243-152EE3C2A529}"/>
+    <hyperlink ref="M98" r:id="rId52" display="https://www.loudoun.gov/1414/Outpatient-Services" xr:uid="{447CAC1E-A75E-5848-B47A-6D1D7156A669}"/>
+    <hyperlink ref="M100" r:id="rId53" xr:uid="{81ABF4B4-0CA5-BF4A-B1A4-0C2E211F9160}"/>
+    <hyperlink ref="M36" r:id="rId54" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx" xr:uid="{4ACE48E9-1180-D841-AED2-BDF15849E408}"/>
+    <hyperlink ref="M40" r:id="rId55" xr:uid="{6A2FCF44-C22E-C642-922F-FBA924D4D9DA}"/>
+    <hyperlink ref="M38" r:id="rId56" xr:uid="{4821ADED-A00E-A84D-8338-FFB5CC7B7E4E}"/>
+    <hyperlink ref="M85" r:id="rId57" xr:uid="{D34B23E2-A200-8645-AF72-A1FB0A8AE90A}"/>
+    <hyperlink ref="M84" r:id="rId58" xr:uid="{CE1C6BD0-F22A-344F-B8F9-266889718E81}"/>
+    <hyperlink ref="M79" r:id="rId59" xr:uid="{94B625DB-2829-614A-91AD-EC40FFC65BB0}"/>
+    <hyperlink ref="M54" r:id="rId60" display="https://www.alleghenycounty.us/Human-Services/About/Contact/Allegheny-Link.aspx" xr:uid="{41FCCC97-6662-6943-80B7-A8A41A5A3C77}"/>
+    <hyperlink ref="M62" r:id="rId61" display="https://www.nhco.org/employment-services" xr:uid="{19A6F497-10A9-5541-A8BC-86FC950C765F}"/>
+    <hyperlink ref="M61" r:id="rId62" display="https://hscc-mvpc.org/community-programs/supports-for-success/" xr:uid="{4C106FDA-8119-6E40-A282-BE3A77FC5862}"/>
+    <hyperlink ref="M60" r:id="rId63" display="https://monvalleyinitiative.com/get-help-with/finding-a-job/" xr:uid="{E9230711-773D-B446-8F19-6695E4D6BE0A}"/>
+    <hyperlink ref="M59" r:id="rId64" display="https://www.partner4work.org/programs/transitional-jobs/" xr:uid="{6B264116-70B9-FA4A-AA4F-D233B6122FA0}"/>
+    <hyperlink ref="M58" r:id="rId65" display="https://www.partner4work.org/programs/strive/" xr:uid="{8205B948-2948-E547-88EA-9CED31771E0A}"/>
+    <hyperlink ref="M57" r:id="rId66" xr:uid="{8CFE70AD-05DB-D142-906B-0DC74F52FA2E}"/>
+    <hyperlink ref="M53" r:id="rId67" display="https://www.valleyyouthhouse.org/programs/transitional-housing/bridge2home-host-homes/" xr:uid="{15E0A920-6E95-7B4F-BB11-050D757A5EAB}"/>
+    <hyperlink ref="M51" r:id="rId68" display="https://loudounliteracy.org/" xr:uid="{9999DF84-E493-E44E-A3EE-CC9DCE69FA8F}"/>
+    <hyperlink ref="M50" r:id="rId69" display="https://www.oarnova.org/services/loudoun-county" xr:uid="{F2FBA2B3-8781-C147-9AA1-AEBC03ECB436}"/>
+    <hyperlink ref="M48" r:id="rId70" display="https://biz.loudoun.gov/work-in-loudoun/" xr:uid="{4982EC8B-FAC5-5640-A062-CBB1672F3253}"/>
+    <hyperlink ref="M47" r:id="rId71" xr:uid="{1A4CA1E2-244B-2C40-8A40-EE156D467B01}"/>
+    <hyperlink ref="M46" r:id="rId72" display="https://www.loudoun.gov/1592/Workforce-Resource-Center" xr:uid="{94B820A0-D3F2-4840-9F07-CA5A487E6333}"/>
+    <hyperlink ref="M45" r:id="rId73" display="https://veteransnavigator.org/program/74824/loudoun-county-rapid-re-housing-program" xr:uid="{7D4B8EF6-3883-A141-A8F0-C51B5B0CFCE3}"/>
+    <hyperlink ref="M44" r:id="rId74" display="https://www.vaoxfordhouse.org/contact-us/" xr:uid="{6ED53666-C4AE-2E40-A60F-93C9F2AF47E8}"/>
+    <hyperlink ref="M52" r:id="rId75" xr:uid="{13FD1025-9919-E14D-A92B-00246A640824}"/>
+    <hyperlink ref="M55" r:id="rId76" display="https://www.partner4work.org/learn-and-earn/" xr:uid="{AC946866-D12C-4141-A0F5-356929FEF69C}"/>
+    <hyperlink ref="M30" r:id="rId77" display="https://www.partner4work.org/corporate-internship-program" xr:uid="{AD08644F-6242-C246-A29F-DBA9063E9589}"/>
+    <hyperlink ref="M27" r:id="rId78" xr:uid="{BA803B63-C457-1646-B625-49C3B0B95A83}"/>
+    <hyperlink ref="M32" r:id="rId79" xr:uid="{EEBCC3DB-0700-1D45-8FF4-D665AC97779C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId80"/>

</xml_diff>